<commit_message>
Column added temporary until RedCap project is adjusted
</commit_message>
<xml_diff>
--- a/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
+++ b/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\D\Eigene Projekte\smith\uc-phep\interpolar\R-db2frontend\db2frontend\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\INTERPOLAR\R-db2frontend\db2frontend\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6C755E-62E2-46D4-80C8-476EA3016808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" tabRatio="791" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" tabRatio="791"/>
   </bookViews>
   <sheets>
     <sheet name="frontend_table_description" sheetId="15" r:id="rId1"/>
     <sheet name="Ward_Patients" sheetId="13" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="344">
   <si>
     <t>pat_id</t>
   </si>
@@ -1052,12 +1051,18 @@
   </si>
   <si>
     <t>VALUE_COUNT</t>
+  </si>
+  <si>
+    <t>record_id_42076f</t>
+  </si>
+  <si>
+    <t>ToDo: zu Entfernen wenn aus RC Projekt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1903,11 +1908,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F476"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2100,35 +2105,35 @@
         <v>332</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>332</v>
+        <v>343</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>82</v>
+        <v>332</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>5</v>
+        <v>332</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>332</v>
+        <v>82</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>331</v>
@@ -2139,10 +2144,10 @@
         <v>332</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>194</v>
+        <v>10</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>331</v>
@@ -2153,13 +2158,13 @@
         <v>332</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2167,10 +2172,10 @@
         <v>332</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>335</v>
@@ -2181,13 +2186,13 @@
         <v>332</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>322</v>
+        <v>205</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2195,10 +2200,10 @@
         <v>332</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>331</v>
@@ -2209,10 +2214,10 @@
         <v>332</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>11</v>
+        <v>185</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>90</v>
+        <v>323</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>331</v>
@@ -2223,10 +2228,10 @@
         <v>332</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>331</v>
@@ -2237,13 +2242,13 @@
         <v>332</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2251,13 +2256,13 @@
         <v>332</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>312</v>
+        <v>58</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2265,13 +2270,13 @@
         <v>332</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>59</v>
+        <v>312</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2279,13 +2284,13 @@
         <v>332</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>330</v>
+        <v>59</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2293,13 +2298,13 @@
         <v>332</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>60</v>
+        <v>330</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2307,13 +2312,13 @@
         <v>332</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>329</v>
+        <v>60</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2321,13 +2326,13 @@
         <v>332</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>61</v>
+        <v>329</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2335,13 +2340,13 @@
         <v>332</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -2349,10 +2354,10 @@
         <v>332</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>326</v>
+        <v>74</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>331</v>
@@ -2363,10 +2368,10 @@
         <v>332</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>75</v>
+        <v>326</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>331</v>
@@ -2377,10 +2382,10 @@
         <v>332</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>331</v>
@@ -2391,10 +2396,10 @@
         <v>332</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>331</v>
@@ -2405,10 +2410,10 @@
         <v>332</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>327</v>
+        <v>77</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>331</v>
@@ -2419,10 +2424,10 @@
         <v>332</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>78</v>
+        <v>327</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>331</v>
@@ -2433,13 +2438,13 @@
         <v>332</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2447,13 +2452,13 @@
         <v>332</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>328</v>
+        <v>62</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -2461,13 +2466,13 @@
         <v>332</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>63</v>
+        <v>328</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2475,13 +2480,13 @@
         <v>332</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>188</v>
+        <v>25</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>186</v>
+        <v>63</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2489,38 +2494,38 @@
         <v>332</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>332</v>
+        <v>188</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>332</v>
+        <v>186</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>83</v>
+        <v>332</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>5</v>
+        <v>332</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>332</v>
+        <v>83</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>202</v>
+        <v>5</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2528,13 +2533,13 @@
         <v>332</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2542,10 +2547,10 @@
         <v>332</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>324</v>
+        <v>203</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>331</v>
@@ -2556,10 +2561,10 @@
         <v>332</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>331</v>
@@ -2570,13 +2575,13 @@
         <v>332</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>26</v>
+        <v>185</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>64</v>
+        <v>323</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2584,13 +2589,13 @@
         <v>332</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2598,10 +2603,10 @@
         <v>332</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>331</v>
@@ -2612,10 +2617,10 @@
         <v>332</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>93</v>
+        <v>28</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>331</v>
@@ -2626,10 +2631,10 @@
         <v>332</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>331</v>
@@ -2640,13 +2645,13 @@
         <v>332</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2654,13 +2659,13 @@
         <v>332</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2668,10 +2673,10 @@
         <v>332</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>189</v>
+        <v>31</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>186</v>
+        <v>66</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>331</v>
@@ -2682,35 +2687,35 @@
         <v>332</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>332</v>
+        <v>189</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>332</v>
+        <v>186</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>84</v>
+        <v>332</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>5</v>
+        <v>332</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>332</v>
+        <v>84</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>204</v>
+        <v>5</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>335</v>
@@ -2721,13 +2726,13 @@
         <v>332</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>325</v>
+        <v>200</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2735,10 +2740,10 @@
         <v>332</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>331</v>
@@ -2749,13 +2754,13 @@
         <v>332</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>32</v>
+        <v>185</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>67</v>
+        <v>323</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2763,13 +2768,13 @@
         <v>332</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2777,10 +2782,10 @@
         <v>332</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>331</v>
@@ -2791,10 +2796,10 @@
         <v>332</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>331</v>
@@ -2805,10 +2810,10 @@
         <v>332</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>331</v>
@@ -2819,10 +2824,10 @@
         <v>332</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>331</v>
@@ -2833,10 +2838,10 @@
         <v>332</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>331</v>
@@ -2847,10 +2852,10 @@
         <v>332</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>331</v>
@@ -2861,10 +2866,10 @@
         <v>332</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>331</v>
@@ -2875,10 +2880,10 @@
         <v>332</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>331</v>
@@ -2889,10 +2894,10 @@
         <v>332</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>331</v>
@@ -2903,10 +2908,10 @@
         <v>332</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>316</v>
+        <v>42</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>317</v>
+        <v>103</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>331</v>
@@ -2917,10 +2922,10 @@
         <v>332</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>331</v>
@@ -2931,10 +2936,10 @@
         <v>332</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>43</v>
+        <v>318</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>104</v>
+        <v>319</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>331</v>
@@ -2945,10 +2950,10 @@
         <v>332</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>331</v>
@@ -2959,10 +2964,10 @@
         <v>332</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>309</v>
+        <v>70</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>331</v>
@@ -2973,10 +2978,10 @@
         <v>332</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>331</v>
@@ -2987,10 +2992,10 @@
         <v>332</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>95</v>
+        <v>46</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>105</v>
+        <v>310</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>331</v>
@@ -3001,10 +3006,10 @@
         <v>332</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>207</v>
+        <v>95</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>234</v>
+        <v>105</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>331</v>
@@ -3015,10 +3020,10 @@
         <v>332</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>331</v>
@@ -3029,10 +3034,10 @@
         <v>332</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>331</v>
@@ -3043,10 +3048,10 @@
         <v>332</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>331</v>
@@ -3057,10 +3062,10 @@
         <v>332</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>331</v>
@@ -3071,10 +3076,10 @@
         <v>332</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>331</v>
@@ -3085,10 +3090,10 @@
         <v>332</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>331</v>
@@ -3099,10 +3104,10 @@
         <v>332</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>331</v>
@@ -3113,10 +3118,10 @@
         <v>332</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>331</v>
@@ -3127,10 +3132,10 @@
         <v>332</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>331</v>
@@ -3141,10 +3146,10 @@
         <v>332</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>331</v>
@@ -3155,10 +3160,10 @@
         <v>332</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>331</v>
@@ -3169,10 +3174,10 @@
         <v>332</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>331</v>
@@ -3183,10 +3188,10 @@
         <v>332</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>331</v>
@@ -3197,10 +3202,10 @@
         <v>332</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>331</v>
@@ -3211,10 +3216,10 @@
         <v>332</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>331</v>
@@ -3225,10 +3230,10 @@
         <v>332</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>331</v>
@@ -3239,10 +3244,10 @@
         <v>332</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>331</v>
@@ -3253,10 +3258,10 @@
         <v>332</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>331</v>
@@ -3267,10 +3272,10 @@
         <v>332</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>331</v>
@@ -3281,10 +3286,10 @@
         <v>332</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>331</v>
@@ -3295,10 +3300,10 @@
         <v>332</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>331</v>
@@ -3309,10 +3314,10 @@
         <v>332</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>331</v>
@@ -3323,10 +3328,10 @@
         <v>332</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>331</v>
@@ -3337,10 +3342,10 @@
         <v>332</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>331</v>
@@ -3351,10 +3356,10 @@
         <v>332</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>331</v>
@@ -3365,10 +3370,10 @@
         <v>332</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>331</v>
@@ -3379,10 +3384,10 @@
         <v>332</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>47</v>
+        <v>233</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>107</v>
+        <v>260</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>331</v>
@@ -3393,10 +3398,10 @@
         <v>332</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>261</v>
+        <v>47</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>266</v>
+        <v>107</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>331</v>
@@ -3407,10 +3412,10 @@
         <v>332</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>331</v>
@@ -3421,10 +3426,10 @@
         <v>332</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>331</v>
@@ -3435,10 +3440,10 @@
         <v>332</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>331</v>
@@ -3449,10 +3454,10 @@
         <v>332</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>331</v>
@@ -3463,10 +3468,10 @@
         <v>332</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>48</v>
+        <v>265</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>71</v>
+        <v>270</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>331</v>
@@ -3477,10 +3482,10 @@
         <v>332</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>331</v>
@@ -3491,10 +3496,10 @@
         <v>332</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>271</v>
+        <v>72</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>331</v>
@@ -3505,10 +3510,10 @@
         <v>332</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>273</v>
+        <v>50</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>331</v>
@@ -3519,10 +3524,10 @@
         <v>332</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>331</v>
@@ -3533,10 +3538,10 @@
         <v>332</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>331</v>
@@ -3547,10 +3552,10 @@
         <v>332</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>331</v>
@@ -3561,10 +3566,10 @@
         <v>332</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>331</v>
@@ -3575,10 +3580,10 @@
         <v>332</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>331</v>
@@ -3589,10 +3594,10 @@
         <v>332</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>331</v>
@@ -3603,10 +3608,10 @@
         <v>332</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>331</v>
@@ -3617,10 +3622,10 @@
         <v>332</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>331</v>
@@ -3631,10 +3636,10 @@
         <v>332</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>331</v>
@@ -3645,10 +3650,10 @@
         <v>332</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>51</v>
+        <v>282</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>331</v>
@@ -3659,10 +3664,10 @@
         <v>332</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>293</v>
+        <v>51</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>301</v>
+        <v>272</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>331</v>
@@ -3673,10 +3678,10 @@
         <v>332</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>331</v>
@@ -3687,10 +3692,10 @@
         <v>332</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>331</v>
@@ -3701,10 +3706,10 @@
         <v>332</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>331</v>
@@ -3715,10 +3720,10 @@
         <v>332</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>331</v>
@@ -3729,10 +3734,10 @@
         <v>332</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>331</v>
@@ -3743,10 +3748,10 @@
         <v>332</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>331</v>
@@ -3757,10 +3762,10 @@
         <v>332</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>331</v>
@@ -3771,10 +3776,10 @@
         <v>332</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>52</v>
+        <v>300</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>73</v>
+        <v>308</v>
       </c>
       <c r="D133" s="2" t="s">
         <v>331</v>
@@ -3785,10 +3790,10 @@
         <v>332</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>331</v>
@@ -3799,10 +3804,10 @@
         <v>332</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>106</v>
+        <v>53</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>331</v>
@@ -3813,10 +3818,10 @@
         <v>332</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>331</v>
@@ -3827,10 +3832,10 @@
         <v>332</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>190</v>
+        <v>54</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>186</v>
+        <v>110</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>331</v>
@@ -3841,38 +3846,38 @@
         <v>332</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>332</v>
+        <v>190</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>332</v>
+        <v>186</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>111</v>
+        <v>332</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>5</v>
+        <v>332</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D139" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>332</v>
+        <v>111</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>192</v>
+        <v>5</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -3880,13 +3885,13 @@
         <v>332</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>112</v>
+        <v>192</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>125</v>
+        <v>199</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -3894,10 +3899,10 @@
         <v>332</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>331</v>
@@ -3908,10 +3913,10 @@
         <v>332</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>331</v>
@@ -3922,10 +3927,10 @@
         <v>332</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>331</v>
@@ -3936,10 +3941,10 @@
         <v>332</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D145" s="2" t="s">
         <v>331</v>
@@ -3950,10 +3955,10 @@
         <v>332</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D146" s="2" t="s">
         <v>331</v>
@@ -3964,10 +3969,10 @@
         <v>332</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>331</v>
@@ -3978,10 +3983,10 @@
         <v>332</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>331</v>
@@ -3992,10 +3997,10 @@
         <v>332</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>331</v>
@@ -4006,10 +4011,10 @@
         <v>332</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>331</v>
@@ -4020,10 +4025,10 @@
         <v>332</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>331</v>
@@ -4034,10 +4039,10 @@
         <v>332</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D152" s="2" t="s">
         <v>331</v>
@@ -4048,10 +4053,10 @@
         <v>332</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>331</v>
@@ -4062,10 +4067,10 @@
         <v>332</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D154" s="2" t="s">
         <v>331</v>
@@ -4076,10 +4081,10 @@
         <v>332</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>191</v>
+        <v>138</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>186</v>
+        <v>139</v>
       </c>
       <c r="D155" s="2" t="s">
         <v>331</v>
@@ -4090,38 +4095,38 @@
         <v>332</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>332</v>
+        <v>191</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>332</v>
+        <v>186</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>140</v>
+        <v>332</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>192</v>
+        <v>332</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="D157" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>332</v>
+        <v>140</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>5</v>
+        <v>192</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -4129,10 +4134,10 @@
         <v>332</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>141</v>
+        <v>5</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>313</v>
+        <v>198</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>331</v>
@@ -4143,10 +4148,10 @@
         <v>332</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>149</v>
+        <v>313</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>331</v>
@@ -4157,10 +4162,10 @@
         <v>332</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>331</v>
@@ -4171,10 +4176,10 @@
         <v>332</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>331</v>
@@ -4185,10 +4190,10 @@
         <v>332</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D163" s="2" t="s">
         <v>331</v>
@@ -4199,10 +4204,10 @@
         <v>332</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>331</v>
@@ -4213,10 +4218,10 @@
         <v>332</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>331</v>
@@ -4227,10 +4232,10 @@
         <v>332</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>331</v>
@@ -4241,10 +4246,10 @@
         <v>332</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>331</v>
@@ -4255,10 +4260,10 @@
         <v>332</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>331</v>
@@ -4269,10 +4274,10 @@
         <v>332</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>331</v>
@@ -4283,10 +4288,10 @@
         <v>332</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>331</v>
@@ -4297,10 +4302,10 @@
         <v>332</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>331</v>
@@ -4311,10 +4316,10 @@
         <v>332</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>331</v>
@@ -4325,10 +4330,10 @@
         <v>332</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>331</v>
@@ -4339,10 +4344,10 @@
         <v>332</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>331</v>
@@ -4353,10 +4358,10 @@
         <v>332</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D175" s="2" t="s">
         <v>331</v>
@@ -4367,10 +4372,10 @@
         <v>332</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>331</v>
@@ -4381,10 +4386,10 @@
         <v>332</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D177" s="2" t="s">
         <v>331</v>
@@ -4395,10 +4400,10 @@
         <v>332</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>331</v>
@@ -4409,10 +4414,10 @@
         <v>332</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D179" s="2" t="s">
         <v>331</v>
@@ -4423,10 +4428,10 @@
         <v>332</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D180" s="2" t="s">
         <v>331</v>
@@ -4437,12 +4442,26 @@
         <v>332</v>
       </c>
       <c r="B181" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D181" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B182" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C181" s="2" t="s">
+      <c r="C182" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D181" s="2" t="s">
+      <c r="D182" s="2" t="s">
         <v>331</v>
       </c>
     </row>
@@ -4455,7 +4474,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Fix empty row frontend tables
</commit_message>
<xml_diff>
--- a/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
+++ b/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
@@ -1368,10 +1368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F476"/>
+  <dimension ref="A1:F475"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1641,672 +1641,654 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A15)&gt;0,[1]table_des_RedCap!A15,"")</f>
-        <v/>
+        <f>IF(LEN([1]table_des_RedCap!A16)&gt;0,[1]table_des_RedCap!A16,"")</f>
+        <v>fall</v>
       </c>
       <c r="B15" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B15)&gt;0,[1]table_des_RedCap!B15,"")</f>
-        <v/>
+        <f>IF(LEN([1]table_des_RedCap!B16)&gt;0,[1]table_des_RedCap!B16,"")</f>
+        <v>record_id</v>
       </c>
       <c r="C15" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B15)&gt;0,[1]table_des_RedCap!C15,"")</f>
-        <v/>
+        <f>IF(LEN([1]table_des_RedCap!B16)&gt;0,[1]table_des_RedCap!C16,"")</f>
+        <v>Record ID RedCap - besetzt/vorgegeben mit Datenbankinternen ID des Patienten - wird im Redcap in allen Instanzen  des Patienten verwendet</v>
       </c>
       <c r="D15" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F15)&gt;0,IF([1]table_des_RedCap!F15="date_ymd","date",IF([1]table_des_RedCap!F15="number","double precision",IF([1]table_des_RedCap!F15="integer","int",IF([1]table_des_RedCap!F15="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <f>IF(LEN([1]table_des_RedCap!F16)&gt;0,IF([1]table_des_RedCap!F16="date_ymd","date",IF([1]table_des_RedCap!F16="number","double precision",IF([1]table_des_RedCap!F16="integer","int",IF([1]table_des_RedCap!F16="autocomplete","varchar","-- setzen --")))),"varchar")</f>
         <v>varchar</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A16)&gt;0,[1]table_des_RedCap!A16,"")</f>
-        <v>fall</v>
+        <f>IF(LEN([1]table_des_RedCap!A17)&gt;0,[1]table_des_RedCap!A17,"")</f>
+        <v/>
       </c>
       <c r="B16" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B16)&gt;0,[1]table_des_RedCap!B16,"")</f>
-        <v>record_id</v>
+        <f>IF(LEN([1]table_des_RedCap!B17)&gt;0,[1]table_des_RedCap!B17,"")</f>
+        <v>fall_header</v>
       </c>
       <c r="C16" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B16)&gt;0,[1]table_des_RedCap!C16,"")</f>
-        <v>Record ID RedCap - besetzt/vorgegeben mit Datenbankinternen ID des Patienten - wird im Redcap in allen Instanzen  des Patienten verwendet</v>
+        <f>IF(LEN([1]table_des_RedCap!B17)&gt;0,[1]table_des_RedCap!C17,"")</f>
+        <v>descriptive item only for frontend</v>
       </c>
       <c r="D16" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F16)&gt;0,IF([1]table_des_RedCap!F16="date_ymd","date",IF([1]table_des_RedCap!F16="number","double precision",IF([1]table_des_RedCap!F16="integer","int",IF([1]table_des_RedCap!F16="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <f>IF(LEN([1]table_des_RedCap!F17)&gt;0,IF([1]table_des_RedCap!F17="date_ymd","date",IF([1]table_des_RedCap!F17="number","double precision",IF([1]table_des_RedCap!F17="integer","int",IF([1]table_des_RedCap!F17="autocomplete","varchar","-- setzen --")))),"varchar")</f>
         <v>varchar</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A17)&gt;0,[1]table_des_RedCap!A17,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A18)&gt;0,[1]table_des_RedCap!A18,"")</f>
         <v/>
       </c>
       <c r="B17" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B17)&gt;0,[1]table_des_RedCap!B17,"")</f>
-        <v>fall_header</v>
+        <f>IF(LEN([1]table_des_RedCap!B18)&gt;0,[1]table_des_RedCap!B18,"")</f>
+        <v>fall_id</v>
       </c>
       <c r="C17" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B17)&gt;0,[1]table_des_RedCap!C17,"")</f>
-        <v>descriptive item only for frontend</v>
+        <f>IF(LEN([1]table_des_RedCap!B18)&gt;0,[1]table_des_RedCap!C18,"")</f>
+        <v>Fall-ID RedCap FHIR Daten</v>
       </c>
       <c r="D17" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F17)&gt;0,IF([1]table_des_RedCap!F17="date_ymd","date",IF([1]table_des_RedCap!F17="number","double precision",IF([1]table_des_RedCap!F17="integer","int",IF([1]table_des_RedCap!F17="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <f>IF(LEN([1]table_des_RedCap!F18)&gt;0,IF([1]table_des_RedCap!F18="date_ymd","date",IF([1]table_des_RedCap!F18="number","double precision",IF([1]table_des_RedCap!F18="integer","int",IF([1]table_des_RedCap!F18="autocomplete","varchar","-- setzen --")))),"varchar")</f>
         <v>varchar</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A18)&gt;0,[1]table_des_RedCap!A18,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A19)&gt;0,[1]table_des_RedCap!A19,"")</f>
         <v/>
       </c>
       <c r="B18" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B18)&gt;0,[1]table_des_RedCap!B18,"")</f>
-        <v>fall_id</v>
+        <f>IF(LEN([1]table_des_RedCap!B19)&gt;0,[1]table_des_RedCap!B19,"")</f>
+        <v>fall_pat_id</v>
       </c>
       <c r="C18" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B18)&gt;0,[1]table_des_RedCap!C18,"")</f>
-        <v>Fall-ID RedCap FHIR Daten</v>
+        <f>IF(LEN([1]table_des_RedCap!B19)&gt;0,[1]table_des_RedCap!C19,"")</f>
+        <v>Patienten-ID zu dem Fall gehört (FHIR Patient:pat_id)</v>
       </c>
       <c r="D18" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F18)&gt;0,IF([1]table_des_RedCap!F18="date_ymd","date",IF([1]table_des_RedCap!F18="number","double precision",IF([1]table_des_RedCap!F18="integer","int",IF([1]table_des_RedCap!F18="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <f>IF(LEN([1]table_des_RedCap!F19)&gt;0,IF([1]table_des_RedCap!F19="date_ymd","date",IF([1]table_des_RedCap!F19="number","double precision",IF([1]table_des_RedCap!F19="integer","int",IF([1]table_des_RedCap!F19="autocomplete","varchar","-- setzen --")))),"varchar")</f>
         <v>varchar</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A19)&gt;0,[1]table_des_RedCap!A19,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A20)&gt;0,[1]table_des_RedCap!A20,"")</f>
         <v/>
       </c>
       <c r="B19" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B19)&gt;0,[1]table_des_RedCap!B19,"")</f>
-        <v>fall_pat_id</v>
+        <f>IF(LEN([1]table_des_RedCap!B20)&gt;0,[1]table_des_RedCap!B20,"")</f>
+        <v>patient_id_fk</v>
       </c>
       <c r="C19" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B19)&gt;0,[1]table_des_RedCap!C19,"")</f>
-        <v>Patienten-ID zu dem Fall gehört (FHIR Patient:pat_id)</v>
+        <f>IF(LEN([1]table_des_RedCap!B20)&gt;0,[1]table_des_RedCap!C20,"")</f>
+        <v>Datenbank-FK des Patienten (Patient: patient_fe_id=Patient.record_id)</v>
       </c>
       <c r="D19" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F19)&gt;0,IF([1]table_des_RedCap!F19="date_ymd","date",IF([1]table_des_RedCap!F19="number","double precision",IF([1]table_des_RedCap!F19="integer","int",IF([1]table_des_RedCap!F19="autocomplete","varchar","-- setzen --")))),"varchar")</f>
-        <v>varchar</v>
+        <f>IF(LEN([1]table_des_RedCap!F20)&gt;0,IF([1]table_des_RedCap!F20="date_ymd","date",IF([1]table_des_RedCap!F20="number","double precision",IF([1]table_des_RedCap!F20="integer","int",IF([1]table_des_RedCap!F20="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <v>int</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A20)&gt;0,[1]table_des_RedCap!A20,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A21)&gt;0,[1]table_des_RedCap!A21,"")</f>
         <v/>
       </c>
       <c r="B20" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B20)&gt;0,[1]table_des_RedCap!B20,"")</f>
-        <v>patient_id_fk</v>
+        <f>IF(LEN([1]table_des_RedCap!B21)&gt;0,[1]table_des_RedCap!B21,"")</f>
+        <v>fall_fe_id</v>
       </c>
       <c r="C20" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B20)&gt;0,[1]table_des_RedCap!C20,"")</f>
-        <v>Datenbank-FK des Patienten (Patient: patient_fe_id=Patient.record_id)</v>
+        <f>IF(LEN([1]table_des_RedCap!B21)&gt;0,[1]table_des_RedCap!C21,"")</f>
+        <v>Datenbank-FK des getypten Falls zur Datenflussverfolgung (Fall: v_fall_all . fall_id)</v>
       </c>
       <c r="D20" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F20)&gt;0,IF([1]table_des_RedCap!F20="date_ymd","date",IF([1]table_des_RedCap!F20="number","double precision",IF([1]table_des_RedCap!F20="integer","int",IF([1]table_des_RedCap!F20="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <f>IF(LEN([1]table_des_RedCap!F21)&gt;0,IF([1]table_des_RedCap!F21="date_ymd","date",IF([1]table_des_RedCap!F21="number","double precision",IF([1]table_des_RedCap!F21="integer","int",IF([1]table_des_RedCap!F21="autocomplete","varchar","-- setzen --")))),"varchar")</f>
         <v>int</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A21)&gt;0,[1]table_des_RedCap!A21,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A22)&gt;0,[1]table_des_RedCap!A22,"")</f>
         <v/>
       </c>
       <c r="B21" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B21)&gt;0,[1]table_des_RedCap!B21,"")</f>
-        <v>fall_fe_id</v>
+        <f>IF(LEN([1]table_des_RedCap!B22)&gt;0,[1]table_des_RedCap!B22,"")</f>
+        <v>fall_femb</v>
       </c>
       <c r="C21" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B21)&gt;0,[1]table_des_RedCap!C21,"")</f>
-        <v>Datenbank-FK des getypten Falls zur Datenflussverfolgung (Fall: v_fall_all . fall_id)</v>
+        <f>IF(LEN([1]table_des_RedCap!B22)&gt;0,[1]table_des_RedCap!C22,"")</f>
+        <v>descriptive item only for frontend</v>
       </c>
       <c r="D21" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F21)&gt;0,IF([1]table_des_RedCap!F21="date_ymd","date",IF([1]table_des_RedCap!F21="number","double precision",IF([1]table_des_RedCap!F21="integer","int",IF([1]table_des_RedCap!F21="autocomplete","varchar","-- setzen --")))),"varchar")</f>
-        <v>int</v>
+        <f>IF(LEN([1]table_des_RedCap!F22)&gt;0,IF([1]table_des_RedCap!F22="date_ymd","date",IF([1]table_des_RedCap!F22="number","double precision",IF([1]table_des_RedCap!F22="integer","int",IF([1]table_des_RedCap!F22="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <v>varchar</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A22)&gt;0,[1]table_des_RedCap!A22,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A23)&gt;0,[1]table_des_RedCap!A23,"")</f>
         <v/>
       </c>
       <c r="B22" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B22)&gt;0,[1]table_des_RedCap!B22,"")</f>
-        <v>fall_femb</v>
+        <f>IF(LEN([1]table_des_RedCap!B23)&gt;0,[1]table_des_RedCap!B23,"")</f>
+        <v>redcap_repeat_instrument</v>
       </c>
       <c r="C22" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B22)&gt;0,[1]table_des_RedCap!C22,"")</f>
-        <v>descriptive item only for frontend</v>
+        <f>IF(LEN([1]table_des_RedCap!B23)&gt;0,[1]table_des_RedCap!C23,"")</f>
+        <v>Frontend interne Datensatzverwaltung - Instrument :   fall</v>
       </c>
       <c r="D22" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F22)&gt;0,IF([1]table_des_RedCap!F22="date_ymd","date",IF([1]table_des_RedCap!F22="number","double precision",IF([1]table_des_RedCap!F22="integer","int",IF([1]table_des_RedCap!F22="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <f>IF(LEN([1]table_des_RedCap!F23)&gt;0,IF([1]table_des_RedCap!F23="date_ymd","date",IF([1]table_des_RedCap!F23="number","double precision",IF([1]table_des_RedCap!F23="integer","int",IF([1]table_des_RedCap!F23="autocomplete","varchar","-- setzen --")))),"varchar")</f>
         <v>varchar</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A23)&gt;0,[1]table_des_RedCap!A23,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A24)&gt;0,[1]table_des_RedCap!A24,"")</f>
         <v/>
       </c>
       <c r="B23" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B23)&gt;0,[1]table_des_RedCap!B23,"")</f>
-        <v>redcap_repeat_instrument</v>
+        <f>IF(LEN([1]table_des_RedCap!B24)&gt;0,[1]table_des_RedCap!B24,"")</f>
+        <v>redcap_repeat_instance</v>
       </c>
       <c r="C23" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B23)&gt;0,[1]table_des_RedCap!C23,"")</f>
-        <v>Frontend interne Datensatzverwaltung - Instrument :   fall</v>
+        <f>IF(LEN([1]table_des_RedCap!B24)&gt;0,[1]table_des_RedCap!C24,"")</f>
+        <v>Frontend interne Datensatzverwaltung - Instanz des Instruments - Numerisch : 1…n</v>
       </c>
       <c r="D23" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F23)&gt;0,IF([1]table_des_RedCap!F23="date_ymd","date",IF([1]table_des_RedCap!F23="number","double precision",IF([1]table_des_RedCap!F23="integer","int",IF([1]table_des_RedCap!F23="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <f>IF(LEN([1]table_des_RedCap!F24)&gt;0,IF([1]table_des_RedCap!F24="date_ymd","date",IF([1]table_des_RedCap!F24="number","double precision",IF([1]table_des_RedCap!F24="integer","int",IF([1]table_des_RedCap!F24="autocomplete","varchar","-- setzen --")))),"varchar")</f>
         <v>varchar</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A24)&gt;0,[1]table_des_RedCap!A24,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A25)&gt;0,[1]table_des_RedCap!A25,"")</f>
         <v/>
       </c>
       <c r="B24" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B24)&gt;0,[1]table_des_RedCap!B24,"")</f>
-        <v>redcap_repeat_instance</v>
+        <f>IF(LEN([1]table_des_RedCap!B25)&gt;0,[1]table_des_RedCap!B25,"")</f>
+        <v>fall_studienphase</v>
       </c>
       <c r="C24" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B24)&gt;0,[1]table_des_RedCap!C24,"")</f>
-        <v>Frontend interne Datensatzverwaltung - Instanz des Instruments - Numerisch : 1…n</v>
+        <f>IF(LEN([1]table_des_RedCap!B25)&gt;0,[1]table_des_RedCap!C25,"")</f>
+        <v>Alt: (1, Usual Care (UC) | 2, Interventional Care (IC) | 3, Pilotphase (P) )</v>
       </c>
       <c r="D24" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F24)&gt;0,IF([1]table_des_RedCap!F24="date_ymd","date",IF([1]table_des_RedCap!F24="number","double precision",IF([1]table_des_RedCap!F24="integer","int",IF([1]table_des_RedCap!F24="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <f>IF(LEN([1]table_des_RedCap!F25)&gt;0,IF([1]table_des_RedCap!F25="date_ymd","date",IF([1]table_des_RedCap!F25="number","double precision",IF([1]table_des_RedCap!F25="integer","int",IF([1]table_des_RedCap!F25="autocomplete","varchar","-- setzen --")))),"varchar")</f>
         <v>varchar</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A25)&gt;0,[1]table_des_RedCap!A25,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A26)&gt;0,[1]table_des_RedCap!A26,"")</f>
         <v/>
       </c>
       <c r="B25" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B25)&gt;0,[1]table_des_RedCap!B25,"")</f>
-        <v>fall_studienphase</v>
+        <f>IF(LEN([1]table_des_RedCap!B26)&gt;0,[1]table_des_RedCap!B26,"")</f>
+        <v>fall_station</v>
       </c>
       <c r="C25" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B25)&gt;0,[1]table_des_RedCap!C25,"")</f>
-        <v>Alt: (1, Usual Care (UC) | 2, Interventional Care (IC) | 3, Pilotphase (P) )</v>
+        <f>IF(LEN([1]table_des_RedCap!B26)&gt;0,[1]table_des_RedCap!C26,"")</f>
+        <v>Station wie vom DIZ Definiert</v>
       </c>
       <c r="D25" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F25)&gt;0,IF([1]table_des_RedCap!F25="date_ymd","date",IF([1]table_des_RedCap!F25="number","double precision",IF([1]table_des_RedCap!F25="integer","int",IF([1]table_des_RedCap!F25="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <f>IF(LEN([1]table_des_RedCap!F26)&gt;0,IF([1]table_des_RedCap!F26="date_ymd","date",IF([1]table_des_RedCap!F26="number","double precision",IF([1]table_des_RedCap!F26="integer","int",IF([1]table_des_RedCap!F26="autocomplete","varchar","-- setzen --")))),"varchar")</f>
         <v>varchar</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A26)&gt;0,[1]table_des_RedCap!A26,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A27)&gt;0,[1]table_des_RedCap!A27,"")</f>
         <v/>
       </c>
       <c r="B26" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B26)&gt;0,[1]table_des_RedCap!B26,"")</f>
-        <v>fall_station</v>
+        <f>IF(LEN([1]table_des_RedCap!B27)&gt;0,[1]table_des_RedCap!B27,"")</f>
+        <v>fall_aufn_dat</v>
       </c>
       <c r="C26" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B26)&gt;0,[1]table_des_RedCap!C26,"")</f>
-        <v>Station wie vom DIZ Definiert</v>
+        <f>IF(LEN([1]table_des_RedCap!B27)&gt;0,[1]table_des_RedCap!C27,"")</f>
+        <v>Aufnahmedatum</v>
       </c>
       <c r="D26" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F26)&gt;0,IF([1]table_des_RedCap!F26="date_ymd","date",IF([1]table_des_RedCap!F26="number","double precision",IF([1]table_des_RedCap!F26="integer","int",IF([1]table_des_RedCap!F26="autocomplete","varchar","-- setzen --")))),"varchar")</f>
-        <v>varchar</v>
+        <f>IF(LEN([1]table_des_RedCap!F27)&gt;0,IF([1]table_des_RedCap!F27="date_ymd","date",IF([1]table_des_RedCap!F27="number","double precision",IF([1]table_des_RedCap!F27="integer","int",IF([1]table_des_RedCap!F27="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <v>date</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A27)&gt;0,[1]table_des_RedCap!A27,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A28)&gt;0,[1]table_des_RedCap!A28,"")</f>
         <v/>
       </c>
       <c r="B27" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B27)&gt;0,[1]table_des_RedCap!B27,"")</f>
-        <v>fall_aufn_dat</v>
+        <f>IF(LEN([1]table_des_RedCap!B28)&gt;0,[1]table_des_RedCap!B28,"")</f>
+        <v>fall_aufn_diag</v>
       </c>
       <c r="C27" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B27)&gt;0,[1]table_des_RedCap!C27,"")</f>
-        <v>Aufnahmedatum</v>
+        <f>IF(LEN([1]table_des_RedCap!B28)&gt;0,[1]table_des_RedCap!C28,"")</f>
+        <v>Diagnose(n) bei Aufnahme (wird nur zum lesen sein</v>
       </c>
       <c r="D27" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F27)&gt;0,IF([1]table_des_RedCap!F27="date_ymd","date",IF([1]table_des_RedCap!F27="number","double precision",IF([1]table_des_RedCap!F27="integer","int",IF([1]table_des_RedCap!F27="autocomplete","varchar","-- setzen --")))),"varchar")</f>
-        <v>date</v>
+        <f>IF(LEN([1]table_des_RedCap!F28)&gt;0,IF([1]table_des_RedCap!F28="date_ymd","date",IF([1]table_des_RedCap!F28="number","double precision",IF([1]table_des_RedCap!F28="integer","int",IF([1]table_des_RedCap!F28="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <v>varchar</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A28)&gt;0,[1]table_des_RedCap!A28,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A29)&gt;0,[1]table_des_RedCap!A29,"")</f>
         <v/>
       </c>
       <c r="B28" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B28)&gt;0,[1]table_des_RedCap!B28,"")</f>
-        <v>fall_aufn_diag</v>
+        <f>IF(LEN([1]table_des_RedCap!B29)&gt;0,[1]table_des_RedCap!B29,"")</f>
+        <v>fall_gewicht_aktuell</v>
       </c>
       <c r="C28" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B28)&gt;0,[1]table_des_RedCap!C28,"")</f>
-        <v>Diagnose(n) bei Aufnahme (wird nur zum lesen sein</v>
+        <f>IF(LEN([1]table_des_RedCap!B29)&gt;0,[1]table_des_RedCap!C29,"")</f>
+        <v>aktuelles Gewicht (Kg)</v>
       </c>
       <c r="D28" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F28)&gt;0,IF([1]table_des_RedCap!F28="date_ymd","date",IF([1]table_des_RedCap!F28="number","double precision",IF([1]table_des_RedCap!F28="integer","int",IF([1]table_des_RedCap!F28="autocomplete","varchar","-- setzen --")))),"varchar")</f>
-        <v>varchar</v>
+        <f>IF(LEN([1]table_des_RedCap!F29)&gt;0,IF([1]table_des_RedCap!F29="date_ymd","date",IF([1]table_des_RedCap!F29="number","double precision",IF([1]table_des_RedCap!F29="integer","int",IF([1]table_des_RedCap!F29="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <v>double precision</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A29)&gt;0,[1]table_des_RedCap!A29,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A30)&gt;0,[1]table_des_RedCap!A30,"")</f>
         <v/>
       </c>
       <c r="B29" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B29)&gt;0,[1]table_des_RedCap!B29,"")</f>
-        <v>fall_gewicht_aktuell</v>
+        <f>IF(LEN([1]table_des_RedCap!B30)&gt;0,[1]table_des_RedCap!B30,"")</f>
+        <v>fall_gewicht_aktl_einheit</v>
       </c>
       <c r="C29" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B29)&gt;0,[1]table_des_RedCap!C29,"")</f>
-        <v>aktuelles Gewicht (Kg)</v>
+        <f>IF(LEN([1]table_des_RedCap!B30)&gt;0,[1]table_des_RedCap!C30,"")</f>
+        <v>Einheit des Gewichts</v>
       </c>
       <c r="D29" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F29)&gt;0,IF([1]table_des_RedCap!F29="date_ymd","date",IF([1]table_des_RedCap!F29="number","double precision",IF([1]table_des_RedCap!F29="integer","int",IF([1]table_des_RedCap!F29="autocomplete","varchar","-- setzen --")))),"varchar")</f>
-        <v>double precision</v>
+        <f>IF(LEN([1]table_des_RedCap!F30)&gt;0,IF([1]table_des_RedCap!F30="date_ymd","date",IF([1]table_des_RedCap!F30="number","double precision",IF([1]table_des_RedCap!F30="integer","int",IF([1]table_des_RedCap!F30="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <v>varchar</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A30)&gt;0,[1]table_des_RedCap!A30,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A31)&gt;0,[1]table_des_RedCap!A31,"")</f>
         <v/>
       </c>
       <c r="B30" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B30)&gt;0,[1]table_des_RedCap!B30,"")</f>
-        <v>fall_gewicht_aktl_einheit</v>
+        <f>IF(LEN([1]table_des_RedCap!B31)&gt;0,[1]table_des_RedCap!B31,"")</f>
+        <v>fall_groesse</v>
       </c>
       <c r="C30" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B30)&gt;0,[1]table_des_RedCap!C30,"")</f>
-        <v>Einheit des Gewichts</v>
+        <f>IF(LEN([1]table_des_RedCap!B31)&gt;0,[1]table_des_RedCap!C31,"")</f>
+        <v>Größe (cm)</v>
       </c>
       <c r="D30" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F30)&gt;0,IF([1]table_des_RedCap!F30="date_ymd","date",IF([1]table_des_RedCap!F30="number","double precision",IF([1]table_des_RedCap!F30="integer","int",IF([1]table_des_RedCap!F30="autocomplete","varchar","-- setzen --")))),"varchar")</f>
-        <v>varchar</v>
+        <f>IF(LEN([1]table_des_RedCap!F31)&gt;0,IF([1]table_des_RedCap!F31="date_ymd","date",IF([1]table_des_RedCap!F31="number","double precision",IF([1]table_des_RedCap!F31="integer","int",IF([1]table_des_RedCap!F31="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <v>double precision</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A31)&gt;0,[1]table_des_RedCap!A31,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A32)&gt;0,[1]table_des_RedCap!A32,"")</f>
         <v/>
       </c>
       <c r="B31" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B31)&gt;0,[1]table_des_RedCap!B31,"")</f>
-        <v>fall_groesse</v>
+        <f>IF(LEN([1]table_des_RedCap!B32)&gt;0,[1]table_des_RedCap!B32,"")</f>
+        <v>fall_groesse_einheit</v>
       </c>
       <c r="C31" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B31)&gt;0,[1]table_des_RedCap!C31,"")</f>
-        <v>Größe (cm)</v>
+        <f>IF(LEN([1]table_des_RedCap!B32)&gt;0,[1]table_des_RedCap!C32,"")</f>
+        <v>Einheit der Größe</v>
       </c>
       <c r="D31" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F31)&gt;0,IF([1]table_des_RedCap!F31="date_ymd","date",IF([1]table_des_RedCap!F31="number","double precision",IF([1]table_des_RedCap!F31="integer","int",IF([1]table_des_RedCap!F31="autocomplete","varchar","-- setzen --")))),"varchar")</f>
-        <v>double precision</v>
+        <f>IF(LEN([1]table_des_RedCap!F32)&gt;0,IF([1]table_des_RedCap!F32="date_ymd","date",IF([1]table_des_RedCap!F32="number","double precision",IF([1]table_des_RedCap!F32="integer","int",IF([1]table_des_RedCap!F32="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <v>varchar</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A32)&gt;0,[1]table_des_RedCap!A32,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A33)&gt;0,[1]table_des_RedCap!A33,"")</f>
         <v/>
       </c>
       <c r="B32" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B32)&gt;0,[1]table_des_RedCap!B32,"")</f>
-        <v>fall_groesse_einheit</v>
+        <f>IF(LEN([1]table_des_RedCap!B33)&gt;0,[1]table_des_RedCap!B33,"")</f>
+        <v>fall_bmi</v>
       </c>
       <c r="C32" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B32)&gt;0,[1]table_des_RedCap!C32,"")</f>
-        <v>Einheit der Größe</v>
+        <f>IF(LEN([1]table_des_RedCap!B33)&gt;0,[1]table_des_RedCap!C33,"")</f>
+        <v>BMI</v>
       </c>
       <c r="D32" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F32)&gt;0,IF([1]table_des_RedCap!F32="date_ymd","date",IF([1]table_des_RedCap!F32="number","double precision",IF([1]table_des_RedCap!F32="integer","int",IF([1]table_des_RedCap!F32="autocomplete","varchar","-- setzen --")))),"varchar")</f>
-        <v>varchar</v>
+        <f>IF(LEN([1]table_des_RedCap!F33)&gt;0,IF([1]table_des_RedCap!F33="date_ymd","date",IF([1]table_des_RedCap!F33="number","double precision",IF([1]table_des_RedCap!F33="integer","int",IF([1]table_des_RedCap!F33="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <v>double precision</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A33)&gt;0,[1]table_des_RedCap!A33,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A34)&gt;0,[1]table_des_RedCap!A34,"")</f>
         <v/>
       </c>
       <c r="B33" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B33)&gt;0,[1]table_des_RedCap!B33,"")</f>
-        <v>fall_bmi</v>
+        <f>IF(LEN([1]table_des_RedCap!B34)&gt;0,[1]table_des_RedCap!B34,"")</f>
+        <v>fall_femb_2</v>
       </c>
       <c r="C33" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B33)&gt;0,[1]table_des_RedCap!C33,"")</f>
-        <v>BMI</v>
+        <f>IF(LEN([1]table_des_RedCap!B34)&gt;0,[1]table_des_RedCap!C34,"")</f>
+        <v>descriptive item only for frontend</v>
       </c>
       <c r="D33" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F33)&gt;0,IF([1]table_des_RedCap!F33="date_ymd","date",IF([1]table_des_RedCap!F33="number","double precision",IF([1]table_des_RedCap!F33="integer","int",IF([1]table_des_RedCap!F33="autocomplete","varchar","-- setzen --")))),"varchar")</f>
-        <v>double precision</v>
+        <f>IF(LEN([1]table_des_RedCap!F34)&gt;0,IF([1]table_des_RedCap!F34="date_ymd","date",IF([1]table_des_RedCap!F34="number","double precision",IF([1]table_des_RedCap!F34="integer","int",IF([1]table_des_RedCap!F34="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <v>varchar</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A34)&gt;0,[1]table_des_RedCap!A34,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A35)&gt;0,[1]table_des_RedCap!A35,"")</f>
         <v/>
       </c>
       <c r="B34" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B34)&gt;0,[1]table_des_RedCap!B34,"")</f>
-        <v>fall_femb_2</v>
+        <f>IF(LEN([1]table_des_RedCap!B35)&gt;0,[1]table_des_RedCap!B35,"")</f>
+        <v>fall_femb_3</v>
       </c>
       <c r="C34" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B34)&gt;0,[1]table_des_RedCap!C34,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!B35)&gt;0,[1]table_des_RedCap!C35,"")</f>
         <v>descriptive item only for frontend</v>
       </c>
       <c r="D34" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F34)&gt;0,IF([1]table_des_RedCap!F34="date_ymd","date",IF([1]table_des_RedCap!F34="number","double precision",IF([1]table_des_RedCap!F34="integer","int",IF([1]table_des_RedCap!F34="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <f>IF(LEN([1]table_des_RedCap!F35)&gt;0,IF([1]table_des_RedCap!F35="date_ymd","date",IF([1]table_des_RedCap!F35="number","double precision",IF([1]table_des_RedCap!F35="integer","int",IF([1]table_des_RedCap!F35="autocomplete","varchar","-- setzen --")))),"varchar")</f>
         <v>varchar</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A35)&gt;0,[1]table_des_RedCap!A35,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A36)&gt;0,[1]table_des_RedCap!A36,"")</f>
         <v/>
       </c>
       <c r="B35" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B35)&gt;0,[1]table_des_RedCap!B35,"")</f>
-        <v>fall_femb_3</v>
+        <f>IF(LEN([1]table_des_RedCap!B36)&gt;0,[1]table_des_RedCap!B36,"")</f>
+        <v>fall_femb_4</v>
       </c>
       <c r="C35" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B35)&gt;0,[1]table_des_RedCap!C35,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!B36)&gt;0,[1]table_des_RedCap!C36,"")</f>
         <v>descriptive item only for frontend</v>
       </c>
       <c r="D35" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F35)&gt;0,IF([1]table_des_RedCap!F35="date_ymd","date",IF([1]table_des_RedCap!F35="number","double precision",IF([1]table_des_RedCap!F35="integer","int",IF([1]table_des_RedCap!F35="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <f>IF(LEN([1]table_des_RedCap!F36)&gt;0,IF([1]table_des_RedCap!F36="date_ymd","date",IF([1]table_des_RedCap!F36="number","double precision",IF([1]table_des_RedCap!F36="integer","int",IF([1]table_des_RedCap!F36="autocomplete","varchar","-- setzen --")))),"varchar")</f>
         <v>varchar</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A36)&gt;0,[1]table_des_RedCap!A36,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A37)&gt;0,[1]table_des_RedCap!A37,"")</f>
         <v/>
       </c>
       <c r="B36" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B36)&gt;0,[1]table_des_RedCap!B36,"")</f>
-        <v>fall_femb_4</v>
+        <f>IF(LEN([1]table_des_RedCap!B37)&gt;0,[1]table_des_RedCap!B37,"")</f>
+        <v>fall_nieren_insuf_chron</v>
       </c>
       <c r="C36" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B36)&gt;0,[1]table_des_RedCap!C36,"")</f>
-        <v>descriptive item only for frontend</v>
+        <f>IF(LEN([1]table_des_RedCap!B37)&gt;0,[1]table_des_RedCap!C37,"")</f>
+        <v>1, ja | 0, nein | -1, nicht bekanntChronische Niereninsuffizienz</v>
       </c>
       <c r="D36" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F36)&gt;0,IF([1]table_des_RedCap!F36="date_ymd","date",IF([1]table_des_RedCap!F36="number","double precision",IF([1]table_des_RedCap!F36="integer","int",IF([1]table_des_RedCap!F36="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <f>IF(LEN([1]table_des_RedCap!F37)&gt;0,IF([1]table_des_RedCap!F37="date_ymd","date",IF([1]table_des_RedCap!F37="number","double precision",IF([1]table_des_RedCap!F37="integer","int",IF([1]table_des_RedCap!F37="autocomplete","varchar","-- setzen --")))),"varchar")</f>
         <v>varchar</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A37)&gt;0,[1]table_des_RedCap!A37,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A38)&gt;0,[1]table_des_RedCap!A38,"")</f>
         <v/>
       </c>
       <c r="B37" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B37)&gt;0,[1]table_des_RedCap!B37,"")</f>
-        <v>fall_nieren_insuf_chron</v>
+        <f>IF(LEN([1]table_des_RedCap!B38)&gt;0,[1]table_des_RedCap!B38,"")</f>
+        <v>fall_nieren_insuf_ausmass_lbl</v>
       </c>
       <c r="C37" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B37)&gt;0,[1]table_des_RedCap!C37,"")</f>
-        <v>1, ja | 0, nein | -1, nicht bekanntChronische Niereninsuffizienz</v>
+        <f>IF(LEN([1]table_des_RedCap!B38)&gt;0,[1]table_des_RedCap!C38,"")</f>
+        <v>descriptive item only for frontend</v>
       </c>
       <c r="D37" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F37)&gt;0,IF([1]table_des_RedCap!F37="date_ymd","date",IF([1]table_des_RedCap!F37="number","double precision",IF([1]table_des_RedCap!F37="integer","int",IF([1]table_des_RedCap!F37="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <f>IF(LEN([1]table_des_RedCap!F38)&gt;0,IF([1]table_des_RedCap!F38="date_ymd","date",IF([1]table_des_RedCap!F38="number","double precision",IF([1]table_des_RedCap!F38="integer","int",IF([1]table_des_RedCap!F38="autocomplete","varchar","-- setzen --")))),"varchar")</f>
         <v>varchar</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A38)&gt;0,[1]table_des_RedCap!A38,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A39)&gt;0,[1]table_des_RedCap!A39,"")</f>
         <v/>
       </c>
       <c r="B38" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B38)&gt;0,[1]table_des_RedCap!B38,"")</f>
-        <v>fall_nieren_insuf_ausmass_lbl</v>
+        <f>IF(LEN([1]table_des_RedCap!B39)&gt;0,[1]table_des_RedCap!B39,"")</f>
+        <v>fall_nieren_insuf_ausmass</v>
       </c>
       <c r="C38" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B38)&gt;0,[1]table_des_RedCap!C38,"")</f>
-        <v>descriptive item only for frontend</v>
+        <f>IF(LEN([1]table_des_RedCap!B39)&gt;0,[1]table_des_RedCap!C39,"")</f>
+        <v>1, Ausmaß unbekannt | 2, 45-59 ml/min/1,73 m2 | 3, 30-44 ml/min/1,73 m2 | 4, 15-29 ml/min/1,73 m2 | 5, &lt; 15 ml/min/1,73 m2</v>
       </c>
       <c r="D38" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F38)&gt;0,IF([1]table_des_RedCap!F38="date_ymd","date",IF([1]table_des_RedCap!F38="number","double precision",IF([1]table_des_RedCap!F38="integer","int",IF([1]table_des_RedCap!F38="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <f>IF(LEN([1]table_des_RedCap!F39)&gt;0,IF([1]table_des_RedCap!F39="date_ymd","date",IF([1]table_des_RedCap!F39="number","double precision",IF([1]table_des_RedCap!F39="integer","int",IF([1]table_des_RedCap!F39="autocomplete","varchar","-- setzen --")))),"varchar")</f>
         <v>varchar</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A39)&gt;0,[1]table_des_RedCap!A39,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A40)&gt;0,[1]table_des_RedCap!A40,"")</f>
         <v/>
       </c>
       <c r="B39" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B39)&gt;0,[1]table_des_RedCap!B39,"")</f>
-        <v>fall_nieren_insuf_ausmass</v>
+        <f>IF(LEN([1]table_des_RedCap!B40)&gt;0,[1]table_des_RedCap!B40,"")</f>
+        <v>fall_nieren_insuf_dialysev_lbl</v>
       </c>
       <c r="C39" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B39)&gt;0,[1]table_des_RedCap!C39,"")</f>
-        <v>1, Ausmaß unbekannt | 2, 45-59 ml/min/1,73 m2 | 3, 30-44 ml/min/1,73 m2 | 4, 15-29 ml/min/1,73 m2 | 5, &lt; 15 ml/min/1,73 m2</v>
+        <f>IF(LEN([1]table_des_RedCap!B40)&gt;0,[1]table_des_RedCap!C40,"")</f>
+        <v>descriptive item only for frontend</v>
       </c>
       <c r="D39" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F39)&gt;0,IF([1]table_des_RedCap!F39="date_ymd","date",IF([1]table_des_RedCap!F39="number","double precision",IF([1]table_des_RedCap!F39="integer","int",IF([1]table_des_RedCap!F39="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <f>IF(LEN([1]table_des_RedCap!F40)&gt;0,IF([1]table_des_RedCap!F40="date_ymd","date",IF([1]table_des_RedCap!F40="number","double precision",IF([1]table_des_RedCap!F40="integer","int",IF([1]table_des_RedCap!F40="autocomplete","varchar","-- setzen --")))),"varchar")</f>
         <v>varchar</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A40)&gt;0,[1]table_des_RedCap!A40,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A41)&gt;0,[1]table_des_RedCap!A41,"")</f>
         <v/>
       </c>
       <c r="B40" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B40)&gt;0,[1]table_des_RedCap!B40,"")</f>
-        <v>fall_nieren_insuf_dialysev_lbl</v>
+        <f>IF(LEN([1]table_des_RedCap!B41)&gt;0,[1]table_des_RedCap!B41,"")</f>
+        <v>fall_nieren_insuf_dialysev</v>
       </c>
       <c r="C40" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B40)&gt;0,[1]table_des_RedCap!C40,"")</f>
-        <v>descriptive item only for frontend</v>
+        <f>IF(LEN([1]table_des_RedCap!B41)&gt;0,[1]table_des_RedCap!C41,"")</f>
+        <v>1, Hämodialyse | 2, Kont. Hämofiltration | 3, Peritonealdialyse | 4, keineDialyseverfahren</v>
       </c>
       <c r="D40" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F40)&gt;0,IF([1]table_des_RedCap!F40="date_ymd","date",IF([1]table_des_RedCap!F40="number","double precision",IF([1]table_des_RedCap!F40="integer","int",IF([1]table_des_RedCap!F40="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <f>IF(LEN([1]table_des_RedCap!F41)&gt;0,IF([1]table_des_RedCap!F41="date_ymd","date",IF([1]table_des_RedCap!F41="number","double precision",IF([1]table_des_RedCap!F41="integer","int",IF([1]table_des_RedCap!F41="autocomplete","varchar","-- setzen --")))),"varchar")</f>
         <v>varchar</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A41)&gt;0,[1]table_des_RedCap!A41,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A42)&gt;0,[1]table_des_RedCap!A42,"")</f>
         <v/>
       </c>
       <c r="B41" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B41)&gt;0,[1]table_des_RedCap!B41,"")</f>
-        <v>fall_nieren_insuf_dialysev</v>
+        <f>IF(LEN([1]table_des_RedCap!B42)&gt;0,[1]table_des_RedCap!B42,"")</f>
+        <v>fall_leber_insuf</v>
       </c>
       <c r="C41" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B41)&gt;0,[1]table_des_RedCap!C41,"")</f>
-        <v>1, Hämodialyse | 2, Kont. Hämofiltration | 3, Peritonealdialyse | 4, keineDialyseverfahren</v>
+        <f>IF(LEN([1]table_des_RedCap!B42)&gt;0,[1]table_des_RedCap!C42,"")</f>
+        <v>1, ja | 0, nein | -1, nicht bekanntLeberinsuffizienz</v>
       </c>
       <c r="D41" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F41)&gt;0,IF([1]table_des_RedCap!F41="date_ymd","date",IF([1]table_des_RedCap!F41="number","double precision",IF([1]table_des_RedCap!F41="integer","int",IF([1]table_des_RedCap!F41="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <f>IF(LEN([1]table_des_RedCap!F42)&gt;0,IF([1]table_des_RedCap!F42="date_ymd","date",IF([1]table_des_RedCap!F42="number","double precision",IF([1]table_des_RedCap!F42="integer","int",IF([1]table_des_RedCap!F42="autocomplete","varchar","-- setzen --")))),"varchar")</f>
         <v>varchar</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A42)&gt;0,[1]table_des_RedCap!A42,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A43)&gt;0,[1]table_des_RedCap!A43,"")</f>
         <v/>
       </c>
       <c r="B42" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B42)&gt;0,[1]table_des_RedCap!B42,"")</f>
-        <v>fall_leber_insuf</v>
+        <f>IF(LEN([1]table_des_RedCap!B43)&gt;0,[1]table_des_RedCap!B43,"")</f>
+        <v>fall_leber_insuf_ausmass_lbl</v>
       </c>
       <c r="C42" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B42)&gt;0,[1]table_des_RedCap!C42,"")</f>
-        <v>1, ja | 0, nein | -1, nicht bekanntLeberinsuffizienz</v>
+        <f>IF(LEN([1]table_des_RedCap!B43)&gt;0,[1]table_des_RedCap!C43,"")</f>
+        <v>descriptive item only for frontend</v>
       </c>
       <c r="D42" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F42)&gt;0,IF([1]table_des_RedCap!F42="date_ymd","date",IF([1]table_des_RedCap!F42="number","double precision",IF([1]table_des_RedCap!F42="integer","int",IF([1]table_des_RedCap!F42="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <f>IF(LEN([1]table_des_RedCap!F43)&gt;0,IF([1]table_des_RedCap!F43="date_ymd","date",IF([1]table_des_RedCap!F43="number","double precision",IF([1]table_des_RedCap!F43="integer","int",IF([1]table_des_RedCap!F43="autocomplete","varchar","-- setzen --")))),"varchar")</f>
         <v>varchar</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A43)&gt;0,[1]table_des_RedCap!A43,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A44)&gt;0,[1]table_des_RedCap!A44,"")</f>
         <v/>
       </c>
       <c r="B43" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B43)&gt;0,[1]table_des_RedCap!B43,"")</f>
-        <v>fall_leber_insuf_ausmass_lbl</v>
+        <f>IF(LEN([1]table_des_RedCap!B44)&gt;0,[1]table_des_RedCap!B44,"")</f>
+        <v>fall_leber_insuf_ausmass</v>
       </c>
       <c r="C43" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B43)&gt;0,[1]table_des_RedCap!C43,"")</f>
-        <v>descriptive item only for frontend</v>
+        <f>IF(LEN([1]table_des_RedCap!B44)&gt;0,[1]table_des_RedCap!C44,"")</f>
+        <v>1, Ausmaß unbekannt | 2, Leicht (Child-Pugh A) | 3, Mittel (Child-Pugh B) | 4, Schwer (Child-Pugh C)aktuelles Ausmaß</v>
       </c>
       <c r="D43" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F43)&gt;0,IF([1]table_des_RedCap!F43="date_ymd","date",IF([1]table_des_RedCap!F43="number","double precision",IF([1]table_des_RedCap!F43="integer","int",IF([1]table_des_RedCap!F43="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <f>IF(LEN([1]table_des_RedCap!F44)&gt;0,IF([1]table_des_RedCap!F44="date_ymd","date",IF([1]table_des_RedCap!F44="number","double precision",IF([1]table_des_RedCap!F44="integer","int",IF([1]table_des_RedCap!F44="autocomplete","varchar","-- setzen --")))),"varchar")</f>
         <v>varchar</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A44)&gt;0,[1]table_des_RedCap!A44,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A45)&gt;0,[1]table_des_RedCap!A45,"")</f>
         <v/>
       </c>
       <c r="B44" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B44)&gt;0,[1]table_des_RedCap!B44,"")</f>
-        <v>fall_leber_insuf_ausmass</v>
+        <f>IF(LEN([1]table_des_RedCap!B45)&gt;0,[1]table_des_RedCap!B45,"")</f>
+        <v>fall_schwanger_mo</v>
       </c>
       <c r="C44" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B44)&gt;0,[1]table_des_RedCap!C44,"")</f>
-        <v>1, Ausmaß unbekannt | 2, Leicht (Child-Pugh A) | 3, Mittel (Child-Pugh B) | 4, Schwer (Child-Pugh C)aktuelles Ausmaß</v>
+        <f>IF(LEN([1]table_des_RedCap!B45)&gt;0,[1]table_des_RedCap!C45,"")</f>
+        <v>0, keine Schwangerschaft | 1, 1 | 2, 2 | 3, 3 | 4, 4 | 5, 5 | 6, 6 | 7, 7 | 8, 8 | 9, 9</v>
       </c>
       <c r="D44" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F44)&gt;0,IF([1]table_des_RedCap!F44="date_ymd","date",IF([1]table_des_RedCap!F44="number","double precision",IF([1]table_des_RedCap!F44="integer","int",IF([1]table_des_RedCap!F44="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <f>IF(LEN([1]table_des_RedCap!F45)&gt;0,IF([1]table_des_RedCap!F45="date_ymd","date",IF([1]table_des_RedCap!F45="number","double precision",IF([1]table_des_RedCap!F45="integer","int",IF([1]table_des_RedCap!F45="autocomplete","varchar","-- setzen --")))),"varchar")</f>
         <v>varchar</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A45)&gt;0,[1]table_des_RedCap!A45,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A46)&gt;0,[1]table_des_RedCap!A46,"")</f>
         <v/>
       </c>
       <c r="B45" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B45)&gt;0,[1]table_des_RedCap!B45,"")</f>
-        <v>fall_schwanger_mo</v>
+        <f>IF(LEN([1]table_des_RedCap!B46)&gt;0,[1]table_des_RedCap!B46,"")</f>
+        <v>fall_op_geplant</v>
       </c>
       <c r="C45" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B45)&gt;0,[1]table_des_RedCap!C45,"")</f>
-        <v>0, keine Schwangerschaft | 1, 1 | 2, 2 | 3, 3 | 4, 4 | 5, 5 | 6, 6 | 7, 7 | 8, 8 | 9, 9</v>
+        <f>IF(LEN([1]table_des_RedCap!B46)&gt;0,[1]table_des_RedCap!C46,"")</f>
+        <v>1, ja | 0, nein | -1, nicht bekanntIst eine Operation geplant?</v>
       </c>
       <c r="D45" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F45)&gt;0,IF([1]table_des_RedCap!F45="date_ymd","date",IF([1]table_des_RedCap!F45="number","double precision",IF([1]table_des_RedCap!F45="integer","int",IF([1]table_des_RedCap!F45="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <f>IF(LEN([1]table_des_RedCap!F46)&gt;0,IF([1]table_des_RedCap!F46="date_ymd","date",IF([1]table_des_RedCap!F46="number","double precision",IF([1]table_des_RedCap!F46="integer","int",IF([1]table_des_RedCap!F46="autocomplete","varchar","-- setzen --")))),"varchar")</f>
         <v>varchar</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A46)&gt;0,[1]table_des_RedCap!A46,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A47)&gt;0,[1]table_des_RedCap!A47,"")</f>
         <v/>
       </c>
       <c r="B46" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B46)&gt;0,[1]table_des_RedCap!B46,"")</f>
-        <v>fall_op_geplant</v>
+        <f>IF(LEN([1]table_des_RedCap!B47)&gt;0,[1]table_des_RedCap!B47,"")</f>
+        <v>fall_op_dat_lbl</v>
       </c>
       <c r="C46" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B46)&gt;0,[1]table_des_RedCap!C46,"")</f>
-        <v>1, ja | 0, nein | -1, nicht bekanntIst eine Operation geplant?</v>
+        <f>IF(LEN([1]table_des_RedCap!B47)&gt;0,[1]table_des_RedCap!C47,"")</f>
+        <v>descriptive item only for frontend</v>
       </c>
       <c r="D46" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F46)&gt;0,IF([1]table_des_RedCap!F46="date_ymd","date",IF([1]table_des_RedCap!F46="number","double precision",IF([1]table_des_RedCap!F46="integer","int",IF([1]table_des_RedCap!F46="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <f>IF(LEN([1]table_des_RedCap!F47)&gt;0,IF([1]table_des_RedCap!F47="date_ymd","date",IF([1]table_des_RedCap!F47="number","double precision",IF([1]table_des_RedCap!F47="integer","int",IF([1]table_des_RedCap!F47="autocomplete","varchar","-- setzen --")))),"varchar")</f>
         <v>varchar</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A47)&gt;0,[1]table_des_RedCap!A47,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A48)&gt;0,[1]table_des_RedCap!A48,"")</f>
         <v/>
       </c>
       <c r="B47" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B47)&gt;0,[1]table_des_RedCap!B47,"")</f>
-        <v>fall_op_dat_lbl</v>
+        <f>IF(LEN([1]table_des_RedCap!B48)&gt;0,[1]table_des_RedCap!B48,"")</f>
+        <v>fall_op_dat</v>
       </c>
       <c r="C47" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B47)&gt;0,[1]table_des_RedCap!C47,"")</f>
-        <v>descriptive item only for frontend</v>
+        <f>IF(LEN([1]table_des_RedCap!B48)&gt;0,[1]table_des_RedCap!C48,"")</f>
+        <v>Operationsdatum</v>
       </c>
       <c r="D47" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F47)&gt;0,IF([1]table_des_RedCap!F47="date_ymd","date",IF([1]table_des_RedCap!F47="number","double precision",IF([1]table_des_RedCap!F47="integer","int",IF([1]table_des_RedCap!F47="autocomplete","varchar","-- setzen --")))),"varchar")</f>
-        <v>varchar</v>
+        <f>IF(LEN([1]table_des_RedCap!F48)&gt;0,IF([1]table_des_RedCap!F48="date_ymd","date",IF([1]table_des_RedCap!F48="number","double precision",IF([1]table_des_RedCap!F48="integer","int",IF([1]table_des_RedCap!F48="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <v>date</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A48)&gt;0,[1]table_des_RedCap!A48,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A49)&gt;0,[1]table_des_RedCap!A49,"")</f>
         <v/>
       </c>
       <c r="B48" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B48)&gt;0,[1]table_des_RedCap!B48,"")</f>
-        <v>fall_op_dat</v>
+        <f>IF(LEN([1]table_des_RedCap!B49)&gt;0,[1]table_des_RedCap!B49,"")</f>
+        <v>fall_status</v>
       </c>
       <c r="C48" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B48)&gt;0,[1]table_des_RedCap!C48,"")</f>
-        <v>Operationsdatum</v>
+        <f>IF(LEN([1]table_des_RedCap!B49)&gt;0,[1]table_des_RedCap!C49,"")</f>
+        <v>Status des Falls</v>
       </c>
       <c r="D48" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F48)&gt;0,IF([1]table_des_RedCap!F48="date_ymd","date",IF([1]table_des_RedCap!F48="number","double precision",IF([1]table_des_RedCap!F48="integer","int",IF([1]table_des_RedCap!F48="autocomplete","varchar","-- setzen --")))),"varchar")</f>
-        <v>date</v>
+        <f>IF(LEN([1]table_des_RedCap!F49)&gt;0,IF([1]table_des_RedCap!F49="date_ymd","date",IF([1]table_des_RedCap!F49="number","double precision",IF([1]table_des_RedCap!F49="integer","int",IF([1]table_des_RedCap!F49="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <v>varchar</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A49)&gt;0,[1]table_des_RedCap!A49,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A50)&gt;0,[1]table_des_RedCap!A50,"")</f>
         <v/>
       </c>
       <c r="B49" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B49)&gt;0,[1]table_des_RedCap!B49,"")</f>
-        <v>fall_status</v>
+        <f>IF(LEN([1]table_des_RedCap!B50)&gt;0,[1]table_des_RedCap!B50,"")</f>
+        <v>fall_ent_dat</v>
       </c>
       <c r="C49" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B49)&gt;0,[1]table_des_RedCap!C49,"")</f>
-        <v>Status des Falls</v>
+        <f>IF(LEN([1]table_des_RedCap!B50)&gt;0,[1]table_des_RedCap!C50,"")</f>
+        <v>Entlassdatum</v>
       </c>
       <c r="D49" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F49)&gt;0,IF([1]table_des_RedCap!F49="date_ymd","date",IF([1]table_des_RedCap!F49="number","double precision",IF([1]table_des_RedCap!F49="integer","int",IF([1]table_des_RedCap!F49="autocomplete","varchar","-- setzen --")))),"varchar")</f>
-        <v>varchar</v>
+        <f>IF(LEN([1]table_des_RedCap!F50)&gt;0,IF([1]table_des_RedCap!F50="date_ymd","date",IF([1]table_des_RedCap!F50="number","double precision",IF([1]table_des_RedCap!F50="integer","int",IF([1]table_des_RedCap!F50="autocomplete","varchar","-- setzen --")))),"varchar")</f>
+        <v>date</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A50)&gt;0,[1]table_des_RedCap!A50,"")</f>
+        <f>IF(LEN([1]table_des_RedCap!A51)&gt;0,[1]table_des_RedCap!A51,"")</f>
         <v/>
       </c>
       <c r="B50" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B50)&gt;0,[1]table_des_RedCap!B50,"")</f>
-        <v>fall_ent_dat</v>
-      </c>
-      <c r="C50" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!B50)&gt;0,[1]table_des_RedCap!C50,"")</f>
-        <v>Entlassdatum</v>
-      </c>
-      <c r="D50" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!F50)&gt;0,IF([1]table_des_RedCap!F50="date_ymd","date",IF([1]table_des_RedCap!F50="number","double precision",IF([1]table_des_RedCap!F50="integer","int",IF([1]table_des_RedCap!F50="autocomplete","varchar","-- setzen --")))),"varchar")</f>
-        <v>date</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="str">
-        <f>IF(LEN([1]table_des_RedCap!A51)&gt;0,[1]table_des_RedCap!A51,"")</f>
-        <v/>
-      </c>
-      <c r="B51" s="3" t="str">
         <f>IF(LEN([1]table_des_RedCap!B51)&gt;0,[1]table_des_RedCap!B51,"")</f>
         <v>fall_complete</v>
       </c>
-      <c r="C51" s="3" t="str">
+      <c r="C50" s="3" t="str">
         <f>IF(LEN([1]table_des_RedCap!B51)&gt;0,[1]table_des_RedCap!C51,"")</f>
         <v>Frontend Complete-Status</v>
       </c>
-      <c r="D51" s="3" t="str">
+      <c r="D50" s="3" t="str">
         <f>IF(LEN([1]table_des_RedCap!F51)&gt;0,IF([1]table_des_RedCap!F51="date_ymd","date",IF([1]table_des_RedCap!F51="number","double precision",IF([1]table_des_RedCap!F51="integer","int",IF([1]table_des_RedCap!F51="autocomplete","varchar","-- setzen --")))),"varchar")</f>
         <v>varchar</v>
       </c>
     </row>
+    <row r="474" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="475" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="476" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add item for checkbox frontend in database
</commit_message>
<xml_diff>
--- a/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
+++ b/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="412">
   <si>
     <t xml:space="preserve">Station </t>
   </si>
@@ -1011,9 +1011,6 @@
     <t>NCC MERP Score</t>
   </si>
   <si>
-    <t>mrp_merp_info</t>
-  </si>
-  <si>
     <t>mrp_merp_txt</t>
   </si>
   <si>
@@ -1249,6 +1246,21 @@
   </si>
   <si>
     <t>trigger_complete</t>
+  </si>
+  <si>
+    <t>meda_risiko_pat_info__1</t>
+  </si>
+  <si>
+    <t>mrp_pi_info__1</t>
+  </si>
+  <si>
+    <t>mrp_mf_info__1</t>
+  </si>
+  <si>
+    <t>mrp_merp_info__1</t>
+  </si>
+  <si>
+    <t>mrpdokumentation_validierung_complete</t>
   </si>
 </sst>
 </file>
@@ -2102,10 +2114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F457"/>
+  <dimension ref="A1:F452"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B226" sqref="B226"/>
+    <sheetView tabSelected="1" topLeftCell="A229" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A219" sqref="A219:XFD219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2812,6 +2824,7 @@
       <c r="D46" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="E46" s="3"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
@@ -2826,6 +2839,7 @@
       <c r="D47" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="E47" s="3"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
@@ -2840,8 +2854,9 @@
       <c r="D48" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>13</v>
       </c>
@@ -2854,8 +2869,9 @@
       <c r="D49" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>13</v>
       </c>
@@ -2868,8 +2884,9 @@
       <c r="D50" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>13</v>
       </c>
@@ -2882,8 +2899,9 @@
       <c r="D51" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>13</v>
       </c>
@@ -2897,7 +2915,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>100</v>
       </c>
@@ -2911,7 +2929,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>13</v>
       </c>
@@ -2925,7 +2943,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>13</v>
       </c>
@@ -2939,7 +2957,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>13</v>
       </c>
@@ -2953,7 +2971,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>13</v>
       </c>
@@ -2967,7 +2985,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>13</v>
       </c>
@@ -2981,7 +2999,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>13</v>
       </c>
@@ -2995,7 +3013,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>13</v>
       </c>
@@ -3009,7 +3027,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>13</v>
       </c>
@@ -3023,7 +3041,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>13</v>
       </c>
@@ -3037,7 +3055,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>13</v>
       </c>
@@ -3051,7 +3069,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>13</v>
       </c>
@@ -3098,7 +3116,7 @@
         <v>13</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>117</v>
+        <v>407</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>15</v>
@@ -3112,10 +3130,10 @@
         <v>13</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>119</v>
+        <v>15</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>12</v>
@@ -3126,10 +3144,10 @@
         <v>13</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>15</v>
+        <v>119</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>12</v>
@@ -3140,10 +3158,10 @@
         <v>13</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>122</v>
+        <v>15</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>12</v>
@@ -3154,10 +3172,10 @@
         <v>13</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>15</v>
+        <v>122</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>12</v>
@@ -3168,10 +3186,10 @@
         <v>13</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>125</v>
+        <v>15</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>12</v>
@@ -3182,10 +3200,10 @@
         <v>13</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>12</v>
@@ -3196,10 +3214,10 @@
         <v>13</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>12</v>
@@ -3210,13 +3228,13 @@
         <v>13</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>15</v>
+        <v>129</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -3224,10 +3242,10 @@
         <v>13</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>132</v>
+        <v>15</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>47</v>
@@ -3238,13 +3256,13 @@
         <v>13</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -3252,10 +3270,10 @@
         <v>13</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>38</v>
+        <v>134</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>12</v>
@@ -3263,13 +3281,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>136</v>
+        <v>13</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>10</v>
+        <v>135</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>12</v>
@@ -3277,16 +3295,16 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>13</v>
+        <v>136</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>137</v>
+        <v>10</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>138</v>
+        <v>11</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -3294,13 +3312,13 @@
         <v>13</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>21</v>
+        <v>137</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -3308,10 +3326,10 @@
         <v>13</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>50</v>
+        <v>139</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>12</v>
@@ -3322,10 +3340,10 @@
         <v>13</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>140</v>
+        <v>23</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>12</v>
@@ -3336,7 +3354,7 @@
         <v>13</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>15</v>
@@ -3350,7 +3368,7 @@
         <v>13</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>15</v>
@@ -3364,7 +3382,7 @@
         <v>13</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>15</v>
@@ -3378,7 +3396,7 @@
         <v>13</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>15</v>
@@ -3392,7 +3410,7 @@
         <v>13</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>15</v>
@@ -3406,7 +3424,7 @@
         <v>13</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>146</v>
+        <v>408</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>15</v>
@@ -3420,7 +3438,7 @@
         <v>13</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>15</v>
@@ -3434,7 +3452,7 @@
         <v>13</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>148</v>
+        <v>409</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>15</v>
@@ -3448,7 +3466,7 @@
         <v>13</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>15</v>
@@ -3462,7 +3480,7 @@
         <v>13</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>15</v>
@@ -3476,13 +3494,13 @@
         <v>13</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>152</v>
+        <v>15</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -3490,10 +3508,10 @@
         <v>13</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>154</v>
+        <v>15</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>12</v>
@@ -3504,10 +3522,10 @@
         <v>13</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>156</v>
+        <v>15</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>12</v>
@@ -3518,13 +3536,13 @@
         <v>13</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>15</v>
+        <v>152</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -3532,10 +3550,10 @@
         <v>13</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>12</v>
@@ -3546,10 +3564,10 @@
         <v>13</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>15</v>
+        <v>156</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>12</v>
@@ -3560,10 +3578,10 @@
         <v>13</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>162</v>
+        <v>15</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>12</v>
@@ -3574,10 +3592,10 @@
         <v>13</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>15</v>
+        <v>159</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>12</v>
@@ -3588,10 +3606,10 @@
         <v>13</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>165</v>
+        <v>15</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>12</v>
@@ -3602,10 +3620,10 @@
         <v>13</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>15</v>
+        <v>162</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>12</v>
@@ -3616,10 +3634,10 @@
         <v>13</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>168</v>
+        <v>15</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>12</v>
@@ -3630,10 +3648,10 @@
         <v>13</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>15</v>
+        <v>165</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>12</v>
@@ -3644,7 +3662,7 @@
         <v>13</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>15</v>
@@ -3658,10 +3676,10 @@
         <v>13</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>15</v>
+        <v>168</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>12</v>
@@ -3672,7 +3690,7 @@
         <v>13</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>15</v>
@@ -3686,7 +3704,7 @@
         <v>13</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>15</v>
@@ -3700,7 +3718,7 @@
         <v>13</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>15</v>
@@ -3714,10 +3732,10 @@
         <v>13</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>176</v>
+        <v>15</v>
       </c>
       <c r="D111" s="3" t="s">
         <v>12</v>
@@ -3728,7 +3746,7 @@
         <v>13</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C112" s="3" t="s">
         <v>15</v>
@@ -3742,10 +3760,10 @@
         <v>13</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>179</v>
+        <v>15</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>12</v>
@@ -3756,10 +3774,10 @@
         <v>13</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>15</v>
+        <v>176</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>12</v>
@@ -3770,10 +3788,10 @@
         <v>13</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>182</v>
+        <v>15</v>
       </c>
       <c r="D115" s="3" t="s">
         <v>12</v>
@@ -3784,10 +3802,10 @@
         <v>13</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>15</v>
+        <v>179</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>12</v>
@@ -3798,10 +3816,10 @@
         <v>13</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>185</v>
+        <v>15</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>12</v>
@@ -3812,10 +3830,10 @@
         <v>13</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>15</v>
+        <v>182</v>
       </c>
       <c r="D118" s="3" t="s">
         <v>12</v>
@@ -3826,10 +3844,10 @@
         <v>13</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>188</v>
+        <v>15</v>
       </c>
       <c r="D119" s="3" t="s">
         <v>12</v>
@@ -3840,10 +3858,10 @@
         <v>13</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>15</v>
+        <v>185</v>
       </c>
       <c r="D120" s="3" t="s">
         <v>12</v>
@@ -3854,10 +3872,10 @@
         <v>13</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>191</v>
+        <v>15</v>
       </c>
       <c r="D121" s="3" t="s">
         <v>12</v>
@@ -3868,10 +3886,10 @@
         <v>13</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>15</v>
+        <v>188</v>
       </c>
       <c r="D122" s="3" t="s">
         <v>12</v>
@@ -3882,10 +3900,10 @@
         <v>13</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>194</v>
+        <v>15</v>
       </c>
       <c r="D123" s="3" t="s">
         <v>12</v>
@@ -3896,10 +3914,10 @@
         <v>13</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>15</v>
+        <v>191</v>
       </c>
       <c r="D124" s="3" t="s">
         <v>12</v>
@@ -3910,10 +3928,10 @@
         <v>13</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>197</v>
+        <v>15</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>12</v>
@@ -3924,10 +3942,10 @@
         <v>13</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>12</v>
@@ -3938,10 +3956,10 @@
         <v>13</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>201</v>
+        <v>15</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>12</v>
@@ -3952,10 +3970,10 @@
         <v>13</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>15</v>
+        <v>197</v>
       </c>
       <c r="D128" s="3" t="s">
         <v>12</v>
@@ -3966,10 +3984,10 @@
         <v>13</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D129" s="3" t="s">
         <v>12</v>
@@ -3980,10 +3998,10 @@
         <v>13</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D130" s="3" t="s">
         <v>12</v>
@@ -3994,10 +4012,10 @@
         <v>13</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>208</v>
+        <v>15</v>
       </c>
       <c r="D131" s="3" t="s">
         <v>12</v>
@@ -4008,10 +4026,10 @@
         <v>13</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D132" s="3" t="s">
         <v>12</v>
@@ -4022,10 +4040,10 @@
         <v>13</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D133" s="3" t="s">
         <v>12</v>
@@ -4036,10 +4054,10 @@
         <v>13</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D134" s="3" t="s">
         <v>12</v>
@@ -4050,10 +4068,10 @@
         <v>13</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="D135" s="3" t="s">
         <v>12</v>
@@ -4064,10 +4082,10 @@
         <v>13</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="D136" s="3" t="s">
         <v>12</v>
@@ -4078,10 +4096,10 @@
         <v>13</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D137" s="3" t="s">
         <v>12</v>
@@ -4092,10 +4110,10 @@
         <v>13</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="D138" s="3" t="s">
         <v>12</v>
@@ -4106,10 +4124,10 @@
         <v>13</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="D139" s="3" t="s">
         <v>12</v>
@@ -4120,10 +4138,10 @@
         <v>13</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="D140" s="3" t="s">
         <v>12</v>
@@ -4134,10 +4152,10 @@
         <v>13</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="D141" s="3" t="s">
         <v>12</v>
@@ -4148,10 +4166,10 @@
         <v>13</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="D142" s="3" t="s">
         <v>12</v>
@@ -4162,10 +4180,10 @@
         <v>13</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="D143" s="3" t="s">
         <v>12</v>
@@ -4176,10 +4194,10 @@
         <v>13</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D144" s="3" t="s">
         <v>12</v>
@@ -4190,10 +4208,10 @@
         <v>13</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="D145" s="3" t="s">
         <v>12</v>
@@ -4204,10 +4222,10 @@
         <v>13</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="D146" s="3" t="s">
         <v>12</v>
@@ -4218,10 +4236,10 @@
         <v>13</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="D147" s="3" t="s">
         <v>12</v>
@@ -4232,10 +4250,10 @@
         <v>13</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="D148" s="3" t="s">
         <v>12</v>
@@ -4246,10 +4264,10 @@
         <v>13</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="D149" s="3" t="s">
         <v>12</v>
@@ -4260,10 +4278,10 @@
         <v>13</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="D150" s="3" t="s">
         <v>12</v>
@@ -4274,10 +4292,10 @@
         <v>13</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="D151" s="3" t="s">
         <v>12</v>
@@ -4288,10 +4306,10 @@
         <v>13</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="D152" s="3" t="s">
         <v>12</v>
@@ -4302,10 +4320,10 @@
         <v>13</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="D153" s="3" t="s">
         <v>12</v>
@@ -4316,10 +4334,10 @@
         <v>13</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D154" s="3" t="s">
         <v>12</v>
@@ -4330,10 +4348,10 @@
         <v>13</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="D155" s="3" t="s">
         <v>12</v>
@@ -4344,10 +4362,10 @@
         <v>13</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="D156" s="3" t="s">
         <v>12</v>
@@ -4358,10 +4376,10 @@
         <v>13</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>15</v>
+        <v>254</v>
       </c>
       <c r="D157" s="3" t="s">
         <v>12</v>
@@ -4372,10 +4390,10 @@
         <v>13</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D158" s="3" t="s">
         <v>12</v>
@@ -4386,10 +4404,10 @@
         <v>13</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D159" s="3" t="s">
         <v>12</v>
@@ -4400,10 +4418,10 @@
         <v>13</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>265</v>
+        <v>15</v>
       </c>
       <c r="D160" s="3" t="s">
         <v>12</v>
@@ -4414,10 +4432,10 @@
         <v>13</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="D161" s="3" t="s">
         <v>12</v>
@@ -4428,10 +4446,10 @@
         <v>13</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="D162" s="3" t="s">
         <v>12</v>
@@ -4442,10 +4460,10 @@
         <v>13</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D163" s="3" t="s">
         <v>12</v>
@@ -4456,10 +4474,10 @@
         <v>13</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>15</v>
+        <v>267</v>
       </c>
       <c r="D164" s="3" t="s">
         <v>12</v>
@@ -4470,10 +4488,10 @@
         <v>13</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>15</v>
+        <v>269</v>
       </c>
       <c r="D165" s="3" t="s">
         <v>12</v>
@@ -4484,10 +4502,10 @@
         <v>13</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D166" s="3" t="s">
         <v>12</v>
@@ -4498,10 +4516,10 @@
         <v>13</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>277</v>
+        <v>15</v>
       </c>
       <c r="D167" s="3" t="s">
         <v>12</v>
@@ -4512,7 +4530,7 @@
         <v>13</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="C168" s="3" t="s">
         <v>15</v>
@@ -4526,10 +4544,10 @@
         <v>13</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D169" s="3" t="s">
         <v>12</v>
@@ -4540,10 +4558,10 @@
         <v>13</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D170" s="3" t="s">
         <v>12</v>
@@ -4554,10 +4572,10 @@
         <v>13</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>284</v>
+        <v>15</v>
       </c>
       <c r="D171" s="3" t="s">
         <v>12</v>
@@ -4568,10 +4586,10 @@
         <v>13</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="D172" s="3" t="s">
         <v>12</v>
@@ -4582,10 +4600,10 @@
         <v>13</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="D173" s="3" t="s">
         <v>12</v>
@@ -4596,10 +4614,10 @@
         <v>13</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D174" s="3" t="s">
         <v>12</v>
@@ -4610,10 +4628,10 @@
         <v>13</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="D175" s="3" t="s">
         <v>12</v>
@@ -4624,10 +4642,10 @@
         <v>13</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="D176" s="3" t="s">
         <v>12</v>
@@ -4638,10 +4656,10 @@
         <v>13</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="D177" s="3" t="s">
         <v>12</v>
@@ -4652,10 +4670,10 @@
         <v>13</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="D178" s="3" t="s">
         <v>12</v>
@@ -4666,10 +4684,10 @@
         <v>13</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="D179" s="3" t="s">
         <v>12</v>
@@ -4680,10 +4698,10 @@
         <v>13</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>15</v>
+        <v>296</v>
       </c>
       <c r="D180" s="3" t="s">
         <v>12</v>
@@ -4694,10 +4712,10 @@
         <v>13</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D181" s="3" t="s">
         <v>12</v>
@@ -4708,10 +4726,10 @@
         <v>13</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="D182" s="3" t="s">
         <v>12</v>
@@ -4722,10 +4740,10 @@
         <v>13</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="C183" s="3" t="s">
-        <v>307</v>
+        <v>15</v>
       </c>
       <c r="D183" s="3" t="s">
         <v>12</v>
@@ -4736,10 +4754,10 @@
         <v>13</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="C184" s="3" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D184" s="3" t="s">
         <v>12</v>
@@ -4750,10 +4768,10 @@
         <v>13</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="D185" s="3" t="s">
         <v>12</v>
@@ -4764,10 +4782,10 @@
         <v>13</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="D186" s="3" t="s">
         <v>12</v>
@@ -4778,10 +4796,10 @@
         <v>13</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="D187" s="3" t="s">
         <v>12</v>
@@ -4792,10 +4810,10 @@
         <v>13</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="D188" s="3" t="s">
         <v>12</v>
@@ -4806,10 +4824,10 @@
         <v>13</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="D189" s="3" t="s">
         <v>12</v>
@@ -4820,10 +4838,10 @@
         <v>13</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>15</v>
+        <v>315</v>
       </c>
       <c r="D190" s="3" t="s">
         <v>12</v>
@@ -4834,10 +4852,10 @@
         <v>13</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="D191" s="3" t="s">
         <v>12</v>
@@ -4848,10 +4866,10 @@
         <v>13</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>15</v>
+        <v>319</v>
       </c>
       <c r="D192" s="3" t="s">
         <v>12</v>
@@ -4862,10 +4880,10 @@
         <v>13</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>325</v>
+        <v>15</v>
       </c>
       <c r="D193" s="3" t="s">
         <v>12</v>
@@ -4876,10 +4894,10 @@
         <v>13</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="D194" s="3" t="s">
         <v>12</v>
@@ -4890,7 +4908,7 @@
         <v>13</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="C195" s="3" t="s">
         <v>15</v>
@@ -4904,10 +4922,10 @@
         <v>13</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>15</v>
+        <v>325</v>
       </c>
       <c r="D196" s="3" t="s">
         <v>12</v>
@@ -4918,10 +4936,10 @@
         <v>13</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D197" s="3" t="s">
         <v>12</v>
@@ -4929,13 +4947,13 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
-        <v>332</v>
+        <v>13</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>10</v>
+        <v>410</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D198" s="3" t="s">
         <v>12</v>
@@ -4946,13 +4964,13 @@
         <v>13</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>45</v>
+        <v>328</v>
       </c>
       <c r="C199" s="3" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="D199" s="3" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -4960,10 +4978,10 @@
         <v>13</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C200" s="3" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="D200" s="3" t="s">
         <v>12</v>
@@ -4974,10 +4992,10 @@
         <v>13</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>335</v>
+        <v>411</v>
       </c>
       <c r="C201" s="3" t="s">
-        <v>336</v>
+        <v>38</v>
       </c>
       <c r="D201" s="3" t="s">
         <v>12</v>
@@ -4985,13 +5003,13 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
-        <v>13</v>
+        <v>331</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>337</v>
+        <v>10</v>
       </c>
       <c r="C202" s="3" t="s">
-        <v>338</v>
+        <v>11</v>
       </c>
       <c r="D202" s="3" t="s">
         <v>12</v>
@@ -5002,10 +5020,10 @@
         <v>13</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>339</v>
+        <v>45</v>
       </c>
       <c r="C203" s="3" t="s">
-        <v>340</v>
+        <v>46</v>
       </c>
       <c r="D203" s="3" t="s">
         <v>12</v>
@@ -5016,13 +5034,13 @@
         <v>13</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="C204" s="3" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -5030,10 +5048,10 @@
         <v>13</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="C205" s="3" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="D205" s="3" t="s">
         <v>12</v>
@@ -5044,10 +5062,10 @@
         <v>13</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="C206" s="3" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="D206" s="3" t="s">
         <v>12</v>
@@ -5058,10 +5076,10 @@
         <v>13</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="C207" s="3" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="D207" s="3" t="s">
         <v>12</v>
@@ -5072,10 +5090,10 @@
         <v>13</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="D208" s="3" t="s">
         <v>12</v>
@@ -5086,10 +5104,10 @@
         <v>13</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="C209" s="3" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="D209" s="3" t="s">
         <v>12</v>
@@ -5100,10 +5118,10 @@
         <v>13</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="C210" s="3" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="D210" s="3" t="s">
         <v>12</v>
@@ -5114,10 +5132,10 @@
         <v>13</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="C211" s="3" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="D211" s="3" t="s">
         <v>12</v>
@@ -5128,10 +5146,10 @@
         <v>13</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="C212" s="3" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="D212" s="3" t="s">
         <v>12</v>
@@ -5142,10 +5160,10 @@
         <v>13</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="C213" s="3" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="D213" s="3" t="s">
         <v>12</v>
@@ -5156,10 +5174,10 @@
         <v>13</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="C214" s="3" t="s">
-        <v>38</v>
+        <v>353</v>
       </c>
       <c r="D214" s="3" t="s">
         <v>12</v>
@@ -5167,16 +5185,16 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="s">
-        <v>362</v>
+        <v>13</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>45</v>
+        <v>354</v>
       </c>
       <c r="C215" s="3" t="s">
-        <v>46</v>
+        <v>355</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -5184,10 +5202,10 @@
         <v>13</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>10</v>
+        <v>356</v>
       </c>
       <c r="C216" s="3" t="s">
-        <v>11</v>
+        <v>357</v>
       </c>
       <c r="D216" s="3" t="s">
         <v>12</v>
@@ -5198,10 +5216,10 @@
         <v>13</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="C217" s="3" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="D217" s="3" t="s">
         <v>12</v>
@@ -5212,10 +5230,10 @@
         <v>13</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="C218" s="3" t="s">
-        <v>366</v>
+        <v>38</v>
       </c>
       <c r="D218" s="3" t="s">
         <v>12</v>
@@ -5223,13 +5241,13 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>13</v>
+        <v>361</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>367</v>
+        <v>45</v>
       </c>
       <c r="C219" s="3" t="s">
-        <v>368</v>
+        <v>46</v>
       </c>
       <c r="D219" s="3" t="s">
         <v>12</v>
@@ -5240,13 +5258,13 @@
         <v>13</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>369</v>
+        <v>10</v>
       </c>
       <c r="C220" s="3" t="s">
-        <v>370</v>
+        <v>11</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -5254,10 +5272,10 @@
         <v>13</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="C221" s="3" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="D221" s="3" t="s">
         <v>12</v>
@@ -5268,10 +5286,10 @@
         <v>13</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="C222" s="3" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="D222" s="3" t="s">
         <v>12</v>
@@ -5282,10 +5300,10 @@
         <v>13</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="C223" s="3" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="D223" s="3" t="s">
         <v>12</v>
@@ -5296,10 +5314,10 @@
         <v>13</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="C224" s="3" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="D224" s="3" t="s">
         <v>12</v>
@@ -5310,10 +5328,10 @@
         <v>13</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="C225" s="3" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="D225" s="3" t="s">
         <v>12</v>
@@ -5324,10 +5342,10 @@
         <v>13</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="C226" s="3" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="D226" s="3" t="s">
         <v>12</v>
@@ -5338,10 +5356,10 @@
         <v>13</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="C227" s="3" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="D227" s="3" t="s">
         <v>12</v>
@@ -5352,10 +5370,10 @@
         <v>13</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="C228" s="3" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="D228" s="3" t="s">
         <v>12</v>
@@ -5366,10 +5384,10 @@
         <v>13</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="C229" s="3" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="D229" s="3" t="s">
         <v>12</v>
@@ -5380,10 +5398,10 @@
         <v>13</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="C230" s="3" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="D230" s="3" t="s">
         <v>12</v>
@@ -5394,10 +5412,10 @@
         <v>13</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="C231" s="3" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="D231" s="3" t="s">
         <v>12</v>
@@ -5408,10 +5426,10 @@
         <v>13</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="C232" s="3" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="D232" s="3" t="s">
         <v>12</v>
@@ -5422,10 +5440,10 @@
         <v>13</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="C233" s="3" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="D233" s="3" t="s">
         <v>12</v>
@@ -5436,10 +5454,10 @@
         <v>13</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="C234" s="3" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="D234" s="3" t="s">
         <v>12</v>
@@ -5450,10 +5468,10 @@
         <v>13</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="C235" s="3" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="D235" s="3" t="s">
         <v>12</v>
@@ -5464,90 +5482,97 @@
         <v>13</v>
       </c>
       <c r="B236" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="C236" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="D236" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A237" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="C237" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="D237" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A238" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B238" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C238" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="D238" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A239" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C239" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D239" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A240" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="C240" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="C236" s="3" t="s">
+      <c r="D240" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A241" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B241" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="D236" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A237" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B237" s="3" t="s">
+      <c r="C241" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="C237" s="3" t="s">
-        <v>404</v>
-      </c>
-      <c r="D237" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A238" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B238" s="3" t="s">
-        <v>405</v>
-      </c>
-      <c r="C238" s="3" t="s">
-        <v>406</v>
-      </c>
-      <c r="D238" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A239" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B239" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="C239" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D239" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A240" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B240" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C240" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D240" s="3"/>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A241" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B241" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C241" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D241" s="3"/>
+      <c r="D241" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>13</v>
+        <v>404</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>13</v>
+        <v>405</v>
+      </c>
+      <c r="D242" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
@@ -5555,10 +5580,13 @@
         <v>13</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>13</v>
+        <v>406</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>13</v>
+        <v>38</v>
+      </c>
+      <c r="D243" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
@@ -5638,63 +5666,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A251" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B251" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C251" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A252" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B252" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C252" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A253" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B253" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C253" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A254" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B254" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C254" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A255" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B255" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C255" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="456" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="457" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating the frontend tables to the current status of the redcap project
</commit_message>
<xml_diff>
--- a/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
+++ b/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="412">
   <si>
     <t xml:space="preserve">Station </t>
   </si>
@@ -93,15 +93,9 @@
     <t>redcap_repeat_instrument</t>
   </si>
   <si>
-    <t>Frontend interne Datensatzverwaltung - Instrument :  patient</t>
-  </si>
-  <si>
     <t>redcap_repeat_instance</t>
   </si>
   <si>
-    <t>Frontend interne Datensatzverwaltung - Instanz des Instruments - Numerisch : 1</t>
-  </si>
-  <si>
     <t>pat_name</t>
   </si>
   <si>
@@ -297,21 +291,6 @@
     <t>fall_schwanger_mo_lbl</t>
   </si>
   <si>
-    <t>fall_op_geplant</t>
-  </si>
-  <si>
-    <t>1, ja | 0, nein | -1, nicht bekanntIst eine Operation geplant?</t>
-  </si>
-  <si>
-    <t>fall_op_dat_lbl</t>
-  </si>
-  <si>
-    <t>fall_op_dat</t>
-  </si>
-  <si>
-    <t>Operationsdatum</t>
-  </si>
-  <si>
     <t>fall_status</t>
   </si>
   <si>
@@ -369,18 +348,6 @@
     <t>Typ der Medikationsanalyse</t>
   </si>
   <si>
-    <t>meda_risiko_pat</t>
-  </si>
-  <si>
-    <t>1, Risikopatient | 2, Medikationsanalyse / Therapieüberwachung in 24-48hMarkieren als Risikopatient</t>
-  </si>
-  <si>
-    <t>meda_risiko_pat_info</t>
-  </si>
-  <si>
-    <t>meda_risiko_pat_info_txt</t>
-  </si>
-  <si>
     <t>meda_ma_thueberw</t>
   </si>
   <si>
@@ -1014,253 +981,286 @@
     <t>mrp_merp_txt</t>
   </si>
   <si>
+    <t>risikofaktor</t>
+  </si>
+  <si>
+    <t>rskfk_gerhemmer</t>
+  </si>
+  <si>
+    <t>Ger.hemmer</t>
+  </si>
+  <si>
+    <t>rskfk_tah</t>
+  </si>
+  <si>
+    <t>TAH</t>
+  </si>
+  <si>
+    <t>rskfk_immunsupp</t>
+  </si>
+  <si>
+    <t>Immunsupp.</t>
+  </si>
+  <si>
+    <t>rskfk_tumorth</t>
+  </si>
+  <si>
+    <t>Tumorth.</t>
+  </si>
+  <si>
+    <t>rskfk_opiat</t>
+  </si>
+  <si>
+    <t>Opiat</t>
+  </si>
+  <si>
+    <t>rskfk_atcn</t>
+  </si>
+  <si>
+    <t>ATC N</t>
+  </si>
+  <si>
+    <t>rskfk_ait</t>
+  </si>
+  <si>
+    <t>AIT</t>
+  </si>
+  <si>
+    <t>rskfk_anzam</t>
+  </si>
+  <si>
+    <t>Anz AM</t>
+  </si>
+  <si>
+    <t>rskfk_priscus</t>
+  </si>
+  <si>
+    <t>PRISCUS</t>
+  </si>
+  <si>
+    <t>rskfk_qtc</t>
+  </si>
+  <si>
+    <t>QTc</t>
+  </si>
+  <si>
+    <t>rskfk_meld</t>
+  </si>
+  <si>
+    <t>MELD</t>
+  </si>
+  <si>
+    <t>rskfk_dialyse</t>
+  </si>
+  <si>
+    <t>Dialyse</t>
+  </si>
+  <si>
+    <t>rskfk_entern</t>
+  </si>
+  <si>
+    <t>ent. Ern.</t>
+  </si>
+  <si>
+    <t>rskfkt_anz_rskamklassen</t>
+  </si>
+  <si>
+    <t>Aggregation der Felder 27-33: Anzahl der Felder mit Ausprägung &gt;0</t>
+  </si>
+  <si>
+    <t>risikofaktor_complete</t>
+  </si>
+  <si>
+    <t>trigger</t>
+  </si>
+  <si>
+    <t>trg_ast</t>
+  </si>
+  <si>
+    <t>AST</t>
+  </si>
+  <si>
+    <t>trg_alt</t>
+  </si>
+  <si>
+    <t>ALT↑</t>
+  </si>
+  <si>
+    <t>trg_crp</t>
+  </si>
+  <si>
+    <t>CRP↑</t>
+  </si>
+  <si>
+    <t>trg_leuk_penie</t>
+  </si>
+  <si>
+    <t>Leuko↓</t>
+  </si>
+  <si>
+    <t>trg_leuk_ose</t>
+  </si>
+  <si>
+    <t>Leuko↑</t>
+  </si>
+  <si>
+    <t>trg_thrmb_penie</t>
+  </si>
+  <si>
+    <t>Thrombo↓</t>
+  </si>
+  <si>
+    <t>trg_aptt</t>
+  </si>
+  <si>
+    <t>aPTT</t>
+  </si>
+  <si>
+    <t>trg_hyp_haem</t>
+  </si>
+  <si>
+    <t>Hb↓</t>
+  </si>
+  <si>
+    <t>trg_hypo_glyk</t>
+  </si>
+  <si>
+    <t>Glc↓</t>
+  </si>
+  <si>
+    <t>trg_hyper_glyk</t>
+  </si>
+  <si>
+    <t>Glc↑</t>
+  </si>
+  <si>
+    <t>trg_hyper_bilirbnm</t>
+  </si>
+  <si>
+    <t>Bili↑</t>
+  </si>
+  <si>
+    <t>trg_ck</t>
+  </si>
+  <si>
+    <t>CK↑</t>
+  </si>
+  <si>
+    <t>trg_hypo_serablmn</t>
+  </si>
+  <si>
+    <t>Alb↓</t>
+  </si>
+  <si>
+    <t>trg_hypo_nat</t>
+  </si>
+  <si>
+    <t>Na+↓</t>
+  </si>
+  <si>
+    <t>trg_hyper_nat</t>
+  </si>
+  <si>
+    <t>Na+↑</t>
+  </si>
+  <si>
+    <t>trg_hyper_kal</t>
+  </si>
+  <si>
+    <t>K+↓</t>
+  </si>
+  <si>
+    <t>trg_hypo_kal</t>
+  </si>
+  <si>
+    <t>K+↑</t>
+  </si>
+  <si>
+    <t>trg_inr_ern</t>
+  </si>
+  <si>
+    <t>INR Antikoag↓</t>
+  </si>
+  <si>
+    <t>trg_inr_erh</t>
+  </si>
+  <si>
+    <t>INR ↑</t>
+  </si>
+  <si>
+    <t>trg_inr_erh_antikoa</t>
+  </si>
+  <si>
+    <t>INR Antikoag↑</t>
+  </si>
+  <si>
+    <t>trg_krea</t>
+  </si>
+  <si>
+    <t>Krea↑</t>
+  </si>
+  <si>
+    <t>trg_egfr</t>
+  </si>
+  <si>
+    <t>eGFR&lt;30</t>
+  </si>
+  <si>
+    <t>trigger_complete</t>
+  </si>
+  <si>
+    <t>mrpdokumentation_validierung_complete</t>
+  </si>
+  <si>
+    <t>mrp_merp_info___1</t>
+  </si>
+  <si>
+    <t>mrp_mf_info___1</t>
+  </si>
+  <si>
+    <t>mrp_pi_info___1</t>
+  </si>
+  <si>
+    <t>fall_bettplatz</t>
+  </si>
+  <si>
+    <t>Bettplatz wie vom DIZ Definiert</t>
+  </si>
+  <si>
+    <t>fall_zimmernr</t>
+  </si>
+  <si>
+    <t>Zimmernummer wie vom DIZ Definiert</t>
+  </si>
+  <si>
+    <t>mrp_femb_22</t>
+  </si>
+  <si>
+    <t>mrp_gewissheit_oth</t>
+  </si>
+  <si>
+    <t>Textfeld, wenn mrp_gewissheit = 2 MRP möglich, weitere Informationen nötig</t>
+  </si>
+  <si>
+    <t>mrp_femb_23</t>
+  </si>
+  <si>
+    <t>mrp_hinweisgeber_oth</t>
+  </si>
+  <si>
+    <t>Textfeld, wenn mrp_hinweisgeber = 7 (andere)</t>
+  </si>
+  <si>
+    <t>mrp_merp_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frontend Complete-Status, wenn ein Pflichtitem fehlt Status bei Import wieder auf Incomplete setzen </t>
+  </si>
+  <si>
     <t>mrp_wiedervorlage</t>
   </si>
   <si>
     <t>MRP Wiedervorlage</t>
-  </si>
-  <si>
-    <t>risikofaktor</t>
-  </si>
-  <si>
-    <t>rskfk_gerhemmer</t>
-  </si>
-  <si>
-    <t>Ger.hemmer</t>
-  </si>
-  <si>
-    <t>rskfk_tah</t>
-  </si>
-  <si>
-    <t>TAH</t>
-  </si>
-  <si>
-    <t>rskfk_immunsupp</t>
-  </si>
-  <si>
-    <t>Immunsupp.</t>
-  </si>
-  <si>
-    <t>rskfk_tumorth</t>
-  </si>
-  <si>
-    <t>Tumorth.</t>
-  </si>
-  <si>
-    <t>rskfk_opiat</t>
-  </si>
-  <si>
-    <t>Opiat</t>
-  </si>
-  <si>
-    <t>rskfk_atcn</t>
-  </si>
-  <si>
-    <t>ATC N</t>
-  </si>
-  <si>
-    <t>rskfk_ait</t>
-  </si>
-  <si>
-    <t>AIT</t>
-  </si>
-  <si>
-    <t>rskfk_anzam</t>
-  </si>
-  <si>
-    <t>Anz AM</t>
-  </si>
-  <si>
-    <t>rskfk_priscus</t>
-  </si>
-  <si>
-    <t>PRISCUS</t>
-  </si>
-  <si>
-    <t>rskfk_qtc</t>
-  </si>
-  <si>
-    <t>QTc</t>
-  </si>
-  <si>
-    <t>rskfk_meld</t>
-  </si>
-  <si>
-    <t>MELD</t>
-  </si>
-  <si>
-    <t>rskfk_dialyse</t>
-  </si>
-  <si>
-    <t>Dialyse</t>
-  </si>
-  <si>
-    <t>rskfk_entern</t>
-  </si>
-  <si>
-    <t>ent. Ern.</t>
-  </si>
-  <si>
-    <t>rskfkt_anz_rskamklassen</t>
-  </si>
-  <si>
-    <t>Aggregation der Felder 27-33: Anzahl der Felder mit Ausprägung &gt;0</t>
-  </si>
-  <si>
-    <t>risikofaktor_complete</t>
-  </si>
-  <si>
-    <t>trigger</t>
-  </si>
-  <si>
-    <t>trg_ast</t>
-  </si>
-  <si>
-    <t>AST</t>
-  </si>
-  <si>
-    <t>trg_alt</t>
-  </si>
-  <si>
-    <t>ALT↑</t>
-  </si>
-  <si>
-    <t>trg_crp</t>
-  </si>
-  <si>
-    <t>CRP↑</t>
-  </si>
-  <si>
-    <t>trg_leuk_penie</t>
-  </si>
-  <si>
-    <t>Leuko↓</t>
-  </si>
-  <si>
-    <t>trg_leuk_ose</t>
-  </si>
-  <si>
-    <t>Leuko↑</t>
-  </si>
-  <si>
-    <t>trg_thrmb_penie</t>
-  </si>
-  <si>
-    <t>Thrombo↓</t>
-  </si>
-  <si>
-    <t>trg_aptt</t>
-  </si>
-  <si>
-    <t>aPTT</t>
-  </si>
-  <si>
-    <t>trg_hyp_haem</t>
-  </si>
-  <si>
-    <t>Hb↓</t>
-  </si>
-  <si>
-    <t>trg_hypo_glyk</t>
-  </si>
-  <si>
-    <t>Glc↓</t>
-  </si>
-  <si>
-    <t>trg_hyper_glyk</t>
-  </si>
-  <si>
-    <t>Glc↑</t>
-  </si>
-  <si>
-    <t>trg_hyper_bilirbnm</t>
-  </si>
-  <si>
-    <t>Bili↑</t>
-  </si>
-  <si>
-    <t>trg_ck</t>
-  </si>
-  <si>
-    <t>CK↑</t>
-  </si>
-  <si>
-    <t>trg_hypo_serablmn</t>
-  </si>
-  <si>
-    <t>Alb↓</t>
-  </si>
-  <si>
-    <t>trg_hypo_nat</t>
-  </si>
-  <si>
-    <t>Na+↓</t>
-  </si>
-  <si>
-    <t>trg_hyper_nat</t>
-  </si>
-  <si>
-    <t>Na+↑</t>
-  </si>
-  <si>
-    <t>trg_hyper_kal</t>
-  </si>
-  <si>
-    <t>K+↓</t>
-  </si>
-  <si>
-    <t>trg_hypo_kal</t>
-  </si>
-  <si>
-    <t>K+↑</t>
-  </si>
-  <si>
-    <t>trg_inr_ern</t>
-  </si>
-  <si>
-    <t>INR Antikoag↓</t>
-  </si>
-  <si>
-    <t>trg_inr_erh</t>
-  </si>
-  <si>
-    <t>INR ↑</t>
-  </si>
-  <si>
-    <t>trg_inr_erh_antikoa</t>
-  </si>
-  <si>
-    <t>INR Antikoag↑</t>
-  </si>
-  <si>
-    <t>trg_krea</t>
-  </si>
-  <si>
-    <t>Krea↑</t>
-  </si>
-  <si>
-    <t>trg_egfr</t>
-  </si>
-  <si>
-    <t>eGFR&lt;30</t>
-  </si>
-  <si>
-    <t>trigger_complete</t>
-  </si>
-  <si>
-    <t>mrpdokumentation_validierung_complete</t>
-  </si>
-  <si>
-    <t>mrp_merp_info___1</t>
-  </si>
-  <si>
-    <t>mrp_mf_info___1</t>
-  </si>
-  <si>
-    <t>mrp_pi_info___1</t>
-  </si>
-  <si>
-    <t>meda_risiko_pat_info___1</t>
   </si>
 </sst>
 </file>
@@ -1750,7 +1750,7 @@
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
@@ -1759,6 +1759,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2114,10 +2115,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F452"/>
+  <dimension ref="A1:F448"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D198" sqref="D198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2231,10 +2232,10 @@
         <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>12</v>
@@ -2246,10 +2247,10 @@
         <v>13</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>12</v>
@@ -2261,13 +2262,13 @@
         <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E9" s="3"/>
     </row>
@@ -2276,13 +2277,13 @@
         <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="E10" s="3"/>
     </row>
@@ -2291,13 +2292,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E11" s="3"/>
     </row>
@@ -2306,25 +2307,25 @@
         <v>13</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>12</v>
@@ -2336,10 +2337,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>12</v>
@@ -2348,13 +2349,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="C15" s="3" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>12</v>
@@ -2366,10 +2367,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>12</v>
@@ -2381,13 +2382,13 @@
         <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="E17" s="3"/>
     </row>
@@ -2396,10 +2397,10 @@
         <v>13</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>12</v>
@@ -2411,13 +2412,13 @@
         <v>13</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="E19" s="3"/>
     </row>
@@ -2426,10 +2427,10 @@
         <v>13</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>12</v>
@@ -2441,10 +2442,10 @@
         <v>13</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>12</v>
@@ -2456,10 +2457,10 @@
         <v>13</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>12</v>
@@ -2471,10 +2472,10 @@
         <v>13</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>51</v>
+        <v>398</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>52</v>
+        <v>399</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>12</v>
@@ -2486,10 +2487,10 @@
         <v>13</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>53</v>
+        <v>400</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>54</v>
+        <v>401</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>12</v>
@@ -2501,13 +2502,13 @@
         <v>13</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E25" s="3"/>
     </row>
@@ -2516,10 +2517,10 @@
         <v>13</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>12</v>
@@ -2531,13 +2532,13 @@
         <v>13</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E27" s="3"/>
     </row>
@@ -2546,10 +2547,10 @@
         <v>13</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>12</v>
@@ -2561,13 +2562,13 @@
         <v>13</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E29" s="3"/>
     </row>
@@ -2576,10 +2577,10 @@
         <v>13</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>12</v>
@@ -2591,13 +2592,13 @@
         <v>13</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E31" s="3"/>
     </row>
@@ -2606,7 +2607,7 @@
         <v>13</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>15</v>
@@ -2621,7 +2622,7 @@
         <v>13</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>15</v>
@@ -2636,7 +2637,7 @@
         <v>13</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>15</v>
@@ -2651,7 +2652,7 @@
         <v>13</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>15</v>
@@ -2666,7 +2667,7 @@
         <v>13</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>15</v>
@@ -2681,10 +2682,10 @@
         <v>13</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>12</v>
@@ -2696,7 +2697,7 @@
         <v>13</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>15</v>
@@ -2711,10 +2712,10 @@
         <v>13</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>12</v>
@@ -2726,7 +2727,7 @@
         <v>13</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>15</v>
@@ -2741,10 +2742,10 @@
         <v>13</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>12</v>
@@ -2756,10 +2757,10 @@
         <v>13</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>12</v>
@@ -2771,7 +2772,7 @@
         <v>13</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>15</v>
@@ -2786,10 +2787,10 @@
         <v>13</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>12</v>
@@ -2801,10 +2802,10 @@
         <v>13</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>12</v>
@@ -2816,7 +2817,7 @@
         <v>13</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>15</v>
@@ -2831,10 +2832,10 @@
         <v>13</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>12</v>
@@ -2846,13 +2847,13 @@
         <v>13</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>15</v>
+        <v>91</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E48" s="3"/>
     </row>
@@ -2861,55 +2862,53 @@
         <v>13</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>94</v>
+        <v>36</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E49" s="3"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>95</v>
+        <v>10</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>96</v>
+        <v>11</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E50" s="3"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>98</v>
+        <v>15</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E51" s="3"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>12</v>
@@ -2917,13 +2916,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>12</v>
@@ -2934,7 +2933,7 @@
         <v>13</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>15</v>
@@ -2948,7 +2947,7 @@
         <v>13</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>15</v>
@@ -2962,7 +2961,7 @@
         <v>13</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>15</v>
@@ -2976,13 +2975,13 @@
         <v>13</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>15</v>
+        <v>101</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2990,10 +2989,10 @@
         <v>13</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>105</v>
+        <v>21</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>15</v>
+        <v>102</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>12</v>
@@ -3004,10 +3003,10 @@
         <v>13</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>106</v>
+        <v>22</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>12</v>
@@ -3018,13 +3017,13 @@
         <v>13</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -3032,10 +3031,10 @@
         <v>13</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>21</v>
+        <v>105</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>12</v>
@@ -3046,10 +3045,10 @@
         <v>13</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>23</v>
+        <v>107</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>50</v>
+        <v>108</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>12</v>
@@ -3060,13 +3059,13 @@
         <v>13</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>111</v>
+        <v>15</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -3074,10 +3073,10 @@
         <v>13</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>12</v>
@@ -3088,10 +3087,10 @@
         <v>13</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>115</v>
+        <v>15</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>12</v>
@@ -3102,10 +3101,10 @@
         <v>13</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>15</v>
+        <v>114</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>12</v>
@@ -3116,10 +3115,10 @@
         <v>13</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>411</v>
+        <v>115</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>12</v>
@@ -3133,7 +3132,7 @@
         <v>117</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>15</v>
+        <v>118</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>12</v>
@@ -3144,13 +3143,13 @@
         <v>13</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>119</v>
+        <v>15</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3161,10 +3160,10 @@
         <v>120</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>15</v>
+        <v>121</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3172,10 +3171,10 @@
         <v>13</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>12</v>
@@ -3186,10 +3185,10 @@
         <v>13</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>12</v>
@@ -3197,13 +3196,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>13</v>
+        <v>125</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>124</v>
+        <v>10</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>125</v>
+        <v>11</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>12</v>
@@ -3220,7 +3219,7 @@
         <v>127</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -3228,10 +3227,10 @@
         <v>13</v>
       </c>
       <c r="B75" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C75" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>129</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>12</v>
@@ -3242,13 +3241,13 @@
         <v>13</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>130</v>
+        <v>22</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -3256,13 +3255,13 @@
         <v>13</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>132</v>
+        <v>15</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -3270,10 +3269,10 @@
         <v>13</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>134</v>
+        <v>15</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>12</v>
@@ -3284,10 +3283,10 @@
         <v>13</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>12</v>
@@ -3295,13 +3294,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>136</v>
+        <v>13</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>10</v>
+        <v>132</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>12</v>
@@ -3312,13 +3311,13 @@
         <v>13</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>138</v>
+        <v>15</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -3326,10 +3325,10 @@
         <v>13</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>21</v>
+        <v>397</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>139</v>
+        <v>15</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>12</v>
@@ -3340,10 +3339,10 @@
         <v>13</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>12</v>
@@ -3354,7 +3353,7 @@
         <v>13</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>140</v>
+        <v>396</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>15</v>
@@ -3368,7 +3367,7 @@
         <v>13</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>15</v>
@@ -3382,7 +3381,7 @@
         <v>13</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>15</v>
@@ -3396,7 +3395,7 @@
         <v>13</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>15</v>
@@ -3410,7 +3409,7 @@
         <v>13</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>15</v>
@@ -3424,7 +3423,7 @@
         <v>13</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>410</v>
+        <v>139</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>15</v>
@@ -3438,13 +3437,13 @@
         <v>13</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>15</v>
+        <v>141</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -3452,10 +3451,10 @@
         <v>13</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>409</v>
+        <v>142</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>15</v>
+        <v>143</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>12</v>
@@ -3466,10 +3465,10 @@
         <v>13</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>15</v>
+        <v>145</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>12</v>
@@ -3480,7 +3479,7 @@
         <v>13</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>15</v>
@@ -3494,10 +3493,10 @@
         <v>13</v>
       </c>
       <c r="B94" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C94" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>12</v>
@@ -3525,7 +3524,7 @@
         <v>150</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>15</v>
+        <v>151</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>12</v>
@@ -3536,13 +3535,13 @@
         <v>13</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>151</v>
+        <v>402</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>152</v>
+        <v>15</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -3550,10 +3549,10 @@
         <v>13</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>153</v>
+        <v>403</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>154</v>
+        <v>404</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>12</v>
@@ -3564,10 +3563,10 @@
         <v>13</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>155</v>
+        <v>405</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>156</v>
+        <v>15</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>12</v>
@@ -3578,10 +3577,10 @@
         <v>13</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>157</v>
+        <v>406</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>15</v>
+        <v>407</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>12</v>
@@ -3592,10 +3591,10 @@
         <v>13</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>159</v>
+        <v>15</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>12</v>
@@ -3606,10 +3605,10 @@
         <v>13</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>15</v>
+        <v>154</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>12</v>
@@ -3620,10 +3619,10 @@
         <v>13</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>162</v>
+        <v>15</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>12</v>
@@ -3634,10 +3633,10 @@
         <v>13</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>15</v>
+        <v>157</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>12</v>
@@ -3648,10 +3647,10 @@
         <v>13</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>165</v>
+        <v>15</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>12</v>
@@ -3662,7 +3661,7 @@
         <v>13</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>15</v>
@@ -3676,10 +3675,10 @@
         <v>13</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>168</v>
+        <v>15</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>12</v>
@@ -3690,7 +3689,7 @@
         <v>13</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>15</v>
@@ -3704,7 +3703,7 @@
         <v>13</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>15</v>
@@ -3718,7 +3717,7 @@
         <v>13</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>15</v>
@@ -3732,10 +3731,10 @@
         <v>13</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>15</v>
+        <v>165</v>
       </c>
       <c r="D111" s="3" t="s">
         <v>12</v>
@@ -3746,7 +3745,7 @@
         <v>13</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C112" s="3" t="s">
         <v>15</v>
@@ -3760,10 +3759,10 @@
         <v>13</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>15</v>
+        <v>168</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>12</v>
@@ -3774,10 +3773,10 @@
         <v>13</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>176</v>
+        <v>15</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>12</v>
@@ -3788,10 +3787,10 @@
         <v>13</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>15</v>
+        <v>171</v>
       </c>
       <c r="D115" s="3" t="s">
         <v>12</v>
@@ -3802,10 +3801,10 @@
         <v>13</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>179</v>
+        <v>15</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>12</v>
@@ -3816,10 +3815,10 @@
         <v>13</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>15</v>
+        <v>174</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>12</v>
@@ -3830,10 +3829,10 @@
         <v>13</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>182</v>
+        <v>15</v>
       </c>
       <c r="D118" s="3" t="s">
         <v>12</v>
@@ -3844,10 +3843,10 @@
         <v>13</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>15</v>
+        <v>177</v>
       </c>
       <c r="D119" s="3" t="s">
         <v>12</v>
@@ -3858,10 +3857,10 @@
         <v>13</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>185</v>
+        <v>15</v>
       </c>
       <c r="D120" s="3" t="s">
         <v>12</v>
@@ -3872,10 +3871,10 @@
         <v>13</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>15</v>
+        <v>180</v>
       </c>
       <c r="D121" s="3" t="s">
         <v>12</v>
@@ -3886,10 +3885,10 @@
         <v>13</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>188</v>
+        <v>15</v>
       </c>
       <c r="D122" s="3" t="s">
         <v>12</v>
@@ -3900,10 +3899,10 @@
         <v>13</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>15</v>
+        <v>183</v>
       </c>
       <c r="D123" s="3" t="s">
         <v>12</v>
@@ -3914,10 +3913,10 @@
         <v>13</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>191</v>
+        <v>15</v>
       </c>
       <c r="D124" s="3" t="s">
         <v>12</v>
@@ -3928,10 +3927,10 @@
         <v>13</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>15</v>
+        <v>186</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>12</v>
@@ -3942,10 +3941,10 @@
         <v>13</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>12</v>
@@ -3956,10 +3955,10 @@
         <v>13</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>15</v>
+        <v>190</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>12</v>
@@ -3970,10 +3969,10 @@
         <v>13</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>197</v>
+        <v>15</v>
       </c>
       <c r="D128" s="3" t="s">
         <v>12</v>
@@ -3984,10 +3983,10 @@
         <v>13</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D129" s="3" t="s">
         <v>12</v>
@@ -3998,10 +3997,10 @@
         <v>13</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D130" s="3" t="s">
         <v>12</v>
@@ -4012,10 +4011,10 @@
         <v>13</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>15</v>
+        <v>197</v>
       </c>
       <c r="D131" s="3" t="s">
         <v>12</v>
@@ -4026,10 +4025,10 @@
         <v>13</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D132" s="3" t="s">
         <v>12</v>
@@ -4040,10 +4039,10 @@
         <v>13</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D133" s="3" t="s">
         <v>12</v>
@@ -4054,10 +4053,10 @@
         <v>13</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D134" s="3" t="s">
         <v>12</v>
@@ -4068,10 +4067,10 @@
         <v>13</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D135" s="3" t="s">
         <v>12</v>
@@ -4082,10 +4081,10 @@
         <v>13</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D136" s="3" t="s">
         <v>12</v>
@@ -4096,10 +4095,10 @@
         <v>13</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D137" s="3" t="s">
         <v>12</v>
@@ -4110,10 +4109,10 @@
         <v>13</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D138" s="3" t="s">
         <v>12</v>
@@ -4124,10 +4123,10 @@
         <v>13</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D139" s="3" t="s">
         <v>12</v>
@@ -4138,10 +4137,10 @@
         <v>13</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D140" s="3" t="s">
         <v>12</v>
@@ -4152,10 +4151,10 @@
         <v>13</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D141" s="3" t="s">
         <v>12</v>
@@ -4166,10 +4165,10 @@
         <v>13</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D142" s="3" t="s">
         <v>12</v>
@@ -4180,10 +4179,10 @@
         <v>13</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D143" s="3" t="s">
         <v>12</v>
@@ -4194,10 +4193,10 @@
         <v>13</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D144" s="3" t="s">
         <v>12</v>
@@ -4208,10 +4207,10 @@
         <v>13</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D145" s="3" t="s">
         <v>12</v>
@@ -4222,10 +4221,10 @@
         <v>13</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D146" s="3" t="s">
         <v>12</v>
@@ -4236,10 +4235,10 @@
         <v>13</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D147" s="3" t="s">
         <v>12</v>
@@ -4250,10 +4249,10 @@
         <v>13</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D148" s="3" t="s">
         <v>12</v>
@@ -4264,10 +4263,10 @@
         <v>13</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D149" s="3" t="s">
         <v>12</v>
@@ -4278,10 +4277,10 @@
         <v>13</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D150" s="3" t="s">
         <v>12</v>
@@ -4292,10 +4291,10 @@
         <v>13</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D151" s="3" t="s">
         <v>12</v>
@@ -4306,10 +4305,10 @@
         <v>13</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D152" s="3" t="s">
         <v>12</v>
@@ -4320,10 +4319,10 @@
         <v>13</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D153" s="3" t="s">
         <v>12</v>
@@ -4334,10 +4333,10 @@
         <v>13</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D154" s="3" t="s">
         <v>12</v>
@@ -4348,10 +4347,10 @@
         <v>13</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D155" s="3" t="s">
         <v>12</v>
@@ -4362,10 +4361,10 @@
         <v>13</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D156" s="3" t="s">
         <v>12</v>
@@ -4376,10 +4375,10 @@
         <v>13</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>254</v>
+        <v>15</v>
       </c>
       <c r="D157" s="3" t="s">
         <v>12</v>
@@ -4390,10 +4389,10 @@
         <v>13</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="D158" s="3" t="s">
         <v>12</v>
@@ -4404,10 +4403,10 @@
         <v>13</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="D159" s="3" t="s">
         <v>12</v>
@@ -4418,10 +4417,10 @@
         <v>13</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>15</v>
+        <v>254</v>
       </c>
       <c r="D160" s="3" t="s">
         <v>12</v>
@@ -4432,10 +4431,10 @@
         <v>13</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D161" s="3" t="s">
         <v>12</v>
@@ -4446,10 +4445,10 @@
         <v>13</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D162" s="3" t="s">
         <v>12</v>
@@ -4460,10 +4459,10 @@
         <v>13</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D163" s="3" t="s">
         <v>12</v>
@@ -4474,10 +4473,10 @@
         <v>13</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>267</v>
+        <v>15</v>
       </c>
       <c r="D164" s="3" t="s">
         <v>12</v>
@@ -4488,10 +4487,10 @@
         <v>13</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>269</v>
+        <v>15</v>
       </c>
       <c r="D165" s="3" t="s">
         <v>12</v>
@@ -4502,10 +4501,10 @@
         <v>13</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="D166" s="3" t="s">
         <v>12</v>
@@ -4516,10 +4515,10 @@
         <v>13</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>15</v>
+        <v>266</v>
       </c>
       <c r="D167" s="3" t="s">
         <v>12</v>
@@ -4530,7 +4529,7 @@
         <v>13</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="C168" s="3" t="s">
         <v>15</v>
@@ -4544,10 +4543,10 @@
         <v>13</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="D169" s="3" t="s">
         <v>12</v>
@@ -4558,10 +4557,10 @@
         <v>13</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D170" s="3" t="s">
         <v>12</v>
@@ -4572,10 +4571,10 @@
         <v>13</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>15</v>
+        <v>273</v>
       </c>
       <c r="D171" s="3" t="s">
         <v>12</v>
@@ -4586,10 +4585,10 @@
         <v>13</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D172" s="3" t="s">
         <v>12</v>
@@ -4600,10 +4599,10 @@
         <v>13</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D173" s="3" t="s">
         <v>12</v>
@@ -4614,10 +4613,10 @@
         <v>13</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D174" s="3" t="s">
         <v>12</v>
@@ -4628,10 +4627,10 @@
         <v>13</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="D175" s="3" t="s">
         <v>12</v>
@@ -4642,10 +4641,10 @@
         <v>13</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D176" s="3" t="s">
         <v>12</v>
@@ -4656,10 +4655,10 @@
         <v>13</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="D177" s="3" t="s">
         <v>12</v>
@@ -4670,10 +4669,10 @@
         <v>13</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="D178" s="3" t="s">
         <v>12</v>
@@ -4684,10 +4683,10 @@
         <v>13</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D179" s="3" t="s">
         <v>12</v>
@@ -4698,10 +4697,10 @@
         <v>13</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>296</v>
+        <v>15</v>
       </c>
       <c r="D180" s="3" t="s">
         <v>12</v>
@@ -4712,10 +4711,10 @@
         <v>13</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="D181" s="3" t="s">
         <v>12</v>
@@ -4726,10 +4725,10 @@
         <v>13</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="D182" s="3" t="s">
         <v>12</v>
@@ -4740,10 +4739,10 @@
         <v>13</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="C183" s="3" t="s">
-        <v>15</v>
+        <v>296</v>
       </c>
       <c r="D183" s="3" t="s">
         <v>12</v>
@@ -4754,10 +4753,10 @@
         <v>13</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="C184" s="3" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D184" s="3" t="s">
         <v>12</v>
@@ -4768,10 +4767,10 @@
         <v>13</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="D185" s="3" t="s">
         <v>12</v>
@@ -4782,10 +4781,10 @@
         <v>13</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="D186" s="3" t="s">
         <v>12</v>
@@ -4796,10 +4795,10 @@
         <v>13</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="D187" s="3" t="s">
         <v>12</v>
@@ -4810,10 +4809,10 @@
         <v>13</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="D188" s="3" t="s">
         <v>12</v>
@@ -4824,10 +4823,10 @@
         <v>13</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D189" s="3" t="s">
         <v>12</v>
@@ -4838,10 +4837,10 @@
         <v>13</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>315</v>
+        <v>15</v>
       </c>
       <c r="D190" s="3" t="s">
         <v>12</v>
@@ -4852,10 +4851,10 @@
         <v>13</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="D191" s="3" t="s">
         <v>12</v>
@@ -4866,10 +4865,10 @@
         <v>13</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>319</v>
+        <v>15</v>
       </c>
       <c r="D192" s="3" t="s">
         <v>12</v>
@@ -4880,10 +4879,10 @@
         <v>13</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>15</v>
+        <v>314</v>
       </c>
       <c r="D193" s="3" t="s">
         <v>12</v>
@@ -4894,10 +4893,10 @@
         <v>13</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="D194" s="3" t="s">
         <v>12</v>
@@ -4908,7 +4907,7 @@
         <v>13</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>323</v>
+        <v>408</v>
       </c>
       <c r="C195" s="3" t="s">
         <v>15</v>
@@ -4922,10 +4921,10 @@
         <v>13</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>324</v>
+        <v>395</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>325</v>
+        <v>15</v>
       </c>
       <c r="D196" s="3" t="s">
         <v>12</v>
@@ -4936,24 +4935,22 @@
         <v>13</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>327</v>
+        <v>15</v>
       </c>
       <c r="D197" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B198" s="3" t="s">
-        <v>408</v>
-      </c>
-      <c r="C198" s="3" t="s">
-        <v>15</v>
+      <c r="A198" s="3"/>
+      <c r="B198" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="C198" s="4" t="s">
+        <v>411</v>
       </c>
       <c r="D198" s="3" t="s">
         <v>12</v>
@@ -4964,10 +4961,10 @@
         <v>13</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>328</v>
+        <v>394</v>
       </c>
       <c r="C199" s="3" t="s">
-        <v>15</v>
+        <v>409</v>
       </c>
       <c r="D199" s="3" t="s">
         <v>12</v>
@@ -4975,13 +4972,13 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="s">
-        <v>13</v>
+        <v>318</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>329</v>
+        <v>10</v>
       </c>
       <c r="C200" s="3" t="s">
-        <v>330</v>
+        <v>11</v>
       </c>
       <c r="D200" s="3" t="s">
         <v>12</v>
@@ -4992,10 +4989,10 @@
         <v>13</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>407</v>
+        <v>43</v>
       </c>
       <c r="C201" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D201" s="3" t="s">
         <v>12</v>
@@ -5003,16 +5000,16 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
-        <v>331</v>
+        <v>13</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>10</v>
+        <v>319</v>
       </c>
       <c r="C202" s="3" t="s">
-        <v>11</v>
+        <v>320</v>
       </c>
       <c r="D202" s="3" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -5020,10 +5017,10 @@
         <v>13</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>45</v>
+        <v>321</v>
       </c>
       <c r="C203" s="3" t="s">
-        <v>46</v>
+        <v>322</v>
       </c>
       <c r="D203" s="3" t="s">
         <v>12</v>
@@ -5034,13 +5031,13 @@
         <v>13</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="C204" s="3" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -5048,10 +5045,10 @@
         <v>13</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="C205" s="3" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="D205" s="3" t="s">
         <v>12</v>
@@ -5062,10 +5059,10 @@
         <v>13</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="C206" s="3" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="D206" s="3" t="s">
         <v>12</v>
@@ -5076,10 +5073,10 @@
         <v>13</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="C207" s="3" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="D207" s="3" t="s">
         <v>12</v>
@@ -5090,10 +5087,10 @@
         <v>13</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="D208" s="3" t="s">
         <v>12</v>
@@ -5104,10 +5101,10 @@
         <v>13</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="C209" s="3" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="D209" s="3" t="s">
         <v>12</v>
@@ -5118,10 +5115,10 @@
         <v>13</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="C210" s="3" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="D210" s="3" t="s">
         <v>12</v>
@@ -5132,10 +5129,10 @@
         <v>13</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="C211" s="3" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="D211" s="3" t="s">
         <v>12</v>
@@ -5146,10 +5143,10 @@
         <v>13</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="C212" s="3" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="D212" s="3" t="s">
         <v>12</v>
@@ -5160,10 +5157,10 @@
         <v>13</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="C213" s="3" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="D213" s="3" t="s">
         <v>12</v>
@@ -5174,10 +5171,10 @@
         <v>13</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="C214" s="3" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="D214" s="3" t="s">
         <v>12</v>
@@ -5188,10 +5185,10 @@
         <v>13</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="C215" s="3" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="D215" s="3" t="s">
         <v>12</v>
@@ -5202,10 +5199,10 @@
         <v>13</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="C216" s="3" t="s">
-        <v>357</v>
+        <v>36</v>
       </c>
       <c r="D216" s="3" t="s">
         <v>12</v>
@@ -5213,13 +5210,13 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
-        <v>13</v>
+        <v>348</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>358</v>
+        <v>43</v>
       </c>
       <c r="C217" s="3" t="s">
-        <v>359</v>
+        <v>44</v>
       </c>
       <c r="D217" s="3" t="s">
         <v>12</v>
@@ -5230,24 +5227,24 @@
         <v>13</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>360</v>
+        <v>10</v>
       </c>
       <c r="C218" s="3" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>361</v>
+        <v>13</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>45</v>
+        <v>349</v>
       </c>
       <c r="C219" s="3" t="s">
-        <v>46</v>
+        <v>350</v>
       </c>
       <c r="D219" s="3" t="s">
         <v>12</v>
@@ -5258,13 +5255,13 @@
         <v>13</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>10</v>
+        <v>351</v>
       </c>
       <c r="C220" s="3" t="s">
-        <v>11</v>
+        <v>352</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -5272,10 +5269,10 @@
         <v>13</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="C221" s="3" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="D221" s="3" t="s">
         <v>12</v>
@@ -5286,10 +5283,10 @@
         <v>13</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="C222" s="3" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="D222" s="3" t="s">
         <v>12</v>
@@ -5300,10 +5297,10 @@
         <v>13</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C223" s="3" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="D223" s="3" t="s">
         <v>12</v>
@@ -5314,10 +5311,10 @@
         <v>13</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="C224" s="3" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="D224" s="3" t="s">
         <v>12</v>
@@ -5328,10 +5325,10 @@
         <v>13</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="C225" s="3" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="D225" s="3" t="s">
         <v>12</v>
@@ -5342,10 +5339,10 @@
         <v>13</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="C226" s="3" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="D226" s="3" t="s">
         <v>12</v>
@@ -5356,10 +5353,10 @@
         <v>13</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="C227" s="3" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="D227" s="3" t="s">
         <v>12</v>
@@ -5370,10 +5367,10 @@
         <v>13</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="C228" s="3" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="D228" s="3" t="s">
         <v>12</v>
@@ -5384,10 +5381,10 @@
         <v>13</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="C229" s="3" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="D229" s="3" t="s">
         <v>12</v>
@@ -5398,10 +5395,10 @@
         <v>13</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="C230" s="3" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="D230" s="3" t="s">
         <v>12</v>
@@ -5412,10 +5409,10 @@
         <v>13</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="C231" s="3" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="D231" s="3" t="s">
         <v>12</v>
@@ -5426,68 +5423,68 @@
         <v>13</v>
       </c>
       <c r="B232" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C232" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="D232" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="D233" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="D234" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A235" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B235" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="C235" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="D235" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A236" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C236" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="C232" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="D232" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B233" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="C233" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="D233" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B234" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="C234" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="D234" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A235" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B235" s="3" t="s">
-        <v>390</v>
-      </c>
-      <c r="C235" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="D235" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A236" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B236" s="3" t="s">
-        <v>392</v>
-      </c>
-      <c r="C236" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="D236" s="3" t="s">
+      <c r="D236" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -5496,10 +5493,10 @@
         <v>13</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="D237" s="2" t="s">
         <v>12</v>
@@ -5510,10 +5507,10 @@
         <v>13</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="D238" s="2" t="s">
         <v>12</v>
@@ -5524,10 +5521,10 @@
         <v>13</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="D239" s="2" t="s">
         <v>12</v>
@@ -5538,10 +5535,10 @@
         <v>13</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="D240" s="2" t="s">
         <v>12</v>
@@ -5552,122 +5549,17 @@
         <v>13</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>403</v>
+        <v>36</v>
       </c>
       <c r="D241" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A242" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B242" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="C242" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="D242" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A243" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B243" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="C243" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D243" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A244" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B244" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C244" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A245" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B245" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C245" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A246" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B246" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C246" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A247" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B247" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C247" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A248" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B248" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C248" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A249" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B249" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C249" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A250" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B250" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C250" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="451" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="452" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add necessary redcap columns also for non-repeating instruments - must not be removed
</commit_message>
<xml_diff>
--- a/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
+++ b/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="413">
   <si>
     <t xml:space="preserve">Station </t>
   </si>
@@ -1261,6 +1261,9 @@
   </si>
   <si>
     <t>MRP Wiedervorlage</t>
+  </si>
+  <si>
+    <t>Frontend interne Datensatzverwaltung - Instrument :  patient - darf nicht besetzt werden muss nur für den sycronisationsvorgang vorhanden sein</t>
   </si>
 </sst>
 </file>
@@ -2117,8 +2120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F448"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D198" sqref="D198"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2168,14 +2171,12 @@
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>15</v>
+        <v>412</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>12</v>
@@ -2183,14 +2184,12 @@
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>17</v>
+        <v>412</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>12</v>
@@ -2202,7 +2201,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>15</v>
@@ -2217,10 +2216,10 @@
         <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>12</v>
@@ -2232,10 +2231,10 @@
         <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>12</v>
@@ -2247,10 +2246,10 @@
         <v>13</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>12</v>
@@ -2262,13 +2261,13 @@
         <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E9" s="3"/>
     </row>
@@ -2277,13 +2276,13 @@
         <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="E10" s="3"/>
     </row>
@@ -2292,13 +2291,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E11" s="3"/>
     </row>
@@ -2307,25 +2306,25 @@
         <v>13</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>12</v>
@@ -2337,10 +2336,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>12</v>
@@ -2349,13 +2348,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>12</v>
@@ -2367,10 +2366,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>12</v>
@@ -2382,13 +2381,13 @@
         <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="E17" s="3"/>
     </row>
@@ -2397,10 +2396,10 @@
         <v>13</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>12</v>
@@ -2412,13 +2411,13 @@
         <v>13</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="E19" s="3"/>
     </row>
@@ -2427,10 +2426,10 @@
         <v>13</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>12</v>
@@ -2442,10 +2441,10 @@
         <v>13</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>12</v>
@@ -2457,10 +2456,10 @@
         <v>13</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>12</v>
@@ -2472,10 +2471,10 @@
         <v>13</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>398</v>
+        <v>49</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>399</v>
+        <v>50</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>12</v>
@@ -2487,10 +2486,10 @@
         <v>13</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>400</v>
+        <v>51</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>401</v>
+        <v>52</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>12</v>
@@ -2502,13 +2501,13 @@
         <v>13</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>53</v>
+        <v>398</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>54</v>
+        <v>399</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E25" s="3"/>
     </row>
@@ -2517,10 +2516,10 @@
         <v>13</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>55</v>
+        <v>400</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>56</v>
+        <v>401</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>12</v>
@@ -2532,13 +2531,13 @@
         <v>13</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E27" s="3"/>
     </row>
@@ -2547,10 +2546,10 @@
         <v>13</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>12</v>
@@ -2562,10 +2561,10 @@
         <v>13</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>32</v>
@@ -2577,10 +2576,10 @@
         <v>13</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>12</v>
@@ -2592,10 +2591,10 @@
         <v>13</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>32</v>
@@ -2607,10 +2606,10 @@
         <v>13</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>12</v>
@@ -2622,13 +2621,13 @@
         <v>13</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="E33" s="3"/>
     </row>
@@ -2637,7 +2636,7 @@
         <v>13</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>15</v>
@@ -2652,7 +2651,7 @@
         <v>13</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>15</v>
@@ -2667,7 +2666,7 @@
         <v>13</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>15</v>
@@ -2682,10 +2681,10 @@
         <v>13</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>12</v>
@@ -2697,7 +2696,7 @@
         <v>13</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>15</v>
@@ -2712,10 +2711,10 @@
         <v>13</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>12</v>
@@ -2727,7 +2726,7 @@
         <v>13</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>15</v>
@@ -2742,10 +2741,10 @@
         <v>13</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>12</v>
@@ -2757,10 +2756,10 @@
         <v>13</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>81</v>
+        <v>15</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>12</v>
@@ -2772,10 +2771,10 @@
         <v>13</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>12</v>
@@ -2787,10 +2786,10 @@
         <v>13</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>12</v>
@@ -2802,10 +2801,10 @@
         <v>13</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>12</v>
@@ -2817,10 +2816,10 @@
         <v>13</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>12</v>
@@ -2832,10 +2831,10 @@
         <v>13</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>12</v>
@@ -2847,13 +2846,13 @@
         <v>13</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>91</v>
+        <v>15</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E48" s="3"/>
     </row>
@@ -2862,10 +2861,10 @@
         <v>13</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>36</v>
+        <v>89</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>12</v>
@@ -2874,41 +2873,43 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>93</v>
+        <v>13</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>12</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E50" s="3"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="E51" s="3"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>95</v>
+        <v>10</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>12</v>
@@ -2919,7 +2920,7 @@
         <v>13</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>15</v>
@@ -2933,7 +2934,7 @@
         <v>13</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>15</v>
@@ -2947,7 +2948,7 @@
         <v>13</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>15</v>
@@ -2961,7 +2962,7 @@
         <v>13</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>15</v>
@@ -2975,13 +2976,13 @@
         <v>13</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>101</v>
+        <v>15</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2989,10 +2990,10 @@
         <v>13</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>21</v>
+        <v>99</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>102</v>
+        <v>15</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>12</v>
@@ -3003,13 +3004,13 @@
         <v>13</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>22</v>
+        <v>100</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>48</v>
+        <v>101</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -3017,13 +3018,13 @@
         <v>13</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>103</v>
+        <v>21</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -3031,10 +3032,10 @@
         <v>13</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>106</v>
+        <v>48</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>12</v>
@@ -3045,13 +3046,13 @@
         <v>13</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -3059,10 +3060,10 @@
         <v>13</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>15</v>
+        <v>106</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>12</v>
@@ -3073,10 +3074,10 @@
         <v>13</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>12</v>
@@ -3087,7 +3088,7 @@
         <v>13</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>15</v>
@@ -3101,10 +3102,10 @@
         <v>13</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>12</v>
@@ -3115,10 +3116,10 @@
         <v>13</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>116</v>
+        <v>15</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>12</v>
@@ -3129,10 +3130,10 @@
         <v>13</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>12</v>
@@ -3143,13 +3144,13 @@
         <v>13</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3157,13 +3158,13 @@
         <v>13</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3171,13 +3172,13 @@
         <v>13</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>123</v>
+        <v>15</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3185,24 +3186,24 @@
         <v>13</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>36</v>
+        <v>121</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>125</v>
+        <v>13</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>10</v>
+        <v>122</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>11</v>
+        <v>123</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>12</v>
@@ -3213,24 +3214,24 @@
         <v>13</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>127</v>
+        <v>36</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>13</v>
+        <v>125</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>128</v>
+        <v>11</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>12</v>
@@ -3241,13 +3242,13 @@
         <v>13</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>22</v>
+        <v>126</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>48</v>
+        <v>127</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -3255,10 +3256,10 @@
         <v>13</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>129</v>
+        <v>21</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>15</v>
+        <v>128</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>12</v>
@@ -3269,10 +3270,10 @@
         <v>13</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>130</v>
+        <v>22</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>12</v>
@@ -3283,7 +3284,7 @@
         <v>13</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>15</v>
@@ -3297,7 +3298,7 @@
         <v>13</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>15</v>
@@ -3311,7 +3312,7 @@
         <v>13</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>15</v>
@@ -3325,7 +3326,7 @@
         <v>13</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>397</v>
+        <v>132</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>15</v>
@@ -3339,7 +3340,7 @@
         <v>13</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>15</v>
@@ -3353,7 +3354,7 @@
         <v>13</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>15</v>
@@ -3367,7 +3368,7 @@
         <v>13</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>15</v>
@@ -3381,7 +3382,7 @@
         <v>13</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>136</v>
+        <v>396</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>15</v>
@@ -3395,7 +3396,7 @@
         <v>13</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>15</v>
@@ -3409,7 +3410,7 @@
         <v>13</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>15</v>
@@ -3423,7 +3424,7 @@
         <v>13</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>15</v>
@@ -3437,13 +3438,13 @@
         <v>13</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>141</v>
+        <v>15</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -3451,10 +3452,10 @@
         <v>13</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>143</v>
+        <v>15</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>12</v>
@@ -3465,13 +3466,13 @@
         <v>13</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -3479,10 +3480,10 @@
         <v>13</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>15</v>
+        <v>143</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>12</v>
@@ -3493,10 +3494,10 @@
         <v>13</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>12</v>
@@ -3507,7 +3508,7 @@
         <v>13</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>15</v>
@@ -3521,10 +3522,10 @@
         <v>13</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>12</v>
@@ -3535,7 +3536,7 @@
         <v>13</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>402</v>
+        <v>149</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>15</v>
@@ -3549,10 +3550,10 @@
         <v>13</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>403</v>
+        <v>150</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>404</v>
+        <v>151</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>12</v>
@@ -3563,7 +3564,7 @@
         <v>13</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>15</v>
@@ -3577,10 +3578,10 @@
         <v>13</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>12</v>
@@ -3591,7 +3592,7 @@
         <v>13</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>152</v>
+        <v>405</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>15</v>
@@ -3605,10 +3606,10 @@
         <v>13</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>153</v>
+        <v>406</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>154</v>
+        <v>407</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>12</v>
@@ -3619,7 +3620,7 @@
         <v>13</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>15</v>
@@ -3633,10 +3634,10 @@
         <v>13</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>12</v>
@@ -3647,7 +3648,7 @@
         <v>13</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>15</v>
@@ -3661,10 +3662,10 @@
         <v>13</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>15</v>
+        <v>157</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>12</v>
@@ -3675,7 +3676,7 @@
         <v>13</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>15</v>
@@ -3689,7 +3690,7 @@
         <v>13</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>15</v>
@@ -3703,7 +3704,7 @@
         <v>13</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>15</v>
@@ -3717,7 +3718,7 @@
         <v>13</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>15</v>
@@ -3731,10 +3732,10 @@
         <v>13</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>165</v>
+        <v>15</v>
       </c>
       <c r="D111" s="3" t="s">
         <v>12</v>
@@ -3745,7 +3746,7 @@
         <v>13</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C112" s="3" t="s">
         <v>15</v>
@@ -3759,10 +3760,10 @@
         <v>13</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>12</v>
@@ -3773,7 +3774,7 @@
         <v>13</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>15</v>
@@ -3787,10 +3788,10 @@
         <v>13</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D115" s="3" t="s">
         <v>12</v>
@@ -3801,7 +3802,7 @@
         <v>13</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>15</v>
@@ -3815,10 +3816,10 @@
         <v>13</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>12</v>
@@ -3829,7 +3830,7 @@
         <v>13</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C118" s="3" t="s">
         <v>15</v>
@@ -3843,10 +3844,10 @@
         <v>13</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D119" s="3" t="s">
         <v>12</v>
@@ -3857,7 +3858,7 @@
         <v>13</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C120" s="3" t="s">
         <v>15</v>
@@ -3871,10 +3872,10 @@
         <v>13</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D121" s="3" t="s">
         <v>12</v>
@@ -3885,7 +3886,7 @@
         <v>13</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C122" s="3" t="s">
         <v>15</v>
@@ -3899,10 +3900,10 @@
         <v>13</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D123" s="3" t="s">
         <v>12</v>
@@ -3913,7 +3914,7 @@
         <v>13</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C124" s="3" t="s">
         <v>15</v>
@@ -3927,10 +3928,10 @@
         <v>13</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>12</v>
@@ -3941,10 +3942,10 @@
         <v>13</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>188</v>
+        <v>15</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>12</v>
@@ -3955,10 +3956,10 @@
         <v>13</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>12</v>
@@ -3969,10 +3970,10 @@
         <v>13</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>15</v>
+        <v>188</v>
       </c>
       <c r="D128" s="3" t="s">
         <v>12</v>
@@ -3983,10 +3984,10 @@
         <v>13</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D129" s="3" t="s">
         <v>12</v>
@@ -3997,10 +3998,10 @@
         <v>13</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>195</v>
+        <v>15</v>
       </c>
       <c r="D130" s="3" t="s">
         <v>12</v>
@@ -4011,10 +4012,10 @@
         <v>13</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D131" s="3" t="s">
         <v>12</v>
@@ -4025,10 +4026,10 @@
         <v>13</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D132" s="3" t="s">
         <v>12</v>
@@ -4039,10 +4040,10 @@
         <v>13</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D133" s="3" t="s">
         <v>12</v>
@@ -4053,10 +4054,10 @@
         <v>13</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D134" s="3" t="s">
         <v>12</v>
@@ -4067,10 +4068,10 @@
         <v>13</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D135" s="3" t="s">
         <v>12</v>
@@ -4081,10 +4082,10 @@
         <v>13</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D136" s="3" t="s">
         <v>12</v>
@@ -4095,10 +4096,10 @@
         <v>13</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D137" s="3" t="s">
         <v>12</v>
@@ -4109,10 +4110,10 @@
         <v>13</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D138" s="3" t="s">
         <v>12</v>
@@ -4123,10 +4124,10 @@
         <v>13</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D139" s="3" t="s">
         <v>12</v>
@@ -4137,10 +4138,10 @@
         <v>13</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D140" s="3" t="s">
         <v>12</v>
@@ -4151,10 +4152,10 @@
         <v>13</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D141" s="3" t="s">
         <v>12</v>
@@ -4165,10 +4166,10 @@
         <v>13</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D142" s="3" t="s">
         <v>12</v>
@@ -4179,10 +4180,10 @@
         <v>13</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D143" s="3" t="s">
         <v>12</v>
@@ -4193,10 +4194,10 @@
         <v>13</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D144" s="3" t="s">
         <v>12</v>
@@ -4207,10 +4208,10 @@
         <v>13</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D145" s="3" t="s">
         <v>12</v>
@@ -4221,10 +4222,10 @@
         <v>13</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D146" s="3" t="s">
         <v>12</v>
@@ -4235,10 +4236,10 @@
         <v>13</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D147" s="3" t="s">
         <v>12</v>
@@ -4249,10 +4250,10 @@
         <v>13</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D148" s="3" t="s">
         <v>12</v>
@@ -4263,10 +4264,10 @@
         <v>13</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D149" s="3" t="s">
         <v>12</v>
@@ -4277,10 +4278,10 @@
         <v>13</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D150" s="3" t="s">
         <v>12</v>
@@ -4291,10 +4292,10 @@
         <v>13</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D151" s="3" t="s">
         <v>12</v>
@@ -4305,10 +4306,10 @@
         <v>13</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D152" s="3" t="s">
         <v>12</v>
@@ -4319,10 +4320,10 @@
         <v>13</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D153" s="3" t="s">
         <v>12</v>
@@ -4333,10 +4334,10 @@
         <v>13</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D154" s="3" t="s">
         <v>12</v>
@@ -4347,10 +4348,10 @@
         <v>13</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D155" s="3" t="s">
         <v>12</v>
@@ -4361,10 +4362,10 @@
         <v>13</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D156" s="3" t="s">
         <v>12</v>
@@ -4375,10 +4376,10 @@
         <v>13</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>15</v>
+        <v>245</v>
       </c>
       <c r="D157" s="3" t="s">
         <v>12</v>
@@ -4389,10 +4390,10 @@
         <v>13</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D158" s="3" t="s">
         <v>12</v>
@@ -4403,10 +4404,10 @@
         <v>13</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>252</v>
+        <v>15</v>
       </c>
       <c r="D159" s="3" t="s">
         <v>12</v>
@@ -4417,10 +4418,10 @@
         <v>13</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D160" s="3" t="s">
         <v>12</v>
@@ -4431,10 +4432,10 @@
         <v>13</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D161" s="3" t="s">
         <v>12</v>
@@ -4445,10 +4446,10 @@
         <v>13</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D162" s="3" t="s">
         <v>12</v>
@@ -4459,10 +4460,10 @@
         <v>13</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D163" s="3" t="s">
         <v>12</v>
@@ -4473,10 +4474,10 @@
         <v>13</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>15</v>
+        <v>258</v>
       </c>
       <c r="D164" s="3" t="s">
         <v>12</v>
@@ -4487,10 +4488,10 @@
         <v>13</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>15</v>
+        <v>260</v>
       </c>
       <c r="D165" s="3" t="s">
         <v>12</v>
@@ -4501,10 +4502,10 @@
         <v>13</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>264</v>
+        <v>15</v>
       </c>
       <c r="D166" s="3" t="s">
         <v>12</v>
@@ -4515,10 +4516,10 @@
         <v>13</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>266</v>
+        <v>15</v>
       </c>
       <c r="D167" s="3" t="s">
         <v>12</v>
@@ -4529,10 +4530,10 @@
         <v>13</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>15</v>
+        <v>264</v>
       </c>
       <c r="D168" s="3" t="s">
         <v>12</v>
@@ -4543,10 +4544,10 @@
         <v>13</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D169" s="3" t="s">
         <v>12</v>
@@ -4557,10 +4558,10 @@
         <v>13</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>271</v>
+        <v>15</v>
       </c>
       <c r="D170" s="3" t="s">
         <v>12</v>
@@ -4571,10 +4572,10 @@
         <v>13</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D171" s="3" t="s">
         <v>12</v>
@@ -4585,10 +4586,10 @@
         <v>13</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D172" s="3" t="s">
         <v>12</v>
@@ -4599,10 +4600,10 @@
         <v>13</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D173" s="3" t="s">
         <v>12</v>
@@ -4613,10 +4614,10 @@
         <v>13</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D174" s="3" t="s">
         <v>12</v>
@@ -4627,10 +4628,10 @@
         <v>13</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D175" s="3" t="s">
         <v>12</v>
@@ -4641,10 +4642,10 @@
         <v>13</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D176" s="3" t="s">
         <v>12</v>
@@ -4655,10 +4656,10 @@
         <v>13</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D177" s="3" t="s">
         <v>12</v>
@@ -4669,10 +4670,10 @@
         <v>13</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D178" s="3" t="s">
         <v>12</v>
@@ -4683,10 +4684,10 @@
         <v>13</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D179" s="3" t="s">
         <v>12</v>
@@ -4697,10 +4698,10 @@
         <v>13</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>15</v>
+        <v>287</v>
       </c>
       <c r="D180" s="3" t="s">
         <v>12</v>
@@ -4711,10 +4712,10 @@
         <v>13</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D181" s="3" t="s">
         <v>12</v>
@@ -4725,10 +4726,10 @@
         <v>13</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>294</v>
+        <v>15</v>
       </c>
       <c r="D182" s="3" t="s">
         <v>12</v>
@@ -4739,10 +4740,10 @@
         <v>13</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C183" s="3" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D183" s="3" t="s">
         <v>12</v>
@@ -4753,10 +4754,10 @@
         <v>13</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C184" s="3" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D184" s="3" t="s">
         <v>12</v>
@@ -4767,10 +4768,10 @@
         <v>13</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D185" s="3" t="s">
         <v>12</v>
@@ -4781,10 +4782,10 @@
         <v>13</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D186" s="3" t="s">
         <v>12</v>
@@ -4795,10 +4796,10 @@
         <v>13</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="D187" s="3" t="s">
         <v>12</v>
@@ -4809,10 +4810,10 @@
         <v>13</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D188" s="3" t="s">
         <v>12</v>
@@ -4823,10 +4824,10 @@
         <v>13</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D189" s="3" t="s">
         <v>12</v>
@@ -4837,10 +4838,10 @@
         <v>13</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>15</v>
+        <v>306</v>
       </c>
       <c r="D190" s="3" t="s">
         <v>12</v>
@@ -4851,10 +4852,10 @@
         <v>13</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D191" s="3" t="s">
         <v>12</v>
@@ -4865,7 +4866,7 @@
         <v>13</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C192" s="3" t="s">
         <v>15</v>
@@ -4879,10 +4880,10 @@
         <v>13</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D193" s="3" t="s">
         <v>12</v>
@@ -4893,10 +4894,10 @@
         <v>13</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>316</v>
+        <v>15</v>
       </c>
       <c r="D194" s="3" t="s">
         <v>12</v>
@@ -4907,10 +4908,10 @@
         <v>13</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>408</v>
+        <v>313</v>
       </c>
       <c r="C195" s="3" t="s">
-        <v>15</v>
+        <v>314</v>
       </c>
       <c r="D195" s="3" t="s">
         <v>12</v>
@@ -4921,10 +4922,10 @@
         <v>13</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>395</v>
+        <v>315</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>15</v>
+        <v>316</v>
       </c>
       <c r="D196" s="3" t="s">
         <v>12</v>
@@ -4935,7 +4936,7 @@
         <v>13</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>317</v>
+        <v>408</v>
       </c>
       <c r="C197" s="3" t="s">
         <v>15</v>
@@ -4945,12 +4946,14 @@
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="3"/>
-      <c r="B198" s="4" t="s">
-        <v>410</v>
-      </c>
-      <c r="C198" s="4" t="s">
-        <v>411</v>
+      <c r="A198" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="C198" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="D198" s="3" t="s">
         <v>12</v>
@@ -4961,24 +4964,22 @@
         <v>13</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>394</v>
+        <v>317</v>
       </c>
       <c r="C199" s="3" t="s">
-        <v>409</v>
+        <v>15</v>
       </c>
       <c r="D199" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="B200" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C200" s="3" t="s">
-        <v>11</v>
+      <c r="A200" s="3"/>
+      <c r="B200" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="C200" s="4" t="s">
+        <v>411</v>
       </c>
       <c r="D200" s="3" t="s">
         <v>12</v>
@@ -4989,10 +4990,10 @@
         <v>13</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>43</v>
+        <v>394</v>
       </c>
       <c r="C201" s="3" t="s">
-        <v>44</v>
+        <v>409</v>
       </c>
       <c r="D201" s="3" t="s">
         <v>12</v>
@@ -5000,16 +5001,16 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
-        <v>13</v>
+        <v>318</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>319</v>
+        <v>10</v>
       </c>
       <c r="C202" s="3" t="s">
-        <v>320</v>
+        <v>11</v>
       </c>
       <c r="D202" s="3" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -5017,10 +5018,10 @@
         <v>13</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>321</v>
+        <v>43</v>
       </c>
       <c r="C203" s="3" t="s">
-        <v>322</v>
+        <v>44</v>
       </c>
       <c r="D203" s="3" t="s">
         <v>12</v>
@@ -5031,13 +5032,13 @@
         <v>13</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C204" s="3" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -5045,10 +5046,10 @@
         <v>13</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C205" s="3" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D205" s="3" t="s">
         <v>12</v>
@@ -5059,10 +5060,10 @@
         <v>13</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C206" s="3" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D206" s="3" t="s">
         <v>12</v>
@@ -5073,10 +5074,10 @@
         <v>13</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C207" s="3" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="D207" s="3" t="s">
         <v>12</v>
@@ -5087,10 +5088,10 @@
         <v>13</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D208" s="3" t="s">
         <v>12</v>
@@ -5101,10 +5102,10 @@
         <v>13</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C209" s="3" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="D209" s="3" t="s">
         <v>12</v>
@@ -5115,10 +5116,10 @@
         <v>13</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C210" s="3" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="D210" s="3" t="s">
         <v>12</v>
@@ -5129,10 +5130,10 @@
         <v>13</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C211" s="3" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="D211" s="3" t="s">
         <v>12</v>
@@ -5143,10 +5144,10 @@
         <v>13</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C212" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="D212" s="3" t="s">
         <v>12</v>
@@ -5157,10 +5158,10 @@
         <v>13</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C213" s="3" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D213" s="3" t="s">
         <v>12</v>
@@ -5171,10 +5172,10 @@
         <v>13</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C214" s="3" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="D214" s="3" t="s">
         <v>12</v>
@@ -5185,10 +5186,10 @@
         <v>13</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C215" s="3" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D215" s="3" t="s">
         <v>12</v>
@@ -5199,10 +5200,10 @@
         <v>13</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C216" s="3" t="s">
-        <v>36</v>
+        <v>344</v>
       </c>
       <c r="D216" s="3" t="s">
         <v>12</v>
@@ -5210,13 +5211,13 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
-        <v>348</v>
+        <v>13</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>43</v>
+        <v>345</v>
       </c>
       <c r="C217" s="3" t="s">
-        <v>44</v>
+        <v>346</v>
       </c>
       <c r="D217" s="3" t="s">
         <v>12</v>
@@ -5227,24 +5228,24 @@
         <v>13</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>10</v>
+        <v>347</v>
       </c>
       <c r="C218" s="3" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>13</v>
+        <v>348</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>349</v>
+        <v>43</v>
       </c>
       <c r="C219" s="3" t="s">
-        <v>350</v>
+        <v>44</v>
       </c>
       <c r="D219" s="3" t="s">
         <v>12</v>
@@ -5255,13 +5256,13 @@
         <v>13</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>351</v>
+        <v>10</v>
       </c>
       <c r="C220" s="3" t="s">
-        <v>352</v>
+        <v>11</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -5269,10 +5270,10 @@
         <v>13</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C221" s="3" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D221" s="3" t="s">
         <v>12</v>
@@ -5283,10 +5284,10 @@
         <v>13</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C222" s="3" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D222" s="3" t="s">
         <v>12</v>
@@ -5297,10 +5298,10 @@
         <v>13</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C223" s="3" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D223" s="3" t="s">
         <v>12</v>
@@ -5311,10 +5312,10 @@
         <v>13</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C224" s="3" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="D224" s="3" t="s">
         <v>12</v>
@@ -5325,10 +5326,10 @@
         <v>13</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C225" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="D225" s="3" t="s">
         <v>12</v>
@@ -5339,10 +5340,10 @@
         <v>13</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C226" s="3" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D226" s="3" t="s">
         <v>12</v>
@@ -5353,10 +5354,10 @@
         <v>13</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C227" s="3" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="D227" s="3" t="s">
         <v>12</v>
@@ -5367,10 +5368,10 @@
         <v>13</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="C228" s="3" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="D228" s="3" t="s">
         <v>12</v>
@@ -5381,10 +5382,10 @@
         <v>13</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="C229" s="3" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="D229" s="3" t="s">
         <v>12</v>
@@ -5395,10 +5396,10 @@
         <v>13</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C230" s="3" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D230" s="3" t="s">
         <v>12</v>
@@ -5409,10 +5410,10 @@
         <v>13</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="C231" s="3" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="D231" s="3" t="s">
         <v>12</v>
@@ -5423,40 +5424,40 @@
         <v>13</v>
       </c>
       <c r="B232" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="C232" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="D232" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B233" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="C233" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="D233" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B234" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="C232" s="3" t="s">
+      <c r="C234" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="D232" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B233" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="C233" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="D233" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B234" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="C234" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="D234" s="2" t="s">
+      <c r="D234" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -5465,10 +5466,10 @@
         <v>13</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="D235" s="2" t="s">
         <v>12</v>
@@ -5479,10 +5480,10 @@
         <v>13</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="D236" s="2" t="s">
         <v>12</v>
@@ -5493,10 +5494,10 @@
         <v>13</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="D237" s="2" t="s">
         <v>12</v>
@@ -5507,10 +5508,10 @@
         <v>13</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D238" s="2" t="s">
         <v>12</v>
@@ -5521,10 +5522,10 @@
         <v>13</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="D239" s="2" t="s">
         <v>12</v>
@@ -5535,10 +5536,10 @@
         <v>13</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="D240" s="2" t="s">
         <v>12</v>
@@ -5549,12 +5550,40 @@
         <v>13</v>
       </c>
       <c r="B241" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="D241" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B242" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C242" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="D242" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A243" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B243" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="C241" s="2" t="s">
+      <c r="C243" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D241" s="2" t="s">
+      <c r="D243" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest changes from the frontend group
</commit_message>
<xml_diff>
--- a/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
+++ b/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="438">
   <si>
     <t xml:space="preserve">Station </t>
   </si>
@@ -81,9 +81,6 @@
     <t>Patient-identifier FHIR Daten</t>
   </si>
   <si>
-    <t>pat_femb</t>
-  </si>
-  <si>
     <t>pat_cis_pid</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t>int</t>
   </si>
   <si>
-    <t>fall_femb</t>
-  </si>
-  <si>
     <t>Frontend interne Datensatzverwaltung - Instrument :   fall</t>
   </si>
   <si>
@@ -255,39 +249,24 @@
     <t>fall_nieren_insuf_ausmass</t>
   </si>
   <si>
-    <t>1, Ausmaß unbekannt | 2, 45-59 ml/min/1,73 m2 | 3, 30-44 ml/min/1,73 m2 | 4, 15-29 ml/min/1,73 m2 | 5, &lt; 15 ml/min/1,73 m2</t>
-  </si>
-  <si>
     <t>fall_nieren_insuf_dialysev_lbl</t>
   </si>
   <si>
     <t>fall_nieren_insuf_dialysev</t>
   </si>
   <si>
-    <t>1, Hämodialyse | 2, Kont. Hämofiltration | 3, Peritonealdialyse | 4, keineDialyseverfahren</t>
-  </si>
-  <si>
     <t>fall_leber_insuf</t>
   </si>
   <si>
-    <t>1, ja | 0, nein | -1, nicht bekanntLeberinsuffizienz</t>
-  </si>
-  <si>
     <t>fall_leber_insuf_ausmass_lbl</t>
   </si>
   <si>
     <t>fall_leber_insuf_ausmass</t>
   </si>
   <si>
-    <t>1, Ausmaß unbekannt | 2, Leicht (Child-Pugh A) | 3, Mittel (Child-Pugh B) | 4, Schwer (Child-Pugh C)aktuelles Ausmaß</t>
-  </si>
-  <si>
     <t>fall_schwanger_mo</t>
   </si>
   <si>
-    <t>0, keine Schwangerschaft | 1, 1 | 2, 2 | 3, 3 | 4, 4 | 5, 5 | 6, 6 | 7, 7 | 8, 8 | 9, 9</t>
-  </si>
-  <si>
     <t>fall_schwanger_mo_lbl</t>
   </si>
   <si>
@@ -312,21 +291,12 @@
     <t>meda_header</t>
   </si>
   <si>
-    <t>meda_femb</t>
-  </si>
-  <si>
     <t>meda_femb_2</t>
   </si>
   <si>
     <t>meda_femb_3</t>
   </si>
   <si>
-    <t>meda_femb_4</t>
-  </si>
-  <si>
-    <t>meda_femb_5</t>
-  </si>
-  <si>
     <t>fall_fe_id</t>
   </si>
   <si>
@@ -345,54 +315,21 @@
     <t>meda_typ</t>
   </si>
   <si>
-    <t>Typ der Medikationsanalyse</t>
-  </si>
-  <si>
     <t>meda_ma_thueberw</t>
   </si>
   <si>
-    <t>Medikationsanalyse / Therapieüberwachung in 24-48h</t>
-  </si>
-  <si>
-    <t>meda_ma_thueberw_comp_lbl</t>
-  </si>
-  <si>
-    <t>meda_ma_thueberw_comp</t>
-  </si>
-  <si>
-    <t>Wiedervorlage abgeschlossen? 1, Ja|0, Nein</t>
-  </si>
-  <si>
-    <t>meda_ma_thueberw_comp_dat_lbl</t>
-  </si>
-  <si>
-    <t>meda_ma_thueberw_comp_dat</t>
-  </si>
-  <si>
-    <t>Abgeschlossen am</t>
-  </si>
-  <si>
     <t>meda_mrp_detekt</t>
   </si>
   <si>
-    <t>MRP detektiert? 1, Ja|0, Nein</t>
-  </si>
-  <si>
     <t>meda_aufwand_zeit</t>
   </si>
   <si>
-    <t>0, &lt;= 5 min | 1, 6-10 min | 2, 11-20 min | 3, 21-30 min | 4, &gt;30 min | 5, Angabe abgelehntZeitaufwand Medikationsanalyse [Min]</t>
-  </si>
-  <si>
     <t>meda_aufwand_zeit_and_lbl</t>
   </si>
   <si>
     <t>meda_aufwand_zeit_and</t>
   </si>
   <si>
-    <t xml:space="preserve">wie lange hat die Medikationsanalyse gedauert? Eingabe in Minuten. </t>
-  </si>
-  <si>
     <t>meda_notiz</t>
   </si>
   <si>
@@ -417,9 +354,6 @@
     <t>mrp_header</t>
   </si>
   <si>
-    <t>mrp_femb</t>
-  </si>
-  <si>
     <t>mrp_femb_2</t>
   </si>
   <si>
@@ -462,9 +396,6 @@
     <t>mrp_entd_algorithmisch</t>
   </si>
   <si>
-    <t>MRP vom INTERPOLAR-Algorithmus entdeckt?</t>
-  </si>
-  <si>
     <t>mrp_hinweisgeber_lbl</t>
   </si>
   <si>
@@ -480,18 +411,12 @@
     <t>mrp_gewissheit</t>
   </si>
   <si>
-    <t>Sicherheit des detektierten MRP</t>
-  </si>
-  <si>
     <t>mrp_gewiss_grund_abl_lbl</t>
   </si>
   <si>
     <t>mrp_gewiss_grund_abl</t>
   </si>
   <si>
-    <t>Grund für nicht Bestätigung</t>
-  </si>
-  <si>
     <t>mrp_gewiss_grund_abl_sonst_lbl</t>
   </si>
   <si>
@@ -522,18 +447,12 @@
     <t>mrp_wirkstoff</t>
   </si>
   <si>
-    <t>Wirkstoff betroffen?</t>
-  </si>
-  <si>
     <t>mrp_atc1_lbl</t>
   </si>
   <si>
     <t>mrp_atc1</t>
   </si>
   <si>
-    <t>1. Medikament ATC / Name:</t>
-  </si>
-  <si>
     <t>mrp_atc2_lbl</t>
   </si>
   <si>
@@ -576,30 +495,18 @@
     <t>mrp_med_prod</t>
   </si>
   <si>
-    <t>Medizinprodukt betroffen?</t>
-  </si>
-  <si>
     <t>mrp_med_prod_sonst_lbl</t>
   </si>
   <si>
     <t>mrp_med_prod_sonst</t>
   </si>
   <si>
-    <t>Sonstigespräparat</t>
-  </si>
-  <si>
     <t>mrp_dokup_fehler</t>
   </si>
   <si>
-    <t>Fehlerbeschreibung </t>
-  </si>
-  <si>
     <t>mrp_dokup_intervention</t>
   </si>
   <si>
-    <t>Intervention -Vorschlag zur Fehlervermeldung</t>
-  </si>
-  <si>
     <t>mrp_femb_14</t>
   </si>
   <si>
@@ -969,15 +876,9 @@
     <t>mrp_dokup_hand_emp_akz</t>
   </si>
   <si>
-    <t>Handlungsempfehlung akzeptiert?</t>
-  </si>
-  <si>
     <t>mrp_merp</t>
   </si>
   <si>
-    <t>NCC MERP Score</t>
-  </si>
-  <si>
     <t>mrp_merp_txt</t>
   </si>
   <si>
@@ -1221,12 +1122,6 @@
     <t>mrp_pi_info___1</t>
   </si>
   <si>
-    <t>fall_bettplatz</t>
-  </si>
-  <si>
-    <t>Bettplatz wie vom DIZ Definiert</t>
-  </si>
-  <si>
     <t>fall_zimmernr</t>
   </si>
   <si>
@@ -1254,16 +1149,196 @@
     <t>mrp_merp_info</t>
   </si>
   <si>
-    <t xml:space="preserve">Frontend Complete-Status, wenn ein Pflichtitem fehlt Status bei Import wieder auf Incomplete setzen </t>
-  </si>
-  <si>
-    <t>mrp_wiedervorlage</t>
-  </si>
-  <si>
-    <t>MRP Wiedervorlage</t>
-  </si>
-  <si>
     <t>Frontend interne Datensatzverwaltung - Instrument :  patient - darf nicht besetzt werden muss nur für den sycronisationsvorgang vorhanden sein</t>
+  </si>
+  <si>
+    <t>pat_femb_1</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - Fieldembedding (femb) der Variablen pat_cis_pid, pat_name, pat_vorname, pat_gebdat,pat_geschlecht</t>
+  </si>
+  <si>
+    <t>Frontend Complete-Status - 0, Incomplete | 1, Unverified | 2, Complete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">descriptive item only for frontend - Gesamtüberischt Patienten, Falldaten, gegenwärtige Formular-Instanz </t>
+  </si>
+  <si>
+    <t>fall_femb_1</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variablen fall_id, fall_station, fall_aufn_dat, fall_zimmernr, fall_aufn_diag, fall_gewicht_aktuell, fall_gewicht_aktl_einheit, fall_groesse, fall_groesse_einheit</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variablen fall_nieren_insuf_chron, fall_nieren_insuf_ausmass_lbl, fall_nieren_insuf_ausmass</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variablen fall_nieren_insuf_dialysev_lbl, fall_nieren_insuf_dialysev</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variablen fall_leber_insuf, fall_leber_insuf_ausmass_lbl, fall_leber_insuf_ausmass</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variablen fall_schwanger_mo_lbl, fall_schwanger_mo</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variablen fall_status, fall_ent_dat</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - Label für femb (korrespondierende Variable)</t>
+  </si>
+  <si>
+    <t>aktuelles Ausmaß - 1, Ausmaß unbekannt | 2, 45-59 ml/min/1,73 m2 | 3, 30-44 ml/min/1,73 m2 | 4, 15-29 ml/min/1,73 m2 | 5, &lt; 15 ml/min/1,73 m2</t>
+  </si>
+  <si>
+    <t>Nierenersatzverfahren - 1, Hämodialyse | 2, Kont. Hämofiltration | 3, Peritonealdialyse | 4, keineDialyseverfahren</t>
+  </si>
+  <si>
+    <t>Leberinsuffizienz - 1, ja | 0, nein | -1, nicht bekanntLeberinsuffizienz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aktuelles Ausmaß -1, Ausmaß unbekannt | 2, Leicht (Child-Pugh A) | 3, Mittel (Child-Pugh B) | 4, Schwer (Child-Pugh C)aktuelles Ausmaß </t>
+  </si>
+  <si>
+    <t>Schwangerschaftsmonat - 0, keine Schwangerschaft | 1, 1 | 2, 2 | 3, 3 | 4, 4 | 5, 5 | 6, 6 | 7, 7 | 8, 8 | 9, 9</t>
+  </si>
+  <si>
+    <t>Frontend Complete-Status - Incomplete | 1, Unverified | 2, Complete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">descriptive item only for frontend - Gesamtüberischt Patienten, Falldaten, gegenwärtige Formular-Instanzen </t>
+  </si>
+  <si>
+    <t>meda_femb_1</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variable meda_dat</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variable meda_ma_thueberw</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variablen meda_mrp_detekt, meda_aufwand_zeit, meda_aufwand_zeit_and_lbl, meda_aufwand_zeit_and, meda_notiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typ der Medikationsanalyse - 1, Typ 1: Einfache MA | 2a, Typ 2a: Erweiterte MA | 2b, Typ 2b: Erweiterte MA | 3, Typ 3: Umfassende MA </t>
+  </si>
+  <si>
+    <t>Medikationsanalyse / Therapieüberwachung in 24-48h - 1, Ja | 0, Nein</t>
+  </si>
+  <si>
+    <t>MRP detektiert? - 1, Ja|0, Nein</t>
+  </si>
+  <si>
+    <t>Zeitaufwand Medikationsanalyse - 0, &lt;= 5 min | 1, 6-10 min | 2, 11-20 min | 3, 21-30 min | 4, &gt;30 min | 5, Angabe abgelehntZeitaufwand Medikationsanalyse [Min]</t>
+  </si>
+  <si>
+    <t>genaue Dauer in Minuten</t>
+  </si>
+  <si>
+    <t>mrp_femb_1</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variable mrp_entd_dat</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variablen mrp_kurzbeschr, mrp_entd_algorithmisch, mrp_hinweisgeber_lbl, mrp_hinweisgeber</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variable mrp_hinweisgeber_oth</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variablen mrp_gewissheit_lbl, mrp_gewissheit</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variable mrp_gewissheit_oth</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variablen mrp_gewiss_grund_abl_lbl, mrp_gewiss_grund_abl</t>
+  </si>
+  <si>
+    <t>MRP vom INTERPOLAR-Algorithmus entdeckt? - 1, Ja | 0, Nein</t>
+  </si>
+  <si>
+    <t>Sicherheit des detektierten MRP - 1, MRP bestätigt | 2, MRP möglich, weitere Informationen nötig | 3, MRP nicht bestätigt</t>
+  </si>
+  <si>
+    <t>Grund für nicht Bestätigung - 1, MRP sachlich falsch (keine Kontraindikation) | 2, MRP sachlich richtig, aber falsche Datengrundlage | 3, MRP sachlich richtig, aber klinisch nicht relevant | 4, MRP sachlich richtig, aber von Stationsapotheker vorher identifiziert | 5, Sonstiges</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variablen mrp_gewiss_grund_abl_sonst_lbl, mrp_gewiss_grund_abl_sonst</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variable mrp_wirkstoff</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variablen mrp_atc1_lbl, mrp_atc1</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variablen mrp_atc2_lbl, mrp_atc2</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variablen mrp_atc3_lbl, mrp_atc3</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variablen mrp_atc4_lbl, mrp_atc4</t>
+  </si>
+  <si>
+    <t>Wirkstoff betroffen? - 1, Ja | 0, Nein</t>
+  </si>
+  <si>
+    <t>1. Medikament ATC / Name- https://www.bfarm.de/SharedDocs/Downloads/DE/Kodiersysteme/ATC/atc-ddd-amtlich-2024.pdf?__blob=publicationFile</t>
+  </si>
+  <si>
+    <t>Medizinprodukt betroffen? - 1, Ja | 0, Nein,</t>
+  </si>
+  <si>
+    <t>Bezeichnung Präparat</t>
+  </si>
+  <si>
+    <t>Frage / Fehlerbeschreibung</t>
+  </si>
+  <si>
+    <t>Intervention / Vorschlag zur Fehlervermeldung</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variablen mrp_med_prod, mrp_med_prod_sonst_lbl, mrp_med_prod_sonst</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variable mrp_ip_klasse</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variable mrp_ip_klasse_disease</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variable mrp_ip_klasse_labor</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variable mrp_massn_am</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variable mrp_massn_orga</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variable mrp_notiz</t>
+  </si>
+  <si>
+    <t>Handlungsempfehlung akzeptiert? - 1, Arzt / Pflege informiert | 2, Intervention vorgeschlagen und umgesetzt | 3, Intervention vorgeschlagen, nicht umgesetzt (keine Kooperation) | 4 , Intervention vorgeschlagen, nicht umgesetzt (Nutzen-Risiko-Abwägung) | 5, Intervention vorgeschlagen, Umsetzung unbekannt | 6, Problem nicht gelöst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NCC MERP Score - A, Category A | B, Category B | C, Category C | D, Category D | E, Category E | F, Category F | G, Category G | H, Category H | I, Category I </t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - Blendet NCC MERP Index ein/aus</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - Beinhaltet NCC MERP Index als PDF</t>
+  </si>
+  <si>
+    <t>descriptive item only for frontend - femb der Variablen</t>
+  </si>
+  <si>
+    <t>Frontend Complete-Status, wenn ein Pflichtitem fehlt Status bei Import wieder auf Incomplete setzen  - 0, Incomplete | 1, Unverified | 2, Complete</t>
   </si>
 </sst>
 </file>
@@ -2118,10 +2193,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F448"/>
+  <dimension ref="A1:F441"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C188" sqref="C188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2171,25 +2246,29 @@
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>412</v>
+        <v>374</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>12</v>
@@ -2231,10 +2310,10 @@
         <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>18</v>
+        <v>375</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>15</v>
+        <v>376</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>12</v>
@@ -2246,10 +2325,10 @@
         <v>13</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>12</v>
@@ -2261,10 +2340,10 @@
         <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>12</v>
@@ -2276,10 +2355,10 @@
         <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>12</v>
@@ -2291,13 +2370,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="E11" s="3"/>
     </row>
@@ -2306,13 +2385,13 @@
         <v>13</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="E12" s="3"/>
     </row>
@@ -2321,10 +2400,10 @@
         <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>12</v>
@@ -2336,10 +2415,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>36</v>
+        <v>377</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>12</v>
@@ -2348,7 +2427,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>10</v>
@@ -2366,10 +2445,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>15</v>
+        <v>378</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>12</v>
@@ -2381,10 +2460,10 @@
         <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>12</v>
@@ -2396,10 +2475,10 @@
         <v>13</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>12</v>
@@ -2411,13 +2490,13 @@
         <v>13</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="E19" s="3"/>
     </row>
@@ -2426,10 +2505,10 @@
         <v>13</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>46</v>
+        <v>379</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>15</v>
+        <v>380</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>12</v>
@@ -2441,10 +2520,10 @@
         <v>13</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>12</v>
@@ -2456,10 +2535,10 @@
         <v>13</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>12</v>
@@ -2471,10 +2550,10 @@
         <v>13</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>12</v>
@@ -2486,10 +2565,10 @@
         <v>13</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>12</v>
@@ -2501,10 +2580,10 @@
         <v>13</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>398</v>
+        <v>365</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>399</v>
+        <v>366</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>12</v>
@@ -2516,13 +2595,13 @@
         <v>13</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>400</v>
+        <v>51</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>401</v>
+        <v>52</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="E26" s="3"/>
     </row>
@@ -2537,7 +2616,7 @@
         <v>54</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E27" s="3"/>
     </row>
@@ -2552,7 +2631,7 @@
         <v>56</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E28" s="3"/>
     </row>
@@ -2567,7 +2646,7 @@
         <v>58</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="E29" s="3"/>
     </row>
@@ -2582,7 +2661,7 @@
         <v>60</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E30" s="3"/>
     </row>
@@ -2597,7 +2676,7 @@
         <v>62</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="E31" s="3"/>
     </row>
@@ -2612,7 +2691,7 @@
         <v>64</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E32" s="3"/>
     </row>
@@ -2624,10 +2703,10 @@
         <v>65</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>66</v>
+        <v>381</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="E33" s="3"/>
     </row>
@@ -2636,10 +2715,10 @@
         <v>13</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>15</v>
+        <v>382</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>12</v>
@@ -2651,10 +2730,10 @@
         <v>13</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>15</v>
+        <v>383</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>12</v>
@@ -2666,10 +2745,10 @@
         <v>13</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>15</v>
+        <v>384</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>12</v>
@@ -2681,10 +2760,10 @@
         <v>13</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>15</v>
+        <v>385</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>12</v>
@@ -2696,10 +2775,10 @@
         <v>13</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>12</v>
@@ -2714,7 +2793,7 @@
         <v>72</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>73</v>
+        <v>386</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>12</v>
@@ -2726,10 +2805,10 @@
         <v>13</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>15</v>
+        <v>387</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>12</v>
@@ -2741,10 +2820,10 @@
         <v>13</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>76</v>
+        <v>386</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>12</v>
@@ -2756,10 +2835,10 @@
         <v>13</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>15</v>
+        <v>388</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>12</v>
@@ -2771,10 +2850,10 @@
         <v>13</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>79</v>
+        <v>389</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>12</v>
@@ -2786,10 +2865,10 @@
         <v>13</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>81</v>
+        <v>386</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>12</v>
@@ -2801,10 +2880,10 @@
         <v>13</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>15</v>
+        <v>390</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>12</v>
@@ -2816,10 +2895,10 @@
         <v>13</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>84</v>
+        <v>391</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>12</v>
@@ -2831,10 +2910,10 @@
         <v>13</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>86</v>
+        <v>386</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>12</v>
@@ -2846,10 +2925,10 @@
         <v>13</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>15</v>
+        <v>82</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>12</v>
@@ -2861,13 +2940,13 @@
         <v>13</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="E49" s="3"/>
     </row>
@@ -2876,40 +2955,38 @@
         <v>13</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>91</v>
+        <v>392</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E50" s="3"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>92</v>
+        <v>10</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E51" s="3"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>93</v>
+        <v>13</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>11</v>
+        <v>393</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>12</v>
@@ -2920,10 +2997,10 @@
         <v>13</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>94</v>
+        <v>394</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>15</v>
+        <v>395</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>12</v>
@@ -2934,10 +3011,10 @@
         <v>13</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>15</v>
+        <v>396</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>12</v>
@@ -2948,10 +3025,10 @@
         <v>13</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>15</v>
+        <v>397</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>12</v>
@@ -2962,13 +3039,13 @@
         <v>13</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>15</v>
+        <v>91</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2976,10 +3053,10 @@
         <v>13</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>98</v>
+        <v>20</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>12</v>
@@ -2990,10 +3067,10 @@
         <v>13</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>12</v>
@@ -3004,13 +3081,13 @@
         <v>13</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -3018,10 +3095,10 @@
         <v>13</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>21</v>
+        <v>95</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>102</v>
+        <v>398</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>12</v>
@@ -3032,10 +3109,10 @@
         <v>13</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>22</v>
+        <v>96</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>48</v>
+        <v>399</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>12</v>
@@ -3046,13 +3123,13 @@
         <v>13</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>104</v>
+        <v>400</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -3060,10 +3137,10 @@
         <v>13</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>106</v>
+        <v>401</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>12</v>
@@ -3074,13 +3151,13 @@
         <v>13</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>108</v>
+        <v>386</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -3088,13 +3165,13 @@
         <v>13</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>15</v>
+        <v>402</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3102,10 +3179,10 @@
         <v>13</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>12</v>
@@ -3116,10 +3193,10 @@
         <v>13</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>15</v>
+        <v>377</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>12</v>
@@ -3127,13 +3204,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>13</v>
+        <v>104</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>113</v>
+        <v>10</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>114</v>
+        <v>11</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>12</v>
@@ -3144,13 +3221,13 @@
         <v>13</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3158,10 +3235,10 @@
         <v>13</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>117</v>
+        <v>20</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>12</v>
@@ -3172,13 +3249,13 @@
         <v>13</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>119</v>
+        <v>21</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3186,13 +3263,13 @@
         <v>13</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>121</v>
+        <v>393</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3200,10 +3277,10 @@
         <v>13</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>122</v>
+        <v>403</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>123</v>
+        <v>404</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>12</v>
@@ -3214,10 +3291,10 @@
         <v>13</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>36</v>
+        <v>405</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>12</v>
@@ -3225,13 +3302,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>125</v>
+        <v>13</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>11</v>
+        <v>406</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>12</v>
@@ -3242,13 +3319,13 @@
         <v>13</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>127</v>
+        <v>15</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -3256,10 +3333,10 @@
         <v>13</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>21</v>
+        <v>364</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>128</v>
+        <v>15</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>12</v>
@@ -3270,10 +3347,10 @@
         <v>13</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>22</v>
+        <v>112</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>12</v>
@@ -3284,7 +3361,7 @@
         <v>13</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>129</v>
+        <v>363</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>15</v>
@@ -3298,7 +3375,7 @@
         <v>13</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>15</v>
@@ -3312,7 +3389,7 @@
         <v>13</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>15</v>
@@ -3326,10 +3403,10 @@
         <v>13</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>15</v>
+        <v>407</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>12</v>
@@ -3340,10 +3417,10 @@
         <v>13</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>15</v>
+        <v>408</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>12</v>
@@ -3354,10 +3431,10 @@
         <v>13</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>397</v>
+        <v>117</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>15</v>
+        <v>409</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>12</v>
@@ -3368,13 +3445,13 @@
         <v>13</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>15</v>
+        <v>119</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -3382,10 +3459,10 @@
         <v>13</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>396</v>
+        <v>120</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>15</v>
+        <v>121</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>12</v>
@@ -3396,10 +3473,10 @@
         <v>13</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>15</v>
+        <v>410</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>12</v>
@@ -3410,7 +3487,7 @@
         <v>13</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>15</v>
@@ -3424,10 +3501,10 @@
         <v>13</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>15</v>
+        <v>125</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>12</v>
@@ -3438,7 +3515,7 @@
         <v>13</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>15</v>
@@ -3452,10 +3529,10 @@
         <v>13</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>15</v>
+        <v>411</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>12</v>
@@ -3466,13 +3543,13 @@
         <v>13</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>140</v>
+        <v>367</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>141</v>
+        <v>15</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -3480,10 +3557,10 @@
         <v>13</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>142</v>
+        <v>368</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>143</v>
+        <v>369</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>12</v>
@@ -3494,10 +3571,10 @@
         <v>13</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>144</v>
+        <v>370</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>145</v>
+        <v>15</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>12</v>
@@ -3508,10 +3585,10 @@
         <v>13</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>146</v>
+        <v>371</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>15</v>
+        <v>372</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>12</v>
@@ -3522,10 +3599,10 @@
         <v>13</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>148</v>
+        <v>15</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>12</v>
@@ -3536,10 +3613,10 @@
         <v>13</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>15</v>
+        <v>412</v>
       </c>
       <c r="D97" s="3" t="s">
         <v>12</v>
@@ -3550,10 +3627,10 @@
         <v>13</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>151</v>
+        <v>15</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>12</v>
@@ -3564,10 +3641,10 @@
         <v>13</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>402</v>
+        <v>131</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>15</v>
+        <v>132</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>12</v>
@@ -3578,10 +3655,10 @@
         <v>13</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>403</v>
+        <v>133</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>12</v>
@@ -3592,10 +3669,10 @@
         <v>13</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>405</v>
+        <v>134</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>15</v>
+        <v>414</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>12</v>
@@ -3606,10 +3683,10 @@
         <v>13</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>406</v>
+        <v>135</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>407</v>
+        <v>415</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>12</v>
@@ -3620,10 +3697,10 @@
         <v>13</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>15</v>
+        <v>416</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>12</v>
@@ -3634,10 +3711,10 @@
         <v>13</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>154</v>
+        <v>417</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>12</v>
@@ -3648,10 +3725,10 @@
         <v>13</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>15</v>
+        <v>418</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>12</v>
@@ -3662,10 +3739,10 @@
         <v>13</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>157</v>
+        <v>419</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>12</v>
@@ -3676,10 +3753,10 @@
         <v>13</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>15</v>
+        <v>386</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>12</v>
@@ -3690,10 +3767,10 @@
         <v>13</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>15</v>
+        <v>420</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>12</v>
@@ -3704,10 +3781,10 @@
         <v>13</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>15</v>
+        <v>386</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>12</v>
@@ -3718,10 +3795,10 @@
         <v>13</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>15</v>
+        <v>144</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>12</v>
@@ -3732,10 +3809,10 @@
         <v>13</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>15</v>
+        <v>386</v>
       </c>
       <c r="D111" s="3" t="s">
         <v>12</v>
@@ -3746,10 +3823,10 @@
         <v>13</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>15</v>
+        <v>147</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>12</v>
@@ -3760,10 +3837,10 @@
         <v>13</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>165</v>
+        <v>386</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>12</v>
@@ -3774,10 +3851,10 @@
         <v>13</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>15</v>
+        <v>150</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>12</v>
@@ -3788,10 +3865,10 @@
         <v>13</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>168</v>
+        <v>386</v>
       </c>
       <c r="D115" s="3" t="s">
         <v>12</v>
@@ -3802,10 +3879,10 @@
         <v>13</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>15</v>
+        <v>153</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>12</v>
@@ -3816,10 +3893,10 @@
         <v>13</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>171</v>
+        <v>386</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>12</v>
@@ -3830,10 +3907,10 @@
         <v>13</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>15</v>
+        <v>421</v>
       </c>
       <c r="D118" s="3" t="s">
         <v>12</v>
@@ -3844,10 +3921,10 @@
         <v>13</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>174</v>
+        <v>386</v>
       </c>
       <c r="D119" s="3" t="s">
         <v>12</v>
@@ -3858,10 +3935,10 @@
         <v>13</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>15</v>
+        <v>422</v>
       </c>
       <c r="D120" s="3" t="s">
         <v>12</v>
@@ -3872,10 +3949,10 @@
         <v>13</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>177</v>
+        <v>423</v>
       </c>
       <c r="D121" s="3" t="s">
         <v>12</v>
@@ -3886,10 +3963,10 @@
         <v>13</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>15</v>
+        <v>424</v>
       </c>
       <c r="D122" s="3" t="s">
         <v>12</v>
@@ -3900,10 +3977,10 @@
         <v>13</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>180</v>
+        <v>425</v>
       </c>
       <c r="D123" s="3" t="s">
         <v>12</v>
@@ -3914,10 +3991,10 @@
         <v>13</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>15</v>
+        <v>162</v>
       </c>
       <c r="D124" s="3" t="s">
         <v>12</v>
@@ -3928,10 +4005,10 @@
         <v>13</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>12</v>
@@ -3942,10 +4019,10 @@
         <v>13</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>15</v>
+        <v>166</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>12</v>
@@ -3956,10 +4033,10 @@
         <v>13</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>12</v>
@@ -3970,10 +4047,10 @@
         <v>13</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="D128" s="3" t="s">
         <v>12</v>
@@ -3984,10 +4061,10 @@
         <v>13</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="D129" s="3" t="s">
         <v>12</v>
@@ -3998,10 +4075,10 @@
         <v>13</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>15</v>
+        <v>174</v>
       </c>
       <c r="D130" s="3" t="s">
         <v>12</v>
@@ -4012,10 +4089,10 @@
         <v>13</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="D131" s="3" t="s">
         <v>12</v>
@@ -4026,10 +4103,10 @@
         <v>13</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="D132" s="3" t="s">
         <v>12</v>
@@ -4040,10 +4117,10 @@
         <v>13</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="D133" s="3" t="s">
         <v>12</v>
@@ -4054,10 +4131,10 @@
         <v>13</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="D134" s="3" t="s">
         <v>12</v>
@@ -4068,10 +4145,10 @@
         <v>13</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="D135" s="3" t="s">
         <v>12</v>
@@ -4082,10 +4159,10 @@
         <v>13</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="D136" s="3" t="s">
         <v>12</v>
@@ -4096,10 +4173,10 @@
         <v>13</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="D137" s="3" t="s">
         <v>12</v>
@@ -4110,10 +4187,10 @@
         <v>13</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="D138" s="3" t="s">
         <v>12</v>
@@ -4124,10 +4201,10 @@
         <v>13</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="D139" s="3" t="s">
         <v>12</v>
@@ -4138,10 +4215,10 @@
         <v>13</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="D140" s="3" t="s">
         <v>12</v>
@@ -4152,10 +4229,10 @@
         <v>13</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="D141" s="3" t="s">
         <v>12</v>
@@ -4166,10 +4243,10 @@
         <v>13</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="D142" s="3" t="s">
         <v>12</v>
@@ -4180,10 +4257,10 @@
         <v>13</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="D143" s="3" t="s">
         <v>12</v>
@@ -4194,10 +4271,10 @@
         <v>13</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="D144" s="3" t="s">
         <v>12</v>
@@ -4208,10 +4285,10 @@
         <v>13</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
       <c r="D145" s="3" t="s">
         <v>12</v>
@@ -4222,10 +4299,10 @@
         <v>13</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="D146" s="3" t="s">
         <v>12</v>
@@ -4236,10 +4313,10 @@
         <v>13</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="D147" s="3" t="s">
         <v>12</v>
@@ -4250,10 +4327,10 @@
         <v>13</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="D148" s="3" t="s">
         <v>12</v>
@@ -4264,10 +4341,10 @@
         <v>13</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="D149" s="3" t="s">
         <v>12</v>
@@ -4278,10 +4355,10 @@
         <v>13</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="D150" s="3" t="s">
         <v>12</v>
@@ -4292,10 +4369,10 @@
         <v>13</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="D151" s="3" t="s">
         <v>12</v>
@@ -4306,10 +4383,10 @@
         <v>13</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>235</v>
+        <v>386</v>
       </c>
       <c r="D152" s="3" t="s">
         <v>12</v>
@@ -4320,10 +4397,10 @@
         <v>13</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
       <c r="D153" s="3" t="s">
         <v>12</v>
@@ -4334,10 +4411,10 @@
         <v>13</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="D154" s="3" t="s">
         <v>12</v>
@@ -4348,10 +4425,10 @@
         <v>13</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="D155" s="3" t="s">
         <v>12</v>
@@ -4362,10 +4439,10 @@
         <v>13</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="D156" s="3" t="s">
         <v>12</v>
@@ -4376,10 +4453,10 @@
         <v>13</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="D157" s="3" t="s">
         <v>12</v>
@@ -4390,10 +4467,10 @@
         <v>13</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="D158" s="3" t="s">
         <v>12</v>
@@ -4404,10 +4481,10 @@
         <v>13</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>15</v>
+        <v>426</v>
       </c>
       <c r="D159" s="3" t="s">
         <v>12</v>
@@ -4418,10 +4495,10 @@
         <v>13</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>250</v>
+        <v>427</v>
       </c>
       <c r="D160" s="3" t="s">
         <v>12</v>
@@ -4432,10 +4509,10 @@
         <v>13</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>251</v>
+        <v>232</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>252</v>
+        <v>233</v>
       </c>
       <c r="D161" s="3" t="s">
         <v>12</v>
@@ -4446,10 +4523,10 @@
         <v>13</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
       <c r="D162" s="3" t="s">
         <v>12</v>
@@ -4460,10 +4537,10 @@
         <v>13</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>255</v>
+        <v>236</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>256</v>
+        <v>428</v>
       </c>
       <c r="D163" s="3" t="s">
         <v>12</v>
@@ -4474,10 +4551,10 @@
         <v>13</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="D164" s="3" t="s">
         <v>12</v>
@@ -4488,10 +4565,10 @@
         <v>13</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="D165" s="3" t="s">
         <v>12</v>
@@ -4502,10 +4579,10 @@
         <v>13</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>15</v>
+        <v>242</v>
       </c>
       <c r="D166" s="3" t="s">
         <v>12</v>
@@ -4516,10 +4593,10 @@
         <v>13</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>262</v>
+        <v>243</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>15</v>
+        <v>244</v>
       </c>
       <c r="D167" s="3" t="s">
         <v>12</v>
@@ -4530,10 +4607,10 @@
         <v>13</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="D168" s="3" t="s">
         <v>12</v>
@@ -4544,10 +4621,10 @@
         <v>13</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="D169" s="3" t="s">
         <v>12</v>
@@ -4558,10 +4635,10 @@
         <v>13</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>15</v>
+        <v>250</v>
       </c>
       <c r="D170" s="3" t="s">
         <v>12</v>
@@ -4572,10 +4649,10 @@
         <v>13</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="D171" s="3" t="s">
         <v>12</v>
@@ -4586,10 +4663,10 @@
         <v>13</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="D172" s="3" t="s">
         <v>12</v>
@@ -4600,10 +4677,10 @@
         <v>13</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="D173" s="3" t="s">
         <v>12</v>
@@ -4614,10 +4691,10 @@
         <v>13</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="D174" s="3" t="s">
         <v>12</v>
@@ -4628,10 +4705,10 @@
         <v>13</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>277</v>
+        <v>429</v>
       </c>
       <c r="D175" s="3" t="s">
         <v>12</v>
@@ -4642,10 +4719,10 @@
         <v>13</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>279</v>
+        <v>261</v>
       </c>
       <c r="D176" s="3" t="s">
         <v>12</v>
@@ -4656,10 +4733,10 @@
         <v>13</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="D177" s="3" t="s">
         <v>12</v>
@@ -4670,10 +4747,10 @@
         <v>13</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>282</v>
+        <v>264</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>283</v>
+        <v>265</v>
       </c>
       <c r="D178" s="3" t="s">
         <v>12</v>
@@ -4684,10 +4761,10 @@
         <v>13</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>285</v>
+        <v>267</v>
       </c>
       <c r="D179" s="3" t="s">
         <v>12</v>
@@ -4698,10 +4775,10 @@
         <v>13</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>286</v>
+        <v>268</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>287</v>
+        <v>269</v>
       </c>
       <c r="D180" s="3" t="s">
         <v>12</v>
@@ -4712,10 +4789,10 @@
         <v>13</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>288</v>
+        <v>270</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>289</v>
+        <v>271</v>
       </c>
       <c r="D181" s="3" t="s">
         <v>12</v>
@@ -4726,10 +4803,10 @@
         <v>13</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>290</v>
+        <v>272</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>15</v>
+        <v>273</v>
       </c>
       <c r="D182" s="3" t="s">
         <v>12</v>
@@ -4740,10 +4817,10 @@
         <v>13</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>291</v>
+        <v>274</v>
       </c>
       <c r="C183" s="3" t="s">
-        <v>292</v>
+        <v>275</v>
       </c>
       <c r="D183" s="3" t="s">
         <v>12</v>
@@ -4754,10 +4831,10 @@
         <v>13</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>293</v>
+        <v>276</v>
       </c>
       <c r="C184" s="3" t="s">
-        <v>294</v>
+        <v>277</v>
       </c>
       <c r="D184" s="3" t="s">
         <v>12</v>
@@ -4768,10 +4845,10 @@
         <v>13</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>296</v>
+        <v>430</v>
       </c>
       <c r="D185" s="3" t="s">
         <v>12</v>
@@ -4782,10 +4859,10 @@
         <v>13</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
       <c r="D186" s="3" t="s">
         <v>12</v>
@@ -4796,10 +4873,10 @@
         <v>13</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>300</v>
+        <v>431</v>
       </c>
       <c r="D187" s="3" t="s">
         <v>12</v>
@@ -4810,10 +4887,10 @@
         <v>13</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>301</v>
+        <v>282</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>302</v>
+        <v>432</v>
       </c>
       <c r="D188" s="3" t="s">
         <v>12</v>
@@ -4824,10 +4901,10 @@
         <v>13</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>304</v>
+        <v>433</v>
       </c>
       <c r="D189" s="3" t="s">
         <v>12</v>
@@ -4838,10 +4915,10 @@
         <v>13</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>305</v>
+        <v>373</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>306</v>
+        <v>15</v>
       </c>
       <c r="D190" s="3" t="s">
         <v>12</v>
@@ -4852,10 +4929,10 @@
         <v>13</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>307</v>
+        <v>362</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>308</v>
+        <v>434</v>
       </c>
       <c r="D191" s="3" t="s">
         <v>12</v>
@@ -4866,10 +4943,10 @@
         <v>13</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>309</v>
+        <v>284</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>15</v>
+        <v>435</v>
       </c>
       <c r="D192" s="3" t="s">
         <v>12</v>
@@ -4880,10 +4957,10 @@
         <v>13</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>311</v>
+        <v>436</v>
       </c>
       <c r="D193" s="3" t="s">
         <v>12</v>
@@ -4894,10 +4971,10 @@
         <v>13</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>312</v>
+        <v>361</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>15</v>
+        <v>437</v>
       </c>
       <c r="D194" s="3" t="s">
         <v>12</v>
@@ -4905,13 +4982,13 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B195" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="C195" s="3" t="s">
-        <v>314</v>
+        <v>285</v>
+      </c>
+      <c r="B195" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C195" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="D195" s="3" t="s">
         <v>12</v>
@@ -4922,13 +4999,13 @@
         <v>13</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>315</v>
+        <v>42</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>316</v>
+        <v>43</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -4936,10 +5013,10 @@
         <v>13</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>408</v>
+        <v>286</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>15</v>
+        <v>287</v>
       </c>
       <c r="D197" s="3" t="s">
         <v>12</v>
@@ -4950,10 +5027,10 @@
         <v>13</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>395</v>
+        <v>288</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>15</v>
+        <v>289</v>
       </c>
       <c r="D198" s="3" t="s">
         <v>12</v>
@@ -4964,22 +5041,24 @@
         <v>13</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>317</v>
+        <v>290</v>
       </c>
       <c r="C199" s="3" t="s">
-        <v>15</v>
+        <v>291</v>
       </c>
       <c r="D199" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="3"/>
-      <c r="B200" s="4" t="s">
-        <v>410</v>
-      </c>
-      <c r="C200" s="4" t="s">
-        <v>411</v>
+      <c r="A200" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C200" s="3" t="s">
+        <v>293</v>
       </c>
       <c r="D200" s="3" t="s">
         <v>12</v>
@@ -4990,10 +5069,10 @@
         <v>13</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>394</v>
+        <v>294</v>
       </c>
       <c r="C201" s="3" t="s">
-        <v>409</v>
+        <v>295</v>
       </c>
       <c r="D201" s="3" t="s">
         <v>12</v>
@@ -5001,13 +5080,13 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
-        <v>318</v>
+        <v>13</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>10</v>
+        <v>296</v>
       </c>
       <c r="C202" s="3" t="s">
-        <v>11</v>
+        <v>297</v>
       </c>
       <c r="D202" s="3" t="s">
         <v>12</v>
@@ -5018,10 +5097,10 @@
         <v>13</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>43</v>
+        <v>298</v>
       </c>
       <c r="C203" s="3" t="s">
-        <v>44</v>
+        <v>299</v>
       </c>
       <c r="D203" s="3" t="s">
         <v>12</v>
@@ -5032,13 +5111,13 @@
         <v>13</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="C204" s="3" t="s">
-        <v>320</v>
+        <v>301</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -5046,10 +5125,10 @@
         <v>13</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>321</v>
+        <v>302</v>
       </c>
       <c r="C205" s="3" t="s">
-        <v>322</v>
+        <v>303</v>
       </c>
       <c r="D205" s="3" t="s">
         <v>12</v>
@@ -5060,10 +5139,10 @@
         <v>13</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>323</v>
+        <v>304</v>
       </c>
       <c r="C206" s="3" t="s">
-        <v>324</v>
+        <v>305</v>
       </c>
       <c r="D206" s="3" t="s">
         <v>12</v>
@@ -5074,10 +5153,10 @@
         <v>13</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>325</v>
+        <v>306</v>
       </c>
       <c r="C207" s="3" t="s">
-        <v>326</v>
+        <v>307</v>
       </c>
       <c r="D207" s="3" t="s">
         <v>12</v>
@@ -5088,10 +5167,10 @@
         <v>13</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>327</v>
+        <v>308</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>328</v>
+        <v>309</v>
       </c>
       <c r="D208" s="3" t="s">
         <v>12</v>
@@ -5102,10 +5181,10 @@
         <v>13</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>329</v>
+        <v>310</v>
       </c>
       <c r="C209" s="3" t="s">
-        <v>330</v>
+        <v>311</v>
       </c>
       <c r="D209" s="3" t="s">
         <v>12</v>
@@ -5116,10 +5195,10 @@
         <v>13</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>331</v>
+        <v>312</v>
       </c>
       <c r="C210" s="3" t="s">
-        <v>332</v>
+        <v>313</v>
       </c>
       <c r="D210" s="3" t="s">
         <v>12</v>
@@ -5130,10 +5209,10 @@
         <v>13</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>333</v>
+        <v>314</v>
       </c>
       <c r="C211" s="3" t="s">
-        <v>334</v>
+        <v>35</v>
       </c>
       <c r="D211" s="3" t="s">
         <v>12</v>
@@ -5141,16 +5220,16 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
-        <v>13</v>
+        <v>315</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>335</v>
+        <v>42</v>
       </c>
       <c r="C212" s="3" t="s">
-        <v>336</v>
+        <v>43</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5158,10 +5237,10 @@
         <v>13</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>337</v>
+        <v>10</v>
       </c>
       <c r="C213" s="3" t="s">
-        <v>338</v>
+        <v>11</v>
       </c>
       <c r="D213" s="3" t="s">
         <v>12</v>
@@ -5172,10 +5251,10 @@
         <v>13</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>339</v>
+        <v>316</v>
       </c>
       <c r="C214" s="3" t="s">
-        <v>340</v>
+        <v>317</v>
       </c>
       <c r="D214" s="3" t="s">
         <v>12</v>
@@ -5186,10 +5265,10 @@
         <v>13</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>341</v>
+        <v>318</v>
       </c>
       <c r="C215" s="3" t="s">
-        <v>342</v>
+        <v>319</v>
       </c>
       <c r="D215" s="3" t="s">
         <v>12</v>
@@ -5200,10 +5279,10 @@
         <v>13</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>343</v>
+        <v>320</v>
       </c>
       <c r="C216" s="3" t="s">
-        <v>344</v>
+        <v>321</v>
       </c>
       <c r="D216" s="3" t="s">
         <v>12</v>
@@ -5214,10 +5293,10 @@
         <v>13</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>345</v>
+        <v>322</v>
       </c>
       <c r="C217" s="3" t="s">
-        <v>346</v>
+        <v>323</v>
       </c>
       <c r="D217" s="3" t="s">
         <v>12</v>
@@ -5228,10 +5307,10 @@
         <v>13</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>347</v>
+        <v>324</v>
       </c>
       <c r="C218" s="3" t="s">
-        <v>36</v>
+        <v>325</v>
       </c>
       <c r="D218" s="3" t="s">
         <v>12</v>
@@ -5239,13 +5318,13 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>348</v>
+        <v>13</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>43</v>
+        <v>326</v>
       </c>
       <c r="C219" s="3" t="s">
-        <v>44</v>
+        <v>327</v>
       </c>
       <c r="D219" s="3" t="s">
         <v>12</v>
@@ -5256,13 +5335,13 @@
         <v>13</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>10</v>
+        <v>328</v>
       </c>
       <c r="C220" s="3" t="s">
-        <v>11</v>
+        <v>329</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -5270,10 +5349,10 @@
         <v>13</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>349</v>
+        <v>330</v>
       </c>
       <c r="C221" s="3" t="s">
-        <v>350</v>
+        <v>331</v>
       </c>
       <c r="D221" s="3" t="s">
         <v>12</v>
@@ -5284,10 +5363,10 @@
         <v>13</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>351</v>
+        <v>332</v>
       </c>
       <c r="C222" s="3" t="s">
-        <v>352</v>
+        <v>333</v>
       </c>
       <c r="D222" s="3" t="s">
         <v>12</v>
@@ -5298,10 +5377,10 @@
         <v>13</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>353</v>
+        <v>334</v>
       </c>
       <c r="C223" s="3" t="s">
-        <v>354</v>
+        <v>335</v>
       </c>
       <c r="D223" s="3" t="s">
         <v>12</v>
@@ -5312,10 +5391,10 @@
         <v>13</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>355</v>
+        <v>336</v>
       </c>
       <c r="C224" s="3" t="s">
-        <v>356</v>
+        <v>337</v>
       </c>
       <c r="D224" s="3" t="s">
         <v>12</v>
@@ -5326,10 +5405,10 @@
         <v>13</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="C225" s="3" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="D225" s="3" t="s">
         <v>12</v>
@@ -5340,10 +5419,10 @@
         <v>13</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>359</v>
+        <v>340</v>
       </c>
       <c r="C226" s="3" t="s">
-        <v>360</v>
+        <v>341</v>
       </c>
       <c r="D226" s="3" t="s">
         <v>12</v>
@@ -5354,10 +5433,10 @@
         <v>13</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>361</v>
+        <v>342</v>
       </c>
       <c r="C227" s="3" t="s">
-        <v>362</v>
+        <v>343</v>
       </c>
       <c r="D227" s="3" t="s">
         <v>12</v>
@@ -5368,96 +5447,96 @@
         <v>13</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>363</v>
+        <v>344</v>
       </c>
       <c r="C228" s="3" t="s">
-        <v>364</v>
+        <v>345</v>
       </c>
       <c r="D228" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A229" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B229" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="C229" s="3" t="s">
-        <v>366</v>
-      </c>
-      <c r="D229" s="3" t="s">
+      <c r="A229" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D229" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A230" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B230" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="C230" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="D230" s="3" t="s">
+      <c r="A230" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="D230" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B231" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="C231" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="D231" s="3" t="s">
+      <c r="A231" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D231" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B232" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="C232" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="D232" s="3" t="s">
+      <c r="A232" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B232" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="D232" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B233" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="C233" s="3" t="s">
-        <v>374</v>
-      </c>
-      <c r="D233" s="3" t="s">
+      <c r="A233" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="D233" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B234" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="C234" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="D234" s="3" t="s">
+      <c r="A234" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D234" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -5466,10 +5545,10 @@
         <v>13</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>377</v>
+        <v>358</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>378</v>
+        <v>359</v>
       </c>
       <c r="D235" s="2" t="s">
         <v>12</v>
@@ -5480,115 +5559,17 @@
         <v>13</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>379</v>
+        <v>360</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>380</v>
+        <v>35</v>
       </c>
       <c r="D236" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A237" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B237" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="C237" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="D237" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A238" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B238" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="C238" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="D238" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A239" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B239" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="C239" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="D239" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A240" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B240" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="C240" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="D240" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A241" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B241" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="C241" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="D241" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A242" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B242" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="C242" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="D242" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A243" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B243" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="C243" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D243" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="447" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="448" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
- optimization of the timestamp in all tables by temporarily replacing the tigger - fix bug in mrp document double display field
</commit_message>
<xml_diff>
--- a/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
+++ b/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\INTERPOLAR\R-db2frontend\db2frontend\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mreusche.LIFE.000\Nextcloud\arbeit\Teilprojekte\Interpolar\Datenbankstruktur\Release 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="438">
   <si>
     <t xml:space="preserve">Station </t>
   </si>
@@ -1883,7 +1883,18 @@
     <cellStyle name="Warnender Text" xfId="15" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Zelle überprüfen" xfId="14" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2193,9 +2204,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F441"/>
+  <dimension ref="A1:F440"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A177" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C188" sqref="C188"/>
     </sheetView>
   </sheetViews>
@@ -3546,7 +3557,7 @@
         <v>367</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>15</v>
+        <v>436</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>12</v>
@@ -4957,10 +4968,10 @@
         <v>13</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D193" s="3" t="s">
         <v>12</v>
@@ -4968,13 +4979,13 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B194" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="C194" s="3" t="s">
-        <v>437</v>
+        <v>285</v>
+      </c>
+      <c r="B194" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C194" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="D194" s="3" t="s">
         <v>12</v>
@@ -4982,16 +4993,16 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="B195" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C195" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C195" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -4999,13 +5010,13 @@
         <v>13</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>42</v>
+        <v>286</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>43</v>
+        <v>287</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -5013,10 +5024,10 @@
         <v>13</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D197" s="3" t="s">
         <v>12</v>
@@ -5027,10 +5038,10 @@
         <v>13</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D198" s="3" t="s">
         <v>12</v>
@@ -5041,10 +5052,10 @@
         <v>13</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C199" s="3" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="D199" s="3" t="s">
         <v>12</v>
@@ -5055,10 +5066,10 @@
         <v>13</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C200" s="3" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D200" s="3" t="s">
         <v>12</v>
@@ -5069,10 +5080,10 @@
         <v>13</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C201" s="3" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D201" s="3" t="s">
         <v>12</v>
@@ -5083,10 +5094,10 @@
         <v>13</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C202" s="3" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D202" s="3" t="s">
         <v>12</v>
@@ -5097,10 +5108,10 @@
         <v>13</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C203" s="3" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D203" s="3" t="s">
         <v>12</v>
@@ -5111,10 +5122,10 @@
         <v>13</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C204" s="3" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D204" s="3" t="s">
         <v>12</v>
@@ -5125,10 +5136,10 @@
         <v>13</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C205" s="3" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D205" s="3" t="s">
         <v>12</v>
@@ -5139,10 +5150,10 @@
         <v>13</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C206" s="3" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D206" s="3" t="s">
         <v>12</v>
@@ -5153,10 +5164,10 @@
         <v>13</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C207" s="3" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D207" s="3" t="s">
         <v>12</v>
@@ -5167,10 +5178,10 @@
         <v>13</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D208" s="3" t="s">
         <v>12</v>
@@ -5181,10 +5192,10 @@
         <v>13</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C209" s="3" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="D209" s="3" t="s">
         <v>12</v>
@@ -5195,10 +5206,10 @@
         <v>13</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C210" s="3" t="s">
-        <v>313</v>
+        <v>35</v>
       </c>
       <c r="D210" s="3" t="s">
         <v>12</v>
@@ -5206,30 +5217,30 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="s">
-        <v>13</v>
+        <v>315</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>314</v>
+        <v>42</v>
       </c>
       <c r="C211" s="3" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
-        <v>315</v>
+        <v>13</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="C212" s="3" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5237,10 +5248,10 @@
         <v>13</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>10</v>
+        <v>316</v>
       </c>
       <c r="C213" s="3" t="s">
-        <v>11</v>
+        <v>317</v>
       </c>
       <c r="D213" s="3" t="s">
         <v>12</v>
@@ -5251,10 +5262,10 @@
         <v>13</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C214" s="3" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D214" s="3" t="s">
         <v>12</v>
@@ -5265,10 +5276,10 @@
         <v>13</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C215" s="3" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D215" s="3" t="s">
         <v>12</v>
@@ -5279,10 +5290,10 @@
         <v>13</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C216" s="3" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D216" s="3" t="s">
         <v>12</v>
@@ -5293,10 +5304,10 @@
         <v>13</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C217" s="3" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D217" s="3" t="s">
         <v>12</v>
@@ -5307,10 +5318,10 @@
         <v>13</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C218" s="3" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="D218" s="3" t="s">
         <v>12</v>
@@ -5321,10 +5332,10 @@
         <v>13</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C219" s="3" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="D219" s="3" t="s">
         <v>12</v>
@@ -5335,10 +5346,10 @@
         <v>13</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C220" s="3" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D220" s="3" t="s">
         <v>12</v>
@@ -5349,10 +5360,10 @@
         <v>13</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C221" s="3" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D221" s="3" t="s">
         <v>12</v>
@@ -5363,10 +5374,10 @@
         <v>13</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C222" s="3" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D222" s="3" t="s">
         <v>12</v>
@@ -5377,10 +5388,10 @@
         <v>13</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C223" s="3" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D223" s="3" t="s">
         <v>12</v>
@@ -5391,10 +5402,10 @@
         <v>13</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C224" s="3" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D224" s="3" t="s">
         <v>12</v>
@@ -5405,10 +5416,10 @@
         <v>13</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="C225" s="3" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="D225" s="3" t="s">
         <v>12</v>
@@ -5419,10 +5430,10 @@
         <v>13</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C226" s="3" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D226" s="3" t="s">
         <v>12</v>
@@ -5433,26 +5444,26 @@
         <v>13</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C227" s="3" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D227" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A228" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B228" s="3" t="s">
-        <v>344</v>
-      </c>
-      <c r="C228" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="D228" s="3" t="s">
+      <c r="A228" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B228" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D228" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -5461,10 +5472,10 @@
         <v>13</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D229" s="2" t="s">
         <v>12</v>
@@ -5475,10 +5486,10 @@
         <v>13</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="D230" s="2" t="s">
         <v>12</v>
@@ -5489,10 +5500,10 @@
         <v>13</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="D231" s="2" t="s">
         <v>12</v>
@@ -5503,10 +5514,10 @@
         <v>13</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="D232" s="2" t="s">
         <v>12</v>
@@ -5517,10 +5528,10 @@
         <v>13</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C233" s="2" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="D233" s="2" t="s">
         <v>12</v>
@@ -5531,10 +5542,10 @@
         <v>13</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C234" s="2" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="D234" s="2" t="s">
         <v>12</v>
@@ -5545,32 +5556,21 @@
         <v>13</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>359</v>
+        <v>35</v>
       </c>
       <c r="D235" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A236" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B236" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="C236" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D236" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
+    <row r="439" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="440" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="441" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
DB - Data type change of study data from date to timestamp
</commit_message>
<xml_diff>
--- a/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
+++ b/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mreusche.LIFE.000\Nextcloud\arbeit\Teilprojekte\Interpolar\Datenbankstruktur\Release 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\borzem\Desktop\IP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="4200" windowHeight="6375" tabRatio="791"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10860" tabRatio="791"/>
   </bookViews>
   <sheets>
     <sheet name="frontend_table_description" sheetId="15" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="439">
   <si>
     <t xml:space="preserve">Station </t>
   </si>
@@ -1339,6 +1339,9 @@
   </si>
   <si>
     <t>Frontend Complete-Status, wenn ein Pflichtitem fehlt Status bei Import wieder auf Incomplete setzen  - 0, Incomplete | 1, Unverified | 2, Complete</t>
+  </si>
+  <si>
+    <t>timestamp</t>
   </si>
 </sst>
 </file>
@@ -2206,8 +2209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F440"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A177" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C188" sqref="C188"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85:XFD85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2612,7 +2615,7 @@
         <v>52</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>28</v>
+        <v>438</v>
       </c>
       <c r="E26" s="3"/>
     </row>
@@ -2957,7 +2960,7 @@
         <v>84</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>28</v>
+        <v>438</v>
       </c>
       <c r="E49" s="3"/>
     </row>
@@ -3098,7 +3101,7 @@
         <v>94</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>28</v>
+        <v>438</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -3462,7 +3465,7 @@
         <v>119</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>28</v>
+        <v>438</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
DB - fix empty descriptions and regenerate the SQL scripts for the frontend for version Table Descr. v03.03.2025 Refs #626
</commit_message>
<xml_diff>
--- a/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
+++ b/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="580">
   <si>
     <t xml:space="preserve">Station </t>
   </si>
@@ -1762,6 +1762,9 @@
   </si>
   <si>
     <t>retrolektive_mrp_bewertung</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -3027,8 +3030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F535"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5504,7 +5507,9 @@
       <c r="B187" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C187" s="3"/>
+      <c r="C187" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="D187" s="3" t="s">
         <v>12</v>
       </c>
@@ -5514,7 +5519,9 @@
       <c r="B188" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C188" s="3"/>
+      <c r="C188" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="D188" s="3" t="s">
         <v>12</v>
       </c>
@@ -5524,7 +5531,9 @@
       <c r="B189" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C189" s="3"/>
+      <c r="C189" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="D189" s="3" t="s">
         <v>12</v>
       </c>
@@ -6219,7 +6228,9 @@
       <c r="B247" s="3" t="s">
         <v>521</v>
       </c>
-      <c r="C247" s="3"/>
+      <c r="C247" s="3" t="s">
+        <v>579</v>
+      </c>
       <c r="D247" s="3" t="s">
         <v>12</v>
       </c>
@@ -6709,7 +6720,9 @@
       <c r="B288" s="3" t="s">
         <v>567</v>
       </c>
-      <c r="C288" s="3"/>
+      <c r="C288" s="3" t="s">
+        <v>579</v>
+      </c>
       <c r="D288" s="3" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
DB - fixing duplicate column labels Refs #625
</commit_message>
<xml_diff>
--- a/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
+++ b/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
@@ -1764,7 +1764,7 @@
     <t>retrolektive_mrp_bewertung</t>
   </si>
   <si>
-    <t>NA</t>
+    <t>ret_massn_orga2</t>
   </si>
 </sst>
 </file>
@@ -2337,7 +2337,397 @@
     <cellStyle name="Warnender Text" xfId="15" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Zelle überprüfen" xfId="14" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="77">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3030,8 +3420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F535"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6229,7 +6619,7 @@
         <v>521</v>
       </c>
       <c r="C247" s="3" t="s">
-        <v>579</v>
+        <v>239</v>
       </c>
       <c r="D247" s="3" t="s">
         <v>12</v>
@@ -6598,7 +6988,7 @@
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" s="3"/>
       <c r="B278" s="3" t="s">
-        <v>509</v>
+        <v>579</v>
       </c>
       <c r="C278" s="8" t="s">
         <v>221</v>
@@ -6721,7 +7111,7 @@
         <v>567</v>
       </c>
       <c r="C288" s="3" t="s">
-        <v>579</v>
+        <v>239</v>
       </c>
       <c r="D288" s="3" t="s">
         <v>12</v>
@@ -7319,118 +7709,121 @@
     <row r="535" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="B65:B67">
-    <cfRule type="duplicateValues" dxfId="37" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="76" priority="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B70">
-    <cfRule type="duplicateValues" dxfId="36" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="75" priority="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B72">
-    <cfRule type="duplicateValues" dxfId="35" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="74" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="duplicateValues" dxfId="34" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="73" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B82">
-    <cfRule type="duplicateValues" dxfId="33" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="72" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B98">
-    <cfRule type="duplicateValues" dxfId="32" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="71" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B109">
-    <cfRule type="duplicateValues" dxfId="31" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="70" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B112">
-    <cfRule type="duplicateValues" dxfId="30" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="69" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B115">
-    <cfRule type="duplicateValues" dxfId="29" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B121">
-    <cfRule type="duplicateValues" dxfId="28" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="67" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B150">
-    <cfRule type="duplicateValues" dxfId="27" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B152">
-    <cfRule type="duplicateValues" dxfId="26" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B154">
-    <cfRule type="duplicateValues" dxfId="25" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="64" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B156">
-    <cfRule type="duplicateValues" dxfId="24" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B168">
-    <cfRule type="duplicateValues" dxfId="23" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="62" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B178">
-    <cfRule type="duplicateValues" dxfId="22" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="61" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B180">
-    <cfRule type="duplicateValues" dxfId="21" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B183">
-    <cfRule type="duplicateValues" dxfId="20" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B190">
-    <cfRule type="duplicateValues" dxfId="19" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B202">
-    <cfRule type="duplicateValues" dxfId="18" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B205">
-    <cfRule type="duplicateValues" dxfId="17" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B212">
-    <cfRule type="duplicateValues" dxfId="16" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B219">
-    <cfRule type="duplicateValues" dxfId="15" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B221">
-    <cfRule type="duplicateValues" dxfId="14" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B224">
-    <cfRule type="duplicateValues" dxfId="13" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B236">
-    <cfRule type="duplicateValues" dxfId="12" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B246">
-    <cfRule type="duplicateValues" dxfId="11" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B248">
-    <cfRule type="duplicateValues" dxfId="10" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B253">
-    <cfRule type="duplicateValues" dxfId="9" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B254:B257">
-    <cfRule type="duplicateValues" dxfId="8" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B258:B259 B261 B263:B264 B266:B276 B278:B286 B288">
-    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B260">
-    <cfRule type="duplicateValues" dxfId="6" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B262">
-    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B265">
-    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B277">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B287">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B289:B1048576 B157:B167 B122:B149 B113:B114 B110:B111 B68:B69 B1:B20 B22 B25:B41 B71 B73:B81 B43:B61 B83:B97 B99:B108 B116:B120 B151 B153 B155 B169:B177 B179 B181:B182 B184:B189 B191:B201 B203:B204 B206:B211 B213:B216">
-    <cfRule type="duplicateValues" dxfId="1" priority="70"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="71"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B217:B218 B220 B222:B223 B225:B235 B237:B245 B247 B249:B252">
-    <cfRule type="duplicateValues" dxfId="0" priority="97"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="98"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Remove multiline comments in  Frontend_Table_Description.xlsx generation
</commit_message>
<xml_diff>
--- a/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
+++ b/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
@@ -233,13 +233,13 @@
     <t xml:space="preserve">meda_anlage</t>
   </si>
   <si>
-    <t xml:space="preserve">Formular angelegt von </t>
+    <t xml:space="preserve">Formular angelegt von</t>
   </si>
   <si>
     <t xml:space="preserve">meda_edit</t>
   </si>
   <si>
-    <t xml:space="preserve">Formular zuletzt bearbeitet von </t>
+    <t xml:space="preserve">Formular zuletzt bearbeitet von</t>
   </si>
   <si>
     <t xml:space="preserve">fall_meda_id</t>
@@ -251,8 +251,7 @@
     <t xml:space="preserve">meda_id</t>
   </si>
   <si>
-    <t xml:space="preserve">ID Medikationsanalyse
-</t>
+    <t xml:space="preserve">ID Medikationsanalyse</t>
   </si>
   <si>
     <t xml:space="preserve">meda_typ</t>
@@ -330,7 +329,7 @@
     <t xml:space="preserve">meda_aufwand_zeit</t>
   </si>
   <si>
-    <t xml:space="preserve">Zeitaufwand Medikationsanalyse </t>
+    <t xml:space="preserve">Zeitaufwand Medikationsanalyse</t>
   </si>
   <si>
     <t xml:space="preserve">meda_aufwand_zeit_and</t>
@@ -396,7 +395,7 @@
     <t xml:space="preserve">mrp_hinweisgeber_oth</t>
   </si>
   <si>
-    <t xml:space="preserve">Anderer Hinweisgeber </t>
+    <t xml:space="preserve">Anderer Hinweisgeber</t>
   </si>
   <si>
     <t xml:space="preserve">mrp_wirkstoff</t>
@@ -780,7 +779,7 @@
     <t xml:space="preserve">ret_bewerter1</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Bewertung von </t>
+    <t xml:space="preserve">1. Bewertung von</t>
   </si>
   <si>
     <t xml:space="preserve">ret_id</t>
@@ -792,8 +791,7 @@
     <t xml:space="preserve">ret_meda_id</t>
   </si>
   <si>
-    <t xml:space="preserve">Zuordnung Meda -&gt; rMRP
-</t>
+    <t xml:space="preserve">Zuordnung Meda -&gt; rMRP</t>
   </si>
   <si>
     <t xml:space="preserve">ret_meda_dat1</t>
@@ -931,7 +929,7 @@
     <t xml:space="preserve">ret_bewerter2</t>
   </si>
   <si>
-    <t xml:space="preserve">2. Bewertung von </t>
+    <t xml:space="preserve">2. Bewertung von</t>
   </si>
   <si>
     <t xml:space="preserve">ret_gewissheit2</t>
@@ -1087,8 +1085,7 @@
     <t xml:space="preserve">rskfk_entern</t>
   </si>
   <si>
-    <t xml:space="preserve">ent. Ern.
-</t>
+    <t xml:space="preserve">ent. Ern.</t>
   </si>
   <si>
     <t xml:space="preserve">rskfkt_anz_rskamklassen</t>
@@ -1148,8 +1145,7 @@
     <t xml:space="preserve">trg_hyp_haem</t>
   </si>
   <si>
-    <t xml:space="preserve">Hb↓
-</t>
+    <t xml:space="preserve">Hb↓</t>
   </si>
   <si>
     <t xml:space="preserve">trg_hypo_glyk</t>

</xml_diff>

<commit_message>
Update Frontend Data Dictionary and generated Table Description
</commit_message>
<xml_diff>
--- a/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
+++ b/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="405">
   <si>
     <t xml:space="preserve">Hint</t>
   </si>
@@ -911,13 +911,7 @@
     <t xml:space="preserve">ret_2ndbewertung___1</t>
   </si>
   <si>
-    <t xml:space="preserve">1 - 2nd Look</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_2ndbewertung___Zweite MRP-Bewertung durchführen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zweite MRP-Bewertung durchführen</t>
+    <t xml:space="preserve">1 - 2nd Look / Zweite MRP-Bewertung durchführen</t>
   </si>
   <si>
     <t xml:space="preserve">ret_bewerter2_pipeline</t>
@@ -4112,7 +4106,7 @@
         <v>304</v>
       </c>
       <c r="C184" t="s">
-        <v>305</v>
+        <v>269</v>
       </c>
       <c r="D184" t="s">
         <v>12</v>
@@ -4123,10 +4117,10 @@
         <v>1</v>
       </c>
       <c r="B185" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C185" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="D185" t="s">
         <v>12</v>
@@ -4137,10 +4131,10 @@
         <v>1</v>
       </c>
       <c r="B186" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C186" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D186" t="s">
         <v>12</v>
@@ -4151,10 +4145,10 @@
         <v>1</v>
       </c>
       <c r="B187" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C187" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D187" t="s">
         <v>12</v>
@@ -4165,10 +4159,10 @@
         <v>1</v>
       </c>
       <c r="B188" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C188" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D188" t="s">
         <v>12</v>
@@ -4179,10 +4173,10 @@
         <v>1</v>
       </c>
       <c r="B189" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C189" t="s">
-        <v>277</v>
+        <v>209</v>
       </c>
       <c r="D189" t="s">
         <v>12</v>
@@ -4193,10 +4187,10 @@
         <v>1</v>
       </c>
       <c r="B190" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C190" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D190" t="s">
         <v>12</v>
@@ -4207,10 +4201,10 @@
         <v>1</v>
       </c>
       <c r="B191" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C191" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D191" t="s">
         <v>12</v>
@@ -4221,10 +4215,10 @@
         <v>1</v>
       </c>
       <c r="B192" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C192" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D192" t="s">
         <v>12</v>
@@ -4235,10 +4229,10 @@
         <v>1</v>
       </c>
       <c r="B193" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C193" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D193" t="s">
         <v>12</v>
@@ -4249,10 +4243,10 @@
         <v>1</v>
       </c>
       <c r="B194" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C194" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D194" t="s">
         <v>12</v>
@@ -4263,10 +4257,10 @@
         <v>1</v>
       </c>
       <c r="B195" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C195" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D195" t="s">
         <v>12</v>
@@ -4277,10 +4271,10 @@
         <v>1</v>
       </c>
       <c r="B196" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C196" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D196" t="s">
         <v>12</v>
@@ -4291,10 +4285,10 @@
         <v>1</v>
       </c>
       <c r="B197" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C197" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D197" t="s">
         <v>12</v>
@@ -4305,10 +4299,10 @@
         <v>1</v>
       </c>
       <c r="B198" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C198" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D198" t="s">
         <v>12</v>
@@ -4319,10 +4313,10 @@
         <v>1</v>
       </c>
       <c r="B199" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C199" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D199" t="s">
         <v>12</v>
@@ -4333,10 +4327,10 @@
         <v>1</v>
       </c>
       <c r="B200" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C200" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D200" t="s">
         <v>12</v>
@@ -4347,10 +4341,10 @@
         <v>1</v>
       </c>
       <c r="B201" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C201" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D201" t="s">
         <v>12</v>
@@ -4361,10 +4355,10 @@
         <v>1</v>
       </c>
       <c r="B202" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C202" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D202" t="s">
         <v>12</v>
@@ -4375,10 +4369,10 @@
         <v>1</v>
       </c>
       <c r="B203" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C203" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D203" t="s">
         <v>12</v>
@@ -4389,10 +4383,10 @@
         <v>1</v>
       </c>
       <c r="B204" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C204" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D204" t="s">
         <v>12</v>
@@ -4403,10 +4397,10 @@
         <v>1</v>
       </c>
       <c r="B205" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C205" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D205" t="s">
         <v>12</v>
@@ -4417,10 +4411,10 @@
         <v>1</v>
       </c>
       <c r="B206" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C206" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D206" t="s">
         <v>12</v>
@@ -4431,10 +4425,10 @@
         <v>1</v>
       </c>
       <c r="B207" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C207" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D207" t="s">
         <v>12</v>
@@ -4445,10 +4439,10 @@
         <v>1</v>
       </c>
       <c r="B208" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C208" t="s">
-        <v>245</v>
+        <v>36</v>
       </c>
       <c r="D208" t="s">
         <v>12</v>
@@ -4456,13 +4450,13 @@
     </row>
     <row r="209">
       <c r="A209" t="s">
-        <v>1</v>
+        <v>329</v>
       </c>
       <c r="B209" t="s">
-        <v>330</v>
+        <v>10</v>
       </c>
       <c r="C209" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="D209" t="s">
         <v>12</v>
@@ -4470,13 +4464,13 @@
     </row>
     <row r="210">
       <c r="A210" t="s">
-        <v>331</v>
+        <v>1</v>
       </c>
       <c r="B210" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C210" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D210" t="s">
         <v>12</v>
@@ -4487,10 +4481,10 @@
         <v>1</v>
       </c>
       <c r="B211" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C211" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D211" t="s">
         <v>12</v>
@@ -4501,10 +4495,10 @@
         <v>1</v>
       </c>
       <c r="B212" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C212" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D212" t="s">
         <v>12</v>
@@ -4515,13 +4509,13 @@
         <v>1</v>
       </c>
       <c r="B213" t="s">
-        <v>17</v>
+        <v>330</v>
       </c>
       <c r="C213" t="s">
-        <v>18</v>
+        <v>331</v>
       </c>
       <c r="D213" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="214">
@@ -4703,7 +4697,7 @@
         <v>357</v>
       </c>
       <c r="D226" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="227">
@@ -4714,21 +4708,21 @@
         <v>358</v>
       </c>
       <c r="C227" t="s">
-        <v>359</v>
+        <v>36</v>
       </c>
       <c r="D227" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="s">
-        <v>1</v>
+        <v>359</v>
       </c>
       <c r="B228" t="s">
-        <v>360</v>
+        <v>10</v>
       </c>
       <c r="C228" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="D228" t="s">
         <v>12</v>
@@ -4736,13 +4730,13 @@
     </row>
     <row r="229">
       <c r="A229" t="s">
-        <v>361</v>
+        <v>1</v>
       </c>
       <c r="B229" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C229" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D229" t="s">
         <v>12</v>
@@ -4753,10 +4747,10 @@
         <v>1</v>
       </c>
       <c r="B230" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C230" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D230" t="s">
         <v>12</v>
@@ -4767,10 +4761,10 @@
         <v>1</v>
       </c>
       <c r="B231" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C231" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D231" t="s">
         <v>12</v>
@@ -4781,13 +4775,13 @@
         <v>1</v>
       </c>
       <c r="B232" t="s">
-        <v>17</v>
+        <v>360</v>
       </c>
       <c r="C232" t="s">
-        <v>18</v>
+        <v>361</v>
       </c>
       <c r="D232" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="233">
@@ -5092,23 +5086,9 @@
         <v>404</v>
       </c>
       <c r="C254" t="s">
-        <v>405</v>
+        <v>36</v>
       </c>
       <c r="D254" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="255">
-      <c r="A255" t="s">
-        <v>1</v>
-      </c>
-      <c r="B255" t="s">
-        <v>406</v>
-      </c>
-      <c r="C255" t="s">
-        <v>36</v>
-      </c>
-      <c r="D255" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new Redcap Data Dictionary and generated Frontend_Table_Description
(cherry picked from commit 350cc8f30d52663c3d1b172cf31bad59170346bd)
</commit_message>
<xml_diff>
--- a/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
+++ b/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="416">
   <si>
     <t xml:space="preserve">Hint</t>
   </si>
@@ -449,7 +449,7 @@
     <t xml:space="preserve">mrp_dokup_fehler</t>
   </si>
   <si>
-    <t xml:space="preserve">Frage / Fehlerbeschreibung   </t>
+    <t xml:space="preserve">Frage / Fehlerbeschreibung </t>
   </si>
   <si>
     <t xml:space="preserve">mrp_dokup_intervention</t>
@@ -626,6 +626,9 @@
     <t xml:space="preserve">MRP-Klasse (INTERPOLAR)</t>
   </si>
   <si>
+    <t xml:space="preserve">mrp_ip_klasse_01</t>
+  </si>
+  <si>
     <t xml:space="preserve">mrp_ip_klasse_disease</t>
   </si>
   <si>
@@ -638,6 +641,12 @@
     <t xml:space="preserve">Labor</t>
   </si>
   <si>
+    <t xml:space="preserve">mrp_ip_klasse_nieren_insuf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grad der Nierenfunktionseinschränkung</t>
+  </si>
+  <si>
     <t xml:space="preserve">mrp_massn_am___1</t>
   </si>
   <si>
@@ -806,6 +815,9 @@
     <t xml:space="preserve">ret_ip_klasse</t>
   </si>
   <si>
+    <t xml:space="preserve">ret_ip_klasse_01</t>
+  </si>
+  <si>
     <t xml:space="preserve">ret_atc1</t>
   </si>
   <si>
@@ -818,6 +830,9 @@
     <t xml:space="preserve">ret_ip_klasse_labor</t>
   </si>
   <si>
+    <t xml:space="preserve">ret_ip_klasse_nieren_insuf</t>
+  </si>
+  <si>
     <t xml:space="preserve">ret_gewissheit1</t>
   </si>
   <si>
@@ -830,13 +845,13 @@
     <t xml:space="preserve">Zuordnung zu manuellem MRP</t>
   </si>
   <si>
-    <t xml:space="preserve">ret_gewissheit_oth1</t>
+    <t xml:space="preserve">ret_gewissheit1_oth</t>
   </si>
   <si>
     <t xml:space="preserve">Weitere Informationen</t>
   </si>
   <si>
-    <t xml:space="preserve">ret_gewiss_grund_abl1</t>
+    <t xml:space="preserve">ret_gewiss_grund1_abl</t>
   </si>
   <si>
     <t xml:space="preserve">Grund für nicht Bestätigung</t>
@@ -848,6 +863,18 @@
     <t xml:space="preserve">Bitte näher beschreiben</t>
   </si>
   <si>
+    <t xml:space="preserve">ret_gewiss_grund_abl_klin1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WARUM ist das MRP nicht klinisch relevant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_grund_abl_klin1_neg___1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Dieses MRP halte ich FÜR KEINEN Patienten auf dieser Station für KLINISCH RELEVANT</t>
+  </si>
+  <si>
     <t xml:space="preserve">ret_massn_am1___1</t>
   </si>
   <si>
@@ -939,6 +966,12 @@
   </si>
   <si>
     <t xml:space="preserve">ret_gewiss_grund_abl_sonst2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_grund_abl_klin2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_grund_abl_klin_neg___1</t>
   </si>
   <si>
     <t xml:space="preserve">ret_massn_am2___1</t>
@@ -3168,7 +3201,7 @@
         <v>204</v>
       </c>
       <c r="C117" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D117" t="s">
         <v>12</v>
@@ -3179,10 +3212,10 @@
         <v>1</v>
       </c>
       <c r="B118" t="s">
+        <v>205</v>
+      </c>
+      <c r="C118" t="s">
         <v>206</v>
-      </c>
-      <c r="C118" t="s">
-        <v>207</v>
       </c>
       <c r="D118" t="s">
         <v>12</v>
@@ -3193,10 +3226,10 @@
         <v>1</v>
       </c>
       <c r="B119" t="s">
+        <v>207</v>
+      </c>
+      <c r="C119" t="s">
         <v>208</v>
-      </c>
-      <c r="C119" t="s">
-        <v>209</v>
       </c>
       <c r="D119" t="s">
         <v>12</v>
@@ -3207,10 +3240,10 @@
         <v>1</v>
       </c>
       <c r="B120" t="s">
+        <v>209</v>
+      </c>
+      <c r="C120" t="s">
         <v>210</v>
-      </c>
-      <c r="C120" t="s">
-        <v>211</v>
       </c>
       <c r="D120" t="s">
         <v>12</v>
@@ -3221,10 +3254,10 @@
         <v>1</v>
       </c>
       <c r="B121" t="s">
+        <v>211</v>
+      </c>
+      <c r="C121" t="s">
         <v>212</v>
-      </c>
-      <c r="C121" t="s">
-        <v>213</v>
       </c>
       <c r="D121" t="s">
         <v>12</v>
@@ -3235,10 +3268,10 @@
         <v>1</v>
       </c>
       <c r="B122" t="s">
+        <v>213</v>
+      </c>
+      <c r="C122" t="s">
         <v>214</v>
-      </c>
-      <c r="C122" t="s">
-        <v>215</v>
       </c>
       <c r="D122" t="s">
         <v>12</v>
@@ -3249,10 +3282,10 @@
         <v>1</v>
       </c>
       <c r="B123" t="s">
+        <v>215</v>
+      </c>
+      <c r="C123" t="s">
         <v>216</v>
-      </c>
-      <c r="C123" t="s">
-        <v>217</v>
       </c>
       <c r="D123" t="s">
         <v>12</v>
@@ -3263,10 +3296,10 @@
         <v>1</v>
       </c>
       <c r="B124" t="s">
+        <v>217</v>
+      </c>
+      <c r="C124" t="s">
         <v>218</v>
-      </c>
-      <c r="C124" t="s">
-        <v>219</v>
       </c>
       <c r="D124" t="s">
         <v>12</v>
@@ -3277,10 +3310,10 @@
         <v>1</v>
       </c>
       <c r="B125" t="s">
+        <v>219</v>
+      </c>
+      <c r="C125" t="s">
         <v>220</v>
-      </c>
-      <c r="C125" t="s">
-        <v>221</v>
       </c>
       <c r="D125" t="s">
         <v>12</v>
@@ -3291,10 +3324,10 @@
         <v>1</v>
       </c>
       <c r="B126" t="s">
+        <v>221</v>
+      </c>
+      <c r="C126" t="s">
         <v>222</v>
-      </c>
-      <c r="C126" t="s">
-        <v>223</v>
       </c>
       <c r="D126" t="s">
         <v>12</v>
@@ -3305,10 +3338,10 @@
         <v>1</v>
       </c>
       <c r="B127" t="s">
+        <v>223</v>
+      </c>
+      <c r="C127" t="s">
         <v>224</v>
-      </c>
-      <c r="C127" t="s">
-        <v>225</v>
       </c>
       <c r="D127" t="s">
         <v>12</v>
@@ -3319,10 +3352,10 @@
         <v>1</v>
       </c>
       <c r="B128" t="s">
+        <v>225</v>
+      </c>
+      <c r="C128" t="s">
         <v>226</v>
-      </c>
-      <c r="C128" t="s">
-        <v>227</v>
       </c>
       <c r="D128" t="s">
         <v>12</v>
@@ -3333,10 +3366,10 @@
         <v>1</v>
       </c>
       <c r="B129" t="s">
+        <v>227</v>
+      </c>
+      <c r="C129" t="s">
         <v>228</v>
-      </c>
-      <c r="C129" t="s">
-        <v>229</v>
       </c>
       <c r="D129" t="s">
         <v>12</v>
@@ -3347,10 +3380,10 @@
         <v>1</v>
       </c>
       <c r="B130" t="s">
+        <v>229</v>
+      </c>
+      <c r="C130" t="s">
         <v>230</v>
-      </c>
-      <c r="C130" t="s">
-        <v>231</v>
       </c>
       <c r="D130" t="s">
         <v>12</v>
@@ -3361,10 +3394,10 @@
         <v>1</v>
       </c>
       <c r="B131" t="s">
+        <v>231</v>
+      </c>
+      <c r="C131" t="s">
         <v>232</v>
-      </c>
-      <c r="C131" t="s">
-        <v>233</v>
       </c>
       <c r="D131" t="s">
         <v>12</v>
@@ -3375,10 +3408,10 @@
         <v>1</v>
       </c>
       <c r="B132" t="s">
+        <v>233</v>
+      </c>
+      <c r="C132" t="s">
         <v>234</v>
-      </c>
-      <c r="C132" t="s">
-        <v>235</v>
       </c>
       <c r="D132" t="s">
         <v>12</v>
@@ -3389,10 +3422,10 @@
         <v>1</v>
       </c>
       <c r="B133" t="s">
+        <v>235</v>
+      </c>
+      <c r="C133" t="s">
         <v>236</v>
-      </c>
-      <c r="C133" t="s">
-        <v>237</v>
       </c>
       <c r="D133" t="s">
         <v>12</v>
@@ -3403,10 +3436,10 @@
         <v>1</v>
       </c>
       <c r="B134" t="s">
+        <v>237</v>
+      </c>
+      <c r="C134" t="s">
         <v>238</v>
-      </c>
-      <c r="C134" t="s">
-        <v>239</v>
       </c>
       <c r="D134" t="s">
         <v>12</v>
@@ -3417,10 +3450,10 @@
         <v>1</v>
       </c>
       <c r="B135" t="s">
+        <v>239</v>
+      </c>
+      <c r="C135" t="s">
         <v>240</v>
-      </c>
-      <c r="C135" t="s">
-        <v>241</v>
       </c>
       <c r="D135" t="s">
         <v>12</v>
@@ -3431,10 +3464,10 @@
         <v>1</v>
       </c>
       <c r="B136" t="s">
+        <v>241</v>
+      </c>
+      <c r="C136" t="s">
         <v>242</v>
-      </c>
-      <c r="C136" t="s">
-        <v>243</v>
       </c>
       <c r="D136" t="s">
         <v>12</v>
@@ -3445,10 +3478,10 @@
         <v>1</v>
       </c>
       <c r="B137" t="s">
+        <v>243</v>
+      </c>
+      <c r="C137" t="s">
         <v>244</v>
-      </c>
-      <c r="C137" t="s">
-        <v>245</v>
       </c>
       <c r="D137" t="s">
         <v>12</v>
@@ -3459,10 +3492,10 @@
         <v>1</v>
       </c>
       <c r="B138" t="s">
+        <v>245</v>
+      </c>
+      <c r="C138" t="s">
         <v>246</v>
-      </c>
-      <c r="C138" t="s">
-        <v>247</v>
       </c>
       <c r="D138" t="s">
         <v>12</v>
@@ -3473,10 +3506,10 @@
         <v>1</v>
       </c>
       <c r="B139" t="s">
+        <v>247</v>
+      </c>
+      <c r="C139" t="s">
         <v>248</v>
-      </c>
-      <c r="C139" t="s">
-        <v>249</v>
       </c>
       <c r="D139" t="s">
         <v>12</v>
@@ -3487,10 +3520,10 @@
         <v>1</v>
       </c>
       <c r="B140" t="s">
+        <v>249</v>
+      </c>
+      <c r="C140" t="s">
         <v>250</v>
-      </c>
-      <c r="C140" t="s">
-        <v>251</v>
       </c>
       <c r="D140" t="s">
         <v>12</v>
@@ -3501,10 +3534,10 @@
         <v>1</v>
       </c>
       <c r="B141" t="s">
+        <v>251</v>
+      </c>
+      <c r="C141" t="s">
         <v>252</v>
-      </c>
-      <c r="C141" t="s">
-        <v>36</v>
       </c>
       <c r="D141" t="s">
         <v>12</v>
@@ -3512,13 +3545,13 @@
     </row>
     <row r="142">
       <c r="A142" t="s">
+        <v>1</v>
+      </c>
+      <c r="B142" t="s">
         <v>253</v>
       </c>
-      <c r="B142" t="s">
-        <v>10</v>
-      </c>
       <c r="C142" t="s">
-        <v>11</v>
+        <v>254</v>
       </c>
       <c r="D142" t="s">
         <v>12</v>
@@ -3529,10 +3562,10 @@
         <v>1</v>
       </c>
       <c r="B143" t="s">
-        <v>13</v>
+        <v>255</v>
       </c>
       <c r="C143" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="D143" t="s">
         <v>12</v>
@@ -3540,13 +3573,13 @@
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>1</v>
+        <v>256</v>
       </c>
       <c r="B144" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C144" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D144" t="s">
         <v>12</v>
@@ -3557,10 +3590,10 @@
         <v>1</v>
       </c>
       <c r="B145" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C145" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D145" t="s">
         <v>12</v>
@@ -3571,10 +3604,10 @@
         <v>1</v>
       </c>
       <c r="B146" t="s">
-        <v>254</v>
+        <v>15</v>
       </c>
       <c r="C146" t="s">
-        <v>255</v>
+        <v>16</v>
       </c>
       <c r="D146" t="s">
         <v>12</v>
@@ -3585,10 +3618,10 @@
         <v>1</v>
       </c>
       <c r="B147" t="s">
-        <v>256</v>
+        <v>17</v>
       </c>
       <c r="C147" t="s">
-        <v>257</v>
+        <v>18</v>
       </c>
       <c r="D147" t="s">
         <v>12</v>
@@ -3599,10 +3632,10 @@
         <v>1</v>
       </c>
       <c r="B148" t="s">
+        <v>257</v>
+      </c>
+      <c r="C148" t="s">
         <v>258</v>
-      </c>
-      <c r="C148" t="s">
-        <v>259</v>
       </c>
       <c r="D148" t="s">
         <v>12</v>
@@ -3613,13 +3646,13 @@
         <v>1</v>
       </c>
       <c r="B149" t="s">
+        <v>259</v>
+      </c>
+      <c r="C149" t="s">
         <v>260</v>
       </c>
-      <c r="C149" t="s">
-        <v>261</v>
-      </c>
       <c r="D149" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
     </row>
     <row r="150">
@@ -3627,10 +3660,10 @@
         <v>1</v>
       </c>
       <c r="B150" t="s">
+        <v>261</v>
+      </c>
+      <c r="C150" t="s">
         <v>262</v>
-      </c>
-      <c r="C150" t="s">
-        <v>123</v>
       </c>
       <c r="D150" t="s">
         <v>12</v>
@@ -3644,10 +3677,10 @@
         <v>263</v>
       </c>
       <c r="C151" t="s">
-        <v>203</v>
+        <v>264</v>
       </c>
       <c r="D151" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
     </row>
     <row r="152">
@@ -3655,10 +3688,10 @@
         <v>1</v>
       </c>
       <c r="B152" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C152" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D152" t="s">
         <v>12</v>
@@ -3669,10 +3702,10 @@
         <v>1</v>
       </c>
       <c r="B153" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C153" t="s">
-        <v>133</v>
+        <v>203</v>
       </c>
       <c r="D153" t="s">
         <v>12</v>
@@ -3683,10 +3716,10 @@
         <v>1</v>
       </c>
       <c r="B154" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C154" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D154" t="s">
         <v>12</v>
@@ -3697,10 +3730,10 @@
         <v>1</v>
       </c>
       <c r="B155" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C155" t="s">
-        <v>207</v>
+        <v>131</v>
       </c>
       <c r="D155" t="s">
         <v>12</v>
@@ -3711,10 +3744,10 @@
         <v>1</v>
       </c>
       <c r="B156" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C156" t="s">
-        <v>269</v>
+        <v>133</v>
       </c>
       <c r="D156" t="s">
         <v>12</v>
@@ -3728,7 +3761,7 @@
         <v>270</v>
       </c>
       <c r="C157" t="s">
-        <v>271</v>
+        <v>206</v>
       </c>
       <c r="D157" t="s">
         <v>12</v>
@@ -3739,10 +3772,10 @@
         <v>1</v>
       </c>
       <c r="B158" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C158" t="s">
-        <v>273</v>
+        <v>208</v>
       </c>
       <c r="D158" t="s">
         <v>12</v>
@@ -3753,10 +3786,10 @@
         <v>1</v>
       </c>
       <c r="B159" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C159" t="s">
-        <v>275</v>
+        <v>210</v>
       </c>
       <c r="D159" t="s">
         <v>12</v>
@@ -3767,10 +3800,10 @@
         <v>1</v>
       </c>
       <c r="B160" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C160" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D160" t="s">
         <v>12</v>
@@ -3781,10 +3814,10 @@
         <v>1</v>
       </c>
       <c r="B161" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C161" t="s">
-        <v>209</v>
+        <v>276</v>
       </c>
       <c r="D161" t="s">
         <v>12</v>
@@ -3795,10 +3828,10 @@
         <v>1</v>
       </c>
       <c r="B162" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C162" t="s">
-        <v>211</v>
+        <v>278</v>
       </c>
       <c r="D162" t="s">
         <v>12</v>
@@ -3809,10 +3842,10 @@
         <v>1</v>
       </c>
       <c r="B163" t="s">
+        <v>279</v>
+      </c>
+      <c r="C163" t="s">
         <v>280</v>
-      </c>
-      <c r="C163" t="s">
-        <v>213</v>
       </c>
       <c r="D163" t="s">
         <v>12</v>
@@ -3826,7 +3859,7 @@
         <v>281</v>
       </c>
       <c r="C164" t="s">
-        <v>215</v>
+        <v>282</v>
       </c>
       <c r="D164" t="s">
         <v>12</v>
@@ -3837,10 +3870,10 @@
         <v>1</v>
       </c>
       <c r="B165" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C165" t="s">
-        <v>217</v>
+        <v>284</v>
       </c>
       <c r="D165" t="s">
         <v>12</v>
@@ -3851,10 +3884,10 @@
         <v>1</v>
       </c>
       <c r="B166" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C166" t="s">
-        <v>219</v>
+        <v>286</v>
       </c>
       <c r="D166" t="s">
         <v>12</v>
@@ -3865,10 +3898,10 @@
         <v>1</v>
       </c>
       <c r="B167" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C167" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="D167" t="s">
         <v>12</v>
@@ -3879,10 +3912,10 @@
         <v>1</v>
       </c>
       <c r="B168" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C168" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D168" t="s">
         <v>12</v>
@@ -3893,10 +3926,10 @@
         <v>1</v>
       </c>
       <c r="B169" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C169" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D169" t="s">
         <v>12</v>
@@ -3907,10 +3940,10 @@
         <v>1</v>
       </c>
       <c r="B170" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C170" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="D170" t="s">
         <v>12</v>
@@ -3921,10 +3954,10 @@
         <v>1</v>
       </c>
       <c r="B171" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C171" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="D171" t="s">
         <v>12</v>
@@ -3935,10 +3968,10 @@
         <v>1</v>
       </c>
       <c r="B172" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C172" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="D172" t="s">
         <v>12</v>
@@ -3949,10 +3982,10 @@
         <v>1</v>
       </c>
       <c r="B173" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="C173" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="D173" t="s">
         <v>12</v>
@@ -3963,10 +3996,10 @@
         <v>1</v>
       </c>
       <c r="B174" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="C174" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D174" t="s">
         <v>12</v>
@@ -3977,10 +4010,10 @@
         <v>1</v>
       </c>
       <c r="B175" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="C175" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="D175" t="s">
         <v>12</v>
@@ -3991,10 +4024,10 @@
         <v>1</v>
       </c>
       <c r="B176" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="C176" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="D176" t="s">
         <v>12</v>
@@ -4005,10 +4038,10 @@
         <v>1</v>
       </c>
       <c r="B177" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C177" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="D177" t="s">
         <v>12</v>
@@ -4019,10 +4052,10 @@
         <v>1</v>
       </c>
       <c r="B178" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C178" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="D178" t="s">
         <v>12</v>
@@ -4033,10 +4066,10 @@
         <v>1</v>
       </c>
       <c r="B179" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="C179" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="D179" t="s">
         <v>12</v>
@@ -4047,13 +4080,13 @@
         <v>1</v>
       </c>
       <c r="B180" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C180" t="s">
-        <v>261</v>
+        <v>238</v>
       </c>
       <c r="D180" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
     </row>
     <row r="181">
@@ -4061,10 +4094,10 @@
         <v>1</v>
       </c>
       <c r="B181" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="C181" t="s">
-        <v>299</v>
+        <v>240</v>
       </c>
       <c r="D181" t="s">
         <v>12</v>
@@ -4075,10 +4108,10 @@
         <v>1</v>
       </c>
       <c r="B182" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C182" t="s">
-        <v>301</v>
+        <v>242</v>
       </c>
       <c r="D182" t="s">
         <v>12</v>
@@ -4089,10 +4122,10 @@
         <v>1</v>
       </c>
       <c r="B183" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C183" t="s">
-        <v>303</v>
+        <v>244</v>
       </c>
       <c r="D183" t="s">
         <v>12</v>
@@ -4106,7 +4139,7 @@
         <v>304</v>
       </c>
       <c r="C184" t="s">
-        <v>269</v>
+        <v>246</v>
       </c>
       <c r="D184" t="s">
         <v>12</v>
@@ -4120,7 +4153,7 @@
         <v>305</v>
       </c>
       <c r="C185" t="s">
-        <v>271</v>
+        <v>248</v>
       </c>
       <c r="D185" t="s">
         <v>12</v>
@@ -4134,10 +4167,10 @@
         <v>306</v>
       </c>
       <c r="C186" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="D186" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
     </row>
     <row r="187">
@@ -4148,7 +4181,7 @@
         <v>307</v>
       </c>
       <c r="C187" t="s">
-        <v>275</v>
+        <v>308</v>
       </c>
       <c r="D187" t="s">
         <v>12</v>
@@ -4159,10 +4192,10 @@
         <v>1</v>
       </c>
       <c r="B188" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C188" t="s">
-        <v>277</v>
+        <v>310</v>
       </c>
       <c r="D188" t="s">
         <v>12</v>
@@ -4173,10 +4206,10 @@
         <v>1</v>
       </c>
       <c r="B189" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="C189" t="s">
-        <v>209</v>
+        <v>312</v>
       </c>
       <c r="D189" t="s">
         <v>12</v>
@@ -4187,10 +4220,10 @@
         <v>1</v>
       </c>
       <c r="B190" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="C190" t="s">
-        <v>211</v>
+        <v>274</v>
       </c>
       <c r="D190" t="s">
         <v>12</v>
@@ -4201,10 +4234,10 @@
         <v>1</v>
       </c>
       <c r="B191" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C191" t="s">
-        <v>213</v>
+        <v>276</v>
       </c>
       <c r="D191" t="s">
         <v>12</v>
@@ -4215,10 +4248,10 @@
         <v>1</v>
       </c>
       <c r="B192" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C192" t="s">
-        <v>215</v>
+        <v>278</v>
       </c>
       <c r="D192" t="s">
         <v>12</v>
@@ -4229,10 +4262,10 @@
         <v>1</v>
       </c>
       <c r="B193" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C193" t="s">
-        <v>217</v>
+        <v>280</v>
       </c>
       <c r="D193" t="s">
         <v>12</v>
@@ -4243,10 +4276,10 @@
         <v>1</v>
       </c>
       <c r="B194" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="C194" t="s">
-        <v>219</v>
+        <v>282</v>
       </c>
       <c r="D194" t="s">
         <v>12</v>
@@ -4257,10 +4290,10 @@
         <v>1</v>
       </c>
       <c r="B195" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="C195" t="s">
-        <v>221</v>
+        <v>284</v>
       </c>
       <c r="D195" t="s">
         <v>12</v>
@@ -4271,10 +4304,10 @@
         <v>1</v>
       </c>
       <c r="B196" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C196" t="s">
-        <v>223</v>
+        <v>286</v>
       </c>
       <c r="D196" t="s">
         <v>12</v>
@@ -4285,10 +4318,10 @@
         <v>1</v>
       </c>
       <c r="B197" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="C197" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="D197" t="s">
         <v>12</v>
@@ -4299,10 +4332,10 @@
         <v>1</v>
       </c>
       <c r="B198" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C198" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="D198" t="s">
         <v>12</v>
@@ -4313,10 +4346,10 @@
         <v>1</v>
       </c>
       <c r="B199" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="C199" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="D199" t="s">
         <v>12</v>
@@ -4327,10 +4360,10 @@
         <v>1</v>
       </c>
       <c r="B200" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C200" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="D200" t="s">
         <v>12</v>
@@ -4341,10 +4374,10 @@
         <v>1</v>
       </c>
       <c r="B201" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="C201" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="D201" t="s">
         <v>12</v>
@@ -4355,10 +4388,10 @@
         <v>1</v>
       </c>
       <c r="B202" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="C202" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="D202" t="s">
         <v>12</v>
@@ -4369,10 +4402,10 @@
         <v>1</v>
       </c>
       <c r="B203" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="C203" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="D203" t="s">
         <v>12</v>
@@ -4383,10 +4416,10 @@
         <v>1</v>
       </c>
       <c r="B204" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="C204" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="D204" t="s">
         <v>12</v>
@@ -4397,10 +4430,10 @@
         <v>1</v>
       </c>
       <c r="B205" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="C205" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="D205" t="s">
         <v>12</v>
@@ -4411,10 +4444,10 @@
         <v>1</v>
       </c>
       <c r="B206" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="C206" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="D206" t="s">
         <v>12</v>
@@ -4425,10 +4458,10 @@
         <v>1</v>
       </c>
       <c r="B207" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="C207" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="D207" t="s">
         <v>12</v>
@@ -4439,10 +4472,10 @@
         <v>1</v>
       </c>
       <c r="B208" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="C208" t="s">
-        <v>36</v>
+        <v>234</v>
       </c>
       <c r="D208" t="s">
         <v>12</v>
@@ -4450,13 +4483,13 @@
     </row>
     <row r="209">
       <c r="A209" t="s">
-        <v>329</v>
+        <v>1</v>
       </c>
       <c r="B209" t="s">
-        <v>10</v>
+        <v>332</v>
       </c>
       <c r="C209" t="s">
-        <v>11</v>
+        <v>236</v>
       </c>
       <c r="D209" t="s">
         <v>12</v>
@@ -4467,10 +4500,10 @@
         <v>1</v>
       </c>
       <c r="B210" t="s">
-        <v>13</v>
+        <v>333</v>
       </c>
       <c r="C210" t="s">
-        <v>14</v>
+        <v>238</v>
       </c>
       <c r="D210" t="s">
         <v>12</v>
@@ -4481,10 +4514,10 @@
         <v>1</v>
       </c>
       <c r="B211" t="s">
-        <v>15</v>
+        <v>334</v>
       </c>
       <c r="C211" t="s">
-        <v>16</v>
+        <v>240</v>
       </c>
       <c r="D211" t="s">
         <v>12</v>
@@ -4495,10 +4528,10 @@
         <v>1</v>
       </c>
       <c r="B212" t="s">
-        <v>17</v>
+        <v>335</v>
       </c>
       <c r="C212" t="s">
-        <v>18</v>
+        <v>242</v>
       </c>
       <c r="D212" t="s">
         <v>12</v>
@@ -4509,13 +4542,13 @@
         <v>1</v>
       </c>
       <c r="B213" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="C213" t="s">
-        <v>331</v>
+        <v>244</v>
       </c>
       <c r="D213" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="214">
@@ -4523,13 +4556,13 @@
         <v>1</v>
       </c>
       <c r="B214" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="C214" t="s">
-        <v>333</v>
+        <v>246</v>
       </c>
       <c r="D214" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="215">
@@ -4537,13 +4570,13 @@
         <v>1</v>
       </c>
       <c r="B215" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="C215" t="s">
-        <v>335</v>
+        <v>248</v>
       </c>
       <c r="D215" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="216">
@@ -4551,27 +4584,27 @@
         <v>1</v>
       </c>
       <c r="B216" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="C216" t="s">
-        <v>337</v>
+        <v>36</v>
       </c>
       <c r="D216" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="s">
-        <v>1</v>
+        <v>340</v>
       </c>
       <c r="B217" t="s">
-        <v>338</v>
+        <v>10</v>
       </c>
       <c r="C217" t="s">
-        <v>339</v>
+        <v>11</v>
       </c>
       <c r="D217" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="218">
@@ -4579,13 +4612,13 @@
         <v>1</v>
       </c>
       <c r="B218" t="s">
-        <v>340</v>
+        <v>13</v>
       </c>
       <c r="C218" t="s">
-        <v>341</v>
+        <v>14</v>
       </c>
       <c r="D218" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="219">
@@ -4593,13 +4626,13 @@
         <v>1</v>
       </c>
       <c r="B219" t="s">
-        <v>342</v>
+        <v>15</v>
       </c>
       <c r="C219" t="s">
-        <v>343</v>
+        <v>16</v>
       </c>
       <c r="D219" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="220">
@@ -4607,13 +4640,13 @@
         <v>1</v>
       </c>
       <c r="B220" t="s">
-        <v>344</v>
+        <v>17</v>
       </c>
       <c r="C220" t="s">
-        <v>345</v>
+        <v>18</v>
       </c>
       <c r="D220" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="221">
@@ -4621,10 +4654,10 @@
         <v>1</v>
       </c>
       <c r="B221" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="C221" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="D221" t="s">
         <v>40</v>
@@ -4635,10 +4668,10 @@
         <v>1</v>
       </c>
       <c r="B222" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="C222" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="D222" t="s">
         <v>40</v>
@@ -4649,10 +4682,10 @@
         <v>1</v>
       </c>
       <c r="B223" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="C223" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="D223" t="s">
         <v>40</v>
@@ -4663,10 +4696,10 @@
         <v>1</v>
       </c>
       <c r="B224" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="C224" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="D224" t="s">
         <v>40</v>
@@ -4677,10 +4710,10 @@
         <v>1</v>
       </c>
       <c r="B225" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="C225" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="D225" t="s">
         <v>40</v>
@@ -4691,13 +4724,13 @@
         <v>1</v>
       </c>
       <c r="B226" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="C226" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="D226" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="227">
@@ -4705,27 +4738,27 @@
         <v>1</v>
       </c>
       <c r="B227" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="C227" t="s">
-        <v>36</v>
+        <v>354</v>
       </c>
       <c r="D227" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="s">
-        <v>359</v>
+        <v>1</v>
       </c>
       <c r="B228" t="s">
-        <v>10</v>
+        <v>355</v>
       </c>
       <c r="C228" t="s">
-        <v>11</v>
+        <v>356</v>
       </c>
       <c r="D228" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="229">
@@ -4733,13 +4766,13 @@
         <v>1</v>
       </c>
       <c r="B229" t="s">
-        <v>13</v>
+        <v>357</v>
       </c>
       <c r="C229" t="s">
-        <v>14</v>
+        <v>358</v>
       </c>
       <c r="D229" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="230">
@@ -4747,13 +4780,13 @@
         <v>1</v>
       </c>
       <c r="B230" t="s">
-        <v>15</v>
+        <v>359</v>
       </c>
       <c r="C230" t="s">
-        <v>16</v>
+        <v>360</v>
       </c>
       <c r="D230" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="231">
@@ -4761,13 +4794,13 @@
         <v>1</v>
       </c>
       <c r="B231" t="s">
-        <v>17</v>
+        <v>361</v>
       </c>
       <c r="C231" t="s">
-        <v>18</v>
+        <v>362</v>
       </c>
       <c r="D231" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="232">
@@ -4775,10 +4808,10 @@
         <v>1</v>
       </c>
       <c r="B232" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="C232" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="D232" t="s">
         <v>40</v>
@@ -4789,10 +4822,10 @@
         <v>1</v>
       </c>
       <c r="B233" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="C233" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="D233" t="s">
         <v>40</v>
@@ -4803,13 +4836,13 @@
         <v>1</v>
       </c>
       <c r="B234" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C234" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D234" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="235">
@@ -4817,27 +4850,27 @@
         <v>1</v>
       </c>
       <c r="B235" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="C235" t="s">
-        <v>367</v>
+        <v>36</v>
       </c>
       <c r="D235" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="s">
-        <v>1</v>
+        <v>370</v>
       </c>
       <c r="B236" t="s">
-        <v>368</v>
+        <v>10</v>
       </c>
       <c r="C236" t="s">
-        <v>369</v>
+        <v>11</v>
       </c>
       <c r="D236" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="237">
@@ -4845,13 +4878,13 @@
         <v>1</v>
       </c>
       <c r="B237" t="s">
-        <v>370</v>
+        <v>13</v>
       </c>
       <c r="C237" t="s">
-        <v>371</v>
+        <v>14</v>
       </c>
       <c r="D237" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="238">
@@ -4859,13 +4892,13 @@
         <v>1</v>
       </c>
       <c r="B238" t="s">
-        <v>372</v>
+        <v>15</v>
       </c>
       <c r="C238" t="s">
-        <v>373</v>
+        <v>16</v>
       </c>
       <c r="D238" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="239">
@@ -4873,13 +4906,13 @@
         <v>1</v>
       </c>
       <c r="B239" t="s">
-        <v>374</v>
+        <v>17</v>
       </c>
       <c r="C239" t="s">
-        <v>375</v>
+        <v>18</v>
       </c>
       <c r="D239" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="240">
@@ -4887,10 +4920,10 @@
         <v>1</v>
       </c>
       <c r="B240" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C240" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="D240" t="s">
         <v>40</v>
@@ -4901,10 +4934,10 @@
         <v>1</v>
       </c>
       <c r="B241" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="C241" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="D241" t="s">
         <v>40</v>
@@ -4915,10 +4948,10 @@
         <v>1</v>
       </c>
       <c r="B242" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="C242" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="D242" t="s">
         <v>40</v>
@@ -4929,10 +4962,10 @@
         <v>1</v>
       </c>
       <c r="B243" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="C243" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D243" t="s">
         <v>40</v>
@@ -4943,10 +4976,10 @@
         <v>1</v>
       </c>
       <c r="B244" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="C244" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="D244" t="s">
         <v>40</v>
@@ -4957,10 +4990,10 @@
         <v>1</v>
       </c>
       <c r="B245" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="C245" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="D245" t="s">
         <v>40</v>
@@ -4971,10 +5004,10 @@
         <v>1</v>
       </c>
       <c r="B246" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="C246" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="D246" t="s">
         <v>40</v>
@@ -4985,10 +5018,10 @@
         <v>1</v>
       </c>
       <c r="B247" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="C247" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="D247" t="s">
         <v>40</v>
@@ -4999,10 +5032,10 @@
         <v>1</v>
       </c>
       <c r="B248" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C248" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="D248" t="s">
         <v>40</v>
@@ -5013,10 +5046,10 @@
         <v>1</v>
       </c>
       <c r="B249" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="C249" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="D249" t="s">
         <v>40</v>
@@ -5027,10 +5060,10 @@
         <v>1</v>
       </c>
       <c r="B250" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="C250" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="D250" t="s">
         <v>40</v>
@@ -5041,10 +5074,10 @@
         <v>1</v>
       </c>
       <c r="B251" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="C251" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="D251" t="s">
         <v>40</v>
@@ -5055,10 +5088,10 @@
         <v>1</v>
       </c>
       <c r="B252" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="C252" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="D252" t="s">
         <v>40</v>
@@ -5069,10 +5102,10 @@
         <v>1</v>
       </c>
       <c r="B253" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="C253" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="D253" t="s">
         <v>40</v>
@@ -5083,12 +5116,124 @@
         <v>1</v>
       </c>
       <c r="B254" t="s">
+        <v>399</v>
+      </c>
+      <c r="C254" t="s">
+        <v>400</v>
+      </c>
+      <c r="D254" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="s">
+        <v>1</v>
+      </c>
+      <c r="B255" t="s">
+        <v>401</v>
+      </c>
+      <c r="C255" t="s">
+        <v>402</v>
+      </c>
+      <c r="D255" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="s">
+        <v>1</v>
+      </c>
+      <c r="B256" t="s">
+        <v>403</v>
+      </c>
+      <c r="C256" t="s">
         <v>404</v>
       </c>
-      <c r="C254" t="s">
+      <c r="D256" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="s">
+        <v>1</v>
+      </c>
+      <c r="B257" t="s">
+        <v>405</v>
+      </c>
+      <c r="C257" t="s">
+        <v>406</v>
+      </c>
+      <c r="D257" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="s">
+        <v>1</v>
+      </c>
+      <c r="B258" t="s">
+        <v>407</v>
+      </c>
+      <c r="C258" t="s">
+        <v>408</v>
+      </c>
+      <c r="D258" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="s">
+        <v>1</v>
+      </c>
+      <c r="B259" t="s">
+        <v>409</v>
+      </c>
+      <c r="C259" t="s">
+        <v>410</v>
+      </c>
+      <c r="D259" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="s">
+        <v>1</v>
+      </c>
+      <c r="B260" t="s">
+        <v>411</v>
+      </c>
+      <c r="C260" t="s">
+        <v>412</v>
+      </c>
+      <c r="D260" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="s">
+        <v>1</v>
+      </c>
+      <c r="B261" t="s">
+        <v>413</v>
+      </c>
+      <c r="C261" t="s">
+        <v>414</v>
+      </c>
+      <c r="D261" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="s">
+        <v>1</v>
+      </c>
+      <c r="B262" t="s">
+        <v>415</v>
+      </c>
+      <c r="C262" t="s">
         <v>36</v>
       </c>
-      <c r="D254" t="s">
+      <c r="D262" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Frontend_Table_Description and dictionary
</commit_message>
<xml_diff>
--- a/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
+++ b/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="424">
   <si>
     <t xml:space="preserve">Hint</t>
   </si>
@@ -119,6 +119,12 @@
     <t xml:space="preserve">Geschlecht</t>
   </si>
   <si>
+    <t xml:space="preserve">pat_additional_values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reserviertes Feld für zusätzliche Werte</t>
+  </si>
+  <si>
     <t xml:space="preserve">patient_complete</t>
   </si>
   <si>
@@ -128,6 +134,12 @@
     <t xml:space="preserve">fall</t>
   </si>
   <si>
+    <t xml:space="preserve">fall_fhir_enc_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verstecktes Feld für FHIR-ID des Encounters</t>
+  </si>
+  <si>
     <t xml:space="preserve">patient_id_fk</t>
   </si>
   <si>
@@ -146,7 +158,7 @@
     <t xml:space="preserve">fall_id</t>
   </si>
   <si>
-    <t xml:space="preserve">Fall-ID</t>
+    <t xml:space="preserve">Fall-ID Encounter-Identifier (KIS)</t>
   </si>
   <si>
     <t xml:space="preserve">fall_studienphase</t>
@@ -224,6 +236,9 @@
     <t xml:space="preserve">Entlassdatum</t>
   </si>
   <si>
+    <t xml:space="preserve">fall_additional_values</t>
+  </si>
+  <si>
     <t xml:space="preserve">fall_complete</t>
   </si>
   <si>
@@ -245,13 +260,13 @@
     <t xml:space="preserve">fall_meda_id</t>
   </si>
   <si>
-    <t xml:space="preserve">Dynamische SQL-Abfrage zur Zuordnung Medikationsanalyse -&gt; Fall</t>
+    <t xml:space="preserve">Dynamische SQL-Abfrage zur Zuordnung Medikationsanalyse zu Fall (Fall-ID Encounter-Identifier (KIS)) Auswahlfeld falls die aktuell dokumentierte Medikationsanalyse sich nicht auf die letzte Instanz des Falls bezieht.  </t>
   </si>
   <si>
     <t xml:space="preserve">meda_id</t>
   </si>
   <si>
-    <t xml:space="preserve">ID Medikationsanalyse</t>
+    <t xml:space="preserve">ID Medikationsanalyse (REDCap) Fall-ID Encounter-Identifier (KIS) mit Instanz der aktuellen Medikationsanalyse aggregiert</t>
   </si>
   <si>
     <t xml:space="preserve">meda_typ</t>
@@ -344,6 +359,9 @@
     <t xml:space="preserve">Notizfeld</t>
   </si>
   <si>
+    <t xml:space="preserve">meda_additional_values</t>
+  </si>
+  <si>
     <t xml:space="preserve">medikationsanalyse_complete</t>
   </si>
   <si>
@@ -359,13 +377,13 @@
     <t xml:space="preserve">mrp_meda_id</t>
   </si>
   <si>
-    <t xml:space="preserve">Dynamische SQL-Abfrage zur Zuordnung Medikationsanalyse -&gt; MRP</t>
+    <t xml:space="preserve">Dynamische SQL-Abfrage zur Zuordnung Medikationsanalyse zu MRP   Auswahlfeld falls die aktuell dokumentiertes MRP  sich nicht auf die letzte Instanz der Medikationsanalyse bezieht.  </t>
   </si>
   <si>
     <t xml:space="preserve">mrp_id</t>
   </si>
   <si>
-    <t xml:space="preserve">MRP-ID</t>
+    <t xml:space="preserve">MRP-ID (REDCap) Fall-ID Encounter-Identifier (KIS) mit Instanz der aktuellen Medikationsanalyse und der Instanz des aktuellen MRP aggregiert</t>
   </si>
   <si>
     <t xml:space="preserve">mrp_entd_dat</t>
@@ -779,6 +797,9 @@
     <t xml:space="preserve">1 - NCC MERP Index</t>
   </si>
   <si>
+    <t xml:space="preserve">mrp_additional_values</t>
+  </si>
+  <si>
     <t xml:space="preserve">mrpdokumentation_validierung_complete</t>
   </si>
   <si>
@@ -794,7 +815,7 @@
     <t xml:space="preserve">ret_id</t>
   </si>
   <si>
-    <t xml:space="preserve">Retrolektive MRP-ID</t>
+    <t xml:space="preserve">Retrolektive MRP-ID (REDCap) Fall-ID Encounter-Identifier (KIS) mit Instanz der aktuellen Medikationsanalyse und der Instanz des aktuellen MRP aggregiert</t>
   </si>
   <si>
     <t xml:space="preserve">ret_meda_id</t>
@@ -1029,6 +1050,9 @@
   </si>
   <si>
     <t xml:space="preserve">ret_notiz2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_additional_values</t>
   </si>
   <si>
     <t xml:space="preserve">retrolektive_mrpbewertung_complete</t>
@@ -1823,13 +1847,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
         <v>37</v>
       </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
@@ -1837,13 +1861,13 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
@@ -1854,10 +1878,10 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D21" t="s">
         <v>12</v>
@@ -1868,10 +1892,10 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
@@ -1882,13 +1906,13 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24">
@@ -1896,10 +1920,10 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
         <v>41</v>
-      </c>
-      <c r="C24" t="s">
-        <v>42</v>
       </c>
       <c r="D24" t="s">
         <v>12</v>
@@ -1910,13 +1934,13 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" t="s">
         <v>43</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>44</v>
-      </c>
-      <c r="D25" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="26">
@@ -1958,7 +1982,7 @@
         <v>50</v>
       </c>
       <c r="D28" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29">
@@ -1966,10 +1990,10 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" t="s">
         <v>52</v>
-      </c>
-      <c r="C29" t="s">
-        <v>53</v>
       </c>
       <c r="D29" t="s">
         <v>12</v>
@@ -1980,13 +2004,13 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" t="s">
         <v>54</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>55</v>
-      </c>
-      <c r="D30" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="31">
@@ -2000,7 +2024,7 @@
         <v>57</v>
       </c>
       <c r="D31" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32">
@@ -2084,7 +2108,7 @@
         <v>69</v>
       </c>
       <c r="D37" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38">
@@ -2095,7 +2119,7 @@
         <v>70</v>
       </c>
       <c r="C38" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="D38" t="s">
         <v>12</v>
@@ -2103,16 +2127,16 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="C39" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D39" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40">
@@ -2120,10 +2144,10 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="C40" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="D40" t="s">
         <v>12</v>
@@ -2134,10 +2158,10 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="C41" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="D41" t="s">
         <v>12</v>
@@ -2145,13 +2169,13 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="B42" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C42" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D42" t="s">
         <v>12</v>
@@ -2162,10 +2186,10 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>72</v>
+        <v>13</v>
       </c>
       <c r="C43" t="s">
-        <v>73</v>
+        <v>14</v>
       </c>
       <c r="D43" t="s">
         <v>12</v>
@@ -2176,10 +2200,10 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="C44" t="s">
-        <v>75</v>
+        <v>16</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
@@ -2190,10 +2214,10 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="C45" t="s">
-        <v>77</v>
+        <v>18</v>
       </c>
       <c r="D45" t="s">
         <v>12</v>
@@ -2204,10 +2228,10 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" t="s">
         <v>78</v>
-      </c>
-      <c r="C46" t="s">
-        <v>79</v>
       </c>
       <c r="D46" t="s">
         <v>12</v>
@@ -2218,10 +2242,10 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47" t="s">
         <v>80</v>
-      </c>
-      <c r="C47" t="s">
-        <v>81</v>
       </c>
       <c r="D47" t="s">
         <v>12</v>
@@ -2232,13 +2256,13 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" t="s">
         <v>82</v>
       </c>
-      <c r="C48" t="s">
-        <v>83</v>
-      </c>
       <c r="D48" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49">
@@ -2246,13 +2270,13 @@
         <v>1</v>
       </c>
       <c r="B49" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" t="s">
         <v>84</v>
       </c>
-      <c r="C49" t="s">
-        <v>57</v>
-      </c>
       <c r="D49" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50">
@@ -2263,7 +2287,7 @@
         <v>85</v>
       </c>
       <c r="C50" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="D50" t="s">
         <v>12</v>
@@ -2274,13 +2298,13 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C51" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="D51" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52">
@@ -2288,13 +2312,13 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C52" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D52" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53">
@@ -2302,13 +2326,13 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C53" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D53" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54">
@@ -2316,13 +2340,13 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C54" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="D54" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55">
@@ -2330,10 +2354,10 @@
         <v>1</v>
       </c>
       <c r="B55" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C55" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="D55" t="s">
         <v>12</v>
@@ -2347,10 +2371,10 @@
         <v>93</v>
       </c>
       <c r="C56" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="D56" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="57">
@@ -2358,10 +2382,10 @@
         <v>1</v>
       </c>
       <c r="B57" t="s">
+        <v>94</v>
+      </c>
+      <c r="C57" t="s">
         <v>95</v>
-      </c>
-      <c r="C57" t="s">
-        <v>96</v>
       </c>
       <c r="D57" t="s">
         <v>12</v>
@@ -2372,10 +2396,10 @@
         <v>1</v>
       </c>
       <c r="B58" t="s">
+        <v>96</v>
+      </c>
+      <c r="C58" t="s">
         <v>97</v>
-      </c>
-      <c r="C58" t="s">
-        <v>92</v>
       </c>
       <c r="D58" t="s">
         <v>12</v>
@@ -2417,7 +2441,7 @@
         <v>102</v>
       </c>
       <c r="C61" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D61" t="s">
         <v>12</v>
@@ -2428,10 +2452,10 @@
         <v>1</v>
       </c>
       <c r="B62" t="s">
+        <v>103</v>
+      </c>
+      <c r="C62" t="s">
         <v>104</v>
-      </c>
-      <c r="C62" t="s">
-        <v>105</v>
       </c>
       <c r="D62" t="s">
         <v>12</v>
@@ -2442,13 +2466,13 @@
         <v>1</v>
       </c>
       <c r="B63" t="s">
+        <v>105</v>
+      </c>
+      <c r="C63" t="s">
         <v>106</v>
       </c>
-      <c r="C63" t="s">
-        <v>107</v>
-      </c>
       <c r="D63" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="64">
@@ -2456,10 +2480,10 @@
         <v>1</v>
       </c>
       <c r="B64" t="s">
+        <v>107</v>
+      </c>
+      <c r="C64" t="s">
         <v>108</v>
-      </c>
-      <c r="C64" t="s">
-        <v>109</v>
       </c>
       <c r="D64" t="s">
         <v>12</v>
@@ -2470,10 +2494,10 @@
         <v>1</v>
       </c>
       <c r="B65" t="s">
+        <v>109</v>
+      </c>
+      <c r="C65" t="s">
         <v>110</v>
-      </c>
-      <c r="C65" t="s">
-        <v>36</v>
       </c>
       <c r="D65" t="s">
         <v>12</v>
@@ -2481,16 +2505,16 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
+        <v>1</v>
+      </c>
+      <c r="B66" t="s">
         <v>111</v>
       </c>
-      <c r="B66" t="s">
-        <v>10</v>
-      </c>
       <c r="C66" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="D66" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="67">
@@ -2498,10 +2522,10 @@
         <v>1</v>
       </c>
       <c r="B67" t="s">
-        <v>13</v>
+        <v>113</v>
       </c>
       <c r="C67" t="s">
-        <v>14</v>
+        <v>114</v>
       </c>
       <c r="D67" t="s">
         <v>12</v>
@@ -2512,10 +2536,10 @@
         <v>1</v>
       </c>
       <c r="B68" t="s">
-        <v>15</v>
+        <v>115</v>
       </c>
       <c r="C68" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="D68" t="s">
         <v>12</v>
@@ -2526,10 +2550,10 @@
         <v>1</v>
       </c>
       <c r="B69" t="s">
-        <v>17</v>
+        <v>116</v>
       </c>
       <c r="C69" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="D69" t="s">
         <v>12</v>
@@ -2537,13 +2561,13 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>1</v>
+        <v>117</v>
       </c>
       <c r="B70" t="s">
-        <v>112</v>
+        <v>10</v>
       </c>
       <c r="C70" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D70" t="s">
         <v>12</v>
@@ -2554,10 +2578,10 @@
         <v>1</v>
       </c>
       <c r="B71" t="s">
-        <v>113</v>
+        <v>13</v>
       </c>
       <c r="C71" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="D71" t="s">
         <v>12</v>
@@ -2568,10 +2592,10 @@
         <v>1</v>
       </c>
       <c r="B72" t="s">
-        <v>114</v>
+        <v>15</v>
       </c>
       <c r="C72" t="s">
-        <v>115</v>
+        <v>16</v>
       </c>
       <c r="D72" t="s">
         <v>12</v>
@@ -2582,10 +2606,10 @@
         <v>1</v>
       </c>
       <c r="B73" t="s">
-        <v>116</v>
+        <v>17</v>
       </c>
       <c r="C73" t="s">
-        <v>117</v>
+        <v>18</v>
       </c>
       <c r="D73" t="s">
         <v>12</v>
@@ -2599,10 +2623,10 @@
         <v>118</v>
       </c>
       <c r="C74" t="s">
-        <v>119</v>
+        <v>78</v>
       </c>
       <c r="D74" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75">
@@ -2610,10 +2634,10 @@
         <v>1</v>
       </c>
       <c r="B75" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C75" t="s">
-        <v>121</v>
+        <v>80</v>
       </c>
       <c r="D75" t="s">
         <v>12</v>
@@ -2624,10 +2648,10 @@
         <v>1</v>
       </c>
       <c r="B76" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C76" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D76" t="s">
         <v>12</v>
@@ -2638,10 +2662,10 @@
         <v>1</v>
       </c>
       <c r="B77" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C77" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D77" t="s">
         <v>12</v>
@@ -2652,13 +2676,13 @@
         <v>1</v>
       </c>
       <c r="B78" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C78" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D78" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
     </row>
     <row r="79">
@@ -2666,10 +2690,10 @@
         <v>1</v>
       </c>
       <c r="B79" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C79" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D79" t="s">
         <v>12</v>
@@ -2680,10 +2704,10 @@
         <v>1</v>
       </c>
       <c r="B80" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C80" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D80" t="s">
         <v>12</v>
@@ -2694,10 +2718,10 @@
         <v>1</v>
       </c>
       <c r="B81" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C81" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D81" t="s">
         <v>12</v>
@@ -2708,10 +2732,10 @@
         <v>1</v>
       </c>
       <c r="B82" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C82" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D82" t="s">
         <v>12</v>
@@ -2722,10 +2746,10 @@
         <v>1</v>
       </c>
       <c r="B83" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C83" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D83" t="s">
         <v>12</v>
@@ -2736,10 +2760,10 @@
         <v>1</v>
       </c>
       <c r="B84" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C84" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D84" t="s">
         <v>12</v>
@@ -2750,10 +2774,10 @@
         <v>1</v>
       </c>
       <c r="B85" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C85" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D85" t="s">
         <v>12</v>
@@ -2764,10 +2788,10 @@
         <v>1</v>
       </c>
       <c r="B86" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C86" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D86" t="s">
         <v>12</v>
@@ -2778,10 +2802,10 @@
         <v>1</v>
       </c>
       <c r="B87" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C87" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D87" t="s">
         <v>12</v>
@@ -2792,10 +2816,10 @@
         <v>1</v>
       </c>
       <c r="B88" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C88" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D88" t="s">
         <v>12</v>
@@ -2806,10 +2830,10 @@
         <v>1</v>
       </c>
       <c r="B89" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C89" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D89" t="s">
         <v>12</v>
@@ -2820,10 +2844,10 @@
         <v>1</v>
       </c>
       <c r="B90" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C90" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D90" t="s">
         <v>12</v>
@@ -2834,10 +2858,10 @@
         <v>1</v>
       </c>
       <c r="B91" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C91" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D91" t="s">
         <v>12</v>
@@ -2848,10 +2872,10 @@
         <v>1</v>
       </c>
       <c r="B92" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C92" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D92" t="s">
         <v>12</v>
@@ -2862,10 +2886,10 @@
         <v>1</v>
       </c>
       <c r="B93" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C93" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D93" t="s">
         <v>12</v>
@@ -2876,10 +2900,10 @@
         <v>1</v>
       </c>
       <c r="B94" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C94" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D94" t="s">
         <v>12</v>
@@ -2890,10 +2914,10 @@
         <v>1</v>
       </c>
       <c r="B95" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C95" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D95" t="s">
         <v>12</v>
@@ -2904,10 +2928,10 @@
         <v>1</v>
       </c>
       <c r="B96" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C96" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D96" t="s">
         <v>12</v>
@@ -2918,10 +2942,10 @@
         <v>1</v>
       </c>
       <c r="B97" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C97" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D97" t="s">
         <v>12</v>
@@ -2932,10 +2956,10 @@
         <v>1</v>
       </c>
       <c r="B98" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C98" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D98" t="s">
         <v>12</v>
@@ -2946,10 +2970,10 @@
         <v>1</v>
       </c>
       <c r="B99" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C99" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D99" t="s">
         <v>12</v>
@@ -2960,10 +2984,10 @@
         <v>1</v>
       </c>
       <c r="B100" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C100" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D100" t="s">
         <v>12</v>
@@ -2974,10 +2998,10 @@
         <v>1</v>
       </c>
       <c r="B101" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C101" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D101" t="s">
         <v>12</v>
@@ -2988,10 +3012,10 @@
         <v>1</v>
       </c>
       <c r="B102" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C102" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D102" t="s">
         <v>12</v>
@@ -3002,10 +3026,10 @@
         <v>1</v>
       </c>
       <c r="B103" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C103" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D103" t="s">
         <v>12</v>
@@ -3016,10 +3040,10 @@
         <v>1</v>
       </c>
       <c r="B104" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C104" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D104" t="s">
         <v>12</v>
@@ -3030,10 +3054,10 @@
         <v>1</v>
       </c>
       <c r="B105" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C105" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D105" t="s">
         <v>12</v>
@@ -3044,10 +3068,10 @@
         <v>1</v>
       </c>
       <c r="B106" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C106" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D106" t="s">
         <v>12</v>
@@ -3058,10 +3082,10 @@
         <v>1</v>
       </c>
       <c r="B107" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C107" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D107" t="s">
         <v>12</v>
@@ -3072,10 +3096,10 @@
         <v>1</v>
       </c>
       <c r="B108" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C108" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D108" t="s">
         <v>12</v>
@@ -3086,10 +3110,10 @@
         <v>1</v>
       </c>
       <c r="B109" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C109" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D109" t="s">
         <v>12</v>
@@ -3100,10 +3124,10 @@
         <v>1</v>
       </c>
       <c r="B110" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C110" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D110" t="s">
         <v>12</v>
@@ -3114,10 +3138,10 @@
         <v>1</v>
       </c>
       <c r="B111" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C111" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D111" t="s">
         <v>12</v>
@@ -3128,10 +3152,10 @@
         <v>1</v>
       </c>
       <c r="B112" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C112" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D112" t="s">
         <v>12</v>
@@ -3142,10 +3166,10 @@
         <v>1</v>
       </c>
       <c r="B113" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C113" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D113" t="s">
         <v>12</v>
@@ -3156,10 +3180,10 @@
         <v>1</v>
       </c>
       <c r="B114" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C114" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D114" t="s">
         <v>12</v>
@@ -3170,10 +3194,10 @@
         <v>1</v>
       </c>
       <c r="B115" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C115" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D115" t="s">
         <v>12</v>
@@ -3184,10 +3208,10 @@
         <v>1</v>
       </c>
       <c r="B116" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C116" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D116" t="s">
         <v>12</v>
@@ -3198,7 +3222,7 @@
         <v>1</v>
       </c>
       <c r="B117" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C117" t="s">
         <v>203</v>
@@ -3212,10 +3236,10 @@
         <v>1</v>
       </c>
       <c r="B118" t="s">
+        <v>204</v>
+      </c>
+      <c r="C118" t="s">
         <v>205</v>
-      </c>
-      <c r="C118" t="s">
-        <v>206</v>
       </c>
       <c r="D118" t="s">
         <v>12</v>
@@ -3226,10 +3250,10 @@
         <v>1</v>
       </c>
       <c r="B119" t="s">
+        <v>206</v>
+      </c>
+      <c r="C119" t="s">
         <v>207</v>
-      </c>
-      <c r="C119" t="s">
-        <v>208</v>
       </c>
       <c r="D119" t="s">
         <v>12</v>
@@ -3240,10 +3264,10 @@
         <v>1</v>
       </c>
       <c r="B120" t="s">
+        <v>208</v>
+      </c>
+      <c r="C120" t="s">
         <v>209</v>
-      </c>
-      <c r="C120" t="s">
-        <v>210</v>
       </c>
       <c r="D120" t="s">
         <v>12</v>
@@ -3254,10 +3278,10 @@
         <v>1</v>
       </c>
       <c r="B121" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C121" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D121" t="s">
         <v>12</v>
@@ -3268,10 +3292,10 @@
         <v>1</v>
       </c>
       <c r="B122" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C122" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D122" t="s">
         <v>12</v>
@@ -3282,10 +3306,10 @@
         <v>1</v>
       </c>
       <c r="B123" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C123" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D123" t="s">
         <v>12</v>
@@ -3296,10 +3320,10 @@
         <v>1</v>
       </c>
       <c r="B124" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C124" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D124" t="s">
         <v>12</v>
@@ -3310,10 +3334,10 @@
         <v>1</v>
       </c>
       <c r="B125" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C125" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D125" t="s">
         <v>12</v>
@@ -3324,10 +3348,10 @@
         <v>1</v>
       </c>
       <c r="B126" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C126" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D126" t="s">
         <v>12</v>
@@ -3338,10 +3362,10 @@
         <v>1</v>
       </c>
       <c r="B127" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C127" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D127" t="s">
         <v>12</v>
@@ -3352,10 +3376,10 @@
         <v>1</v>
       </c>
       <c r="B128" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C128" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D128" t="s">
         <v>12</v>
@@ -3366,10 +3390,10 @@
         <v>1</v>
       </c>
       <c r="B129" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C129" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D129" t="s">
         <v>12</v>
@@ -3380,10 +3404,10 @@
         <v>1</v>
       </c>
       <c r="B130" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C130" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D130" t="s">
         <v>12</v>
@@ -3394,10 +3418,10 @@
         <v>1</v>
       </c>
       <c r="B131" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C131" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D131" t="s">
         <v>12</v>
@@ -3408,10 +3432,10 @@
         <v>1</v>
       </c>
       <c r="B132" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C132" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D132" t="s">
         <v>12</v>
@@ -3422,10 +3446,10 @@
         <v>1</v>
       </c>
       <c r="B133" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C133" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D133" t="s">
         <v>12</v>
@@ -3436,10 +3460,10 @@
         <v>1</v>
       </c>
       <c r="B134" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C134" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D134" t="s">
         <v>12</v>
@@ -3450,10 +3474,10 @@
         <v>1</v>
       </c>
       <c r="B135" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C135" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D135" t="s">
         <v>12</v>
@@ -3464,10 +3488,10 @@
         <v>1</v>
       </c>
       <c r="B136" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C136" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D136" t="s">
         <v>12</v>
@@ -3478,10 +3502,10 @@
         <v>1</v>
       </c>
       <c r="B137" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C137" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D137" t="s">
         <v>12</v>
@@ -3492,10 +3516,10 @@
         <v>1</v>
       </c>
       <c r="B138" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C138" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D138" t="s">
         <v>12</v>
@@ -3506,10 +3530,10 @@
         <v>1</v>
       </c>
       <c r="B139" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C139" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D139" t="s">
         <v>12</v>
@@ -3520,10 +3544,10 @@
         <v>1</v>
       </c>
       <c r="B140" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C140" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D140" t="s">
         <v>12</v>
@@ -3534,10 +3558,10 @@
         <v>1</v>
       </c>
       <c r="B141" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C141" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D141" t="s">
         <v>12</v>
@@ -3548,10 +3572,10 @@
         <v>1</v>
       </c>
       <c r="B142" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C142" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D142" t="s">
         <v>12</v>
@@ -3562,10 +3586,10 @@
         <v>1</v>
       </c>
       <c r="B143" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C143" t="s">
-        <v>36</v>
+        <v>254</v>
       </c>
       <c r="D143" t="s">
         <v>12</v>
@@ -3573,13 +3597,13 @@
     </row>
     <row r="144">
       <c r="A144" t="s">
+        <v>1</v>
+      </c>
+      <c r="B144" t="s">
+        <v>255</v>
+      </c>
+      <c r="C144" t="s">
         <v>256</v>
-      </c>
-      <c r="B144" t="s">
-        <v>10</v>
-      </c>
-      <c r="C144" t="s">
-        <v>11</v>
       </c>
       <c r="D144" t="s">
         <v>12</v>
@@ -3590,10 +3614,10 @@
         <v>1</v>
       </c>
       <c r="B145" t="s">
-        <v>13</v>
+        <v>257</v>
       </c>
       <c r="C145" t="s">
-        <v>14</v>
+        <v>258</v>
       </c>
       <c r="D145" t="s">
         <v>12</v>
@@ -3604,10 +3628,10 @@
         <v>1</v>
       </c>
       <c r="B146" t="s">
-        <v>15</v>
+        <v>259</v>
       </c>
       <c r="C146" t="s">
-        <v>16</v>
+        <v>260</v>
       </c>
       <c r="D146" t="s">
         <v>12</v>
@@ -3618,10 +3642,10 @@
         <v>1</v>
       </c>
       <c r="B147" t="s">
-        <v>17</v>
+        <v>261</v>
       </c>
       <c r="C147" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="D147" t="s">
         <v>12</v>
@@ -3632,10 +3656,10 @@
         <v>1</v>
       </c>
       <c r="B148" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="C148" t="s">
-        <v>258</v>
+        <v>38</v>
       </c>
       <c r="D148" t="s">
         <v>12</v>
@@ -3643,13 +3667,13 @@
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>1</v>
+        <v>263</v>
       </c>
       <c r="B149" t="s">
-        <v>259</v>
+        <v>10</v>
       </c>
       <c r="C149" t="s">
-        <v>260</v>
+        <v>11</v>
       </c>
       <c r="D149" t="s">
         <v>12</v>
@@ -3660,10 +3684,10 @@
         <v>1</v>
       </c>
       <c r="B150" t="s">
-        <v>261</v>
+        <v>13</v>
       </c>
       <c r="C150" t="s">
-        <v>262</v>
+        <v>14</v>
       </c>
       <c r="D150" t="s">
         <v>12</v>
@@ -3674,13 +3698,13 @@
         <v>1</v>
       </c>
       <c r="B151" t="s">
-        <v>263</v>
+        <v>15</v>
       </c>
       <c r="C151" t="s">
-        <v>264</v>
+        <v>16</v>
       </c>
       <c r="D151" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
     </row>
     <row r="152">
@@ -3688,10 +3712,10 @@
         <v>1</v>
       </c>
       <c r="B152" t="s">
-        <v>265</v>
+        <v>17</v>
       </c>
       <c r="C152" t="s">
-        <v>123</v>
+        <v>18</v>
       </c>
       <c r="D152" t="s">
         <v>12</v>
@@ -3702,10 +3726,10 @@
         <v>1</v>
       </c>
       <c r="B153" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C153" t="s">
-        <v>203</v>
+        <v>265</v>
       </c>
       <c r="D153" t="s">
         <v>12</v>
@@ -3716,10 +3740,10 @@
         <v>1</v>
       </c>
       <c r="B154" t="s">
+        <v>266</v>
+      </c>
+      <c r="C154" t="s">
         <v>267</v>
-      </c>
-      <c r="C154" t="s">
-        <v>203</v>
       </c>
       <c r="D154" t="s">
         <v>12</v>
@@ -3733,7 +3757,7 @@
         <v>268</v>
       </c>
       <c r="C155" t="s">
-        <v>131</v>
+        <v>269</v>
       </c>
       <c r="D155" t="s">
         <v>12</v>
@@ -3744,13 +3768,13 @@
         <v>1</v>
       </c>
       <c r="B156" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C156" t="s">
-        <v>133</v>
+        <v>271</v>
       </c>
       <c r="D156" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
     </row>
     <row r="157">
@@ -3758,10 +3782,10 @@
         <v>1</v>
       </c>
       <c r="B157" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C157" t="s">
-        <v>206</v>
+        <v>129</v>
       </c>
       <c r="D157" t="s">
         <v>12</v>
@@ -3772,10 +3796,10 @@
         <v>1</v>
       </c>
       <c r="B158" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C158" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D158" t="s">
         <v>12</v>
@@ -3786,10 +3810,10 @@
         <v>1</v>
       </c>
       <c r="B159" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C159" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D159" t="s">
         <v>12</v>
@@ -3800,10 +3824,10 @@
         <v>1</v>
       </c>
       <c r="B160" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C160" t="s">
-        <v>274</v>
+        <v>137</v>
       </c>
       <c r="D160" t="s">
         <v>12</v>
@@ -3814,10 +3838,10 @@
         <v>1</v>
       </c>
       <c r="B161" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C161" t="s">
-        <v>276</v>
+        <v>139</v>
       </c>
       <c r="D161" t="s">
         <v>12</v>
@@ -3831,7 +3855,7 @@
         <v>277</v>
       </c>
       <c r="C162" t="s">
-        <v>278</v>
+        <v>212</v>
       </c>
       <c r="D162" t="s">
         <v>12</v>
@@ -3842,10 +3866,10 @@
         <v>1</v>
       </c>
       <c r="B163" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C163" t="s">
-        <v>280</v>
+        <v>214</v>
       </c>
       <c r="D163" t="s">
         <v>12</v>
@@ -3856,10 +3880,10 @@
         <v>1</v>
       </c>
       <c r="B164" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C164" t="s">
-        <v>282</v>
+        <v>216</v>
       </c>
       <c r="D164" t="s">
         <v>12</v>
@@ -3870,10 +3894,10 @@
         <v>1</v>
       </c>
       <c r="B165" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C165" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D165" t="s">
         <v>12</v>
@@ -3884,10 +3908,10 @@
         <v>1</v>
       </c>
       <c r="B166" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C166" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D166" t="s">
         <v>12</v>
@@ -3898,10 +3922,10 @@
         <v>1</v>
       </c>
       <c r="B167" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C167" t="s">
-        <v>212</v>
+        <v>285</v>
       </c>
       <c r="D167" t="s">
         <v>12</v>
@@ -3912,10 +3936,10 @@
         <v>1</v>
       </c>
       <c r="B168" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C168" t="s">
-        <v>214</v>
+        <v>287</v>
       </c>
       <c r="D168" t="s">
         <v>12</v>
@@ -3926,10 +3950,10 @@
         <v>1</v>
       </c>
       <c r="B169" t="s">
+        <v>288</v>
+      </c>
+      <c r="C169" t="s">
         <v>289</v>
-      </c>
-      <c r="C169" t="s">
-        <v>216</v>
       </c>
       <c r="D169" t="s">
         <v>12</v>
@@ -3943,7 +3967,7 @@
         <v>290</v>
       </c>
       <c r="C170" t="s">
-        <v>218</v>
+        <v>291</v>
       </c>
       <c r="D170" t="s">
         <v>12</v>
@@ -3954,10 +3978,10 @@
         <v>1</v>
       </c>
       <c r="B171" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C171" t="s">
-        <v>220</v>
+        <v>293</v>
       </c>
       <c r="D171" t="s">
         <v>12</v>
@@ -3968,10 +3992,10 @@
         <v>1</v>
       </c>
       <c r="B172" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C172" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D172" t="s">
         <v>12</v>
@@ -3982,10 +4006,10 @@
         <v>1</v>
       </c>
       <c r="B173" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C173" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D173" t="s">
         <v>12</v>
@@ -3996,10 +4020,10 @@
         <v>1</v>
       </c>
       <c r="B174" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C174" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D174" t="s">
         <v>12</v>
@@ -4010,10 +4034,10 @@
         <v>1</v>
       </c>
       <c r="B175" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="C175" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D175" t="s">
         <v>12</v>
@@ -4024,10 +4048,10 @@
         <v>1</v>
       </c>
       <c r="B176" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C176" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D176" t="s">
         <v>12</v>
@@ -4038,10 +4062,10 @@
         <v>1</v>
       </c>
       <c r="B177" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C177" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D177" t="s">
         <v>12</v>
@@ -4052,10 +4076,10 @@
         <v>1</v>
       </c>
       <c r="B178" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C178" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D178" t="s">
         <v>12</v>
@@ -4066,10 +4090,10 @@
         <v>1</v>
       </c>
       <c r="B179" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="C179" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D179" t="s">
         <v>12</v>
@@ -4080,10 +4104,10 @@
         <v>1</v>
       </c>
       <c r="B180" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C180" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D180" t="s">
         <v>12</v>
@@ -4094,10 +4118,10 @@
         <v>1</v>
       </c>
       <c r="B181" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C181" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D181" t="s">
         <v>12</v>
@@ -4108,10 +4132,10 @@
         <v>1</v>
       </c>
       <c r="B182" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C182" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D182" t="s">
         <v>12</v>
@@ -4122,10 +4146,10 @@
         <v>1</v>
       </c>
       <c r="B183" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C183" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D183" t="s">
         <v>12</v>
@@ -4136,10 +4160,10 @@
         <v>1</v>
       </c>
       <c r="B184" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C184" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D184" t="s">
         <v>12</v>
@@ -4150,10 +4174,10 @@
         <v>1</v>
       </c>
       <c r="B185" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="C185" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D185" t="s">
         <v>12</v>
@@ -4164,13 +4188,13 @@
         <v>1</v>
       </c>
       <c r="B186" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C186" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="D186" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
     </row>
     <row r="187">
@@ -4178,10 +4202,10 @@
         <v>1</v>
       </c>
       <c r="B187" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C187" t="s">
-        <v>308</v>
+        <v>248</v>
       </c>
       <c r="D187" t="s">
         <v>12</v>
@@ -4192,10 +4216,10 @@
         <v>1</v>
       </c>
       <c r="B188" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C188" t="s">
-        <v>310</v>
+        <v>250</v>
       </c>
       <c r="D188" t="s">
         <v>12</v>
@@ -4209,7 +4233,7 @@
         <v>311</v>
       </c>
       <c r="C189" t="s">
-        <v>312</v>
+        <v>252</v>
       </c>
       <c r="D189" t="s">
         <v>12</v>
@@ -4220,10 +4244,10 @@
         <v>1</v>
       </c>
       <c r="B190" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C190" t="s">
-        <v>274</v>
+        <v>254</v>
       </c>
       <c r="D190" t="s">
         <v>12</v>
@@ -4234,13 +4258,13 @@
         <v>1</v>
       </c>
       <c r="B191" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C191" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D191" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
     </row>
     <row r="192">
@@ -4248,10 +4272,10 @@
         <v>1</v>
       </c>
       <c r="B192" t="s">
+        <v>314</v>
+      </c>
+      <c r="C192" t="s">
         <v>315</v>
-      </c>
-      <c r="C192" t="s">
-        <v>278</v>
       </c>
       <c r="D192" t="s">
         <v>12</v>
@@ -4265,7 +4289,7 @@
         <v>316</v>
       </c>
       <c r="C193" t="s">
-        <v>280</v>
+        <v>317</v>
       </c>
       <c r="D193" t="s">
         <v>12</v>
@@ -4276,10 +4300,10 @@
         <v>1</v>
       </c>
       <c r="B194" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C194" t="s">
-        <v>282</v>
+        <v>319</v>
       </c>
       <c r="D194" t="s">
         <v>12</v>
@@ -4290,10 +4314,10 @@
         <v>1</v>
       </c>
       <c r="B195" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C195" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D195" t="s">
         <v>12</v>
@@ -4304,10 +4328,10 @@
         <v>1</v>
       </c>
       <c r="B196" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C196" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D196" t="s">
         <v>12</v>
@@ -4318,10 +4342,10 @@
         <v>1</v>
       </c>
       <c r="B197" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C197" t="s">
-        <v>212</v>
+        <v>285</v>
       </c>
       <c r="D197" t="s">
         <v>12</v>
@@ -4332,10 +4356,10 @@
         <v>1</v>
       </c>
       <c r="B198" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C198" t="s">
-        <v>214</v>
+        <v>287</v>
       </c>
       <c r="D198" t="s">
         <v>12</v>
@@ -4346,10 +4370,10 @@
         <v>1</v>
       </c>
       <c r="B199" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C199" t="s">
-        <v>216</v>
+        <v>289</v>
       </c>
       <c r="D199" t="s">
         <v>12</v>
@@ -4360,10 +4384,10 @@
         <v>1</v>
       </c>
       <c r="B200" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C200" t="s">
-        <v>218</v>
+        <v>291</v>
       </c>
       <c r="D200" t="s">
         <v>12</v>
@@ -4374,10 +4398,10 @@
         <v>1</v>
       </c>
       <c r="B201" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C201" t="s">
-        <v>220</v>
+        <v>293</v>
       </c>
       <c r="D201" t="s">
         <v>12</v>
@@ -4388,10 +4412,10 @@
         <v>1</v>
       </c>
       <c r="B202" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C202" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D202" t="s">
         <v>12</v>
@@ -4402,10 +4426,10 @@
         <v>1</v>
       </c>
       <c r="B203" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C203" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D203" t="s">
         <v>12</v>
@@ -4416,10 +4440,10 @@
         <v>1</v>
       </c>
       <c r="B204" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C204" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D204" t="s">
         <v>12</v>
@@ -4430,10 +4454,10 @@
         <v>1</v>
       </c>
       <c r="B205" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C205" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D205" t="s">
         <v>12</v>
@@ -4444,10 +4468,10 @@
         <v>1</v>
       </c>
       <c r="B206" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C206" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D206" t="s">
         <v>12</v>
@@ -4458,10 +4482,10 @@
         <v>1</v>
       </c>
       <c r="B207" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C207" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D207" t="s">
         <v>12</v>
@@ -4472,10 +4496,10 @@
         <v>1</v>
       </c>
       <c r="B208" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C208" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D208" t="s">
         <v>12</v>
@@ -4486,10 +4510,10 @@
         <v>1</v>
       </c>
       <c r="B209" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C209" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D209" t="s">
         <v>12</v>
@@ -4500,10 +4524,10 @@
         <v>1</v>
       </c>
       <c r="B210" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C210" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D210" t="s">
         <v>12</v>
@@ -4514,10 +4538,10 @@
         <v>1</v>
       </c>
       <c r="B211" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C211" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D211" t="s">
         <v>12</v>
@@ -4528,10 +4552,10 @@
         <v>1</v>
       </c>
       <c r="B212" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C212" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D212" t="s">
         <v>12</v>
@@ -4542,10 +4566,10 @@
         <v>1</v>
       </c>
       <c r="B213" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C213" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D213" t="s">
         <v>12</v>
@@ -4556,10 +4580,10 @@
         <v>1</v>
       </c>
       <c r="B214" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C214" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D214" t="s">
         <v>12</v>
@@ -4570,10 +4594,10 @@
         <v>1</v>
       </c>
       <c r="B215" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="C215" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D215" t="s">
         <v>12</v>
@@ -4584,10 +4608,10 @@
         <v>1</v>
       </c>
       <c r="B216" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="C216" t="s">
-        <v>36</v>
+        <v>246</v>
       </c>
       <c r="D216" t="s">
         <v>12</v>
@@ -4595,13 +4619,13 @@
     </row>
     <row r="217">
       <c r="A217" t="s">
-        <v>340</v>
+        <v>1</v>
       </c>
       <c r="B217" t="s">
-        <v>10</v>
+        <v>342</v>
       </c>
       <c r="C217" t="s">
-        <v>11</v>
+        <v>248</v>
       </c>
       <c r="D217" t="s">
         <v>12</v>
@@ -4612,10 +4636,10 @@
         <v>1</v>
       </c>
       <c r="B218" t="s">
-        <v>13</v>
+        <v>343</v>
       </c>
       <c r="C218" t="s">
-        <v>14</v>
+        <v>250</v>
       </c>
       <c r="D218" t="s">
         <v>12</v>
@@ -4626,10 +4650,10 @@
         <v>1</v>
       </c>
       <c r="B219" t="s">
-        <v>15</v>
+        <v>344</v>
       </c>
       <c r="C219" t="s">
-        <v>16</v>
+        <v>252</v>
       </c>
       <c r="D219" t="s">
         <v>12</v>
@@ -4640,10 +4664,10 @@
         <v>1</v>
       </c>
       <c r="B220" t="s">
-        <v>17</v>
+        <v>345</v>
       </c>
       <c r="C220" t="s">
-        <v>18</v>
+        <v>254</v>
       </c>
       <c r="D220" t="s">
         <v>12</v>
@@ -4654,13 +4678,13 @@
         <v>1</v>
       </c>
       <c r="B221" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="C221" t="s">
-        <v>342</v>
+        <v>36</v>
       </c>
       <c r="D221" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="222">
@@ -4668,27 +4692,27 @@
         <v>1</v>
       </c>
       <c r="B222" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="C222" t="s">
-        <v>344</v>
+        <v>38</v>
       </c>
       <c r="D222" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="s">
-        <v>1</v>
+        <v>348</v>
       </c>
       <c r="B223" t="s">
-        <v>345</v>
+        <v>10</v>
       </c>
       <c r="C223" t="s">
-        <v>346</v>
+        <v>11</v>
       </c>
       <c r="D223" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="224">
@@ -4696,13 +4720,13 @@
         <v>1</v>
       </c>
       <c r="B224" t="s">
-        <v>347</v>
+        <v>13</v>
       </c>
       <c r="C224" t="s">
-        <v>348</v>
+        <v>14</v>
       </c>
       <c r="D224" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="225">
@@ -4710,13 +4734,13 @@
         <v>1</v>
       </c>
       <c r="B225" t="s">
-        <v>349</v>
+        <v>15</v>
       </c>
       <c r="C225" t="s">
-        <v>350</v>
+        <v>16</v>
       </c>
       <c r="D225" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="226">
@@ -4724,13 +4748,13 @@
         <v>1</v>
       </c>
       <c r="B226" t="s">
-        <v>351</v>
+        <v>17</v>
       </c>
       <c r="C226" t="s">
-        <v>352</v>
+        <v>18</v>
       </c>
       <c r="D226" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="227">
@@ -4738,13 +4762,13 @@
         <v>1</v>
       </c>
       <c r="B227" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C227" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D227" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="228">
@@ -4752,13 +4776,13 @@
         <v>1</v>
       </c>
       <c r="B228" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C228" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D228" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="229">
@@ -4766,13 +4790,13 @@
         <v>1</v>
       </c>
       <c r="B229" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C229" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D229" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="230">
@@ -4780,13 +4804,13 @@
         <v>1</v>
       </c>
       <c r="B230" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C230" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="D230" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="231">
@@ -4794,13 +4818,13 @@
         <v>1</v>
       </c>
       <c r="B231" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C231" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="D231" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="232">
@@ -4808,13 +4832,13 @@
         <v>1</v>
       </c>
       <c r="B232" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C232" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D232" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="233">
@@ -4822,13 +4846,13 @@
         <v>1</v>
       </c>
       <c r="B233" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C233" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="D233" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="234">
@@ -4836,13 +4860,13 @@
         <v>1</v>
       </c>
       <c r="B234" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="C234" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="D234" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="235">
@@ -4850,27 +4874,27 @@
         <v>1</v>
       </c>
       <c r="B235" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="C235" t="s">
-        <v>36</v>
+        <v>366</v>
       </c>
       <c r="D235" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="s">
-        <v>370</v>
+        <v>1</v>
       </c>
       <c r="B236" t="s">
-        <v>10</v>
+        <v>367</v>
       </c>
       <c r="C236" t="s">
-        <v>11</v>
+        <v>368</v>
       </c>
       <c r="D236" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="237">
@@ -4878,13 +4902,13 @@
         <v>1</v>
       </c>
       <c r="B237" t="s">
-        <v>13</v>
+        <v>369</v>
       </c>
       <c r="C237" t="s">
-        <v>14</v>
+        <v>370</v>
       </c>
       <c r="D237" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="238">
@@ -4892,13 +4916,13 @@
         <v>1</v>
       </c>
       <c r="B238" t="s">
-        <v>15</v>
+        <v>371</v>
       </c>
       <c r="C238" t="s">
-        <v>16</v>
+        <v>372</v>
       </c>
       <c r="D238" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="239">
@@ -4906,13 +4930,13 @@
         <v>1</v>
       </c>
       <c r="B239" t="s">
-        <v>17</v>
+        <v>373</v>
       </c>
       <c r="C239" t="s">
-        <v>18</v>
+        <v>374</v>
       </c>
       <c r="D239" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="240">
@@ -4920,13 +4944,13 @@
         <v>1</v>
       </c>
       <c r="B240" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="C240" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="D240" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="241">
@@ -4934,27 +4958,27 @@
         <v>1</v>
       </c>
       <c r="B241" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="C241" t="s">
-        <v>374</v>
+        <v>38</v>
       </c>
       <c r="D241" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="s">
-        <v>1</v>
+        <v>378</v>
       </c>
       <c r="B242" t="s">
-        <v>375</v>
+        <v>10</v>
       </c>
       <c r="C242" t="s">
-        <v>376</v>
+        <v>11</v>
       </c>
       <c r="D242" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="243">
@@ -4962,13 +4986,13 @@
         <v>1</v>
       </c>
       <c r="B243" t="s">
-        <v>377</v>
+        <v>13</v>
       </c>
       <c r="C243" t="s">
-        <v>378</v>
+        <v>14</v>
       </c>
       <c r="D243" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="244">
@@ -4976,13 +5000,13 @@
         <v>1</v>
       </c>
       <c r="B244" t="s">
-        <v>379</v>
+        <v>15</v>
       </c>
       <c r="C244" t="s">
-        <v>380</v>
+        <v>16</v>
       </c>
       <c r="D244" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="245">
@@ -4990,13 +5014,13 @@
         <v>1</v>
       </c>
       <c r="B245" t="s">
-        <v>381</v>
+        <v>17</v>
       </c>
       <c r="C245" t="s">
-        <v>382</v>
+        <v>18</v>
       </c>
       <c r="D245" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="246">
@@ -5004,13 +5028,13 @@
         <v>1</v>
       </c>
       <c r="B246" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="C246" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="D246" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="247">
@@ -5018,13 +5042,13 @@
         <v>1</v>
       </c>
       <c r="B247" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="C247" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="D247" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="248">
@@ -5032,13 +5056,13 @@
         <v>1</v>
       </c>
       <c r="B248" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="C248" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D248" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="249">
@@ -5046,13 +5070,13 @@
         <v>1</v>
       </c>
       <c r="B249" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="C249" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="D249" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="250">
@@ -5060,13 +5084,13 @@
         <v>1</v>
       </c>
       <c r="B250" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="C250" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="D250" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="251">
@@ -5074,13 +5098,13 @@
         <v>1</v>
       </c>
       <c r="B251" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="C251" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="D251" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="252">
@@ -5088,13 +5112,13 @@
         <v>1</v>
       </c>
       <c r="B252" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="C252" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="D252" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="253">
@@ -5102,13 +5126,13 @@
         <v>1</v>
       </c>
       <c r="B253" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C253" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D253" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="254">
@@ -5116,13 +5140,13 @@
         <v>1</v>
       </c>
       <c r="B254" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="C254" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="D254" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="255">
@@ -5130,13 +5154,13 @@
         <v>1</v>
       </c>
       <c r="B255" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="C255" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="D255" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="256">
@@ -5144,13 +5168,13 @@
         <v>1</v>
       </c>
       <c r="B256" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="C256" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="D256" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="257">
@@ -5158,13 +5182,13 @@
         <v>1</v>
       </c>
       <c r="B257" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="C257" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="D257" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="258">
@@ -5172,13 +5196,13 @@
         <v>1</v>
       </c>
       <c r="B258" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="C258" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D258" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="259">
@@ -5186,13 +5210,13 @@
         <v>1</v>
       </c>
       <c r="B259" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="C259" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="D259" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="260">
@@ -5200,13 +5224,13 @@
         <v>1</v>
       </c>
       <c r="B260" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C260" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D260" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="261">
@@ -5214,13 +5238,13 @@
         <v>1</v>
       </c>
       <c r="B261" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C261" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="D261" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="262">
@@ -5228,12 +5252,96 @@
         <v>1</v>
       </c>
       <c r="B262" t="s">
+        <v>411</v>
+      </c>
+      <c r="C262" t="s">
+        <v>412</v>
+      </c>
+      <c r="D262" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="s">
+        <v>1</v>
+      </c>
+      <c r="B263" t="s">
+        <v>413</v>
+      </c>
+      <c r="C263" t="s">
+        <v>414</v>
+      </c>
+      <c r="D263" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="s">
+        <v>1</v>
+      </c>
+      <c r="B264" t="s">
         <v>415</v>
       </c>
-      <c r="C262" t="s">
-        <v>36</v>
-      </c>
-      <c r="D262" t="s">
+      <c r="C264" t="s">
+        <v>416</v>
+      </c>
+      <c r="D264" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="s">
+        <v>1</v>
+      </c>
+      <c r="B265" t="s">
+        <v>417</v>
+      </c>
+      <c r="C265" t="s">
+        <v>418</v>
+      </c>
+      <c r="D265" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="s">
+        <v>1</v>
+      </c>
+      <c r="B266" t="s">
+        <v>419</v>
+      </c>
+      <c r="C266" t="s">
+        <v>420</v>
+      </c>
+      <c r="D266" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="s">
+        <v>1</v>
+      </c>
+      <c r="B267" t="s">
+        <v>421</v>
+      </c>
+      <c r="C267" t="s">
+        <v>422</v>
+      </c>
+      <c r="D267" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="s">
+        <v>1</v>
+      </c>
+      <c r="B268" t="s">
+        <v>423</v>
+      </c>
+      <c r="C268" t="s">
+        <v>38</v>
+      </c>
+      <c r="D268" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Redcap data dictionary and table description
</commit_message>
<xml_diff>
--- a/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
+++ b/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="426">
   <si>
     <t xml:space="preserve">Hint</t>
   </si>
@@ -794,7 +794,7 @@
     <t xml:space="preserve">mrp_merp_info___1</t>
   </si>
   <si>
-    <t xml:space="preserve">1 - NCC MERP Index</t>
+    <t xml:space="preserve">1 - NCC MERP Index anzeigen</t>
   </si>
   <si>
     <t xml:space="preserve">mrp_additional_values</t>
@@ -815,7 +815,7 @@
     <t xml:space="preserve">ret_id</t>
   </si>
   <si>
-    <t xml:space="preserve">Retrolektive MRP-ID (REDCap) Fall-ID Encounter-Identifier (KIS) mit Instanz der aktuellen Medikationsanalyse und der Instanz des aktuellen MRP aggregiert</t>
+    <t xml:space="preserve">Retrolektive MRP-ID (REDCap) Hier wird die MEDA-ID der Medikationsanalyse angegeben, zu deren Zeitpunkt dieses MRP vom Apotheker hätte gefunden werden können. Wenn keine Medikationsanalyse dokumentiert ist wir eine ID aus Fall-ID-x eingetragen</t>
   </si>
   <si>
     <t xml:space="preserve">ret_meda_id</t>
@@ -971,6 +971,12 @@
     <t xml:space="preserve">ret_bewerter2</t>
   </si>
   <si>
+    <t xml:space="preserve">2. Bewertung von  @DEFAULT = @SETVALUE = '[ret_bewerter2_pipeline]'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_bewerter3</t>
+  </si>
+  <si>
     <t xml:space="preserve">2. Bewertung von</t>
   </si>
   <si>
@@ -992,7 +998,7 @@
     <t xml:space="preserve">ret_gewiss_grund_abl_klin2</t>
   </si>
   <si>
-    <t xml:space="preserve">ret_gewiss_grund_abl_klin_neg___1</t>
+    <t xml:space="preserve">ret_gewiss_grund_abl_klin2_neg___1</t>
   </si>
   <si>
     <t xml:space="preserve">ret_massn_am2___1</t>
@@ -4317,7 +4323,7 @@
         <v>320</v>
       </c>
       <c r="C195" t="s">
-        <v>281</v>
+        <v>321</v>
       </c>
       <c r="D195" t="s">
         <v>12</v>
@@ -4328,10 +4334,10 @@
         <v>1</v>
       </c>
       <c r="B196" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C196" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D196" t="s">
         <v>12</v>
@@ -4342,10 +4348,10 @@
         <v>1</v>
       </c>
       <c r="B197" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C197" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D197" t="s">
         <v>12</v>
@@ -4356,10 +4362,10 @@
         <v>1</v>
       </c>
       <c r="B198" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C198" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D198" t="s">
         <v>12</v>
@@ -4370,10 +4376,10 @@
         <v>1</v>
       </c>
       <c r="B199" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C199" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D199" t="s">
         <v>12</v>
@@ -4384,10 +4390,10 @@
         <v>1</v>
       </c>
       <c r="B200" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C200" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D200" t="s">
         <v>12</v>
@@ -4398,10 +4404,10 @@
         <v>1</v>
       </c>
       <c r="B201" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C201" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D201" t="s">
         <v>12</v>
@@ -4412,10 +4418,10 @@
         <v>1</v>
       </c>
       <c r="B202" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C202" t="s">
-        <v>218</v>
+        <v>293</v>
       </c>
       <c r="D202" t="s">
         <v>12</v>
@@ -4426,10 +4432,10 @@
         <v>1</v>
       </c>
       <c r="B203" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C203" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D203" t="s">
         <v>12</v>
@@ -4440,10 +4446,10 @@
         <v>1</v>
       </c>
       <c r="B204" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C204" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D204" t="s">
         <v>12</v>
@@ -4454,10 +4460,10 @@
         <v>1</v>
       </c>
       <c r="B205" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C205" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D205" t="s">
         <v>12</v>
@@ -4468,10 +4474,10 @@
         <v>1</v>
       </c>
       <c r="B206" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C206" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D206" t="s">
         <v>12</v>
@@ -4482,10 +4488,10 @@
         <v>1</v>
       </c>
       <c r="B207" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C207" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D207" t="s">
         <v>12</v>
@@ -4496,10 +4502,10 @@
         <v>1</v>
       </c>
       <c r="B208" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C208" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D208" t="s">
         <v>12</v>
@@ -4510,10 +4516,10 @@
         <v>1</v>
       </c>
       <c r="B209" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C209" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D209" t="s">
         <v>12</v>
@@ -4524,10 +4530,10 @@
         <v>1</v>
       </c>
       <c r="B210" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C210" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D210" t="s">
         <v>12</v>
@@ -4538,10 +4544,10 @@
         <v>1</v>
       </c>
       <c r="B211" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C211" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D211" t="s">
         <v>12</v>
@@ -4552,10 +4558,10 @@
         <v>1</v>
       </c>
       <c r="B212" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C212" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D212" t="s">
         <v>12</v>
@@ -4566,10 +4572,10 @@
         <v>1</v>
       </c>
       <c r="B213" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C213" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D213" t="s">
         <v>12</v>
@@ -4580,10 +4586,10 @@
         <v>1</v>
       </c>
       <c r="B214" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C214" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D214" t="s">
         <v>12</v>
@@ -4594,10 +4600,10 @@
         <v>1</v>
       </c>
       <c r="B215" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C215" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D215" t="s">
         <v>12</v>
@@ -4608,10 +4614,10 @@
         <v>1</v>
       </c>
       <c r="B216" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C216" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D216" t="s">
         <v>12</v>
@@ -4622,10 +4628,10 @@
         <v>1</v>
       </c>
       <c r="B217" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C217" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D217" t="s">
         <v>12</v>
@@ -4636,10 +4642,10 @@
         <v>1</v>
       </c>
       <c r="B218" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C218" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D218" t="s">
         <v>12</v>
@@ -4650,10 +4656,10 @@
         <v>1</v>
       </c>
       <c r="B219" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C219" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D219" t="s">
         <v>12</v>
@@ -4664,10 +4670,10 @@
         <v>1</v>
       </c>
       <c r="B220" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C220" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D220" t="s">
         <v>12</v>
@@ -4678,10 +4684,10 @@
         <v>1</v>
       </c>
       <c r="B221" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C221" t="s">
-        <v>36</v>
+        <v>254</v>
       </c>
       <c r="D221" t="s">
         <v>12</v>
@@ -4692,10 +4698,10 @@
         <v>1</v>
       </c>
       <c r="B222" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C222" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D222" t="s">
         <v>12</v>
@@ -4703,13 +4709,13 @@
     </row>
     <row r="223">
       <c r="A223" t="s">
-        <v>348</v>
+        <v>1</v>
       </c>
       <c r="B223" t="s">
-        <v>10</v>
+        <v>349</v>
       </c>
       <c r="C223" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D223" t="s">
         <v>12</v>
@@ -4717,13 +4723,13 @@
     </row>
     <row r="224">
       <c r="A224" t="s">
-        <v>1</v>
+        <v>350</v>
       </c>
       <c r="B224" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C224" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D224" t="s">
         <v>12</v>
@@ -4734,10 +4740,10 @@
         <v>1</v>
       </c>
       <c r="B225" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C225" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D225" t="s">
         <v>12</v>
@@ -4748,10 +4754,10 @@
         <v>1</v>
       </c>
       <c r="B226" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C226" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D226" t="s">
         <v>12</v>
@@ -4762,13 +4768,13 @@
         <v>1</v>
       </c>
       <c r="B227" t="s">
-        <v>349</v>
+        <v>17</v>
       </c>
       <c r="C227" t="s">
-        <v>350</v>
+        <v>18</v>
       </c>
       <c r="D227" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
     </row>
     <row r="228">
@@ -4950,7 +4956,7 @@
         <v>376</v>
       </c>
       <c r="D240" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="241">
@@ -4961,21 +4967,21 @@
         <v>377</v>
       </c>
       <c r="C241" t="s">
-        <v>38</v>
+        <v>378</v>
       </c>
       <c r="D241" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="s">
-        <v>378</v>
+        <v>1</v>
       </c>
       <c r="B242" t="s">
-        <v>10</v>
+        <v>379</v>
       </c>
       <c r="C242" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D242" t="s">
         <v>12</v>
@@ -4983,13 +4989,13 @@
     </row>
     <row r="243">
       <c r="A243" t="s">
-        <v>1</v>
+        <v>380</v>
       </c>
       <c r="B243" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C243" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D243" t="s">
         <v>12</v>
@@ -5000,10 +5006,10 @@
         <v>1</v>
       </c>
       <c r="B244" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C244" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D244" t="s">
         <v>12</v>
@@ -5014,10 +5020,10 @@
         <v>1</v>
       </c>
       <c r="B245" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C245" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D245" t="s">
         <v>12</v>
@@ -5028,13 +5034,13 @@
         <v>1</v>
       </c>
       <c r="B246" t="s">
-        <v>379</v>
+        <v>17</v>
       </c>
       <c r="C246" t="s">
-        <v>380</v>
+        <v>18</v>
       </c>
       <c r="D246" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
     </row>
     <row r="247">
@@ -5339,9 +5345,23 @@
         <v>423</v>
       </c>
       <c r="C268" t="s">
+        <v>424</v>
+      </c>
+      <c r="D268" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="s">
+        <v>1</v>
+      </c>
+      <c r="B269" t="s">
+        <v>425</v>
+      </c>
+      <c r="C269" t="s">
         <v>38</v>
       </c>
-      <c r="D268" t="s">
+      <c r="D269" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Enable adding columns per extension file in frontend DB tables
</commit_message>
<xml_diff>
--- a/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
+++ b/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
@@ -12,47 +12,47 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="431">
   <si>
     <t xml:space="preserve">Hint</t>
   </si>
   <si>
+    <t xml:space="preserve">This file is generated by the R script 'RedcapDataDictionaryToFrontend'. Do not change it directly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you want to add or remove columns for a resource or an entire table, change the Redcap exported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'Frontend_DataDictionary.csv' and execute the generation process via the init script in the db2frontend module.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TABLE_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLUMN_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLUMN_DESCRIPTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLUMN_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">record_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Record ID RedCap - predefined with the database internal ID of the patient - used in all instances of the patient in RedCap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">varchar</t>
+  </si>
+  <si>
     <t xml:space="preserve"/>
   </si>
   <si>
-    <t xml:space="preserve">This file is generated by the R script 'RedcapDataDictionaryToFrontend'. Do not change it directly.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If you want to add or remove columns for a resource or an entire table, change the Redcap exported</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'Frontend_DataDictionary.csv' and execute the generation process via the init script in the db2frontend module.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TABLE_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COLUMN_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COLUMN_DESCRIPTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COLUMN_TYPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">patient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">record_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Record ID RedCap - predefined with the database internal ID of the patient - used in all instances of the patient in RedCap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">varchar</t>
-  </si>
-  <si>
     <t xml:space="preserve">redcap_repeat_instrument</t>
   </si>
   <si>
@@ -1062,6 +1062,18 @@
   </si>
   <si>
     <t xml:space="preserve">ret_additional_values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db_ret_main_enc_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FHIR ID of the main Encounter to which this evaluation belongs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db_ret_medical_case_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HIS internal Identifier of the medical case to which this evaluation belongs</t>
   </si>
   <si>
     <t xml:space="preserve">retrolektive_mrpbewertung_complete</t>
@@ -1630,79 +1642,69 @@
       </c>
       <c r="B1"/>
       <c r="C1"/>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
+      <c r="D1"/>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2"/>
       <c r="C2"/>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3"/>
       <c r="C3"/>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
+      <c r="D4"/>
     </row>
     <row r="5">
       <c r="A5"/>
       <c r="B5"/>
       <c r="C5"/>
-      <c r="D5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -1711,12 +1713,12 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
@@ -1725,12 +1727,12 @@
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
@@ -1739,12 +1741,12 @@
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -1753,12 +1755,12 @@
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
@@ -1767,12 +1769,12 @@
         <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
@@ -1781,12 +1783,12 @@
         <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>25</v>
@@ -1795,12 +1797,12 @@
         <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
         <v>27</v>
@@ -1814,7 +1816,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
         <v>30</v>
@@ -1828,7 +1830,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
         <v>33</v>
@@ -1837,12 +1839,12 @@
         <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
         <v>35</v>
@@ -1851,12 +1853,12 @@
         <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
         <v>37</v>
@@ -1865,7 +1867,7 @@
         <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20">
@@ -1873,18 +1875,18 @@
         <v>39</v>
       </c>
       <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
         <v>10</v>
       </c>
-      <c r="C20" t="s">
-        <v>11</v>
-      </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
         <v>13</v>
@@ -1893,12 +1895,12 @@
         <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B22" t="s">
         <v>15</v>
@@ -1907,12 +1909,12 @@
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B23" t="s">
         <v>17</v>
@@ -1921,12 +1923,12 @@
         <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
         <v>40</v>
@@ -1935,12 +1937,12 @@
         <v>41</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B25" t="s">
         <v>42</v>
@@ -1954,7 +1956,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B26" t="s">
         <v>45</v>
@@ -1963,12 +1965,12 @@
         <v>46</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B27" t="s">
         <v>47</v>
@@ -1977,12 +1979,12 @@
         <v>48</v>
       </c>
       <c r="D27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B28" t="s">
         <v>49</v>
@@ -1991,12 +1993,12 @@
         <v>50</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B29" t="s">
         <v>51</v>
@@ -2005,12 +2007,12 @@
         <v>52</v>
       </c>
       <c r="D29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B30" t="s">
         <v>53</v>
@@ -2024,7 +2026,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B31" t="s">
         <v>56</v>
@@ -2033,12 +2035,12 @@
         <v>57</v>
       </c>
       <c r="D31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B32" t="s">
         <v>58</v>
@@ -2047,12 +2049,12 @@
         <v>59</v>
       </c>
       <c r="D32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B33" t="s">
         <v>60</v>
@@ -2066,7 +2068,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B34" t="s">
         <v>62</v>
@@ -2075,12 +2077,12 @@
         <v>63</v>
       </c>
       <c r="D34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B35" t="s">
         <v>64</v>
@@ -2094,7 +2096,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B36" t="s">
         <v>66</v>
@@ -2103,12 +2105,12 @@
         <v>67</v>
       </c>
       <c r="D36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B37" t="s">
         <v>68</v>
@@ -2122,7 +2124,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B38" t="s">
         <v>70</v>
@@ -2131,12 +2133,12 @@
         <v>71</v>
       </c>
       <c r="D38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B39" t="s">
         <v>72</v>
@@ -2150,7 +2152,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B40" t="s">
         <v>74</v>
@@ -2159,12 +2161,12 @@
         <v>36</v>
       </c>
       <c r="D40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B41" t="s">
         <v>75</v>
@@ -2173,7 +2175,7 @@
         <v>38</v>
       </c>
       <c r="D41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42">
@@ -2181,18 +2183,18 @@
         <v>76</v>
       </c>
       <c r="B42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" t="s">
         <v>10</v>
       </c>
-      <c r="C42" t="s">
-        <v>11</v>
-      </c>
       <c r="D42" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B43" t="s">
         <v>13</v>
@@ -2201,12 +2203,12 @@
         <v>14</v>
       </c>
       <c r="D43" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B44" t="s">
         <v>15</v>
@@ -2215,12 +2217,12 @@
         <v>16</v>
       </c>
       <c r="D44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B45" t="s">
         <v>17</v>
@@ -2229,12 +2231,12 @@
         <v>18</v>
       </c>
       <c r="D45" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B46" t="s">
         <v>77</v>
@@ -2243,12 +2245,12 @@
         <v>78</v>
       </c>
       <c r="D46" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B47" t="s">
         <v>79</v>
@@ -2257,12 +2259,12 @@
         <v>80</v>
       </c>
       <c r="D47" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B48" t="s">
         <v>81</v>
@@ -2271,12 +2273,12 @@
         <v>82</v>
       </c>
       <c r="D48" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B49" t="s">
         <v>83</v>
@@ -2285,12 +2287,12 @@
         <v>84</v>
       </c>
       <c r="D49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B50" t="s">
         <v>85</v>
@@ -2299,12 +2301,12 @@
         <v>86</v>
       </c>
       <c r="D50" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B51" t="s">
         <v>87</v>
@@ -2318,7 +2320,7 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B52" t="s">
         <v>89</v>
@@ -2332,7 +2334,7 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B53" t="s">
         <v>90</v>
@@ -2341,12 +2343,12 @@
         <v>63</v>
       </c>
       <c r="D53" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B54" t="s">
         <v>91</v>
@@ -2360,7 +2362,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B55" t="s">
         <v>92</v>
@@ -2369,12 +2371,12 @@
         <v>67</v>
       </c>
       <c r="D55" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B56" t="s">
         <v>93</v>
@@ -2388,7 +2390,7 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B57" t="s">
         <v>94</v>
@@ -2397,12 +2399,12 @@
         <v>95</v>
       </c>
       <c r="D57" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B58" t="s">
         <v>96</v>
@@ -2411,12 +2413,12 @@
         <v>97</v>
       </c>
       <c r="D58" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B59" t="s">
         <v>98</v>
@@ -2425,12 +2427,12 @@
         <v>99</v>
       </c>
       <c r="D59" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B60" t="s">
         <v>100</v>
@@ -2439,12 +2441,12 @@
         <v>101</v>
       </c>
       <c r="D60" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B61" t="s">
         <v>102</v>
@@ -2453,12 +2455,12 @@
         <v>97</v>
       </c>
       <c r="D61" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B62" t="s">
         <v>103</v>
@@ -2467,12 +2469,12 @@
         <v>104</v>
       </c>
       <c r="D62" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B63" t="s">
         <v>105</v>
@@ -2481,12 +2483,12 @@
         <v>106</v>
       </c>
       <c r="D63" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B64" t="s">
         <v>107</v>
@@ -2495,12 +2497,12 @@
         <v>108</v>
       </c>
       <c r="D64" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B65" t="s">
         <v>109</v>
@@ -2509,12 +2511,12 @@
         <v>110</v>
       </c>
       <c r="D65" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B66" t="s">
         <v>111</v>
@@ -2528,7 +2530,7 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B67" t="s">
         <v>113</v>
@@ -2537,12 +2539,12 @@
         <v>114</v>
       </c>
       <c r="D67" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B68" t="s">
         <v>115</v>
@@ -2551,12 +2553,12 @@
         <v>36</v>
       </c>
       <c r="D68" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B69" t="s">
         <v>116</v>
@@ -2565,7 +2567,7 @@
         <v>38</v>
       </c>
       <c r="D69" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70">
@@ -2573,18 +2575,18 @@
         <v>117</v>
       </c>
       <c r="B70" t="s">
+        <v>9</v>
+      </c>
+      <c r="C70" t="s">
         <v>10</v>
       </c>
-      <c r="C70" t="s">
-        <v>11</v>
-      </c>
       <c r="D70" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B71" t="s">
         <v>13</v>
@@ -2593,12 +2595,12 @@
         <v>14</v>
       </c>
       <c r="D71" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B72" t="s">
         <v>15</v>
@@ -2607,12 +2609,12 @@
         <v>16</v>
       </c>
       <c r="D72" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B73" t="s">
         <v>17</v>
@@ -2621,12 +2623,12 @@
         <v>18</v>
       </c>
       <c r="D73" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B74" t="s">
         <v>118</v>
@@ -2635,12 +2637,12 @@
         <v>78</v>
       </c>
       <c r="D74" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B75" t="s">
         <v>119</v>
@@ -2649,12 +2651,12 @@
         <v>80</v>
       </c>
       <c r="D75" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B76" t="s">
         <v>120</v>
@@ -2663,12 +2665,12 @@
         <v>121</v>
       </c>
       <c r="D76" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B77" t="s">
         <v>122</v>
@@ -2677,12 +2679,12 @@
         <v>123</v>
       </c>
       <c r="D77" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B78" t="s">
         <v>124</v>
@@ -2696,7 +2698,7 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B79" t="s">
         <v>126</v>
@@ -2705,12 +2707,12 @@
         <v>127</v>
       </c>
       <c r="D79" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B80" t="s">
         <v>128</v>
@@ -2719,12 +2721,12 @@
         <v>129</v>
       </c>
       <c r="D80" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B81" t="s">
         <v>130</v>
@@ -2733,12 +2735,12 @@
         <v>131</v>
       </c>
       <c r="D81" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B82" t="s">
         <v>132</v>
@@ -2747,12 +2749,12 @@
         <v>133</v>
       </c>
       <c r="D82" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B83" t="s">
         <v>134</v>
@@ -2761,12 +2763,12 @@
         <v>135</v>
       </c>
       <c r="D83" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B84" t="s">
         <v>136</v>
@@ -2775,12 +2777,12 @@
         <v>137</v>
       </c>
       <c r="D84" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B85" t="s">
         <v>138</v>
@@ -2789,12 +2791,12 @@
         <v>139</v>
       </c>
       <c r="D85" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B86" t="s">
         <v>140</v>
@@ -2803,12 +2805,12 @@
         <v>141</v>
       </c>
       <c r="D86" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B87" t="s">
         <v>142</v>
@@ -2817,12 +2819,12 @@
         <v>143</v>
       </c>
       <c r="D87" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B88" t="s">
         <v>144</v>
@@ -2831,12 +2833,12 @@
         <v>145</v>
       </c>
       <c r="D88" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B89" t="s">
         <v>146</v>
@@ -2845,12 +2847,12 @@
         <v>147</v>
       </c>
       <c r="D89" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B90" t="s">
         <v>148</v>
@@ -2859,12 +2861,12 @@
         <v>149</v>
       </c>
       <c r="D90" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B91" t="s">
         <v>150</v>
@@ -2873,12 +2875,12 @@
         <v>151</v>
       </c>
       <c r="D91" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B92" t="s">
         <v>152</v>
@@ -2887,12 +2889,12 @@
         <v>153</v>
       </c>
       <c r="D92" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B93" t="s">
         <v>154</v>
@@ -2901,12 +2903,12 @@
         <v>155</v>
       </c>
       <c r="D93" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B94" t="s">
         <v>156</v>
@@ -2915,12 +2917,12 @@
         <v>157</v>
       </c>
       <c r="D94" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B95" t="s">
         <v>158</v>
@@ -2929,12 +2931,12 @@
         <v>159</v>
       </c>
       <c r="D95" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B96" t="s">
         <v>160</v>
@@ -2943,12 +2945,12 @@
         <v>161</v>
       </c>
       <c r="D96" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B97" t="s">
         <v>162</v>
@@ -2957,12 +2959,12 @@
         <v>163</v>
       </c>
       <c r="D97" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B98" t="s">
         <v>164</v>
@@ -2971,12 +2973,12 @@
         <v>165</v>
       </c>
       <c r="D98" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B99" t="s">
         <v>166</v>
@@ -2985,12 +2987,12 @@
         <v>167</v>
       </c>
       <c r="D99" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B100" t="s">
         <v>168</v>
@@ -2999,12 +3001,12 @@
         <v>169</v>
       </c>
       <c r="D100" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B101" t="s">
         <v>170</v>
@@ -3013,12 +3015,12 @@
         <v>171</v>
       </c>
       <c r="D101" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B102" t="s">
         <v>172</v>
@@ -3027,12 +3029,12 @@
         <v>173</v>
       </c>
       <c r="D102" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B103" t="s">
         <v>174</v>
@@ -3041,12 +3043,12 @@
         <v>175</v>
       </c>
       <c r="D103" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B104" t="s">
         <v>176</v>
@@ -3055,12 +3057,12 @@
         <v>177</v>
       </c>
       <c r="D104" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B105" t="s">
         <v>178</v>
@@ -3069,12 +3071,12 @@
         <v>179</v>
       </c>
       <c r="D105" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B106" t="s">
         <v>180</v>
@@ -3083,12 +3085,12 @@
         <v>181</v>
       </c>
       <c r="D106" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B107" t="s">
         <v>182</v>
@@ -3097,12 +3099,12 @@
         <v>183</v>
       </c>
       <c r="D107" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B108" t="s">
         <v>184</v>
@@ -3111,12 +3113,12 @@
         <v>185</v>
       </c>
       <c r="D108" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B109" t="s">
         <v>186</v>
@@ -3125,12 +3127,12 @@
         <v>187</v>
       </c>
       <c r="D109" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B110" t="s">
         <v>188</v>
@@ -3139,12 +3141,12 @@
         <v>189</v>
       </c>
       <c r="D110" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B111" t="s">
         <v>190</v>
@@ -3153,12 +3155,12 @@
         <v>191</v>
       </c>
       <c r="D111" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B112" t="s">
         <v>192</v>
@@ -3167,12 +3169,12 @@
         <v>193</v>
       </c>
       <c r="D112" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B113" t="s">
         <v>194</v>
@@ -3181,12 +3183,12 @@
         <v>195</v>
       </c>
       <c r="D113" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B114" t="s">
         <v>196</v>
@@ -3195,12 +3197,12 @@
         <v>197</v>
       </c>
       <c r="D114" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B115" t="s">
         <v>198</v>
@@ -3209,12 +3211,12 @@
         <v>199</v>
       </c>
       <c r="D115" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B116" t="s">
         <v>200</v>
@@ -3223,12 +3225,12 @@
         <v>201</v>
       </c>
       <c r="D116" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B117" t="s">
         <v>202</v>
@@ -3237,12 +3239,12 @@
         <v>203</v>
       </c>
       <c r="D117" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B118" t="s">
         <v>204</v>
@@ -3251,12 +3253,12 @@
         <v>205</v>
       </c>
       <c r="D118" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B119" t="s">
         <v>206</v>
@@ -3265,12 +3267,12 @@
         <v>207</v>
       </c>
       <c r="D119" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B120" t="s">
         <v>208</v>
@@ -3279,12 +3281,12 @@
         <v>209</v>
       </c>
       <c r="D120" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B121" t="s">
         <v>210</v>
@@ -3293,12 +3295,12 @@
         <v>209</v>
       </c>
       <c r="D121" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B122" t="s">
         <v>211</v>
@@ -3307,12 +3309,12 @@
         <v>212</v>
       </c>
       <c r="D122" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B123" t="s">
         <v>213</v>
@@ -3321,12 +3323,12 @@
         <v>214</v>
       </c>
       <c r="D123" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B124" t="s">
         <v>215</v>
@@ -3335,12 +3337,12 @@
         <v>216</v>
       </c>
       <c r="D124" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B125" t="s">
         <v>217</v>
@@ -3349,12 +3351,12 @@
         <v>218</v>
       </c>
       <c r="D125" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B126" t="s">
         <v>219</v>
@@ -3363,12 +3365,12 @@
         <v>220</v>
       </c>
       <c r="D126" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B127" t="s">
         <v>221</v>
@@ -3377,12 +3379,12 @@
         <v>222</v>
       </c>
       <c r="D127" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B128" t="s">
         <v>223</v>
@@ -3391,12 +3393,12 @@
         <v>224</v>
       </c>
       <c r="D128" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B129" t="s">
         <v>225</v>
@@ -3405,12 +3407,12 @@
         <v>226</v>
       </c>
       <c r="D129" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B130" t="s">
         <v>227</v>
@@ -3419,12 +3421,12 @@
         <v>228</v>
       </c>
       <c r="D130" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B131" t="s">
         <v>229</v>
@@ -3433,12 +3435,12 @@
         <v>230</v>
       </c>
       <c r="D131" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B132" t="s">
         <v>231</v>
@@ -3447,12 +3449,12 @@
         <v>232</v>
       </c>
       <c r="D132" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B133" t="s">
         <v>233</v>
@@ -3461,12 +3463,12 @@
         <v>234</v>
       </c>
       <c r="D133" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B134" t="s">
         <v>235</v>
@@ -3475,12 +3477,12 @@
         <v>236</v>
       </c>
       <c r="D134" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B135" t="s">
         <v>237</v>
@@ -3489,12 +3491,12 @@
         <v>238</v>
       </c>
       <c r="D135" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B136" t="s">
         <v>239</v>
@@ -3503,12 +3505,12 @@
         <v>240</v>
       </c>
       <c r="D136" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B137" t="s">
         <v>241</v>
@@ -3517,12 +3519,12 @@
         <v>242</v>
       </c>
       <c r="D137" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B138" t="s">
         <v>243</v>
@@ -3531,12 +3533,12 @@
         <v>244</v>
       </c>
       <c r="D138" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B139" t="s">
         <v>245</v>
@@ -3545,12 +3547,12 @@
         <v>246</v>
       </c>
       <c r="D139" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B140" t="s">
         <v>247</v>
@@ -3559,12 +3561,12 @@
         <v>248</v>
       </c>
       <c r="D140" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B141" t="s">
         <v>249</v>
@@ -3573,12 +3575,12 @@
         <v>250</v>
       </c>
       <c r="D141" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B142" t="s">
         <v>251</v>
@@ -3587,12 +3589,12 @@
         <v>252</v>
       </c>
       <c r="D142" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B143" t="s">
         <v>253</v>
@@ -3601,12 +3603,12 @@
         <v>254</v>
       </c>
       <c r="D143" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B144" t="s">
         <v>255</v>
@@ -3615,12 +3617,12 @@
         <v>256</v>
       </c>
       <c r="D144" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B145" t="s">
         <v>257</v>
@@ -3629,12 +3631,12 @@
         <v>258</v>
       </c>
       <c r="D145" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B146" t="s">
         <v>259</v>
@@ -3643,12 +3645,12 @@
         <v>260</v>
       </c>
       <c r="D146" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B147" t="s">
         <v>261</v>
@@ -3657,12 +3659,12 @@
         <v>36</v>
       </c>
       <c r="D147" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B148" t="s">
         <v>262</v>
@@ -3671,7 +3673,7 @@
         <v>38</v>
       </c>
       <c r="D148" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="149">
@@ -3679,18 +3681,18 @@
         <v>263</v>
       </c>
       <c r="B149" t="s">
+        <v>9</v>
+      </c>
+      <c r="C149" t="s">
         <v>10</v>
       </c>
-      <c r="C149" t="s">
-        <v>11</v>
-      </c>
       <c r="D149" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B150" t="s">
         <v>13</v>
@@ -3699,12 +3701,12 @@
         <v>14</v>
       </c>
       <c r="D150" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B151" t="s">
         <v>15</v>
@@ -3713,12 +3715,12 @@
         <v>16</v>
       </c>
       <c r="D151" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B152" t="s">
         <v>17</v>
@@ -3727,12 +3729,12 @@
         <v>18</v>
       </c>
       <c r="D152" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B153" t="s">
         <v>264</v>
@@ -3741,12 +3743,12 @@
         <v>265</v>
       </c>
       <c r="D153" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B154" t="s">
         <v>266</v>
@@ -3755,12 +3757,12 @@
         <v>267</v>
       </c>
       <c r="D154" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B155" t="s">
         <v>268</v>
@@ -3769,12 +3771,12 @@
         <v>269</v>
       </c>
       <c r="D155" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B156" t="s">
         <v>270</v>
@@ -3788,7 +3790,7 @@
     </row>
     <row r="157">
       <c r="A157" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B157" t="s">
         <v>272</v>
@@ -3797,12 +3799,12 @@
         <v>273</v>
       </c>
       <c r="D157" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B158" t="s">
         <v>274</v>
@@ -3811,12 +3813,12 @@
         <v>209</v>
       </c>
       <c r="D158" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B159" t="s">
         <v>275</v>
@@ -3825,12 +3827,12 @@
         <v>209</v>
       </c>
       <c r="D159" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B160" t="s">
         <v>276</v>
@@ -3839,12 +3841,12 @@
         <v>137</v>
       </c>
       <c r="D160" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B161" t="s">
         <v>277</v>
@@ -3853,12 +3855,12 @@
         <v>139</v>
       </c>
       <c r="D161" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B162" t="s">
         <v>278</v>
@@ -3867,12 +3869,12 @@
         <v>212</v>
       </c>
       <c r="D162" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B163" t="s">
         <v>279</v>
@@ -3881,12 +3883,12 @@
         <v>214</v>
       </c>
       <c r="D163" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B164" t="s">
         <v>280</v>
@@ -3895,12 +3897,12 @@
         <v>216</v>
       </c>
       <c r="D164" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B165" t="s">
         <v>281</v>
@@ -3909,12 +3911,12 @@
         <v>282</v>
       </c>
       <c r="D165" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B166" t="s">
         <v>283</v>
@@ -3923,12 +3925,12 @@
         <v>284</v>
       </c>
       <c r="D166" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B167" t="s">
         <v>285</v>
@@ -3937,12 +3939,12 @@
         <v>286</v>
       </c>
       <c r="D167" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B168" t="s">
         <v>287</v>
@@ -3951,12 +3953,12 @@
         <v>288</v>
       </c>
       <c r="D168" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B169" t="s">
         <v>289</v>
@@ -3965,12 +3967,12 @@
         <v>290</v>
       </c>
       <c r="D169" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B170" t="s">
         <v>291</v>
@@ -3979,12 +3981,12 @@
         <v>292</v>
       </c>
       <c r="D170" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B171" t="s">
         <v>293</v>
@@ -3993,12 +3995,12 @@
         <v>294</v>
       </c>
       <c r="D171" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B172" t="s">
         <v>295</v>
@@ -4007,12 +4009,12 @@
         <v>218</v>
       </c>
       <c r="D172" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B173" t="s">
         <v>296</v>
@@ -4021,12 +4023,12 @@
         <v>220</v>
       </c>
       <c r="D173" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B174" t="s">
         <v>297</v>
@@ -4035,12 +4037,12 @@
         <v>222</v>
       </c>
       <c r="D174" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B175" t="s">
         <v>298</v>
@@ -4049,12 +4051,12 @@
         <v>224</v>
       </c>
       <c r="D175" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B176" t="s">
         <v>299</v>
@@ -4063,12 +4065,12 @@
         <v>226</v>
       </c>
       <c r="D176" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B177" t="s">
         <v>300</v>
@@ -4077,12 +4079,12 @@
         <v>228</v>
       </c>
       <c r="D177" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B178" t="s">
         <v>301</v>
@@ -4091,12 +4093,12 @@
         <v>230</v>
       </c>
       <c r="D178" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B179" t="s">
         <v>302</v>
@@ -4105,12 +4107,12 @@
         <v>232</v>
       </c>
       <c r="D179" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B180" t="s">
         <v>303</v>
@@ -4119,12 +4121,12 @@
         <v>234</v>
       </c>
       <c r="D180" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B181" t="s">
         <v>304</v>
@@ -4133,12 +4135,12 @@
         <v>236</v>
       </c>
       <c r="D181" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B182" t="s">
         <v>305</v>
@@ -4147,12 +4149,12 @@
         <v>238</v>
       </c>
       <c r="D182" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B183" t="s">
         <v>306</v>
@@ -4161,12 +4163,12 @@
         <v>240</v>
       </c>
       <c r="D183" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B184" t="s">
         <v>307</v>
@@ -4175,12 +4177,12 @@
         <v>242</v>
       </c>
       <c r="D184" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B185" t="s">
         <v>308</v>
@@ -4189,12 +4191,12 @@
         <v>244</v>
       </c>
       <c r="D185" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B186" t="s">
         <v>309</v>
@@ -4203,12 +4205,12 @@
         <v>246</v>
       </c>
       <c r="D186" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B187" t="s">
         <v>310</v>
@@ -4217,12 +4219,12 @@
         <v>248</v>
       </c>
       <c r="D187" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B188" t="s">
         <v>311</v>
@@ -4231,12 +4233,12 @@
         <v>250</v>
       </c>
       <c r="D188" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B189" t="s">
         <v>312</v>
@@ -4245,12 +4247,12 @@
         <v>252</v>
       </c>
       <c r="D189" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B190" t="s">
         <v>313</v>
@@ -4259,12 +4261,12 @@
         <v>254</v>
       </c>
       <c r="D190" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B191" t="s">
         <v>314</v>
@@ -4278,7 +4280,7 @@
     </row>
     <row r="192">
       <c r="A192" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B192" t="s">
         <v>315</v>
@@ -4287,12 +4289,12 @@
         <v>316</v>
       </c>
       <c r="D192" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B193" t="s">
         <v>317</v>
@@ -4301,12 +4303,12 @@
         <v>318</v>
       </c>
       <c r="D193" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B194" t="s">
         <v>319</v>
@@ -4315,12 +4317,12 @@
         <v>320</v>
       </c>
       <c r="D194" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B195" t="s">
         <v>321</v>
@@ -4329,12 +4331,12 @@
         <v>322</v>
       </c>
       <c r="D195" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B196" t="s">
         <v>323</v>
@@ -4343,12 +4345,12 @@
         <v>282</v>
       </c>
       <c r="D196" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B197" t="s">
         <v>324</v>
@@ -4357,12 +4359,12 @@
         <v>284</v>
       </c>
       <c r="D197" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B198" t="s">
         <v>325</v>
@@ -4371,12 +4373,12 @@
         <v>286</v>
       </c>
       <c r="D198" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B199" t="s">
         <v>326</v>
@@ -4385,12 +4387,12 @@
         <v>288</v>
       </c>
       <c r="D199" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B200" t="s">
         <v>327</v>
@@ -4399,12 +4401,12 @@
         <v>290</v>
       </c>
       <c r="D200" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B201" t="s">
         <v>328</v>
@@ -4413,12 +4415,12 @@
         <v>292</v>
       </c>
       <c r="D201" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B202" t="s">
         <v>329</v>
@@ -4427,12 +4429,12 @@
         <v>294</v>
       </c>
       <c r="D202" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B203" t="s">
         <v>330</v>
@@ -4441,12 +4443,12 @@
         <v>218</v>
       </c>
       <c r="D203" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B204" t="s">
         <v>331</v>
@@ -4455,12 +4457,12 @@
         <v>220</v>
       </c>
       <c r="D204" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B205" t="s">
         <v>332</v>
@@ -4469,12 +4471,12 @@
         <v>222</v>
       </c>
       <c r="D205" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B206" t="s">
         <v>333</v>
@@ -4483,12 +4485,12 @@
         <v>224</v>
       </c>
       <c r="D206" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B207" t="s">
         <v>334</v>
@@ -4497,12 +4499,12 @@
         <v>226</v>
       </c>
       <c r="D207" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B208" t="s">
         <v>335</v>
@@ -4511,12 +4513,12 @@
         <v>228</v>
       </c>
       <c r="D208" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B209" t="s">
         <v>336</v>
@@ -4525,12 +4527,12 @@
         <v>230</v>
       </c>
       <c r="D209" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B210" t="s">
         <v>337</v>
@@ -4539,12 +4541,12 @@
         <v>232</v>
       </c>
       <c r="D210" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B211" t="s">
         <v>338</v>
@@ -4553,12 +4555,12 @@
         <v>234</v>
       </c>
       <c r="D211" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B212" t="s">
         <v>339</v>
@@ -4567,12 +4569,12 @@
         <v>236</v>
       </c>
       <c r="D212" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B213" t="s">
         <v>340</v>
@@ -4581,12 +4583,12 @@
         <v>238</v>
       </c>
       <c r="D213" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B214" t="s">
         <v>341</v>
@@ -4595,12 +4597,12 @@
         <v>240</v>
       </c>
       <c r="D214" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B215" t="s">
         <v>342</v>
@@ -4609,12 +4611,12 @@
         <v>242</v>
       </c>
       <c r="D215" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B216" t="s">
         <v>343</v>
@@ -4623,12 +4625,12 @@
         <v>244</v>
       </c>
       <c r="D216" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B217" t="s">
         <v>344</v>
@@ -4637,12 +4639,12 @@
         <v>246</v>
       </c>
       <c r="D217" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B218" t="s">
         <v>345</v>
@@ -4651,12 +4653,12 @@
         <v>248</v>
       </c>
       <c r="D218" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B219" t="s">
         <v>346</v>
@@ -4665,12 +4667,12 @@
         <v>250</v>
       </c>
       <c r="D219" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B220" t="s">
         <v>347</v>
@@ -4679,12 +4681,12 @@
         <v>252</v>
       </c>
       <c r="D220" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B221" t="s">
         <v>348</v>
@@ -4693,12 +4695,12 @@
         <v>254</v>
       </c>
       <c r="D221" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B222" t="s">
         <v>349</v>
@@ -4707,110 +4709,110 @@
         <v>36</v>
       </c>
       <c r="D222" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B223" t="s">
         <v>350</v>
       </c>
       <c r="C223" t="s">
-        <v>38</v>
+        <v>351</v>
       </c>
       <c r="D223" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="s">
-        <v>351</v>
+        <v>12</v>
       </c>
       <c r="B224" t="s">
-        <v>10</v>
+        <v>352</v>
       </c>
       <c r="C224" t="s">
-        <v>11</v>
+        <v>353</v>
       </c>
       <c r="D224" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B225" t="s">
-        <v>13</v>
+        <v>354</v>
       </c>
       <c r="C225" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="D225" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="s">
-        <v>1</v>
+        <v>355</v>
       </c>
       <c r="B226" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C226" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D226" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B227" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C227" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D227" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B228" t="s">
-        <v>352</v>
+        <v>15</v>
       </c>
       <c r="C228" t="s">
-        <v>353</v>
+        <v>16</v>
       </c>
       <c r="D228" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B229" t="s">
-        <v>354</v>
+        <v>17</v>
       </c>
       <c r="C229" t="s">
-        <v>355</v>
+        <v>18</v>
       </c>
       <c r="D229" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B230" t="s">
         <v>356</v>
@@ -4824,7 +4826,7 @@
     </row>
     <row r="231">
       <c r="A231" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B231" t="s">
         <v>358</v>
@@ -4838,7 +4840,7 @@
     </row>
     <row r="232">
       <c r="A232" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B232" t="s">
         <v>360</v>
@@ -4852,7 +4854,7 @@
     </row>
     <row r="233">
       <c r="A233" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B233" t="s">
         <v>362</v>
@@ -4866,7 +4868,7 @@
     </row>
     <row r="234">
       <c r="A234" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B234" t="s">
         <v>364</v>
@@ -4880,7 +4882,7 @@
     </row>
     <row r="235">
       <c r="A235" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B235" t="s">
         <v>366</v>
@@ -4894,7 +4896,7 @@
     </row>
     <row r="236">
       <c r="A236" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B236" t="s">
         <v>368</v>
@@ -4908,7 +4910,7 @@
     </row>
     <row r="237">
       <c r="A237" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B237" t="s">
         <v>370</v>
@@ -4922,7 +4924,7 @@
     </row>
     <row r="238">
       <c r="A238" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B238" t="s">
         <v>372</v>
@@ -4936,7 +4938,7 @@
     </row>
     <row r="239">
       <c r="A239" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B239" t="s">
         <v>374</v>
@@ -4950,7 +4952,7 @@
     </row>
     <row r="240">
       <c r="A240" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B240" t="s">
         <v>376</v>
@@ -4964,7 +4966,7 @@
     </row>
     <row r="241">
       <c r="A241" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B241" t="s">
         <v>378</v>
@@ -4973,110 +4975,110 @@
         <v>379</v>
       </c>
       <c r="D241" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B242" t="s">
         <v>380</v>
       </c>
       <c r="C242" t="s">
-        <v>38</v>
+        <v>381</v>
       </c>
       <c r="D242" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="s">
-        <v>381</v>
+        <v>12</v>
       </c>
       <c r="B243" t="s">
-        <v>10</v>
+        <v>382</v>
       </c>
       <c r="C243" t="s">
-        <v>11</v>
+        <v>383</v>
       </c>
       <c r="D243" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B244" t="s">
-        <v>13</v>
+        <v>384</v>
       </c>
       <c r="C244" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="D244" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="s">
-        <v>1</v>
+        <v>385</v>
       </c>
       <c r="B245" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C245" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D245" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B246" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C246" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D246" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B247" t="s">
-        <v>382</v>
+        <v>15</v>
       </c>
       <c r="C247" t="s">
-        <v>383</v>
+        <v>16</v>
       </c>
       <c r="D247" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B248" t="s">
-        <v>384</v>
+        <v>17</v>
       </c>
       <c r="C248" t="s">
-        <v>385</v>
+        <v>18</v>
       </c>
       <c r="D248" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B249" t="s">
         <v>386</v>
@@ -5090,7 +5092,7 @@
     </row>
     <row r="250">
       <c r="A250" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B250" t="s">
         <v>388</v>
@@ -5104,7 +5106,7 @@
     </row>
     <row r="251">
       <c r="A251" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B251" t="s">
         <v>390</v>
@@ -5118,7 +5120,7 @@
     </row>
     <row r="252">
       <c r="A252" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B252" t="s">
         <v>392</v>
@@ -5132,7 +5134,7 @@
     </row>
     <row r="253">
       <c r="A253" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B253" t="s">
         <v>394</v>
@@ -5146,7 +5148,7 @@
     </row>
     <row r="254">
       <c r="A254" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B254" t="s">
         <v>396</v>
@@ -5160,7 +5162,7 @@
     </row>
     <row r="255">
       <c r="A255" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B255" t="s">
         <v>398</v>
@@ -5174,7 +5176,7 @@
     </row>
     <row r="256">
       <c r="A256" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B256" t="s">
         <v>400</v>
@@ -5188,7 +5190,7 @@
     </row>
     <row r="257">
       <c r="A257" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B257" t="s">
         <v>402</v>
@@ -5202,7 +5204,7 @@
     </row>
     <row r="258">
       <c r="A258" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B258" t="s">
         <v>404</v>
@@ -5216,7 +5218,7 @@
     </row>
     <row r="259">
       <c r="A259" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B259" t="s">
         <v>406</v>
@@ -5230,7 +5232,7 @@
     </row>
     <row r="260">
       <c r="A260" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B260" t="s">
         <v>408</v>
@@ -5244,7 +5246,7 @@
     </row>
     <row r="261">
       <c r="A261" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B261" t="s">
         <v>410</v>
@@ -5258,7 +5260,7 @@
     </row>
     <row r="262">
       <c r="A262" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B262" t="s">
         <v>412</v>
@@ -5272,7 +5274,7 @@
     </row>
     <row r="263">
       <c r="A263" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B263" t="s">
         <v>414</v>
@@ -5286,7 +5288,7 @@
     </row>
     <row r="264">
       <c r="A264" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B264" t="s">
         <v>416</v>
@@ -5300,7 +5302,7 @@
     </row>
     <row r="265">
       <c r="A265" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B265" t="s">
         <v>418</v>
@@ -5314,7 +5316,7 @@
     </row>
     <row r="266">
       <c r="A266" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B266" t="s">
         <v>420</v>
@@ -5328,7 +5330,7 @@
     </row>
     <row r="267">
       <c r="A267" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B267" t="s">
         <v>422</v>
@@ -5342,7 +5344,7 @@
     </row>
     <row r="268">
       <c r="A268" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B268" t="s">
         <v>424</v>
@@ -5356,16 +5358,44 @@
     </row>
     <row r="269">
       <c r="A269" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B269" t="s">
         <v>426</v>
       </c>
       <c r="C269" t="s">
+        <v>427</v>
+      </c>
+      <c r="D269" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="s">
+        <v>12</v>
+      </c>
+      <c r="B270" t="s">
+        <v>428</v>
+      </c>
+      <c r="C270" t="s">
+        <v>429</v>
+      </c>
+      <c r="D270" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="s">
+        <v>12</v>
+      </c>
+      <c r="B271" t="s">
+        <v>430</v>
+      </c>
+      <c r="C271" t="s">
         <v>38</v>
       </c>
-      <c r="D269" t="s">
-        <v>12</v>
+      <c r="D271" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Frontend TableDescription and SQL scripts
</commit_message>
<xml_diff>
--- a/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
+++ b/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="433">
   <si>
     <t xml:space="preserve">Hint</t>
   </si>
@@ -71,6 +71,12 @@
     <t xml:space="preserve">Function as dataset filter by stations</t>
   </si>
   <si>
+    <t xml:space="preserve">projekt_versionsnummer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Versionsnummer zum Matching von REDCap-Projektversion mit weiteren Versionselementen der Toolchain</t>
+  </si>
+  <si>
     <t xml:space="preserve">pat_id</t>
   </si>
   <si>
@@ -134,6 +140,12 @@
     <t xml:space="preserve">fall</t>
   </si>
   <si>
+    <t xml:space="preserve">db_filter_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dashboard Filter 8</t>
+  </si>
+  <si>
     <t xml:space="preserve">fall_fhir_enc_id</t>
   </si>
   <si>
@@ -245,6 +257,18 @@
     <t xml:space="preserve">medikationsanalyse</t>
   </si>
   <si>
+    <t xml:space="preserve">db_filter_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dashboard Filter 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db_filter_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dashboard Filter 7</t>
+  </si>
+  <si>
     <t xml:space="preserve">meda_anlage</t>
   </si>
   <si>
@@ -260,7 +284,7 @@
     <t xml:space="preserve">fall_meda_id</t>
   </si>
   <si>
-    <t xml:space="preserve">Dynamische SQL-Abfrage zur Zuordnung Medikationsanalyse zu Fall (Fall-ID Encounter-Identifier (KIS)) Auswahlfeld falls die aktuell dokumentierte Medikationsanalyse sich nicht auf die letzte Instanz des Falls bezieht.  </t>
+    <t xml:space="preserve">1 Dynamische SQL-Abfrage zur Zuordnung Medikationsanalyse zu Fall (Fall-ID Encounter-Identifier (KIS)) Auswahlfeld falls die aktuell dokumentierte Medikationsanalyse sich nicht auf die letzte Instanz des Falls bezieht.  </t>
   </si>
   <si>
     <t xml:space="preserve">meda_id</t>
@@ -368,6 +392,12 @@
     <t xml:space="preserve">mrpdokumentation_validierung</t>
   </si>
   <si>
+    <t xml:space="preserve">db_filter_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dashboard Filter 6</t>
+  </si>
+  <si>
     <t xml:space="preserve">mrp_anlage</t>
   </si>
   <si>
@@ -377,7 +407,7 @@
     <t xml:space="preserve">mrp_meda_id</t>
   </si>
   <si>
-    <t xml:space="preserve">Dynamische SQL-Abfrage zur Zuordnung Medikationsanalyse zu MRP   Auswahlfeld falls die aktuell dokumentiertes MRP  sich nicht auf die letzte Instanz der Medikationsanalyse bezieht.  </t>
+    <t xml:space="preserve">2 Dynamische SQL-Abfrage zur Zuordnung Medikationsanalyse zu MRP   Auswahlfeld falls die aktuell dokumentiertes MRP  sich nicht auf die letzte Instanz der Medikationsanalyse bezieht.  </t>
   </si>
   <si>
     <t xml:space="preserve">mrp_id</t>
@@ -965,21 +995,9 @@
     <t xml:space="preserve">1 - 2nd Look / Zweite MRP-Bewertung durchführen</t>
   </si>
   <si>
-    <t xml:space="preserve">ret_bewerter2_pipeline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bewerter2 Pipeline</t>
-  </si>
-  <si>
     <t xml:space="preserve">ret_bewerter2</t>
   </si>
   <si>
-    <t xml:space="preserve">2. Bewertung von  @DEFAULT = @SETVALUE = ret_bewerter2_pipeline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_bewerter3</t>
-  </si>
-  <si>
     <t xml:space="preserve">2. Bewertung von</t>
   </si>
   <si>
@@ -1062,18 +1080,6 @@
   </si>
   <si>
     <t xml:space="preserve">ret_additional_values</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db_ret_main_enc_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FHIR ID of the main Encounter to which this evaluation belongs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db_ret_medical_case_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HIS internal Identifier of the medical case to which this evaluation belongs</t>
   </si>
   <si>
     <t xml:space="preserve">retrolektive_mrpbewertung_complete</t>
@@ -1811,7 +1817,7 @@
         <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16">
@@ -1819,13 +1825,13 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
         <v>30</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>31</v>
-      </c>
-      <c r="D16" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="17">
@@ -1833,13 +1839,13 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
         <v>33</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>34</v>
-      </c>
-      <c r="D17" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="18">
@@ -1872,13 +1878,13 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
         <v>39</v>
       </c>
-      <c r="B20" t="s">
-        <v>9</v>
-      </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
@@ -1886,13 +1892,13 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
@@ -1903,10 +1909,10 @@
         <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
@@ -1917,10 +1923,10 @@
         <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D23" t="s">
         <v>11</v>
@@ -1931,10 +1937,10 @@
         <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
@@ -1951,7 +1957,7 @@
         <v>43</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26">
@@ -1959,10 +1965,10 @@
         <v>12</v>
       </c>
       <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" t="s">
         <v>45</v>
-      </c>
-      <c r="C26" t="s">
-        <v>46</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -1973,13 +1979,13 @@
         <v>12</v>
       </c>
       <c r="B27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" t="s">
         <v>47</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>48</v>
-      </c>
-      <c r="D27" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="28">
@@ -2021,7 +2027,7 @@
         <v>54</v>
       </c>
       <c r="D30" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31">
@@ -2029,10 +2035,10 @@
         <v>12</v>
       </c>
       <c r="B31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" t="s">
         <v>56</v>
-      </c>
-      <c r="C31" t="s">
-        <v>57</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -2043,13 +2049,13 @@
         <v>12</v>
       </c>
       <c r="B32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" t="s">
         <v>58</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>59</v>
-      </c>
-      <c r="D32" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="33">
@@ -2063,7 +2069,7 @@
         <v>61</v>
       </c>
       <c r="D33" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34">
@@ -2091,7 +2097,7 @@
         <v>65</v>
       </c>
       <c r="D35" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36">
@@ -2119,7 +2125,7 @@
         <v>69</v>
       </c>
       <c r="D37" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38">
@@ -2147,7 +2153,7 @@
         <v>73</v>
       </c>
       <c r="D39" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40">
@@ -2158,7 +2164,7 @@
         <v>74</v>
       </c>
       <c r="C40" t="s">
-        <v>36</v>
+        <v>75</v>
       </c>
       <c r="D40" t="s">
         <v>11</v>
@@ -2169,24 +2175,24 @@
         <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C41" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="D41" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="B42" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="D42" t="s">
         <v>11</v>
@@ -2197,10 +2203,10 @@
         <v>12</v>
       </c>
       <c r="B43" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="C43" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
@@ -2208,13 +2214,13 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="B44" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
@@ -2225,10 +2231,10 @@
         <v>12</v>
       </c>
       <c r="B45" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C45" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D45" t="s">
         <v>11</v>
@@ -2239,10 +2245,10 @@
         <v>12</v>
       </c>
       <c r="B46" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
+        <v>16</v>
       </c>
       <c r="D46" t="s">
         <v>11</v>
@@ -2253,10 +2259,10 @@
         <v>12</v>
       </c>
       <c r="B47" t="s">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="C47" t="s">
-        <v>80</v>
+        <v>18</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
@@ -2273,7 +2279,7 @@
         <v>82</v>
       </c>
       <c r="D48" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49">
@@ -2287,7 +2293,7 @@
         <v>84</v>
       </c>
       <c r="D49" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50">
@@ -2315,7 +2321,7 @@
         <v>88</v>
       </c>
       <c r="D51" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52">
@@ -2326,10 +2332,10 @@
         <v>89</v>
       </c>
       <c r="C52" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="D52" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53">
@@ -2337,10 +2343,10 @@
         <v>12</v>
       </c>
       <c r="B53" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C53" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="D53" t="s">
         <v>11</v>
@@ -2351,13 +2357,13 @@
         <v>12</v>
       </c>
       <c r="B54" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C54" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="D54" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="55">
@@ -2365,13 +2371,13 @@
         <v>12</v>
       </c>
       <c r="B55" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C55" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="D55" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56">
@@ -2379,13 +2385,13 @@
         <v>12</v>
       </c>
       <c r="B56" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C56" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D56" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="57">
@@ -2393,10 +2399,10 @@
         <v>12</v>
       </c>
       <c r="B57" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C57" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="D57" t="s">
         <v>11</v>
@@ -2407,13 +2413,13 @@
         <v>12</v>
       </c>
       <c r="B58" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C58" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="D58" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
     </row>
     <row r="59">
@@ -2421,10 +2427,10 @@
         <v>12</v>
       </c>
       <c r="B59" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C59" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="D59" t="s">
         <v>11</v>
@@ -2435,13 +2441,13 @@
         <v>12</v>
       </c>
       <c r="B60" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C60" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="D60" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
     </row>
     <row r="61">
@@ -2452,7 +2458,7 @@
         <v>102</v>
       </c>
       <c r="C61" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D61" t="s">
         <v>11</v>
@@ -2463,10 +2469,10 @@
         <v>12</v>
       </c>
       <c r="B62" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C62" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D62" t="s">
         <v>11</v>
@@ -2477,10 +2483,10 @@
         <v>12</v>
       </c>
       <c r="B63" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C63" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D63" t="s">
         <v>11</v>
@@ -2491,10 +2497,10 @@
         <v>12</v>
       </c>
       <c r="B64" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C64" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D64" t="s">
         <v>11</v>
@@ -2505,10 +2511,10 @@
         <v>12</v>
       </c>
       <c r="B65" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C65" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D65" t="s">
         <v>11</v>
@@ -2525,7 +2531,7 @@
         <v>112</v>
       </c>
       <c r="D66" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67">
@@ -2550,7 +2556,7 @@
         <v>115</v>
       </c>
       <c r="C68" t="s">
-        <v>36</v>
+        <v>116</v>
       </c>
       <c r="D68" t="s">
         <v>11</v>
@@ -2561,10 +2567,10 @@
         <v>12</v>
       </c>
       <c r="B69" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C69" t="s">
-        <v>38</v>
+        <v>118</v>
       </c>
       <c r="D69" t="s">
         <v>11</v>
@@ -2572,16 +2578,16 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>117</v>
+        <v>12</v>
       </c>
       <c r="B70" t="s">
-        <v>9</v>
+        <v>119</v>
       </c>
       <c r="C70" t="s">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="D70" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
     </row>
     <row r="71">
@@ -2589,10 +2595,10 @@
         <v>12</v>
       </c>
       <c r="B71" t="s">
-        <v>13</v>
+        <v>121</v>
       </c>
       <c r="C71" t="s">
-        <v>14</v>
+        <v>122</v>
       </c>
       <c r="D71" t="s">
         <v>11</v>
@@ -2603,10 +2609,10 @@
         <v>12</v>
       </c>
       <c r="B72" t="s">
-        <v>15</v>
+        <v>123</v>
       </c>
       <c r="C72" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="D72" t="s">
         <v>11</v>
@@ -2617,10 +2623,10 @@
         <v>12</v>
       </c>
       <c r="B73" t="s">
-        <v>17</v>
+        <v>124</v>
       </c>
       <c r="C73" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="D73" t="s">
         <v>11</v>
@@ -2628,13 +2634,13 @@
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>12</v>
+        <v>125</v>
       </c>
       <c r="B74" t="s">
-        <v>118</v>
+        <v>9</v>
       </c>
       <c r="C74" t="s">
-        <v>78</v>
+        <v>10</v>
       </c>
       <c r="D74" t="s">
         <v>11</v>
@@ -2645,10 +2651,10 @@
         <v>12</v>
       </c>
       <c r="B75" t="s">
-        <v>119</v>
+        <v>13</v>
       </c>
       <c r="C75" t="s">
-        <v>80</v>
+        <v>14</v>
       </c>
       <c r="D75" t="s">
         <v>11</v>
@@ -2659,10 +2665,10 @@
         <v>12</v>
       </c>
       <c r="B76" t="s">
-        <v>120</v>
+        <v>15</v>
       </c>
       <c r="C76" t="s">
-        <v>121</v>
+        <v>16</v>
       </c>
       <c r="D76" t="s">
         <v>11</v>
@@ -2673,10 +2679,10 @@
         <v>12</v>
       </c>
       <c r="B77" t="s">
-        <v>122</v>
+        <v>17</v>
       </c>
       <c r="C77" t="s">
-        <v>123</v>
+        <v>18</v>
       </c>
       <c r="D77" t="s">
         <v>11</v>
@@ -2687,13 +2693,13 @@
         <v>12</v>
       </c>
       <c r="B78" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C78" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D78" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
     </row>
     <row r="79">
@@ -2701,10 +2707,10 @@
         <v>12</v>
       </c>
       <c r="B79" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C79" t="s">
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="D79" t="s">
         <v>11</v>
@@ -2715,10 +2721,10 @@
         <v>12</v>
       </c>
       <c r="B80" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C80" t="s">
-        <v>129</v>
+        <v>88</v>
       </c>
       <c r="D80" t="s">
         <v>11</v>
@@ -2763,7 +2769,7 @@
         <v>135</v>
       </c>
       <c r="D83" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
     </row>
     <row r="84">
@@ -3292,7 +3298,7 @@
         <v>210</v>
       </c>
       <c r="C121" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D121" t="s">
         <v>11</v>
@@ -3303,10 +3309,10 @@
         <v>12</v>
       </c>
       <c r="B122" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C122" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D122" t="s">
         <v>11</v>
@@ -3317,10 +3323,10 @@
         <v>12</v>
       </c>
       <c r="B123" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C123" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D123" t="s">
         <v>11</v>
@@ -3331,10 +3337,10 @@
         <v>12</v>
       </c>
       <c r="B124" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C124" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D124" t="s">
         <v>11</v>
@@ -3345,10 +3351,10 @@
         <v>12</v>
       </c>
       <c r="B125" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C125" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D125" t="s">
         <v>11</v>
@@ -3359,10 +3365,10 @@
         <v>12</v>
       </c>
       <c r="B126" t="s">
+        <v>220</v>
+      </c>
+      <c r="C126" t="s">
         <v>219</v>
-      </c>
-      <c r="C126" t="s">
-        <v>220</v>
       </c>
       <c r="D126" t="s">
         <v>11</v>
@@ -3656,7 +3662,7 @@
         <v>261</v>
       </c>
       <c r="C147" t="s">
-        <v>36</v>
+        <v>262</v>
       </c>
       <c r="D147" t="s">
         <v>11</v>
@@ -3667,10 +3673,10 @@
         <v>12</v>
       </c>
       <c r="B148" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C148" t="s">
-        <v>38</v>
+        <v>264</v>
       </c>
       <c r="D148" t="s">
         <v>11</v>
@@ -3678,13 +3684,13 @@
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>263</v>
+        <v>12</v>
       </c>
       <c r="B149" t="s">
-        <v>9</v>
+        <v>265</v>
       </c>
       <c r="C149" t="s">
-        <v>10</v>
+        <v>266</v>
       </c>
       <c r="D149" t="s">
         <v>11</v>
@@ -3695,10 +3701,10 @@
         <v>12</v>
       </c>
       <c r="B150" t="s">
-        <v>13</v>
+        <v>267</v>
       </c>
       <c r="C150" t="s">
-        <v>14</v>
+        <v>268</v>
       </c>
       <c r="D150" t="s">
         <v>11</v>
@@ -3709,10 +3715,10 @@
         <v>12</v>
       </c>
       <c r="B151" t="s">
-        <v>15</v>
+        <v>269</v>
       </c>
       <c r="C151" t="s">
-        <v>16</v>
+        <v>270</v>
       </c>
       <c r="D151" t="s">
         <v>11</v>
@@ -3723,10 +3729,10 @@
         <v>12</v>
       </c>
       <c r="B152" t="s">
-        <v>17</v>
+        <v>271</v>
       </c>
       <c r="C152" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="D152" t="s">
         <v>11</v>
@@ -3737,10 +3743,10 @@
         <v>12</v>
       </c>
       <c r="B153" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="C153" t="s">
-        <v>265</v>
+        <v>40</v>
       </c>
       <c r="D153" t="s">
         <v>11</v>
@@ -3748,13 +3754,13 @@
     </row>
     <row r="154">
       <c r="A154" t="s">
-        <v>12</v>
+        <v>273</v>
       </c>
       <c r="B154" t="s">
-        <v>266</v>
+        <v>9</v>
       </c>
       <c r="C154" t="s">
-        <v>267</v>
+        <v>10</v>
       </c>
       <c r="D154" t="s">
         <v>11</v>
@@ -3765,10 +3771,10 @@
         <v>12</v>
       </c>
       <c r="B155" t="s">
-        <v>268</v>
+        <v>13</v>
       </c>
       <c r="C155" t="s">
-        <v>269</v>
+        <v>14</v>
       </c>
       <c r="D155" t="s">
         <v>11</v>
@@ -3779,13 +3785,13 @@
         <v>12</v>
       </c>
       <c r="B156" t="s">
-        <v>270</v>
+        <v>15</v>
       </c>
       <c r="C156" t="s">
-        <v>271</v>
+        <v>16</v>
       </c>
       <c r="D156" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
     </row>
     <row r="157">
@@ -3793,10 +3799,10 @@
         <v>12</v>
       </c>
       <c r="B157" t="s">
-        <v>272</v>
+        <v>17</v>
       </c>
       <c r="C157" t="s">
-        <v>273</v>
+        <v>18</v>
       </c>
       <c r="D157" t="s">
         <v>11</v>
@@ -3810,7 +3816,7 @@
         <v>274</v>
       </c>
       <c r="C158" t="s">
-        <v>209</v>
+        <v>275</v>
       </c>
       <c r="D158" t="s">
         <v>11</v>
@@ -3821,10 +3827,10 @@
         <v>12</v>
       </c>
       <c r="B159" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C159" t="s">
-        <v>209</v>
+        <v>277</v>
       </c>
       <c r="D159" t="s">
         <v>11</v>
@@ -3835,10 +3841,10 @@
         <v>12</v>
       </c>
       <c r="B160" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C160" t="s">
-        <v>137</v>
+        <v>279</v>
       </c>
       <c r="D160" t="s">
         <v>11</v>
@@ -3849,13 +3855,13 @@
         <v>12</v>
       </c>
       <c r="B161" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C161" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="D161" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
     </row>
     <row r="162">
@@ -3863,10 +3869,10 @@
         <v>12</v>
       </c>
       <c r="B162" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="C162" t="s">
-        <v>212</v>
+        <v>283</v>
       </c>
       <c r="D162" t="s">
         <v>11</v>
@@ -3877,10 +3883,10 @@
         <v>12</v>
       </c>
       <c r="B163" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="C163" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="D163" t="s">
         <v>11</v>
@@ -3891,10 +3897,10 @@
         <v>12</v>
       </c>
       <c r="B164" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="C164" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D164" t="s">
         <v>11</v>
@@ -3905,10 +3911,10 @@
         <v>12</v>
       </c>
       <c r="B165" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="C165" t="s">
-        <v>282</v>
+        <v>147</v>
       </c>
       <c r="D165" t="s">
         <v>11</v>
@@ -3919,10 +3925,10 @@
         <v>12</v>
       </c>
       <c r="B166" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="C166" t="s">
-        <v>284</v>
+        <v>149</v>
       </c>
       <c r="D166" t="s">
         <v>11</v>
@@ -3933,10 +3939,10 @@
         <v>12</v>
       </c>
       <c r="B167" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C167" t="s">
-        <v>286</v>
+        <v>222</v>
       </c>
       <c r="D167" t="s">
         <v>11</v>
@@ -3947,10 +3953,10 @@
         <v>12</v>
       </c>
       <c r="B168" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C168" t="s">
-        <v>288</v>
+        <v>224</v>
       </c>
       <c r="D168" t="s">
         <v>11</v>
@@ -3961,10 +3967,10 @@
         <v>12</v>
       </c>
       <c r="B169" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C169" t="s">
-        <v>290</v>
+        <v>226</v>
       </c>
       <c r="D169" t="s">
         <v>11</v>
@@ -4006,7 +4012,7 @@
         <v>295</v>
       </c>
       <c r="C172" t="s">
-        <v>218</v>
+        <v>296</v>
       </c>
       <c r="D172" t="s">
         <v>11</v>
@@ -4017,10 +4023,10 @@
         <v>12</v>
       </c>
       <c r="B173" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C173" t="s">
-        <v>220</v>
+        <v>298</v>
       </c>
       <c r="D173" t="s">
         <v>11</v>
@@ -4031,10 +4037,10 @@
         <v>12</v>
       </c>
       <c r="B174" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C174" t="s">
-        <v>222</v>
+        <v>300</v>
       </c>
       <c r="D174" t="s">
         <v>11</v>
@@ -4045,10 +4051,10 @@
         <v>12</v>
       </c>
       <c r="B175" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="C175" t="s">
-        <v>224</v>
+        <v>302</v>
       </c>
       <c r="D175" t="s">
         <v>11</v>
@@ -4059,10 +4065,10 @@
         <v>12</v>
       </c>
       <c r="B176" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="C176" t="s">
-        <v>226</v>
+        <v>304</v>
       </c>
       <c r="D176" t="s">
         <v>11</v>
@@ -4073,7 +4079,7 @@
         <v>12</v>
       </c>
       <c r="B177" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C177" t="s">
         <v>228</v>
@@ -4087,7 +4093,7 @@
         <v>12</v>
       </c>
       <c r="B178" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="C178" t="s">
         <v>230</v>
@@ -4101,7 +4107,7 @@
         <v>12</v>
       </c>
       <c r="B179" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="C179" t="s">
         <v>232</v>
@@ -4115,7 +4121,7 @@
         <v>12</v>
       </c>
       <c r="B180" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="C180" t="s">
         <v>234</v>
@@ -4129,7 +4135,7 @@
         <v>12</v>
       </c>
       <c r="B181" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="C181" t="s">
         <v>236</v>
@@ -4143,7 +4149,7 @@
         <v>12</v>
       </c>
       <c r="B182" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="C182" t="s">
         <v>238</v>
@@ -4157,7 +4163,7 @@
         <v>12</v>
       </c>
       <c r="B183" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="C183" t="s">
         <v>240</v>
@@ -4171,7 +4177,7 @@
         <v>12</v>
       </c>
       <c r="B184" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="C184" t="s">
         <v>242</v>
@@ -4185,7 +4191,7 @@
         <v>12</v>
       </c>
       <c r="B185" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="C185" t="s">
         <v>244</v>
@@ -4199,7 +4205,7 @@
         <v>12</v>
       </c>
       <c r="B186" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="C186" t="s">
         <v>246</v>
@@ -4213,7 +4219,7 @@
         <v>12</v>
       </c>
       <c r="B187" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="C187" t="s">
         <v>248</v>
@@ -4227,7 +4233,7 @@
         <v>12</v>
       </c>
       <c r="B188" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="C188" t="s">
         <v>250</v>
@@ -4241,7 +4247,7 @@
         <v>12</v>
       </c>
       <c r="B189" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="C189" t="s">
         <v>252</v>
@@ -4255,7 +4261,7 @@
         <v>12</v>
       </c>
       <c r="B190" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="C190" t="s">
         <v>254</v>
@@ -4269,13 +4275,13 @@
         <v>12</v>
       </c>
       <c r="B191" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="C191" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="D191" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
     </row>
     <row r="192">
@@ -4283,10 +4289,10 @@
         <v>12</v>
       </c>
       <c r="B192" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="C192" t="s">
-        <v>316</v>
+        <v>258</v>
       </c>
       <c r="D192" t="s">
         <v>11</v>
@@ -4297,10 +4303,10 @@
         <v>12</v>
       </c>
       <c r="B193" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="C193" t="s">
-        <v>318</v>
+        <v>260</v>
       </c>
       <c r="D193" t="s">
         <v>11</v>
@@ -4311,10 +4317,10 @@
         <v>12</v>
       </c>
       <c r="B194" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="C194" t="s">
-        <v>320</v>
+        <v>262</v>
       </c>
       <c r="D194" t="s">
         <v>11</v>
@@ -4325,10 +4331,10 @@
         <v>12</v>
       </c>
       <c r="B195" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C195" t="s">
-        <v>322</v>
+        <v>264</v>
       </c>
       <c r="D195" t="s">
         <v>11</v>
@@ -4339,13 +4345,13 @@
         <v>12</v>
       </c>
       <c r="B196" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C196" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D196" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
     </row>
     <row r="197">
@@ -4353,10 +4359,10 @@
         <v>12</v>
       </c>
       <c r="B197" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C197" t="s">
-        <v>284</v>
+        <v>326</v>
       </c>
       <c r="D197" t="s">
         <v>11</v>
@@ -4367,10 +4373,10 @@
         <v>12</v>
       </c>
       <c r="B198" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C198" t="s">
-        <v>286</v>
+        <v>328</v>
       </c>
       <c r="D198" t="s">
         <v>11</v>
@@ -4381,10 +4387,10 @@
         <v>12</v>
       </c>
       <c r="B199" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="C199" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="D199" t="s">
         <v>11</v>
@@ -4395,10 +4401,10 @@
         <v>12</v>
       </c>
       <c r="B200" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="C200" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="D200" t="s">
         <v>11</v>
@@ -4409,10 +4415,10 @@
         <v>12</v>
       </c>
       <c r="B201" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="C201" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="D201" t="s">
         <v>11</v>
@@ -4423,10 +4429,10 @@
         <v>12</v>
       </c>
       <c r="B202" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="C202" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="D202" t="s">
         <v>11</v>
@@ -4437,10 +4443,10 @@
         <v>12</v>
       </c>
       <c r="B203" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="C203" t="s">
-        <v>218</v>
+        <v>300</v>
       </c>
       <c r="D203" t="s">
         <v>11</v>
@@ -4451,10 +4457,10 @@
         <v>12</v>
       </c>
       <c r="B204" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="C204" t="s">
-        <v>220</v>
+        <v>302</v>
       </c>
       <c r="D204" t="s">
         <v>11</v>
@@ -4465,10 +4471,10 @@
         <v>12</v>
       </c>
       <c r="B205" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C205" t="s">
-        <v>222</v>
+        <v>304</v>
       </c>
       <c r="D205" t="s">
         <v>11</v>
@@ -4479,10 +4485,10 @@
         <v>12</v>
       </c>
       <c r="B206" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="C206" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="D206" t="s">
         <v>11</v>
@@ -4493,10 +4499,10 @@
         <v>12</v>
       </c>
       <c r="B207" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="C207" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="D207" t="s">
         <v>11</v>
@@ -4507,10 +4513,10 @@
         <v>12</v>
       </c>
       <c r="B208" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="C208" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="D208" t="s">
         <v>11</v>
@@ -4521,10 +4527,10 @@
         <v>12</v>
       </c>
       <c r="B209" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="C209" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="D209" t="s">
         <v>11</v>
@@ -4535,10 +4541,10 @@
         <v>12</v>
       </c>
       <c r="B210" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="C210" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="D210" t="s">
         <v>11</v>
@@ -4549,10 +4555,10 @@
         <v>12</v>
       </c>
       <c r="B211" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="C211" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D211" t="s">
         <v>11</v>
@@ -4563,10 +4569,10 @@
         <v>12</v>
       </c>
       <c r="B212" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="C212" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="D212" t="s">
         <v>11</v>
@@ -4577,10 +4583,10 @@
         <v>12</v>
       </c>
       <c r="B213" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="C213" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="D213" t="s">
         <v>11</v>
@@ -4591,10 +4597,10 @@
         <v>12</v>
       </c>
       <c r="B214" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="C214" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="D214" t="s">
         <v>11</v>
@@ -4605,10 +4611,10 @@
         <v>12</v>
       </c>
       <c r="B215" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="C215" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="D215" t="s">
         <v>11</v>
@@ -4619,10 +4625,10 @@
         <v>12</v>
       </c>
       <c r="B216" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C216" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D216" t="s">
         <v>11</v>
@@ -4633,10 +4639,10 @@
         <v>12</v>
       </c>
       <c r="B217" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="C217" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="D217" t="s">
         <v>11</v>
@@ -4647,10 +4653,10 @@
         <v>12</v>
       </c>
       <c r="B218" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="C218" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="D218" t="s">
         <v>11</v>
@@ -4661,10 +4667,10 @@
         <v>12</v>
       </c>
       <c r="B219" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C219" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="D219" t="s">
         <v>11</v>
@@ -4675,10 +4681,10 @@
         <v>12</v>
       </c>
       <c r="B220" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="C220" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="D220" t="s">
         <v>11</v>
@@ -4689,10 +4695,10 @@
         <v>12</v>
       </c>
       <c r="B221" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="C221" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="D221" t="s">
         <v>11</v>
@@ -4703,10 +4709,10 @@
         <v>12</v>
       </c>
       <c r="B222" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C222" t="s">
-        <v>36</v>
+        <v>260</v>
       </c>
       <c r="D222" t="s">
         <v>11</v>
@@ -4717,10 +4723,10 @@
         <v>12</v>
       </c>
       <c r="B223" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="C223" t="s">
-        <v>351</v>
+        <v>262</v>
       </c>
       <c r="D223" t="s">
         <v>11</v>
@@ -4731,10 +4737,10 @@
         <v>12</v>
       </c>
       <c r="B224" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C224" t="s">
-        <v>353</v>
+        <v>264</v>
       </c>
       <c r="D224" t="s">
         <v>11</v>
@@ -4745,7 +4751,7 @@
         <v>12</v>
       </c>
       <c r="B225" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C225" t="s">
         <v>38</v>
@@ -4756,13 +4762,13 @@
     </row>
     <row r="226">
       <c r="A226" t="s">
-        <v>355</v>
+        <v>12</v>
       </c>
       <c r="B226" t="s">
-        <v>9</v>
+        <v>356</v>
       </c>
       <c r="C226" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D226" t="s">
         <v>11</v>
@@ -4770,13 +4776,13 @@
     </row>
     <row r="227">
       <c r="A227" t="s">
-        <v>12</v>
+        <v>357</v>
       </c>
       <c r="B227" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C227" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D227" t="s">
         <v>11</v>
@@ -4787,10 +4793,10 @@
         <v>12</v>
       </c>
       <c r="B228" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C228" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D228" t="s">
         <v>11</v>
@@ -4801,10 +4807,10 @@
         <v>12</v>
       </c>
       <c r="B229" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C229" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D229" t="s">
         <v>11</v>
@@ -4815,13 +4821,13 @@
         <v>12</v>
       </c>
       <c r="B230" t="s">
-        <v>356</v>
+        <v>17</v>
       </c>
       <c r="C230" t="s">
-        <v>357</v>
+        <v>18</v>
       </c>
       <c r="D230" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="231">
@@ -4835,7 +4841,7 @@
         <v>359</v>
       </c>
       <c r="D231" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="232">
@@ -4849,7 +4855,7 @@
         <v>361</v>
       </c>
       <c r="D232" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="233">
@@ -4863,7 +4869,7 @@
         <v>363</v>
       </c>
       <c r="D233" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="234">
@@ -4877,7 +4883,7 @@
         <v>365</v>
       </c>
       <c r="D234" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="235">
@@ -4891,7 +4897,7 @@
         <v>367</v>
       </c>
       <c r="D235" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="236">
@@ -4905,7 +4911,7 @@
         <v>369</v>
       </c>
       <c r="D236" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="237">
@@ -4919,7 +4925,7 @@
         <v>371</v>
       </c>
       <c r="D237" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="238">
@@ -4933,7 +4939,7 @@
         <v>373</v>
       </c>
       <c r="D238" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="239">
@@ -4947,7 +4953,7 @@
         <v>375</v>
       </c>
       <c r="D239" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="240">
@@ -4961,7 +4967,7 @@
         <v>377</v>
       </c>
       <c r="D240" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="241">
@@ -4975,7 +4981,7 @@
         <v>379</v>
       </c>
       <c r="D241" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="242">
@@ -4989,7 +4995,7 @@
         <v>381</v>
       </c>
       <c r="D242" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="243">
@@ -5003,7 +5009,7 @@
         <v>383</v>
       </c>
       <c r="D243" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="244">
@@ -5014,21 +5020,21 @@
         <v>384</v>
       </c>
       <c r="C244" t="s">
-        <v>38</v>
+        <v>385</v>
       </c>
       <c r="D244" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="s">
-        <v>385</v>
+        <v>12</v>
       </c>
       <c r="B245" t="s">
-        <v>9</v>
+        <v>386</v>
       </c>
       <c r="C245" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D245" t="s">
         <v>11</v>
@@ -5036,13 +5042,13 @@
     </row>
     <row r="246">
       <c r="A246" t="s">
-        <v>12</v>
+        <v>387</v>
       </c>
       <c r="B246" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C246" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D246" t="s">
         <v>11</v>
@@ -5053,10 +5059,10 @@
         <v>12</v>
       </c>
       <c r="B247" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C247" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D247" t="s">
         <v>11</v>
@@ -5067,10 +5073,10 @@
         <v>12</v>
       </c>
       <c r="B248" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C248" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D248" t="s">
         <v>11</v>
@@ -5081,13 +5087,13 @@
         <v>12</v>
       </c>
       <c r="B249" t="s">
-        <v>386</v>
+        <v>17</v>
       </c>
       <c r="C249" t="s">
-        <v>387</v>
+        <v>18</v>
       </c>
       <c r="D249" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="250">
@@ -5101,7 +5107,7 @@
         <v>389</v>
       </c>
       <c r="D250" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="251">
@@ -5115,7 +5121,7 @@
         <v>391</v>
       </c>
       <c r="D251" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="252">
@@ -5129,7 +5135,7 @@
         <v>393</v>
       </c>
       <c r="D252" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="253">
@@ -5143,7 +5149,7 @@
         <v>395</v>
       </c>
       <c r="D253" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="254">
@@ -5157,7 +5163,7 @@
         <v>397</v>
       </c>
       <c r="D254" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="255">
@@ -5171,7 +5177,7 @@
         <v>399</v>
       </c>
       <c r="D255" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="256">
@@ -5185,7 +5191,7 @@
         <v>401</v>
       </c>
       <c r="D256" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="257">
@@ -5199,7 +5205,7 @@
         <v>403</v>
       </c>
       <c r="D257" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="258">
@@ -5213,7 +5219,7 @@
         <v>405</v>
       </c>
       <c r="D258" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="259">
@@ -5227,7 +5233,7 @@
         <v>407</v>
       </c>
       <c r="D259" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="260">
@@ -5241,7 +5247,7 @@
         <v>409</v>
       </c>
       <c r="D260" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="261">
@@ -5255,7 +5261,7 @@
         <v>411</v>
       </c>
       <c r="D261" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="262">
@@ -5269,7 +5275,7 @@
         <v>413</v>
       </c>
       <c r="D262" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="263">
@@ -5283,7 +5289,7 @@
         <v>415</v>
       </c>
       <c r="D263" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="264">
@@ -5297,7 +5303,7 @@
         <v>417</v>
       </c>
       <c r="D264" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="265">
@@ -5311,7 +5317,7 @@
         <v>419</v>
       </c>
       <c r="D265" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="266">
@@ -5325,7 +5331,7 @@
         <v>421</v>
       </c>
       <c r="D266" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="267">
@@ -5339,7 +5345,7 @@
         <v>423</v>
       </c>
       <c r="D267" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="268">
@@ -5353,7 +5359,7 @@
         <v>425</v>
       </c>
       <c r="D268" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="269">
@@ -5367,7 +5373,7 @@
         <v>427</v>
       </c>
       <c r="D269" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="270">
@@ -5381,7 +5387,7 @@
         <v>429</v>
       </c>
       <c r="D270" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="271">
@@ -5392,9 +5398,23 @@
         <v>430</v>
       </c>
       <c r="C271" t="s">
-        <v>38</v>
+        <v>431</v>
       </c>
       <c r="D271" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="s">
+        <v>12</v>
+      </c>
+      <c r="B272" t="s">
+        <v>432</v>
+      </c>
+      <c r="C272" t="s">
+        <v>40</v>
+      </c>
+      <c r="D272" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert remove frontend columns ret_bewerter2_pipeline and ret_bewerter3
</commit_message>
<xml_diff>
--- a/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
+++ b/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="435">
   <si>
     <t xml:space="preserve">Hint</t>
   </si>
@@ -845,7 +845,7 @@
     <t xml:space="preserve">ret_id</t>
   </si>
   <si>
-    <t xml:space="preserve">Retrolektive MRP-ID (REDCap) Hier wird die MEDA-ID der Medikationsanalyse angegeben, zu deren Zeitpunkt dieses MRP vom Apotheker hätte gefunden werden können. Wenn keine Medikationsanalyse dokumentiert ist wir eine ID aus Fall-ID-x eingetragen</t>
+    <t xml:space="preserve">Retrolektive MRP-ID (REDCap) Hier wird die vom Datenprozessor MEDA-ID-r-Instanz aggregiert.</t>
   </si>
   <si>
     <t xml:space="preserve">ret_meda_id</t>
@@ -999,6 +999,12 @@
   </si>
   <si>
     <t xml:space="preserve">2. Bewertung von</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_bewerter3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_bewerter2_pipeline</t>
   </si>
   <si>
     <t xml:space="preserve">ret_gewissheit2</t>
@@ -4390,7 +4396,7 @@
         <v>329</v>
       </c>
       <c r="C199" t="s">
-        <v>292</v>
+        <v>12</v>
       </c>
       <c r="D199" t="s">
         <v>11</v>
@@ -4404,7 +4410,7 @@
         <v>330</v>
       </c>
       <c r="C200" t="s">
-        <v>294</v>
+        <v>12</v>
       </c>
       <c r="D200" t="s">
         <v>11</v>
@@ -4418,7 +4424,7 @@
         <v>331</v>
       </c>
       <c r="C201" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D201" t="s">
         <v>11</v>
@@ -4432,7 +4438,7 @@
         <v>332</v>
       </c>
       <c r="C202" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D202" t="s">
         <v>11</v>
@@ -4446,7 +4452,7 @@
         <v>333</v>
       </c>
       <c r="C203" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D203" t="s">
         <v>11</v>
@@ -4460,7 +4466,7 @@
         <v>334</v>
       </c>
       <c r="C204" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D204" t="s">
         <v>11</v>
@@ -4474,7 +4480,7 @@
         <v>335</v>
       </c>
       <c r="C205" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="D205" t="s">
         <v>11</v>
@@ -4488,7 +4494,7 @@
         <v>336</v>
       </c>
       <c r="C206" t="s">
-        <v>228</v>
+        <v>302</v>
       </c>
       <c r="D206" t="s">
         <v>11</v>
@@ -4502,7 +4508,7 @@
         <v>337</v>
       </c>
       <c r="C207" t="s">
-        <v>230</v>
+        <v>304</v>
       </c>
       <c r="D207" t="s">
         <v>11</v>
@@ -4516,7 +4522,7 @@
         <v>338</v>
       </c>
       <c r="C208" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D208" t="s">
         <v>11</v>
@@ -4530,7 +4536,7 @@
         <v>339</v>
       </c>
       <c r="C209" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D209" t="s">
         <v>11</v>
@@ -4544,7 +4550,7 @@
         <v>340</v>
       </c>
       <c r="C210" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D210" t="s">
         <v>11</v>
@@ -4558,7 +4564,7 @@
         <v>341</v>
       </c>
       <c r="C211" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D211" t="s">
         <v>11</v>
@@ -4572,7 +4578,7 @@
         <v>342</v>
       </c>
       <c r="C212" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D212" t="s">
         <v>11</v>
@@ -4586,7 +4592,7 @@
         <v>343</v>
       </c>
       <c r="C213" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D213" t="s">
         <v>11</v>
@@ -4600,7 +4606,7 @@
         <v>344</v>
       </c>
       <c r="C214" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D214" t="s">
         <v>11</v>
@@ -4614,7 +4620,7 @@
         <v>345</v>
       </c>
       <c r="C215" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D215" t="s">
         <v>11</v>
@@ -4628,7 +4634,7 @@
         <v>346</v>
       </c>
       <c r="C216" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D216" t="s">
         <v>11</v>
@@ -4642,7 +4648,7 @@
         <v>347</v>
       </c>
       <c r="C217" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D217" t="s">
         <v>11</v>
@@ -4656,7 +4662,7 @@
         <v>348</v>
       </c>
       <c r="C218" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D218" t="s">
         <v>11</v>
@@ -4670,7 +4676,7 @@
         <v>349</v>
       </c>
       <c r="C219" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D219" t="s">
         <v>11</v>
@@ -4684,7 +4690,7 @@
         <v>350</v>
       </c>
       <c r="C220" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D220" t="s">
         <v>11</v>
@@ -4698,7 +4704,7 @@
         <v>351</v>
       </c>
       <c r="C221" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D221" t="s">
         <v>11</v>
@@ -4712,7 +4718,7 @@
         <v>352</v>
       </c>
       <c r="C222" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D222" t="s">
         <v>11</v>
@@ -4726,7 +4732,7 @@
         <v>353</v>
       </c>
       <c r="C223" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D223" t="s">
         <v>11</v>
@@ -4740,7 +4746,7 @@
         <v>354</v>
       </c>
       <c r="C224" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D224" t="s">
         <v>11</v>
@@ -4754,7 +4760,7 @@
         <v>355</v>
       </c>
       <c r="C225" t="s">
-        <v>38</v>
+        <v>262</v>
       </c>
       <c r="D225" t="s">
         <v>11</v>
@@ -4768,7 +4774,7 @@
         <v>356</v>
       </c>
       <c r="C226" t="s">
-        <v>40</v>
+        <v>264</v>
       </c>
       <c r="D226" t="s">
         <v>11</v>
@@ -4776,13 +4782,13 @@
     </row>
     <row r="227">
       <c r="A227" t="s">
+        <v>12</v>
+      </c>
+      <c r="B227" t="s">
         <v>357</v>
       </c>
-      <c r="B227" t="s">
-        <v>9</v>
-      </c>
       <c r="C227" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="D227" t="s">
         <v>11</v>
@@ -4793,10 +4799,10 @@
         <v>12</v>
       </c>
       <c r="B228" t="s">
-        <v>13</v>
+        <v>358</v>
       </c>
       <c r="C228" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="D228" t="s">
         <v>11</v>
@@ -4804,13 +4810,13 @@
     </row>
     <row r="229">
       <c r="A229" t="s">
-        <v>12</v>
+        <v>359</v>
       </c>
       <c r="B229" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C229" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D229" t="s">
         <v>11</v>
@@ -4821,10 +4827,10 @@
         <v>12</v>
       </c>
       <c r="B230" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C230" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D230" t="s">
         <v>11</v>
@@ -4835,13 +4841,13 @@
         <v>12</v>
       </c>
       <c r="B231" t="s">
-        <v>358</v>
+        <v>15</v>
       </c>
       <c r="C231" t="s">
-        <v>359</v>
+        <v>16</v>
       </c>
       <c r="D231" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="232">
@@ -4849,13 +4855,13 @@
         <v>12</v>
       </c>
       <c r="B232" t="s">
-        <v>360</v>
+        <v>17</v>
       </c>
       <c r="C232" t="s">
-        <v>361</v>
+        <v>18</v>
       </c>
       <c r="D232" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="233">
@@ -4863,10 +4869,10 @@
         <v>12</v>
       </c>
       <c r="B233" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C233" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D233" t="s">
         <v>48</v>
@@ -4877,10 +4883,10 @@
         <v>12</v>
       </c>
       <c r="B234" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C234" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D234" t="s">
         <v>48</v>
@@ -4891,10 +4897,10 @@
         <v>12</v>
       </c>
       <c r="B235" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C235" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D235" t="s">
         <v>48</v>
@@ -4905,10 +4911,10 @@
         <v>12</v>
       </c>
       <c r="B236" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C236" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D236" t="s">
         <v>48</v>
@@ -4919,10 +4925,10 @@
         <v>12</v>
       </c>
       <c r="B237" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C237" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D237" t="s">
         <v>48</v>
@@ -4933,10 +4939,10 @@
         <v>12</v>
       </c>
       <c r="B238" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C238" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D238" t="s">
         <v>48</v>
@@ -4947,10 +4953,10 @@
         <v>12</v>
       </c>
       <c r="B239" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C239" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D239" t="s">
         <v>48</v>
@@ -4961,10 +4967,10 @@
         <v>12</v>
       </c>
       <c r="B240" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C240" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D240" t="s">
         <v>48</v>
@@ -4975,10 +4981,10 @@
         <v>12</v>
       </c>
       <c r="B241" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C241" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D241" t="s">
         <v>48</v>
@@ -4989,10 +4995,10 @@
         <v>12</v>
       </c>
       <c r="B242" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C242" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D242" t="s">
         <v>48</v>
@@ -5003,10 +5009,10 @@
         <v>12</v>
       </c>
       <c r="B243" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C243" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D243" t="s">
         <v>48</v>
@@ -5017,13 +5023,13 @@
         <v>12</v>
       </c>
       <c r="B244" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C244" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D244" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="245">
@@ -5031,27 +5037,27 @@
         <v>12</v>
       </c>
       <c r="B245" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C245" t="s">
-        <v>40</v>
+        <v>385</v>
       </c>
       <c r="D245" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="s">
+        <v>12</v>
+      </c>
+      <c r="B246" t="s">
+        <v>386</v>
+      </c>
+      <c r="C246" t="s">
         <v>387</v>
       </c>
-      <c r="B246" t="s">
-        <v>9</v>
-      </c>
-      <c r="C246" t="s">
-        <v>10</v>
-      </c>
       <c r="D246" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
     </row>
     <row r="247">
@@ -5059,10 +5065,10 @@
         <v>12</v>
       </c>
       <c r="B247" t="s">
-        <v>13</v>
+        <v>388</v>
       </c>
       <c r="C247" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="D247" t="s">
         <v>11</v>
@@ -5070,13 +5076,13 @@
     </row>
     <row r="248">
       <c r="A248" t="s">
-        <v>12</v>
+        <v>389</v>
       </c>
       <c r="B248" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C248" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D248" t="s">
         <v>11</v>
@@ -5087,10 +5093,10 @@
         <v>12</v>
       </c>
       <c r="B249" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C249" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D249" t="s">
         <v>11</v>
@@ -5101,13 +5107,13 @@
         <v>12</v>
       </c>
       <c r="B250" t="s">
-        <v>388</v>
+        <v>15</v>
       </c>
       <c r="C250" t="s">
-        <v>389</v>
+        <v>16</v>
       </c>
       <c r="D250" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="251">
@@ -5115,13 +5121,13 @@
         <v>12</v>
       </c>
       <c r="B251" t="s">
-        <v>390</v>
+        <v>17</v>
       </c>
       <c r="C251" t="s">
-        <v>391</v>
+        <v>18</v>
       </c>
       <c r="D251" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="252">
@@ -5129,10 +5135,10 @@
         <v>12</v>
       </c>
       <c r="B252" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C252" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D252" t="s">
         <v>48</v>
@@ -5143,10 +5149,10 @@
         <v>12</v>
       </c>
       <c r="B253" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C253" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D253" t="s">
         <v>48</v>
@@ -5157,10 +5163,10 @@
         <v>12</v>
       </c>
       <c r="B254" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C254" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D254" t="s">
         <v>48</v>
@@ -5171,10 +5177,10 @@
         <v>12</v>
       </c>
       <c r="B255" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C255" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D255" t="s">
         <v>48</v>
@@ -5185,10 +5191,10 @@
         <v>12</v>
       </c>
       <c r="B256" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C256" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D256" t="s">
         <v>48</v>
@@ -5199,10 +5205,10 @@
         <v>12</v>
       </c>
       <c r="B257" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C257" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D257" t="s">
         <v>48</v>
@@ -5213,10 +5219,10 @@
         <v>12</v>
       </c>
       <c r="B258" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C258" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D258" t="s">
         <v>48</v>
@@ -5227,10 +5233,10 @@
         <v>12</v>
       </c>
       <c r="B259" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C259" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D259" t="s">
         <v>48</v>
@@ -5241,10 +5247,10 @@
         <v>12</v>
       </c>
       <c r="B260" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C260" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D260" t="s">
         <v>48</v>
@@ -5255,10 +5261,10 @@
         <v>12</v>
       </c>
       <c r="B261" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C261" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D261" t="s">
         <v>48</v>
@@ -5269,10 +5275,10 @@
         <v>12</v>
       </c>
       <c r="B262" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C262" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D262" t="s">
         <v>48</v>
@@ -5283,10 +5289,10 @@
         <v>12</v>
       </c>
       <c r="B263" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C263" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D263" t="s">
         <v>48</v>
@@ -5297,10 +5303,10 @@
         <v>12</v>
       </c>
       <c r="B264" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C264" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D264" t="s">
         <v>48</v>
@@ -5311,10 +5317,10 @@
         <v>12</v>
       </c>
       <c r="B265" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C265" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D265" t="s">
         <v>48</v>
@@ -5325,10 +5331,10 @@
         <v>12</v>
       </c>
       <c r="B266" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C266" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D266" t="s">
         <v>48</v>
@@ -5339,10 +5345,10 @@
         <v>12</v>
       </c>
       <c r="B267" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C267" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D267" t="s">
         <v>48</v>
@@ -5353,10 +5359,10 @@
         <v>12</v>
       </c>
       <c r="B268" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C268" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D268" t="s">
         <v>48</v>
@@ -5367,10 +5373,10 @@
         <v>12</v>
       </c>
       <c r="B269" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C269" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D269" t="s">
         <v>48</v>
@@ -5381,10 +5387,10 @@
         <v>12</v>
       </c>
       <c r="B270" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C270" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D270" t="s">
         <v>48</v>
@@ -5395,10 +5401,10 @@
         <v>12</v>
       </c>
       <c r="B271" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C271" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D271" t="s">
         <v>48</v>
@@ -5409,12 +5415,40 @@
         <v>12</v>
       </c>
       <c r="B272" t="s">
+        <v>430</v>
+      </c>
+      <c r="C272" t="s">
+        <v>431</v>
+      </c>
+      <c r="D272" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="s">
+        <v>12</v>
+      </c>
+      <c r="B273" t="s">
         <v>432</v>
       </c>
-      <c r="C272" t="s">
+      <c r="C273" t="s">
+        <v>433</v>
+      </c>
+      <c r="D273" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="s">
+        <v>12</v>
+      </c>
+      <c r="B274" t="s">
+        <v>434</v>
+      </c>
+      <c r="C274" t="s">
         <v>40</v>
       </c>
-      <c r="D272" t="s">
+      <c r="D274" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Frontent_DataDictionary and Frontend_Table_Description
refs #1012
</commit_message>
<xml_diff>
--- a/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
+++ b/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="474">
   <si>
     <t xml:space="preserve">Hint</t>
   </si>
@@ -854,141 +854,222 @@
     <t xml:space="preserve">Zuordnung Meda -&gt; rMRP</t>
   </si>
   <si>
+    <t xml:space="preserve">ret_meda_dat_referenz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Referenzdatum der Medikationsanalyse</t>
+  </si>
+  <si>
     <t xml:space="preserve">ret_meda_dat1</t>
   </si>
   <si>
+    <t xml:space="preserve">Datum der retrolektiven Bewertung*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_kurzbeschr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kurzbeschreibung des MRPs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_ip_klasse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_ip_klasse_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_atc1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_atc2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_ip_klasse_disease</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_ip_klasse_labor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_ip_klasse_nieren_insuf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewissheit1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bewertung des detektierten MRP*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_mrp_zuordnung1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zuordnung zu manuellem MRP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewissheit1_oth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weitere Informationen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_grund1_abl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grund für nicht Bestätigung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_trigger1_falsch___1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - ret_atc1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_trigger1_falsch___2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 - ret_atc2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_trigger1_falsch___3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 - ret_ip_klasse_disease</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_trigger1_falsch___4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 - ret_ip_klasse_nieren_insuf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_datengrundl1_1___1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Der Indikator (bzw. alle Indikatoren - falls mehrere) liegt nicht wie in der Kurzbeschreibung angezeigt im EMR vor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_datengrundl1_1___2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 - Indikator/Indikatoren zum Zeitpunkt der Medikationsanalyse nicht gültig (z.B. pausiert - inaktiv - Fehldiagnose)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_datengrundl1_1___3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 - Zusätzliche Informationen nicht berücksichtigt (z.B. aus Briefen - sonstigen Systemen)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_datengrundl1_1___4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 - Anderer Fehler (bitte näher erläutern)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_datengrundl1_2___1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_datengrundl1_2___2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_datengrundl1_2___3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_datengrundl1_2___4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_datengrundl1_1_oth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kommentar (1. Trigger)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_datengrundl1_2_oth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kommentar (2. Trigger)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_grund_abl_sonst1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bitte näher beschreiben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_grund_abl_klin1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WARUM ist das MRP nicht klinisch relevant?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_grund_abl_klin1_neg___1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Dieses MRP halte ich FÜR KEINEN Patienten auf dieser Station für KLINISCH RELEVANT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_massn_am1___1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_massn_am1___2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_massn_am1___3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_massn_am1___4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_massn_am1___5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_massn_am1___6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_massn_am1___7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_massn_am1___8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_massn_am1___9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_massn_am1___10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_massn_orga1___1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_massn_orga1___2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_massn_orga1___3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_massn_orga1___4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_massn_orga1___5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_massn_orga1___6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_massn_orga1___7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_massn_orga1___8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_notiz1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_meda_dat2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Datum der retrolektiven Betrachtung*</t>
   </si>
   <si>
-    <t xml:space="preserve">ret_kurzbeschr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kurzbeschreibung des MRPs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_ip_klasse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_ip_klasse_01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_atc1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_atc2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_ip_klasse_disease</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_ip_klasse_labor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_ip_klasse_nieren_insuf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_gewissheit1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sicherheit des detektierten MRP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_mrp_zuordnung1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zuordnung zu manuellem MRP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_gewissheit1_oth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weitere Informationen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_gewiss_grund1_abl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grund für nicht Bestätigung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_gewiss_grund_abl_sonst1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bitte näher beschreiben</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_gewiss_grund_abl_klin1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WARUM ist das MRP nicht klinisch relevant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_gewiss_grund_abl_klin1_neg___1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 - Dieses MRP halte ich FÜR KEINEN Patienten auf dieser Station für KLINISCH RELEVANT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_massn_am1___1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_massn_am1___2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_massn_am1___3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_massn_am1___4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_massn_am1___5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_massn_am1___6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_massn_am1___7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_massn_am1___8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_massn_am1___9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_massn_am1___10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_massn_orga1___1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_massn_orga1___2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_massn_orga1___3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_massn_orga1___4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_massn_orga1___5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_massn_orga1___6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_massn_orga1___7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_massn_orga1___8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_notiz1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ret_meda_dat2</t>
-  </si>
-  <si>
     <t xml:space="preserve">ret_2ndbewertung___1</t>
   </si>
   <si>
@@ -1022,6 +1103,48 @@
     <t xml:space="preserve">ret_gewiss_grund_abl_sonst2</t>
   </si>
   <si>
+    <t xml:space="preserve">ret_gewiss_trigger2_falsch___1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_trigger2_falsch___2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_trigger2_falsch___3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_trigger2_falsch___4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_datengrundl2_1___1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_datengrundl2_1___2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_datengrundl2_1___3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_datengrundl2_1___4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_datengrundl2_2___1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_datengrundl2_2___2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_datengrundl2_2___3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_datengrundl2_2___4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_datengrundl2_1_oth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_gewiss_datengrundl2_2_oth</t>
+  </si>
+  <si>
     <t xml:space="preserve">ret_gewiss_grund_abl_klin2</t>
   </si>
   <si>
@@ -1170,12 +1293,6 @@
   </si>
   <si>
     <t xml:space="preserve">ent. Ern.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rskfkt_anz_rskamklassen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aggregation der Felder 27-33: Anzahl der Felder mit Ausprägung &gt;0</t>
   </si>
   <si>
     <t xml:space="preserve">risikofaktor_complete</t>
@@ -3881,7 +3998,7 @@
         <v>283</v>
       </c>
       <c r="D162" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
     </row>
     <row r="163">
@@ -3892,7 +4009,7 @@
         <v>284</v>
       </c>
       <c r="C163" t="s">
-        <v>219</v>
+        <v>285</v>
       </c>
       <c r="D163" t="s">
         <v>11</v>
@@ -3903,7 +4020,7 @@
         <v>12</v>
       </c>
       <c r="B164" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C164" t="s">
         <v>219</v>
@@ -3917,10 +4034,10 @@
         <v>12</v>
       </c>
       <c r="B165" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C165" t="s">
-        <v>147</v>
+        <v>219</v>
       </c>
       <c r="D165" t="s">
         <v>11</v>
@@ -3931,10 +4048,10 @@
         <v>12</v>
       </c>
       <c r="B166" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C166" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D166" t="s">
         <v>11</v>
@@ -3945,10 +4062,10 @@
         <v>12</v>
       </c>
       <c r="B167" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C167" t="s">
-        <v>222</v>
+        <v>149</v>
       </c>
       <c r="D167" t="s">
         <v>11</v>
@@ -3959,10 +4076,10 @@
         <v>12</v>
       </c>
       <c r="B168" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C168" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D168" t="s">
         <v>11</v>
@@ -3973,10 +4090,10 @@
         <v>12</v>
       </c>
       <c r="B169" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C169" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D169" t="s">
         <v>11</v>
@@ -3987,10 +4104,10 @@
         <v>12</v>
       </c>
       <c r="B170" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C170" t="s">
-        <v>292</v>
+        <v>226</v>
       </c>
       <c r="D170" t="s">
         <v>11</v>
@@ -4088,7 +4205,7 @@
         <v>305</v>
       </c>
       <c r="C177" t="s">
-        <v>228</v>
+        <v>306</v>
       </c>
       <c r="D177" t="s">
         <v>11</v>
@@ -4099,10 +4216,10 @@
         <v>12</v>
       </c>
       <c r="B178" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C178" t="s">
-        <v>230</v>
+        <v>308</v>
       </c>
       <c r="D178" t="s">
         <v>11</v>
@@ -4113,10 +4230,10 @@
         <v>12</v>
       </c>
       <c r="B179" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C179" t="s">
-        <v>232</v>
+        <v>310</v>
       </c>
       <c r="D179" t="s">
         <v>11</v>
@@ -4127,10 +4244,10 @@
         <v>12</v>
       </c>
       <c r="B180" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="C180" t="s">
-        <v>234</v>
+        <v>312</v>
       </c>
       <c r="D180" t="s">
         <v>11</v>
@@ -4141,10 +4258,10 @@
         <v>12</v>
       </c>
       <c r="B181" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="C181" t="s">
-        <v>236</v>
+        <v>314</v>
       </c>
       <c r="D181" t="s">
         <v>11</v>
@@ -4155,10 +4272,10 @@
         <v>12</v>
       </c>
       <c r="B182" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="C182" t="s">
-        <v>238</v>
+        <v>316</v>
       </c>
       <c r="D182" t="s">
         <v>11</v>
@@ -4169,10 +4286,10 @@
         <v>12</v>
       </c>
       <c r="B183" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="C183" t="s">
-        <v>240</v>
+        <v>310</v>
       </c>
       <c r="D183" t="s">
         <v>11</v>
@@ -4183,10 +4300,10 @@
         <v>12</v>
       </c>
       <c r="B184" t="s">
+        <v>318</v>
+      </c>
+      <c r="C184" t="s">
         <v>312</v>
-      </c>
-      <c r="C184" t="s">
-        <v>242</v>
       </c>
       <c r="D184" t="s">
         <v>11</v>
@@ -4197,10 +4314,10 @@
         <v>12</v>
       </c>
       <c r="B185" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="C185" t="s">
-        <v>244</v>
+        <v>314</v>
       </c>
       <c r="D185" t="s">
         <v>11</v>
@@ -4211,10 +4328,10 @@
         <v>12</v>
       </c>
       <c r="B186" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="C186" t="s">
-        <v>246</v>
+        <v>316</v>
       </c>
       <c r="D186" t="s">
         <v>11</v>
@@ -4225,10 +4342,10 @@
         <v>12</v>
       </c>
       <c r="B187" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="C187" t="s">
-        <v>248</v>
+        <v>322</v>
       </c>
       <c r="D187" t="s">
         <v>11</v>
@@ -4239,10 +4356,10 @@
         <v>12</v>
       </c>
       <c r="B188" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="C188" t="s">
-        <v>250</v>
+        <v>324</v>
       </c>
       <c r="D188" t="s">
         <v>11</v>
@@ -4253,10 +4370,10 @@
         <v>12</v>
       </c>
       <c r="B189" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="C189" t="s">
-        <v>252</v>
+        <v>326</v>
       </c>
       <c r="D189" t="s">
         <v>11</v>
@@ -4267,10 +4384,10 @@
         <v>12</v>
       </c>
       <c r="B190" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
       <c r="C190" t="s">
-        <v>254</v>
+        <v>328</v>
       </c>
       <c r="D190" t="s">
         <v>11</v>
@@ -4281,10 +4398,10 @@
         <v>12</v>
       </c>
       <c r="B191" t="s">
-        <v>319</v>
+        <v>329</v>
       </c>
       <c r="C191" t="s">
-        <v>256</v>
+        <v>330</v>
       </c>
       <c r="D191" t="s">
         <v>11</v>
@@ -4295,10 +4412,10 @@
         <v>12</v>
       </c>
       <c r="B192" t="s">
-        <v>320</v>
+        <v>331</v>
       </c>
       <c r="C192" t="s">
-        <v>258</v>
+        <v>228</v>
       </c>
       <c r="D192" t="s">
         <v>11</v>
@@ -4309,10 +4426,10 @@
         <v>12</v>
       </c>
       <c r="B193" t="s">
-        <v>321</v>
+        <v>332</v>
       </c>
       <c r="C193" t="s">
-        <v>260</v>
+        <v>230</v>
       </c>
       <c r="D193" t="s">
         <v>11</v>
@@ -4323,10 +4440,10 @@
         <v>12</v>
       </c>
       <c r="B194" t="s">
-        <v>322</v>
+        <v>333</v>
       </c>
       <c r="C194" t="s">
-        <v>262</v>
+        <v>232</v>
       </c>
       <c r="D194" t="s">
         <v>11</v>
@@ -4337,10 +4454,10 @@
         <v>12</v>
       </c>
       <c r="B195" t="s">
-        <v>323</v>
+        <v>334</v>
       </c>
       <c r="C195" t="s">
-        <v>264</v>
+        <v>234</v>
       </c>
       <c r="D195" t="s">
         <v>11</v>
@@ -4351,13 +4468,13 @@
         <v>12</v>
       </c>
       <c r="B196" t="s">
-        <v>324</v>
+        <v>335</v>
       </c>
       <c r="C196" t="s">
-        <v>281</v>
+        <v>236</v>
       </c>
       <c r="D196" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
     </row>
     <row r="197">
@@ -4365,10 +4482,10 @@
         <v>12</v>
       </c>
       <c r="B197" t="s">
-        <v>325</v>
+        <v>336</v>
       </c>
       <c r="C197" t="s">
-        <v>326</v>
+        <v>238</v>
       </c>
       <c r="D197" t="s">
         <v>11</v>
@@ -4379,10 +4496,10 @@
         <v>12</v>
       </c>
       <c r="B198" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C198" t="s">
-        <v>328</v>
+        <v>240</v>
       </c>
       <c r="D198" t="s">
         <v>11</v>
@@ -4393,10 +4510,10 @@
         <v>12</v>
       </c>
       <c r="B199" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="C199" t="s">
-        <v>12</v>
+        <v>242</v>
       </c>
       <c r="D199" t="s">
         <v>11</v>
@@ -4407,10 +4524,10 @@
         <v>12</v>
       </c>
       <c r="B200" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="C200" t="s">
-        <v>12</v>
+        <v>244</v>
       </c>
       <c r="D200" t="s">
         <v>11</v>
@@ -4421,10 +4538,10 @@
         <v>12</v>
       </c>
       <c r="B201" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="C201" t="s">
-        <v>292</v>
+        <v>246</v>
       </c>
       <c r="D201" t="s">
         <v>11</v>
@@ -4435,10 +4552,10 @@
         <v>12</v>
       </c>
       <c r="B202" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="C202" t="s">
-        <v>294</v>
+        <v>248</v>
       </c>
       <c r="D202" t="s">
         <v>11</v>
@@ -4449,10 +4566,10 @@
         <v>12</v>
       </c>
       <c r="B203" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="C203" t="s">
-        <v>296</v>
+        <v>250</v>
       </c>
       <c r="D203" t="s">
         <v>11</v>
@@ -4463,10 +4580,10 @@
         <v>12</v>
       </c>
       <c r="B204" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="C204" t="s">
-        <v>298</v>
+        <v>252</v>
       </c>
       <c r="D204" t="s">
         <v>11</v>
@@ -4477,10 +4594,10 @@
         <v>12</v>
       </c>
       <c r="B205" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="C205" t="s">
-        <v>300</v>
+        <v>254</v>
       </c>
       <c r="D205" t="s">
         <v>11</v>
@@ -4491,10 +4608,10 @@
         <v>12</v>
       </c>
       <c r="B206" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="C206" t="s">
-        <v>302</v>
+        <v>256</v>
       </c>
       <c r="D206" t="s">
         <v>11</v>
@@ -4505,10 +4622,10 @@
         <v>12</v>
       </c>
       <c r="B207" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="C207" t="s">
-        <v>304</v>
+        <v>258</v>
       </c>
       <c r="D207" t="s">
         <v>11</v>
@@ -4519,10 +4636,10 @@
         <v>12</v>
       </c>
       <c r="B208" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
       <c r="C208" t="s">
-        <v>228</v>
+        <v>260</v>
       </c>
       <c r="D208" t="s">
         <v>11</v>
@@ -4533,10 +4650,10 @@
         <v>12</v>
       </c>
       <c r="B209" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
       <c r="C209" t="s">
-        <v>230</v>
+        <v>262</v>
       </c>
       <c r="D209" t="s">
         <v>11</v>
@@ -4547,10 +4664,10 @@
         <v>12</v>
       </c>
       <c r="B210" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
       <c r="C210" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
       <c r="D210" t="s">
         <v>11</v>
@@ -4561,13 +4678,13 @@
         <v>12</v>
       </c>
       <c r="B211" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="C211" t="s">
-        <v>234</v>
+        <v>351</v>
       </c>
       <c r="D211" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
     </row>
     <row r="212">
@@ -4575,10 +4692,10 @@
         <v>12</v>
       </c>
       <c r="B212" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C212" t="s">
-        <v>236</v>
+        <v>353</v>
       </c>
       <c r="D212" t="s">
         <v>11</v>
@@ -4589,10 +4706,10 @@
         <v>12</v>
       </c>
       <c r="B213" t="s">
-        <v>343</v>
+        <v>354</v>
       </c>
       <c r="C213" t="s">
-        <v>238</v>
+        <v>355</v>
       </c>
       <c r="D213" t="s">
         <v>11</v>
@@ -4603,10 +4720,10 @@
         <v>12</v>
       </c>
       <c r="B214" t="s">
-        <v>344</v>
+        <v>356</v>
       </c>
       <c r="C214" t="s">
-        <v>240</v>
+        <v>12</v>
       </c>
       <c r="D214" t="s">
         <v>11</v>
@@ -4617,10 +4734,10 @@
         <v>12</v>
       </c>
       <c r="B215" t="s">
-        <v>345</v>
+        <v>357</v>
       </c>
       <c r="C215" t="s">
-        <v>242</v>
+        <v>12</v>
       </c>
       <c r="D215" t="s">
         <v>11</v>
@@ -4631,10 +4748,10 @@
         <v>12</v>
       </c>
       <c r="B216" t="s">
-        <v>346</v>
+        <v>358</v>
       </c>
       <c r="C216" t="s">
-        <v>244</v>
+        <v>294</v>
       </c>
       <c r="D216" t="s">
         <v>11</v>
@@ -4645,10 +4762,10 @@
         <v>12</v>
       </c>
       <c r="B217" t="s">
-        <v>347</v>
+        <v>359</v>
       </c>
       <c r="C217" t="s">
-        <v>246</v>
+        <v>296</v>
       </c>
       <c r="D217" t="s">
         <v>11</v>
@@ -4659,10 +4776,10 @@
         <v>12</v>
       </c>
       <c r="B218" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
       <c r="C218" t="s">
-        <v>248</v>
+        <v>298</v>
       </c>
       <c r="D218" t="s">
         <v>11</v>
@@ -4673,10 +4790,10 @@
         <v>12</v>
       </c>
       <c r="B219" t="s">
-        <v>349</v>
+        <v>361</v>
       </c>
       <c r="C219" t="s">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="D219" t="s">
         <v>11</v>
@@ -4687,10 +4804,10 @@
         <v>12</v>
       </c>
       <c r="B220" t="s">
-        <v>350</v>
+        <v>362</v>
       </c>
       <c r="C220" t="s">
-        <v>252</v>
+        <v>326</v>
       </c>
       <c r="D220" t="s">
         <v>11</v>
@@ -4701,10 +4818,10 @@
         <v>12</v>
       </c>
       <c r="B221" t="s">
-        <v>351</v>
+        <v>363</v>
       </c>
       <c r="C221" t="s">
-        <v>254</v>
+        <v>302</v>
       </c>
       <c r="D221" t="s">
         <v>11</v>
@@ -4715,10 +4832,10 @@
         <v>12</v>
       </c>
       <c r="B222" t="s">
-        <v>352</v>
+        <v>364</v>
       </c>
       <c r="C222" t="s">
-        <v>256</v>
+        <v>304</v>
       </c>
       <c r="D222" t="s">
         <v>11</v>
@@ -4729,10 +4846,10 @@
         <v>12</v>
       </c>
       <c r="B223" t="s">
-        <v>353</v>
+        <v>365</v>
       </c>
       <c r="C223" t="s">
-        <v>258</v>
+        <v>306</v>
       </c>
       <c r="D223" t="s">
         <v>11</v>
@@ -4743,10 +4860,10 @@
         <v>12</v>
       </c>
       <c r="B224" t="s">
-        <v>354</v>
+        <v>366</v>
       </c>
       <c r="C224" t="s">
-        <v>260</v>
+        <v>308</v>
       </c>
       <c r="D224" t="s">
         <v>11</v>
@@ -4757,10 +4874,10 @@
         <v>12</v>
       </c>
       <c r="B225" t="s">
-        <v>355</v>
+        <v>367</v>
       </c>
       <c r="C225" t="s">
-        <v>262</v>
+        <v>310</v>
       </c>
       <c r="D225" t="s">
         <v>11</v>
@@ -4771,10 +4888,10 @@
         <v>12</v>
       </c>
       <c r="B226" t="s">
-        <v>356</v>
+        <v>368</v>
       </c>
       <c r="C226" t="s">
-        <v>264</v>
+        <v>312</v>
       </c>
       <c r="D226" t="s">
         <v>11</v>
@@ -4785,10 +4902,10 @@
         <v>12</v>
       </c>
       <c r="B227" t="s">
-        <v>357</v>
+        <v>369</v>
       </c>
       <c r="C227" t="s">
-        <v>38</v>
+        <v>314</v>
       </c>
       <c r="D227" t="s">
         <v>11</v>
@@ -4799,10 +4916,10 @@
         <v>12</v>
       </c>
       <c r="B228" t="s">
-        <v>358</v>
+        <v>370</v>
       </c>
       <c r="C228" t="s">
-        <v>40</v>
+        <v>316</v>
       </c>
       <c r="D228" t="s">
         <v>11</v>
@@ -4810,13 +4927,13 @@
     </row>
     <row r="229">
       <c r="A229" t="s">
-        <v>359</v>
+        <v>12</v>
       </c>
       <c r="B229" t="s">
-        <v>9</v>
+        <v>371</v>
       </c>
       <c r="C229" t="s">
-        <v>10</v>
+        <v>310</v>
       </c>
       <c r="D229" t="s">
         <v>11</v>
@@ -4827,10 +4944,10 @@
         <v>12</v>
       </c>
       <c r="B230" t="s">
-        <v>13</v>
+        <v>372</v>
       </c>
       <c r="C230" t="s">
-        <v>14</v>
+        <v>312</v>
       </c>
       <c r="D230" t="s">
         <v>11</v>
@@ -4841,10 +4958,10 @@
         <v>12</v>
       </c>
       <c r="B231" t="s">
-        <v>15</v>
+        <v>373</v>
       </c>
       <c r="C231" t="s">
-        <v>16</v>
+        <v>314</v>
       </c>
       <c r="D231" t="s">
         <v>11</v>
@@ -4855,10 +4972,10 @@
         <v>12</v>
       </c>
       <c r="B232" t="s">
-        <v>17</v>
+        <v>374</v>
       </c>
       <c r="C232" t="s">
-        <v>18</v>
+        <v>316</v>
       </c>
       <c r="D232" t="s">
         <v>11</v>
@@ -4869,13 +4986,13 @@
         <v>12</v>
       </c>
       <c r="B233" t="s">
-        <v>360</v>
+        <v>375</v>
       </c>
       <c r="C233" t="s">
-        <v>361</v>
+        <v>322</v>
       </c>
       <c r="D233" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="234">
@@ -4883,13 +5000,13 @@
         <v>12</v>
       </c>
       <c r="B234" t="s">
-        <v>362</v>
+        <v>376</v>
       </c>
       <c r="C234" t="s">
-        <v>363</v>
+        <v>324</v>
       </c>
       <c r="D234" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="235">
@@ -4897,13 +5014,13 @@
         <v>12</v>
       </c>
       <c r="B235" t="s">
-        <v>364</v>
+        <v>377</v>
       </c>
       <c r="C235" t="s">
-        <v>365</v>
+        <v>328</v>
       </c>
       <c r="D235" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="236">
@@ -4911,13 +5028,13 @@
         <v>12</v>
       </c>
       <c r="B236" t="s">
-        <v>366</v>
+        <v>378</v>
       </c>
       <c r="C236" t="s">
-        <v>367</v>
+        <v>330</v>
       </c>
       <c r="D236" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="237">
@@ -4925,13 +5042,13 @@
         <v>12</v>
       </c>
       <c r="B237" t="s">
-        <v>368</v>
+        <v>379</v>
       </c>
       <c r="C237" t="s">
-        <v>369</v>
+        <v>228</v>
       </c>
       <c r="D237" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="238">
@@ -4939,13 +5056,13 @@
         <v>12</v>
       </c>
       <c r="B238" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="C238" t="s">
-        <v>371</v>
+        <v>230</v>
       </c>
       <c r="D238" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="239">
@@ -4953,13 +5070,13 @@
         <v>12</v>
       </c>
       <c r="B239" t="s">
-        <v>372</v>
+        <v>381</v>
       </c>
       <c r="C239" t="s">
-        <v>373</v>
+        <v>232</v>
       </c>
       <c r="D239" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="240">
@@ -4967,13 +5084,13 @@
         <v>12</v>
       </c>
       <c r="B240" t="s">
-        <v>374</v>
+        <v>382</v>
       </c>
       <c r="C240" t="s">
-        <v>375</v>
+        <v>234</v>
       </c>
       <c r="D240" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="241">
@@ -4981,13 +5098,13 @@
         <v>12</v>
       </c>
       <c r="B241" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="C241" t="s">
-        <v>377</v>
+        <v>236</v>
       </c>
       <c r="D241" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="242">
@@ -4995,13 +5112,13 @@
         <v>12</v>
       </c>
       <c r="B242" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="C242" t="s">
-        <v>379</v>
+        <v>238</v>
       </c>
       <c r="D242" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="243">
@@ -5009,13 +5126,13 @@
         <v>12</v>
       </c>
       <c r="B243" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="C243" t="s">
-        <v>381</v>
+        <v>240</v>
       </c>
       <c r="D243" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="244">
@@ -5023,13 +5140,13 @@
         <v>12</v>
       </c>
       <c r="B244" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="C244" t="s">
-        <v>383</v>
+        <v>242</v>
       </c>
       <c r="D244" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="245">
@@ -5037,13 +5154,13 @@
         <v>12</v>
       </c>
       <c r="B245" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="C245" t="s">
-        <v>385</v>
+        <v>244</v>
       </c>
       <c r="D245" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="246">
@@ -5051,13 +5168,13 @@
         <v>12</v>
       </c>
       <c r="B246" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C246" t="s">
-        <v>387</v>
+        <v>246</v>
       </c>
       <c r="D246" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="247">
@@ -5065,10 +5182,10 @@
         <v>12</v>
       </c>
       <c r="B247" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C247" t="s">
-        <v>40</v>
+        <v>248</v>
       </c>
       <c r="D247" t="s">
         <v>11</v>
@@ -5076,13 +5193,13 @@
     </row>
     <row r="248">
       <c r="A248" t="s">
-        <v>389</v>
+        <v>12</v>
       </c>
       <c r="B248" t="s">
-        <v>9</v>
+        <v>390</v>
       </c>
       <c r="C248" t="s">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="D248" t="s">
         <v>11</v>
@@ -5093,10 +5210,10 @@
         <v>12</v>
       </c>
       <c r="B249" t="s">
-        <v>13</v>
+        <v>391</v>
       </c>
       <c r="C249" t="s">
-        <v>14</v>
+        <v>252</v>
       </c>
       <c r="D249" t="s">
         <v>11</v>
@@ -5107,10 +5224,10 @@
         <v>12</v>
       </c>
       <c r="B250" t="s">
-        <v>15</v>
+        <v>392</v>
       </c>
       <c r="C250" t="s">
-        <v>16</v>
+        <v>254</v>
       </c>
       <c r="D250" t="s">
         <v>11</v>
@@ -5121,10 +5238,10 @@
         <v>12</v>
       </c>
       <c r="B251" t="s">
-        <v>17</v>
+        <v>393</v>
       </c>
       <c r="C251" t="s">
-        <v>18</v>
+        <v>256</v>
       </c>
       <c r="D251" t="s">
         <v>11</v>
@@ -5135,13 +5252,13 @@
         <v>12</v>
       </c>
       <c r="B252" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="C252" t="s">
-        <v>391</v>
+        <v>258</v>
       </c>
       <c r="D252" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="253">
@@ -5149,13 +5266,13 @@
         <v>12</v>
       </c>
       <c r="B253" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="C253" t="s">
-        <v>393</v>
+        <v>260</v>
       </c>
       <c r="D253" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="254">
@@ -5163,13 +5280,13 @@
         <v>12</v>
       </c>
       <c r="B254" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="C254" t="s">
-        <v>395</v>
+        <v>262</v>
       </c>
       <c r="D254" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="255">
@@ -5177,13 +5294,13 @@
         <v>12</v>
       </c>
       <c r="B255" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C255" t="s">
-        <v>397</v>
+        <v>264</v>
       </c>
       <c r="D255" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="256">
@@ -5194,10 +5311,10 @@
         <v>398</v>
       </c>
       <c r="C256" t="s">
-        <v>399</v>
+        <v>38</v>
       </c>
       <c r="D256" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="257">
@@ -5205,27 +5322,27 @@
         <v>12</v>
       </c>
       <c r="B257" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C257" t="s">
-        <v>401</v>
+        <v>40</v>
       </c>
       <c r="D257" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="s">
-        <v>12</v>
+        <v>400</v>
       </c>
       <c r="B258" t="s">
-        <v>402</v>
+        <v>9</v>
       </c>
       <c r="C258" t="s">
-        <v>403</v>
+        <v>10</v>
       </c>
       <c r="D258" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="259">
@@ -5233,13 +5350,13 @@
         <v>12</v>
       </c>
       <c r="B259" t="s">
-        <v>404</v>
+        <v>13</v>
       </c>
       <c r="C259" t="s">
-        <v>405</v>
+        <v>14</v>
       </c>
       <c r="D259" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="260">
@@ -5247,13 +5364,13 @@
         <v>12</v>
       </c>
       <c r="B260" t="s">
-        <v>406</v>
+        <v>15</v>
       </c>
       <c r="C260" t="s">
-        <v>407</v>
+        <v>16</v>
       </c>
       <c r="D260" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="261">
@@ -5261,13 +5378,13 @@
         <v>12</v>
       </c>
       <c r="B261" t="s">
-        <v>408</v>
+        <v>17</v>
       </c>
       <c r="C261" t="s">
-        <v>409</v>
+        <v>18</v>
       </c>
       <c r="D261" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="262">
@@ -5275,10 +5392,10 @@
         <v>12</v>
       </c>
       <c r="B262" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="C262" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="D262" t="s">
         <v>48</v>
@@ -5289,10 +5406,10 @@
         <v>12</v>
       </c>
       <c r="B263" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="C263" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="D263" t="s">
         <v>48</v>
@@ -5303,10 +5420,10 @@
         <v>12</v>
       </c>
       <c r="B264" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="C264" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="D264" t="s">
         <v>48</v>
@@ -5317,10 +5434,10 @@
         <v>12</v>
       </c>
       <c r="B265" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="C265" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="D265" t="s">
         <v>48</v>
@@ -5331,10 +5448,10 @@
         <v>12</v>
       </c>
       <c r="B266" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="C266" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="D266" t="s">
         <v>48</v>
@@ -5345,10 +5462,10 @@
         <v>12</v>
       </c>
       <c r="B267" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="C267" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="D267" t="s">
         <v>48</v>
@@ -5359,10 +5476,10 @@
         <v>12</v>
       </c>
       <c r="B268" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="C268" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="D268" t="s">
         <v>48</v>
@@ -5373,10 +5490,10 @@
         <v>12</v>
       </c>
       <c r="B269" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="C269" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="D269" t="s">
         <v>48</v>
@@ -5387,10 +5504,10 @@
         <v>12</v>
       </c>
       <c r="B270" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
       <c r="C270" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
       <c r="D270" t="s">
         <v>48</v>
@@ -5401,10 +5518,10 @@
         <v>12</v>
       </c>
       <c r="B271" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
       <c r="C271" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="D271" t="s">
         <v>48</v>
@@ -5415,10 +5532,10 @@
         <v>12</v>
       </c>
       <c r="B272" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="C272" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="D272" t="s">
         <v>48</v>
@@ -5429,10 +5546,10 @@
         <v>12</v>
       </c>
       <c r="B273" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="C273" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="D273" t="s">
         <v>48</v>
@@ -5443,12 +5560,404 @@
         <v>12</v>
       </c>
       <c r="B274" t="s">
+        <v>425</v>
+      </c>
+      <c r="C274" t="s">
+        <v>426</v>
+      </c>
+      <c r="D274" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="s">
+        <v>12</v>
+      </c>
+      <c r="B275" t="s">
+        <v>427</v>
+      </c>
+      <c r="C275" t="s">
+        <v>40</v>
+      </c>
+      <c r="D275" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="s">
+        <v>428</v>
+      </c>
+      <c r="B276" t="s">
+        <v>9</v>
+      </c>
+      <c r="C276" t="s">
+        <v>10</v>
+      </c>
+      <c r="D276" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="s">
+        <v>12</v>
+      </c>
+      <c r="B277" t="s">
+        <v>13</v>
+      </c>
+      <c r="C277" t="s">
+        <v>14</v>
+      </c>
+      <c r="D277" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="s">
+        <v>12</v>
+      </c>
+      <c r="B278" t="s">
+        <v>15</v>
+      </c>
+      <c r="C278" t="s">
+        <v>16</v>
+      </c>
+      <c r="D278" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="s">
+        <v>12</v>
+      </c>
+      <c r="B279" t="s">
+        <v>17</v>
+      </c>
+      <c r="C279" t="s">
+        <v>18</v>
+      </c>
+      <c r="D279" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="s">
+        <v>12</v>
+      </c>
+      <c r="B280" t="s">
+        <v>429</v>
+      </c>
+      <c r="C280" t="s">
+        <v>430</v>
+      </c>
+      <c r="D280" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="s">
+        <v>12</v>
+      </c>
+      <c r="B281" t="s">
+        <v>431</v>
+      </c>
+      <c r="C281" t="s">
+        <v>432</v>
+      </c>
+      <c r="D281" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="s">
+        <v>12</v>
+      </c>
+      <c r="B282" t="s">
+        <v>433</v>
+      </c>
+      <c r="C282" t="s">
         <v>434</v>
       </c>
-      <c r="C274" t="s">
+      <c r="D282" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="s">
+        <v>12</v>
+      </c>
+      <c r="B283" t="s">
+        <v>435</v>
+      </c>
+      <c r="C283" t="s">
+        <v>436</v>
+      </c>
+      <c r="D283" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="s">
+        <v>12</v>
+      </c>
+      <c r="B284" t="s">
+        <v>437</v>
+      </c>
+      <c r="C284" t="s">
+        <v>438</v>
+      </c>
+      <c r="D284" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="s">
+        <v>12</v>
+      </c>
+      <c r="B285" t="s">
+        <v>439</v>
+      </c>
+      <c r="C285" t="s">
+        <v>440</v>
+      </c>
+      <c r="D285" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="s">
+        <v>12</v>
+      </c>
+      <c r="B286" t="s">
+        <v>441</v>
+      </c>
+      <c r="C286" t="s">
+        <v>442</v>
+      </c>
+      <c r="D286" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="s">
+        <v>12</v>
+      </c>
+      <c r="B287" t="s">
+        <v>443</v>
+      </c>
+      <c r="C287" t="s">
+        <v>444</v>
+      </c>
+      <c r="D287" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="s">
+        <v>12</v>
+      </c>
+      <c r="B288" t="s">
+        <v>445</v>
+      </c>
+      <c r="C288" t="s">
+        <v>446</v>
+      </c>
+      <c r="D288" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="s">
+        <v>12</v>
+      </c>
+      <c r="B289" t="s">
+        <v>447</v>
+      </c>
+      <c r="C289" t="s">
+        <v>448</v>
+      </c>
+      <c r="D289" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="s">
+        <v>12</v>
+      </c>
+      <c r="B290" t="s">
+        <v>449</v>
+      </c>
+      <c r="C290" t="s">
+        <v>450</v>
+      </c>
+      <c r="D290" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="s">
+        <v>12</v>
+      </c>
+      <c r="B291" t="s">
+        <v>451</v>
+      </c>
+      <c r="C291" t="s">
+        <v>452</v>
+      </c>
+      <c r="D291" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="s">
+        <v>12</v>
+      </c>
+      <c r="B292" t="s">
+        <v>453</v>
+      </c>
+      <c r="C292" t="s">
+        <v>454</v>
+      </c>
+      <c r="D292" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="s">
+        <v>12</v>
+      </c>
+      <c r="B293" t="s">
+        <v>455</v>
+      </c>
+      <c r="C293" t="s">
+        <v>456</v>
+      </c>
+      <c r="D293" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="s">
+        <v>12</v>
+      </c>
+      <c r="B294" t="s">
+        <v>457</v>
+      </c>
+      <c r="C294" t="s">
+        <v>458</v>
+      </c>
+      <c r="D294" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="s">
+        <v>12</v>
+      </c>
+      <c r="B295" t="s">
+        <v>459</v>
+      </c>
+      <c r="C295" t="s">
+        <v>460</v>
+      </c>
+      <c r="D295" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="s">
+        <v>12</v>
+      </c>
+      <c r="B296" t="s">
+        <v>461</v>
+      </c>
+      <c r="C296" t="s">
+        <v>462</v>
+      </c>
+      <c r="D296" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="s">
+        <v>12</v>
+      </c>
+      <c r="B297" t="s">
+        <v>463</v>
+      </c>
+      <c r="C297" t="s">
+        <v>464</v>
+      </c>
+      <c r="D297" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="s">
+        <v>12</v>
+      </c>
+      <c r="B298" t="s">
+        <v>465</v>
+      </c>
+      <c r="C298" t="s">
+        <v>466</v>
+      </c>
+      <c r="D298" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="s">
+        <v>12</v>
+      </c>
+      <c r="B299" t="s">
+        <v>467</v>
+      </c>
+      <c r="C299" t="s">
+        <v>468</v>
+      </c>
+      <c r="D299" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="s">
+        <v>12</v>
+      </c>
+      <c r="B300" t="s">
+        <v>469</v>
+      </c>
+      <c r="C300" t="s">
+        <v>470</v>
+      </c>
+      <c r="D300" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="s">
+        <v>12</v>
+      </c>
+      <c r="B301" t="s">
+        <v>471</v>
+      </c>
+      <c r="C301" t="s">
+        <v>472</v>
+      </c>
+      <c r="D301" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="s">
+        <v>12</v>
+      </c>
+      <c r="B302" t="s">
+        <v>473</v>
+      </c>
+      <c r="C302" t="s">
         <v>40</v>
       </c>
-      <c r="D274" t="s">
+      <c r="D302" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>